<commit_message>
Fixing bug for Slim_go
</commit_message>
<xml_diff>
--- a/Project_Output/POIs_sorted.xlsx
+++ b/Project_Output/POIs_sorted.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">uniprotswissprot</t>
   </si>
@@ -41,6 +41,51 @@
     <t xml:space="preserve">Go_count_PPI2</t>
   </si>
   <si>
+    <t xml:space="preserve">Q9UPP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHD finger protein 8 [Source:HGNC Symbol;Acc:HGNC:20672]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHF8_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET1A_HUMAN, HCFC1_HUMAN, E2F1_HUMAN, RBL1_HUMAN, RS3_HUMAN, H14_HUMAN, Q15156_HUMAN, RARA_HUMAN, NOTC1_HUMAN, SUH_HUMAN, NCOR2_HUMAN, KDM1A_HUMAN, FRYL_HUMAN, HMGN2_HUMAN, H15_HUMAN, RARA_HUMAN.ZBT16_HUMAN, PB1_HUMAN, SMCA4_HUMAN, RPAP1_HUMAN, H31_HUMAN, WDR5_HUMAN, ASH2L_HUMAN, ZN711_HUMAN, RPB1_HUMAN, RPB3_HUMAN, TAF1_HUMAN, H31T_HUMAN, MAML1_HUMAN, CDC27_HUMAN, CDC23_HUMAN, APC1_HUMAN, APC5_HUMAN, CDC26_HUMAN, APC4_HUMAN, CDC16_HUMAN, APC7_HUMAN, ANC2_HUMAN, CDC20_HUMAN, FZR1_HUMAN, SUMO2_HUMAN, CCNA2_HUMAN, CENPB_HUMAN, INCE_HUMAN, IF6_HUMAN, XPC_HUMAN, H2B2E_HUMAN, H2AY_HUMAN, RT27_HUMAN, HNRPU_HUMAN, TDIF2_HUMAN, NIP7_HUMAN, NOL8_HUMAN, RIF1_HUMAN, RCC2_HUMAN, THA11_HUMAN, RT35_HUMAN, RT15_HUMAN, REN3A_HUMAN, BRAT1_HUMAN, H3C_HUMAN, BLM_HUMAN, UBP7_HUMAN, OGT1_HUMAN, CC14B_HUMAN, EGLN3_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBC9_HUMAN, MDC1_HUMAN, RMI2_HUMAN, TOP3A_HUMAN, RMI1_HUMAN, DNA2_HUMAN, RA51B_HUMAN, RA51D_HUMAN, RA51C_HUMAN, XRCC2_HUMAN, SPIDR_HUMAN, AP2A_HUMAN, NPM_HUMAN.RARA_HUMAN, CH60_HUMAN, NOP2_HUMAN, MYBB_HUMAN, RUNX1_HUMAN, PML_HUMAN.RARA_HUMAN, HM20B_HUMAN, PF21A_HUMAN, HDAC2_HUMAN, RCOR1_HUMAN, HDAC1_HUMAN, GABPA_HUMAN, TFB1M_HUMAN, GABP1_HUMAN, NRF1_HUMAN, PPRC1_HUMAN, TFB2M_HUMAN, SNW1_HUMAN, HIF1A_HUMAN, JAG1_HUMAN, JAG2_HUMAN, DLK1_HUMAN, ITCH_HUMAN, NUMB_HUMAN, CBP_HUMAN, CCND1_HUMAN, MD2L1_HUMAN, BUB3_HUMAN, BUB1B_HUMAN, CDK1_HUMAN, FBX5_HUMAN, SAE2_HUMAN, SAE1_HUMAN, BRWD1_HUMAN, BAP1_HUMAN, UBP44_HUMAN, SUMO1_HUMAN, REST_HUMAN, RXRA_HUMAN, CALM1_HUMAN.CALM3_HUMAN, KPBB_HUMAN, PHKG1_HUMAN, KPB1_HUMAN, PPARG_HUMAN, HDAC3_HUMAN, NCOR1_HUMAN, AURKB_HUMAN, BOREA_HUMAN, BIRC5_HUMAN, RUVB1_HUMAN, RBBP7_HUMAN, HJURP_HUMAN, RBBP4_HUMAN, CALM3_HUMAN, PPB1_HUMAN, DLL1_HUMAN, AURKC_HUMAN, CDK2_HUMAN, SNF5_HUMAN, SMCE1_HUMAN, ESR2_HUMAN, ZNF14_HUMAN, CNTN1_HUMAN, CTBP1_HUMAN, MINT_HUMAN, CTIP_HUMAN, HEY1_HUMAN, DTX1_HUMAN, CNTN6_HUMAN, MK08_HUMAN, TYY1_HUMAN, HES1_HUMAN, DNER_HUMAN, JUND_HUMAN, ATF2_HUMAN, ESR1_HUMAN, TERF2_HUMAN, FANCJ_HUMAN, NSE3_HUMAN, HDAC4_HUMAN, DAXX_HUMAN, EVI5_HUMAN, DVL1_HUMAN, SIR1_HUMAN, NECD_HUMAN, SMRC1_HUMAN, SMRD1_HUMAN, SMRC2_HUMAN, RB_HUMAN, ABL1_HUMAN, TFDP1_HUMAN, HSPB1_HUMAN, E2F4_HUMAN, RBL2_HUMAN, CYC_HUMAN, SUMO3_HUMAN, P53_HUMAN, RFA1_HUMAN, EP300_HUMAN, ETS1_HUMAN, ETS2_HUMAN, ACTS_HUMAN, ITB4_HUMAN, STAT6_HUMAN, ANDR_HUMAN, TF2H4_HUMAN, ERCC3_HUMAN, TF2H1_HUMAN, ERCC2_HUMAN, TF2H2_HUMAN, TF2H3_HUMAN, CIR1_HUMAN, FHL1_HUMAN, NOTC2_HUMAN, MAML2_HUMAN, MAML3_HUMAN, LEF1_HUMAN, NFKB1_HUMAN, NOTC4_HUMAN, MK01_HUMAN, FRS3_HUMAN, ID2_HUMAN, E2F5_HUMAN, SMAD3_HUMAN, SMAD4_HUMAN, SMAD2_HUMAN, SKIL_HUMAN, GRB2_HUMAN, RELB_HUMAN, IKBA_HUMAN, NOTC1_HUMAN.NOTC2_HUMAN.NOTC3_HUMAN.NOTC4_HUMAN, DTX1_HUMAN.DTX2_HUMAN.DTX3_HUMAN, SKIL_HUMAN.SKI_HUMAN.TLE1_HUMAN.TLE2_HUMAN.TLE3_HUMAN.TLE4_HUMAN, ZMY10_HUMAN, EED_HUMAN, SMRD3_HUMAN, ARF_HUMAN.CDN2A_HUMAN, FBW1A_HUMAN, BMI1_HUMAN, BIRC3_HUMAN, SQSTM_HUMAN, BECN1_HUMAN, A4_HUMAN, GRAB_HUMAN, FUT7_HUMAN, MYH14_HUMAN, SUZ12_HUMAN, BMP2_HUMAN, PHF8_HUMAN, DDIT3_HUMAN, ARNT_HUMAN, PIN1_HUMAN, SRC_HUMAN, KPCD1_HUMAN, PHB_HUMAN, TF65_HUMAN, TRAF3_HUMAN, FOS_HUMAN, C2TA_HUMAN, H2B3B_HUMAN, NEMO_HUMAN, RASF1_HUMAN, MYD88_HUMAN, CYLD_HUMAN, IKKA_HUMAN, IKKB_HUMAN, RING2_HUMAN, CEBPD_HUMAN, TSC2_HUMAN, MK09_HUMAN, EGLN1_HUMAN, EZH2_HUMAN, BAX_HUMAN, BIRC2_HUMAN, MRP1_HUMAN, EGLN2_HUMAN, BRD7_HUMAN, LYL1_HUMAN, DFB4A_HUMAN, MK10_HUMAN, TRAF6_HUMAN, MAVS_HUMAN, PRS10_HUMAN, CUL1_HUMAN, ADRB2_HUMAN, CREB1_HUMAN, UBP11_HUMAN, EPAS1_HUMAN, SKP1_HUMAN, BYST_HUMAN, TMOD3_HUMAN, XIAP_HUMAN, 1433E_HUMAN, IRF1_HUMAN, ULK1_HUMAN, TRAF2_HUMAN, CEBPA_HUMAN, KLF4_HUMAN, IFIT1_HUMAN, H2A2C_HUMAN, MK12_HUMAN, UBB_HUMAN, NEDD8_HUMAN, SEC63_HUMAN, TRM2A_HUMAN, KEAP1_HUMAN, IF16_HUMAN, NR2E3_HUMAN, H32_HUMAN, RXRG_HUMAN, GDIB_HUMAN, PPARD_HUMAN, SIN3A_HUMAN, KRT35_HUMAN, KRT85_HUMAN, TBP_HUMAN, SSXT_HUMAN, PP1G_HUMAN, MAX_HUMAN, ZN121_HUMAN, MYC_HUMAN, MCM7_HUMAN, CCAR2_HUMAN, PDCD5_HUMAN, TRAF4_HUMAN, CAF1A_HUMAN, PO4F2_HUMAN, TAL1_HUMAN, PCSK5_HUMAN, RBBP5_HUMAN, PAXI1_HUMAN, PAGR1_HUMAN, MSH2_HUMAN, RMP_HUMAN, RRP1B_HUMAN, RNF10_HUMAN, ZN333_HUMAN, ARI1A_HUMAN, UBP16_HUMAN, ZBT16_HUMAN, ARI1B_HUMAN, RRP5_HUMAN, MED25_HUMAN, ING4_HUMAN, NREP_HUMAN, SETX_HUMAN, SMN_HUMAN, XRN2_HUMAN, ANM5_HUMAN, SNAI1_HUMAN, NIBAN_HUMAN, MGN_HUMAN, CASC3_HUMAN, RBM8A_HUMAN, PRP18_HUMAN, SENP3_HUMAN, H2AX_HUMAN, TRIP6_HUMAN, REL_HUMAN, CDX2_HUMAN, LNX1_HUMAN, RAGP1_HUMAN, SENP2_HUMAN, ZDH15_HUMAN, PACR_HUMAN, K1C15_HUMAN, RPR1B_HUMAN, RPR1A_HUMAN, NECA2_HUMAN, WWP2_HUMAN, EME1_HUMAN, RBM39_HUMAN, EF1D_HUMAN, NASP_HUMAN, TRADD_HUMAN, ATX1_HUMAN, ATX1L_HUMAN, RAD51_HUMAN, TSN4_HUMAN, ZN124_HUMAN, APBP2_HUMAN, KIF6_HUMAN, NOG1_HUMAN, HD_HUMAN, KCTD9_HUMAN, CALR_HUMAN, DNSL3_HUMAN, RBM44_HUMAN, ACTN2_HUMAN, SGF29_HUMAN, INCA1_HUMAN, RS19_HUMAN, RUXF_HUMAN, ARID2_HUMAN, NBN_HUMAN, ATM_HUMAN, KAT2B_HUMAN, PRS4_HUMAN, HEM1_HUMAN, ZBT39_HUMAN, CDN1A_HUMAN, ADDG_HUMAN, GSC2_HUMAN, NCOA3_HUMAN, CARM1_HUMAN, NF2L2_HUMAN, EHMT2_HUMAN, PSA3_HUMAN, UTP18_HUMAN, HCFC2_HUMAN, KMT2A_HUMAN, MEN1_HUMAN, SAT1_HUMAN, STAT3_HUMAN, CTSR1_HUMAN, KANL1_HUMAN, CDN1B_HUMAN, PLLP_HUMAN, FBLI1_HUMAN, WASC3_HUMAN, SIR2_HUMAN, OPA3_HUMAN, RPC6_HUMAN, PPID_HUMAN, DPF3_HUMAN, H2A1H_HUMAN, H2A1B_HUMAN, MDM2_HUMAN, LERL1_HUMAN, CDYL_HUMAN, CD79A_HUMAN, CCNB1_HUMAN, N62CL_HUMAN, MDM4_HUMAN, A0A024QZ45_HUMAN.FANCJ_HUMAN, SPY2_HUMAN, MTG8_HUMAN.RUNX1_HUMAN, LZTS2_HUMAN, TCTP_HUMAN, FBXW7_HUMAN, KIF22_HUMAN, BTG3_HUMAN, PARP1_HUMAN, DYR1A_HUMAN, SP140_HUMAN, ZN496_HUMAN, HNRPK_HUMAN, CTNB1_HUMAN, PITX2_HUMAN, YBOX1_HUMAN, NUCL_HUMAN, A0A087WYV2_HUMAN.IQCAL_HUMAN, GCC1_HUMAN, ERG28_HUMAN, IGBP1_HUMAN, ATG9A_HUMAN, MD2BP_HUMAN, SIAH1_HUMAN, RD23B_HUMAN, CETN2_HUMAN, CREB3_HUMAN, ZHANG_HUMAN, NRIP1_HUMAN, ANXA7_HUMAN, TE2IP_HUMAN, LANC2_HUMAN, BICL1_HUMAN, CDC5L_HUMAN, BAZ1B_HUMAN, DJC21_HUMAN, DNJA3_HUMAN, CR3L3_HUMAN, RFC5_HUMAN, MYO5C_HUMAN, TNR5_HUMAN, CCNK_HUMAN, CDK12_HUMAN, VIGLN_HUMAN, CENPR_HUMAN, LZTS1_HUMAN, FHL2_HUMAN, REQU_HUMAN, ACTB_HUMAN, AP2B1_HUMAN, RUS1_HUMAN, PKN1_HUMAN, KPCB_HUMAN, CENPA_HUMAN, KAT2A_HUMAN, AXIN1_HUMAN, PRP31_HUMAN, COX8A_HUMAN, MMS19_HUMAN, MIC60_HUMAN, PELP1_HUMAN, PSB3_HUMAN, NCK1_HUMAN, SMCA2_HUMAN, CC190_HUMAN, CBX5_HUMAN, TUFT1_HUMAN, COX17_HUMAN, FHL3_HUMAN, FIGL1_HUMAN, ELMO3_HUMAN, H2B1M_HUMAN, CHD1_HUMAN, MSL1_HUMAN, LSME1_HUMAN, MD2L2_HUMAN, FA35A_HUMAN, KMT2D_HUMAN, NCOA6_HUMAN, RXRB_HUMAN, RT18B_HUMAN, PCBP1_HUMAN, CBX1_HUMAN, GATA1_HUMAN, NFKB2_HUMAN, PP4C_HUMAN, RT29_HUMAN, RED_HUMAN, CTBP2_HUMAN, ZN217_HUMAN, KLH20_HUMAN, LIGO1_HUMAN, E2AK2_HUMAN, ASXL1_HUMAN, NR1H3_HUMAN, RIR1_HUMAN, SBP1_HUMAN, PLCZ1_HUMAN, IF1AX_HUMAN, TBX2_HUMAN, CD2B2_HUMAN, TOPB1_HUMAN, CDC45_HUMAN, RITA1_HUMAN, DYH10_HUMAN, ZN829_HUMAN, MBIP1_HUMAN, MUC18_HUMAN, PLAK_HUMAN, GNAS1_HUMAN, ARP3_HUMAN, CATA_HUMAN, PPIE_HUMAN, ZBT17_HUMAN, KDM4A_HUMAN, A0A024R4Z9_HUMAN.G5E933_HUMAN.MTMR5_HUMAN, G6PD_HUMAN, K2C6A_HUMAN, PA2G4_HUMAN, LECT2_HUMAN, DPY30_HUMAN, K22O_HUMAN, KNL1_HUMAN, AGO2_HUMAN, RACK1_HUMAN, LMTD1_HUMAN, ZBED1_HUMAN, UFD1_HUMAN, MCM2_HUMAN, NMI_HUMAN, DPF1_HUMAN, T2H2L_HUMAN, HIRP3_HUMAN, OS9_HUMAN, TFP11_HUMAN, MSRB3_HUMAN, PHF19_HUMAN, RPAB5_HUMAN, CAN3_HUMAN, CRCM_HUMAN, DISC1_HUMAN, COMT_HUMAN, RS27_HUMAN, KIFC3_HUMAN, RLP24_HUMAN, T22D1_HUMAN, LRIF1_HUMAN, GNPAT_HUMAN, ATG5_HUMAN, UBXN1_HUMAN, SH2B1_HUMAN, K2C8_HUMAN, PIAS4_HUMAN, ZN641_HUMAN, VWC2_HUMAN, ABH15_HUMAN, CLSPN_HUMAN, TF2H5_HUMAN, PRD15_HUMAN, ZMYM3_HUMAN, HEXDC_HUMAN, F264_HUMAN, STAT1_HUMAN, RTF1_HUMAN, CDC73_HUMAN, LEO1_HUMAN, CTR9_HUMAN, PAF1_HUMAN, NACA_HUMAN, VPS53_HUMAN, EVA1A_HUMAN, GOGA2_HUMAN, VRK1_HUMAN, MERL_HUMAN, PTEN_HUMAN, H2A2B_HUMAN, DDB2_HUMAN, HAUS6_HUMAN, BATF_HUMAN, TPSNR_HUMAN, TDRKH_HUMAN, T2FB_HUMAN, SMCA5_HUMAN, CHD3_HUMAN, HELZ_HUMAN, MRGBP_HUMAN, SRRM4_HUMAN, PR20D_HUMAN.PR20E_HUMAN, ZCH14_HUMAN, CISY_HUMAN, WRN_HUMAN, CDK8_HUMAN, RECQ5_HUMAN, CRYAB_HUMAN, ZNF71_HUMAN, AP2M1_HUMAN, UHRF2_HUMAN, TNKS1_HUMAN, PSB10_HUMAN, TCF20_HUMAN, CE290_HUMAN, ARF6_HUMAN, PSPC1_HUMAN, NGRN_HUMAN, NLGN3_HUMAN, SLU7_HUMAN, PCGF2_HUMAN, TIF1A_HUMAN, SEC13_HUMAN, MED1_HUMAN, CXXC1_HUMAN, PIHD1_HUMAN, SF3B2_HUMAN, FYV1_HUMAN, WWOX_HUMAN, OPA1_HUMAN, EF1G_HUMAN, MBD4_HUMAN, CK049_HUMAN, MEX3C_HUMAN, NDST4_HUMAN, SATB1_HUMAN, ZN436_HUMAN, XPF_HUMAN, MPH6_HUMAN, MOFA1_HUMAN, GFI1B_HUMAN, CDK13_HUMAN, DICER_HUMAN, CCNC_HUMAN, MED27_HUMAN, MYOM2_HUMAN, HOMEZ_HUMAN, TBL1X_HUMAN, A0A024RBS3_HUMAN.NCOR2_HUMAN, SYNE1_HUMAN.SYNE2_HUMAN, PCH2_HUMAN, HAUS8_HUMAN, HS90B_HUMAN, KLH14_HUMAN, H2B1N_HUMAN, CLOCK_HUMAN, GOGA5_HUMAN, CD123_HUMAN, SPB1_HUMAN, VHL_HUMAN, U119A_HUMAN, KCTD6_HUMAN, KT33A_HUMAN, BRD1_HUMAN, NCKPL_HUMAN, UBE2S_HUMAN, HMGA2_HUMAN, TR10B_HUMAN, U520_HUMAN, BMAL1_HUMAN, MCRS1_HUMAN, DP13A_HUMAN, DHX58_HUMAN, MTF2_HUMAN.Q96G26_HUMAN, ZBT24_HUMAN, RASF2_HUMAN, TCEA1_HUMAN, NUP62_HUMAN, CBX8_HUMAN, SKAP_HUMAN, BIG1_HUMAN, GORS2_HUMAN, UQCC2_HUMAN, TRI27_HUMAN, NSE4A_HUMAN, HASP_HUMAN, IMA7_HUMAN, EHMT1_HUMAN, HERC5_HUMAN, FBXL6_HUMAN, AIRE_HUMAN, SNP29_HUMAN, FUS_HUMAN, ITBP2_HUMAN, RHG28_HUMAN, MAK_HUMAN, MCPH1_HUMAN, ALPK3_HUMAN, CHD7_HUMAN, RAB43_HUMAN, RT06_HUMAN, AURKA_HUMAN, HNRPD_HUMAN, CIAO1_HUMAN, DPOD1_HUMAN, MIP18_HUMAN, RBPMS_HUMAN, ZO2_HUMAN, EXOC7_HUMAN, UBC_HUMAN, PRAF2_HUMAN, EWS_HUMAN, NSD3_HUMAN, PDIA4_HUMAN, NPM2_HUMAN, DDX3X_HUMAN, CCD14_HUMAN, LMBL2_HUMAN, BANP_HUMAN, PSB1_HUMAN, TP53B_HUMAN, SPICE_HUMAN, PNPH_HUMAN, TRBP2_HUMAN, HAT1_HUMAN, ZN622_HUMAN, NPM_HUMAN, RN125_HUMAN, RALA_HUMAN, PKCB1_HUMAN, WNK4_HUMAN, BCL6_HUMAN, RCOR2_HUMAN, FOXJ2_HUMAN, SNF8_HUMAN, TBA4A_HUMAN, GCR_HUMAN, POGZ_HUMAN, TIF1B_HUMAN, EFC4B_HUMAN, MYOG_HUMAN, 1433Z_HUMAN, MEP50_HUMAN, CDK4_HUMAN, TSKS_HUMAN, K2C78_HUMAN, C2CD3_HUMAN, CHD4_HUMAN, QCR6_HUMAN, ANXA1_HUMAN.B5BU38_HUMAN, EGR2_HUMAN, REXO1_HUMAN, SVIL_HUMAN, YETS4_HUMAN, BAG3_HUMAN, K2C80_HUMAN, NOSTN_HUMAN, CAC1A_HUMAN, MTUS1_HUMAN, MOV10_HUMAN, DHX9_HUMAN, PRKDC_HUMAN, TOP2B_HUMAN, RB15B_HUMAN, H4_HUMAN, NR2E1_HUMAN, SYF1_HUMAN, ERCC6_HUMAN, NRBF2_HUMAN, APEX1_HUMAN, 2AAA_HUMAN, RENT2_HUMAN, RENT1_HUMAN, SRRM1_HUMAN, U5S1_HUMAN, HOT_HUMAN, Q86WV8_HUMAN, CFLAR_HUMAN, TNR6_HUMAN, TDRD3_HUMAN, RBM6_HUMAN, VA0D2_HUMAN, CBX4_HUMAN, M3K14_HUMAN, CSN6_HUMAN, LRRK2_HUMAN, TRDN_HUMAN, HSP77_HUMAN, A4PIV7_HUMAN, AHSA1_HUMAN, MK07_HUMAN, MASU1_HUMAN, H10_HUMAN, PTCD3_HUMAN, GPS2_HUMAN, THOC5_HUMAN, GIMA1_HUMAN, HEMGN_HUMAN, MPP8_HUMAN, NUP50_HUMAN, TERF1_HUMAN, H2B1J_HUMAN, MLH3_HUMAN, SUN2_HUMAN, CEP63_HUMAN, RABE1_HUMAN, 1433B_HUMAN, FUMH_HUMAN, KDM5B_HUMAN, GNL3_HUMAN, TERT_HUMAN, MALT1_HUMAN, H2B2C_HUMAN, SUV91_HUMAN, EIF3E_HUMAN, OPTN_HUMAN, TIMP1_HUMAN, HNRPF_HUMAN, ZN423_HUMAN, RL34_HUMAN, DMAP1_HUMAN, CPSF5_HUMAN, KAT6A_HUMAN, CSK21_HUMAN, CCR1_HUMAN, EGFR_HUMAN, HXA1_HUMAN, FIBP_HUMAN, LMBL1_HUMAN, NRBP_HUMAN, BCAS3_HUMAN.BCAS4_HUMAN, DBF4B_HUMAN, SNORC_HUMAN, NCOA1_HUMAN, CCDB1_HUMAN, STX5_HUMAN, MAF1_HUMAN, SYK_HUMAN, SPT5H_HUMAN, CBX3_HUMAN, T2FA_HUMAN, CRX_HUMAN, DBLOH_HUMAN, PAWR_HUMAN, ERR1_HUMAN, P53_HUMAN.RARA_HUMAN, FWCH1_HUMAN, DCP1A_HUMAN, REN3B_HUMAN, PR40A_HUMAN, CLC10_HUMAN, BICD2_HUMAN, AKT1_HUMAN, ZN674_HUMAN, SOMA_HUMAN, K2C71_HUMAN, SH3G1_HUMAN, KMT2C_HUMAN, SF3A3_HUMAN, IF4A2_HUMAN, K22E_HUMAN, CSK2B_HUMAN, RFA2_HUMAN, RFA3_HUMAN, FRIH_HUMAN, MARF1_HUMAN, ERR3_HUMAN, DYH2_HUMAN, RGS20_HUMAN, CDCA5_HUMAN, LA_HUMAN, PRP8_HUMAN, NUP54_HUMAN, UBE2W_HUMAN, H12_HUMAN, TFAP4_HUMAN, GEM_HUMAN, ARIP4_HUMAN, H2B1L_HUMAN, GNPTA_HUMAN, SET1B_HUMAN, NVL_HUMAN, D0VY79_HUMAN, K2C79_HUMAN, MTMRD_HUMAN, RBG1L_HUMAN, NH2L1_HUMAN, K1C17_HUMAN, SMBT1_HUMAN, CEP76_HUMAN, RL36_HUMAN, NFAC1_HUMAN, RS20_HUMAN, RL4_HUMAN, RL5_HUMAN, RM18_HUMAN, FEN1_HUMAN, EIF3K_HUMAN, SHOC2_HUMAN, R3HD4_HUMAN, H11_HUMAN, TNR1A_HUMAN, UBP28_HUMAN, AQR_HUMAN, RIR2_HUMAN, RS16_HUMAN, A8K3Z6_HUMAN, UBP25_HUMAN, GT253_HUMAN, NRAC_HUMAN, ZN695_HUMAN, RASF9_HUMAN, RN220_HUMAN, PNRC2_HUMAN, ATN1_HUMAN, MS18B_HUMAN, INP5K_HUMAN, GARS_HUMAN, NDRG1_HUMAN, HNRPC_HUMAN, THOC4_HUMAN, ROA1_HUMAN, RAC1_HUMAN, H2B2F_HUMAN, ACTC_HUMAN, JTB_HUMAN, PA1B3_HUMAN, IMA3_HUMAN, PSMD1_HUMAN, SKP2_HUMAN, PIGT_HUMAN, CUL4B_HUMAN, CUL4A_HUMAN, PHF20_HUMAN, PQBP1_HUMAN, CPSF3_HUMAN, UBA3_HUMAN, TSYL5_HUMAN, FLIP1_HUMAN, DZIP3_HUMAN, IQGA2_HUMAN, PRS6B_HUMAN, GA45A_HUMAN, ANM6_HUMAN, 1433F_HUMAN, TXNL1_HUMAN, TAF3_HUMAN, CETN3_HUMAN, ML12A_HUMAN, IF4G3_HUMAN, HNF4G_HUMAN, ADIP_HUMAN, SMAD9_HUMAN, ATF4_HUMAN, TAB1_HUMAN, BC11B_HUMAN, VATB1_HUMAN, MAPK3_HUMAN, ALX1_HUMAN, CHD8_HUMAN, AKAP9_HUMAN, SMG1_HUMAN, NXF1_HUMAN, FGF14_HUMAN, BRMS1_HUMAN, VAPB_HUMAN, P85A_HUMAN, ARF_HUMAN, MYT1_HUMAN, ATX7_HUMAN, TRI16_HUMAN, ATRX_HUMAN, KAT6B_HUMAN, BACD2_HUMAN, EXOS5_HUMAN, TNNT2_HUMAN, SSRB_HUMAN, BTAF1_HUMAN, S10A8_HUMAN, EMAL5_HUMAN, RL40_HUMAN.UBC_HUMAN, PTN4_HUMAN, ZSC29_HUMAN, RHOH_HUMAN, SNIP1_HUMAN, MAPK2_HUMAN, IF5_HUMAN, NAB2_HUMAN, MYB_HUMAN, Z512B_HUMAN, ARI5A_HUMAN, HNRPL_HUMAN, VDAC1_HUMAN, ML12B_HUMAN, RERE_HUMAN, TEAD3_HUMAN, FYN_HUMAN, ZN410_HUMAN, PRGC1_HUMAN, K2C75_HUMAN, PRS8_HUMAN, PSA6_HUMAN, HS71B_HUMAN.HSP77_HUMAN, NEP_HUMAN, ACSF2_HUMAN, FAM9A_HUMAN, NEK2_HUMAN, AKAP8_HUMAN, RPRD2_HUMAN, APAF_HUMAN, PCNA_HUMAN, FOXO3_HUMAN, K1C39_HUMAN, 1B42_HUMAN, VIME_HUMAN, CBX2_HUMAN, VP37B_HUMAN, PDLI7_HUMAN, UBP19_HUMAN, TEKT4_HUMAN, K2C6B_HUMAN, PARP2_HUMAN, RBP2_HUMAN, KANL2_HUMAN, HGS_HUMAN, CBR1_HUMAN, SDS3_HUMAN, DFFA_HUMAN, NCOA2_HUMAN, MATK_HUMAN, ANKS3_HUMAN, AF10_HUMAN, ZSA5B_HUMAN, IF4A3_HUMAN, RNPS1_HUMAN, SMG5_HUMAN, PP1A_HUMAN, PRP19_HUMAN, DAAF4_HUMAN, AIPL1_HUMAN, TRAK1_HUMAN, NEK9_HUMAN, KRA93_HUMAN, DPB1_HUMAN, ROBO2_HUMAN, LMNA_HUMAN, TEFF2_HUMAN, VWF_HUMAN, HSP74_HUMAN, GCP4_HUMAN, LIRB2_HUMAN, NR2C1_HUMAN, K2C6C_HUMAN, KMT2B_HUMAN, HNRPQ_HUMAN, TGIF1_HUMAN, HSF2_HUMAN, ARHG7_HUMAN, PHC3_HUMAN, TADA3_HUMAN, RABX5_HUMAN, UIMC1_HUMAN, NTH_HUMAN, GABP2_HUMAN, CDK7_HUMAN, MD1L1_HUMAN, TRI54_HUMAN, SP1_HUMAN, K2C7_HUMAN, BEND5_HUMAN, HECW1_HUMAN, QCR7_HUMAN, TSR1_HUMAN, BRD4_HUMAN.NUTM1_HUMAN, SYT7_HUMAN, ZN696_HUMAN, IKIP_HUMAN, TITIN_HUMAN, K1H1_HUMAN, CENPQ_HUMAN, KCY_HUMAN, TOP2A_HUMAN, SPERT_HUMAN, THB_HUMAN, TPPP_HUMAN, PSB2_HUMAN, F241B_HUMAN, PMS2_HUMAN, CCNH_HUMAN, GATA4_HUMAN, BRPF3_HUMAN, ASAP2_HUMAN, HNRH2_HUMAN, FOXO4_HUMAN, CNDH2_HUMAN, RCOR3_HUMAN, TROP_HUMAN, PHF10_HUMAN, IN80E_HUMAN, LHX3_HUMAN, CUL2_HUMAN, SHLB2_HUMAN, SHLB1_HUMAN, PPARA_HUMAN, STK11_HUMAN, VAC14_HUMAN, DEDD_HUMAN, DLG1_HUMAN, CEP70_HUMAN, KAT8_HUMAN, BDP1_HUMAN, BRCA1_HUMAN, MSGN1_HUMAN, CHMP5_HUMAN, EIF3I_HUMAN, CCNA1_HUMAN, ORC1_HUMAN, ORC2_HUMAN, SGCA_HUMAN, CAF1B_HUMAN, DYH1_HUMAN, TNNT3_HUMAN, H1X_HUMAN, STXB3_HUMAN, RIPP1_HUMAN, ANKR1_HUMAN, CASQ2_HUMAN, ECI2_HUMAN, SENP1_HUMAN, MYDGF_HUMAN, IMA5_HUMAN, UBQL2_HUMAN, LRC45_HUMAN, APC10_HUMAN, CFA97_HUMAN, GTPBA_HUMAN, GA45G_HUMAN, HDA10_HUMAN, NSD1_HUMAN, MICA1_HUMAN, NR4A1_HUMAN, CUL3_HUMAN, ZNF76_HUMAN, SMG7_HUMAN, BRNP1_HUMAN, ZN326_HUMAN, GNAQ_HUMAN, FLOT2_HUMAN, AHR_HUMAN, PRI2_HUMAN, NDC80_HUMAN, UB2V2_HUMAN, MAPK5_HUMAN, DNMT1_HUMAN, HESX1_HUMAN, MPIP2_HUMAN, CEP44_HUMAN, HCK_HUMAN, RYBP_HUMAN, RHG04_HUMAN, TOP1_HUMAN, TNNT1_HUMAN, FSCN1_HUMAN, NUDC_HUMAN, HEMK1_HUMAN, MED26_HUMAN, MED12_HUMAN, MED8_HUMAN, MK06_HUMAN, THOC2_HUMAN, S39A9_HUMAN, CERS3_HUMAN, BACH1_HUMAN, 1433T_HUMAN, CNTRL_HUMAN, NF1_HUMAN, AKT2_HUMAN, H2B1D_HUMAN, H2AW_HUMAN, K2C5_HUMAN, ACTN4_HUMAN, TM52B_HUMAN, RL7A_HUMAN, CC106_HUMAN, AAKB1_HUMAN, ERC6L_HUMAN, PLK1_HUMAN, XRCC5_HUMAN, MTO1_HUMAN, ZCHC7_HUMAN, GP152_HUMAN, SPN90_HUMAN, DTBP1_HUMAN, CDCA7_HUMAN, NEXN_HUMAN, USF2_HUMAN, RASF3_HUMAN, PMF1_HUMAN, VP37A_HUMAN, CC113_HUMAN, FST_HUMAN, TAF2_HUMAN, P73_HUMAN, ERGI3_HUMAN, SOX5_HUMAN, ETHE1_HUMAN, HP1B3_HUMAN, YBOX3_HUMAN, MAGI2_HUMAN, GANAB_HUMAN, GSTM4_HUMAN, TCRG1_HUMAN, UBF1_HUMAN, MBB1A_HUMAN, COIL_HUMAN, LDB2_HUMAN, ORML1_HUMAN, E41L1_HUMAN, BAD_HUMAN, SEPT1_HUMAN, RSPO1_HUMAN, KLC1_HUMAN, ORML3_HUMAN, TET2_HUMAN, 1433G_HUMAN, E41L3_HUMAN, RA54B_HUMAN, LRC59_HUMAN, PI3R4_HUMAN, PSMD9_HUMAN, GLYR1_HUMAN, SYCE1_HUMAN, SAS10_HUMAN, FR1OP_HUMAN, JPH2_HUMAN, CLCN3_HUMAN, CAPG_HUMAN, BHLH9_HUMAN, TENS1_HUMAN, MON2_HUMAN, ARHG9_HUMAN, WDR62_HUMAN, RBX1_HUMAN, RL10_HUMAN, B4DYC6_HUMAN, SYIM_HUMAN, TEAN2_HUMAN, AKA11_HUMAN, ZC3H8_HUMAN, CENPK_HUMAN, IF4G2_HUMAN, ORML2_HUMAN, MBD1_HUMAN, WDR5B_HUMAN, PHC2_HUMAN, ENKD1_HUMAN, SRPK2_HUMAN, NOC2L_HUMAN, SMYD1_HUMAN, MKL2_HUMAN, USH1C_HUMAN, CBX6_HUMAN, CAN7_HUMAN, GNAI2_HUMAN, HAUS1_HUMAN, ZN655_HUMAN, MOONR_HUMAN, KPYM_HUMAN, SMC5_HUMAN, FXR1_HUMAN, CADH1_HUMAN, RT33_HUMAN, RPC9_HUMAN, TNIK_HUMAN, VINC_HUMAN, PML_HUMAN, CNBP_HUMAN, CAMP3_HUMAN, DNJB5_HUMAN, SPTB2_HUMAN, PNRC1_HUMAN, PRC2A_HUMAN, MBD3_HUMAN, GOG8C_HUMAN, PSD11_HUMAN, CRBN_HUMAN, SYNE2_HUMAN, RBM48_HUMAN, KT222_HUMAN, DHX15_HUMAN, KIF2C_HUMAN, IF5A2_HUMAN, NUF2_HUMAN, ELP1_HUMAN, IKZF3_HUMAN, H2AZ_HUMAN, RTN4_HUMAN, SGO2_HUMAN, ST1E1_HUMAN, RPAB2_HUMAN, RL3_HUMAN, CDCA4_HUMAN, RSMN_HUMAN, FANCA_HUMAN, IMDH2_HUMAN, ELOF1_HUMAN, GOG6A_HUMAN, NPHP3_HUMAN, KT33B_HUMAN, ZNF35_HUMAN, LTN1_HUMAN, RFIP2_HUMAN, A0A075B747_HUMAN.BAHC1_HUMAN, A0A087WTE7_HUMAN.LENG8_HUMAN, GSTO1_HUMAN, RL23_HUMAN, RGS6_HUMAN, GO45_HUMAN, SRBS1_HUMAN, PP2AA_HUMAN, EXOC8_HUMAN, NC2A_HUMAN, SSBP2_HUMAN, FKBP4_HUMAN, CEP78_HUMAN, FAM9B_HUMAN, CH10_HUMAN, RAN_HUMAN, APC_HUMAN, SRP72_HUMAN, PDS5A_HUMAN, MRCKA_HUMAN, HM20A_HUMAN, IL16_HUMAN, TACC1_HUMAN, PABP2_HUMAN, RS30_HUMAN.UBIM_HUMAN, OBSCN_HUMAN, TOX4_HUMAN, VINEX_HUMAN, TCF21_HUMAN, ROCK2_HUMAN, CCNF_HUMAN, K2C3_HUMAN, SMUG1_HUMAN, RAD17_HUMAN, HUWE1_HUMAN, SPB9_HUMAN, SP100_HUMAN, MYLK_HUMAN, TBCB_HUMAN, ABCF1_HUMAN, CNOT7_HUMAN, TM222_HUMAN, SETB1_HUMAN, KRT81_HUMAN, DHX30_HUMAN, H2B1H_HUMAN, BCOR_HUMAN, RL19_HUMAN, MTA2_HUMAN, GOR_HUMAN, PO2F1_HUMAN, TAF6_HUMAN, SUV92_HUMAN, RPC5_HUMAN, SSRP1_HUMAN, RPA34_HUMAN, SP16H_HUMAN, AKT3_HUMAN, LUZP1_HUMAN, MAGD1_HUMAN, KRT83_HUMAN, BCCIP_HUMAN, BARD1_HUMAN, S27A6_HUMAN, HS71L_HUMAN, RT12_HUMAN, SYYC_HUMAN, MYH15_HUMAN, PPIP1_HUMAN, RLA1_HUMAN, TPRKB_HUMAN, F161A_HUMAN, PEPL_HUMAN, CRTC2_HUMAN, RING1_HUMAN, H0YDQ3_HUMAN, RINI_HUMAN, PSMD2_HUMAN, E7EN19_HUMAN, SETD2_HUMAN, TCAL2_HUMAN, TCAL4_HUMAN, AP1G2_HUMAN, TWF2_HUMAN, TRI22_HUMAN, H13_HUMAN, ATAT_HUMAN, ATRIP_HUMAN, SETD7_HUMAN, ITAL_HUMAN, TLN1_HUMAN, ATF3_HUMAN, IFT74_HUMAN, ARFG2_HUMAN, SCAI_HUMAN, SIN3B_HUMAN, KCRS_HUMAN, LMO7_HUMAN, ZN611_HUMAN, PLS1_HUMAN, DIP2A_HUMAN, S30BP_HUMAN, SMYD3_HUMAN, PSA_HUMAN, CAVN1_HUMAN, CBX7_HUMAN, K2C1_HUMAN, RPF2_HUMAN, CALD1_HUMAN, CA112_HUMAN, T22D3_HUMAN, IRF3_HUMAN, ATPO_HUMAN, K2C74_HUMAN, NSMA2_HUMAN, GRB14_HUMAN, RUSD4_HUMAN, ACY1_HUMAN, ZFAT_HUMAN, LEMD1_HUMAN, RA1L2_HUMAN, RBM5_HUMAN, RTRAF_HUMAN, A0AVG3_HUMAN, RS10_HUMAN, HMOX2_HUMAN, AAKB2_HUMAN, TRPM7_HUMAN, PPM1A_HUMAN, NU133_HUMAN, RHXF2_HUMAN, HMGA1_HUMAN, RRP15_HUMAN, KS6A6_HUMAN, ANM2_HUMAN, NAA16_HUMAN, CHIP_HUMAN, PHOCN_HUMAN, COPB_HUMAN, GEMI_HUMAN, CAR10_HUMAN, BAP31_HUMAN, M3K7_HUMAN, NP1L1_HUMAN, PP1B_HUMAN, GRWD1_HUMAN, DDB1_HUMAN, FADD_HUMAN, CASP8_HUMAN, EF1A1_HUMAN, EIF3M_HUMAN, LIPB1_HUMAN, PDIA1_HUMAN, DDX5_HUMAN, PTPRA_HUMAN, TPR_HUMAN, STX7_HUMAN, TSC1_HUMAN, VPS11_HUMAN, P2R3C_HUMAN, PP1R7_HUMAN, ACTN1_HUMAN, VPS4B_HUMAN, HSC20_HUMAN, GLYM_HUMAN, POTE1_HUMAN, BICD1_HUMAN, OAT_HUMAN, BUB1_HUMAN, TAF1D_HUMAN, ADH1B_HUMAN, HIRA_HUMAN, KRT86_HUMAN, DDX52_HUMAN, ZN536_HUMAN, MCM6_HUMAN, HOOK1_HUMAN, DCAM_HUMAN, K1C18_HUMAN, UBB_HUMAN.UBC_HUMAN, RHG30_HUMAN, ZEP1_HUMAN, RN111_HUMAN, KCNA5_HUMAN, HABP4_HUMAN, CFA54_HUMAN, TM14C_HUMAN, KAISO_HUMAN, ASPM_HUMAN, SCMC1_HUMAN, AT11B_HUMAN, LMBL3_HUMAN, MAT1_HUMAN, TYB4_HUMAN, ZN395_HUMAN, KCRU_HUMAN, CAPR2_HUMAN, CENPI_HUMAN, WWP1_HUMAN, CDC42_HUMAN, TOM20_HUMAN, BAHD1_HUMAN, DMD_HUMAN, GSK3B_HUMAN, MED10_HUMAN, Z280A_HUMAN, WDR18_HUMAN, TEX10_HUMAN, LAS1L_HUMAN, H1T_HUMAN, YYAP1_HUMAN, PSF2_HUMAN, SMIM1_HUMAN, SYYM_HUMAN, KR195_HUMAN, SRGEF_HUMAN, ZN341_HUMAN, ZC3HE_HUMAN, AK1C3_HUMAN, TM10B_HUMAN, EHD1_HUMAN, DEK_HUMAN, KDM4B_HUMAN, ROA2_HUMAN, MYPC1_HUMAN, STIP1_HUMAN, PTTG1_HUMAN, WDR82_HUMAN, FOXN1_HUMAN, K1C40_HUMAN, CENPC_HUMAN, BAZ2B_HUMAN, AIM2_HUMAN, KIF2B_HUMAN, ASF1A_HUMAN, YIPF4_HUMAN, PINX1_HUMAN, ZN800_HUMAN, RL26_HUMAN, IMA4_HUMAN, ARI3B_HUMAN, TFPT_HUMAN, E41L2_HUMAN, TRAF1_HUMAN, DC1I1_HUMAN, RREB1_HUMAN, K2C72_HUMAN, TS101_HUMAN, RD23A_HUMAN, KLHL7_HUMAN, TRDMT_HUMAN, NEBU_HUMAN, APC16_HUMAN, LARP7_HUMAN, 1433S_HUMAN, DESP_HUMAN, ERCC5_HUMAN, KRA92_HUMAN, IPYR_HUMAN, USF3_HUMAN, LYAR_HUMAN, H2BFS_HUMAN, SPEB_HUMAN, GIT2_HUMAN, PIAS2_HUMAN, AF9_HUMAN, Q6PK50_HUMAN, MNS1_HUMAN, PPAC_HUMAN, RAD9A_HUMAN, KPCD_HUMAN, BI2L1_HUMAN, GOGB1_HUMAN, MA2A2_HUMAN, MEOX2_HUMAN, ECM29_HUMAN, PP2AB_HUMAN, NEK6_HUMAN, CO8A1_HUMAN, PO6F2_HUMAN, SYTC_HUMAN, CYBP_HUMAN, GAPD1_HUMAN, INT2_HUMAN, SPF27_HUMAN, TEAD2_HUMAN, TGM1_HUMAN, CLRN1_HUMAN, TOM70_HUMAN, TZAP_HUMAN, EIF3A_HUMAN, RHG07_HUMAN, AKP8L_HUMAN, TCPB_HUMAN, DSCR3_HUMAN, CE162_HUMAN, GOG8A_HUMAN.GOG8B_HUMAN, TM1L1_HUMAN, BBC3B_HUMAN, PRP4B_HUMAN, BAIP2_HUMAN, IKKE_HUMAN, TAF5_HUMAN, FA50A_HUMAN, PFD2_HUMAN, UBE3A_HUMAN, CND2_HUMAN, ATPF2_HUMAN, DGKZ_HUMAN, HYOU1_HUMAN, NEK11_HUMAN, AIMP2_HUMAN, KAT5_HUMAN, PAL4C_HUMAN.PAL4G_HUMAN, DYH17_HUMAN, SPIN1_HUMAN, IF2B1_HUMAN, RBM25_HUMAN, RSSA_HUMAN, ARNT2_HUMAN, PEG3_HUMAN, NELFA_HUMAN, GPC3_HUMAN, ATPK_HUMAN, COPRS_HUMAN, KAT7_HUMAN, NBPF1_HUMAN.S4R3K2_HUMAN, TPM3_HUMAN, UBE2U_HUMAN, TDIF1_HUMAN, PDIA3_HUMAN, DYH14_HUMAN, GPAA1_HUMAN, SRSF1_HUMAN, CTDP1_HUMAN, SNAA_HUMAN, KR108_HUMAN, T22D4_HUMAN, FINC_HUMAN, ITB1_HUMAN, BAG1_HUMAN, ZFP28_HUMAN, PSMD6_HUMAN, BOP1_HUMAN, DLDH_HUMAN, FLOT1_HUMAN, OGG1_HUMAN, STK16_HUMAN, TCHP_HUMAN, MCM4_HUMAN, SCML2_HUMAN, IPSP_HUMAN, CDN2C_HUMAN, ITB5_HUMAN, ARL3_HUMAN, GRPE1_HUMAN, MCEM1_HUMAN, GET4_HUMAN, MED31_HUMAN, ADCY9_HUMAN, CALY_HUMAN, HXA7_HUMAN, FLNB_HUMAN, HIF1N_HUMAN, BIP_HUMAN, E2F2_HUMAN, HS90A_HUMAN, BBS4_HUMAN, EFTU_HUMAN, A0A0A0MRV0_HUMAN.RRBP1_HUMAN, CDN2A_HUMAN.G3XAG3_HUMAN, DYR1B_HUMAN, PEO1_HUMAN, PDIP3_HUMAN, CPSF1_HUMAN, PAPOA_HUMAN, SAP18_HUMAN, MRE11_HUMAN, RNF8_HUMAN, STAB2_HUMAN, BSH_HUMAN, A0A087X1W2_HUMAN.ANM1_HUMAN.H7C2I1_HUMAN, TCPZ_HUMAN, PFD6_HUMAN, HNRH3_HUMAN, A0A0A0MRM0_HUMAN.MYOME_HUMAN, ISL1_HUMAN, LSM3_HUMAN, H4G_HUMAN, DYL1_HUMAN, NR2C2_HUMAN, TSYL4_HUMAN, ZBTB9_HUMAN, IF4G1_HUMAN, SYEP_HUMAN, DFFB_HUMAN, ENPL_HUMAN, PARP3_HUMAN, XRCC6_HUMAN, CTC1_HUMAN, DPOLL_HUMAN, MYL9_HUMAN, ZN480_HUMAN, H2B1A_HUMAN, H2A1A_HUMAN, UBP2_HUMAN, PNKP_HUMAN, TGIF2_HUMAN, CDC6_HUMAN, PEX16_HUMAN, CDK6_HUMAN, CD047_HUMAN, SPTA1_HUMAN, CC125_HUMAN, S10A2_HUMAN, IMA1_HUMAN, FOSL2_HUMAN, STAG2_HUMAN, PFD5_HUMAN, MLRV_HUMAN, LAP2A_HUMAN, SYVN1_HUMAN, WNK1_HUMAN, RUVB2_HUMAN, GTPB8_HUMAN, RFX1_HUMAN, FBW1B_HUMAN, FOXN2_HUMAN, AXIN2_HUMAN, GPI8_HUMAN, THOC1_HUMAN, RL41_HUMAN, GOGA3_HUMAN, MYL6_HUMAN, MAP4_HUMAN, TPPP3_HUMAN, MGT4C_HUMAN, KI18A_HUMAN, LARP4_HUMAN, ZNF24_HUMAN, FYB1_HUMAN, PTBP1_HUMAN, SH3G3_HUMAN, LTV1_HUMAN, TAP26_HUMAN, IL7RA_HUMAN, PLEC_HUMAN, PRD16_HUMAN, MMRN1_HUMAN, WEE1_HUMAN, SF3B3_HUMAN, RBP56_HUMAN, TTF1_HUMAN, FER_HUMAN, UCHL1_HUMAN, SMAD1_HUMAN, POLK_HUMAN, ASF1B_HUMAN, RM28_HUMAN, TRPM6_HUMAN, PFD1_HUMAN, KPCD3_HUMAN, K2C4_HUMAN, TNIP1_HUMAN, NTAQ1_HUMAN, ZN181_HUMAN, B7Z2Q3_HUMAN.CCD14_HUMAN, PROF1_HUMAN, DTL_HUMAN, DLG3_HUMAN, SARDH_HUMAN, ENTP5_HUMAN, GAS8_HUMAN, FANCG_HUMAN, APC11_HUMAN, HSPB3_HUMAN, CCHCR_HUMAN, CP110_HUMAN, SAP30_HUMAN, TLX3_HUMAN, RABL6_HUMAN, SNR40_HUMAN, PRIO_HUMAN, EMSY_HUMAN, WRP73_HUMAN, K1C19_HUMAN, XPO1_HUMAN, MYO9B_HUMAN, IF4E_HUMAN, FOLH1_HUMAN, PIDD1_HUMAN, THAP7_HUMAN, ODB2_HUMAN, FRMD8_HUMAN, CCD89_HUMAN, ACD_HUMAN, OBSL1_HUMAN, KLD10_HUMAN, NUDC3_HUMAN, CDK9_HUMAN, TPX2_HUMAN, RT23_HUMAN, PHF2_HUMAN, VASP_HUMAN, AASD1_HUMAN, TET1_HUMAN, SASH3_HUMAN, AHNK_HUMAN, IF2A_HUMAN, H33_HUMAN, H2B1B_HUMAN, ANR26_HUMAN, TEX35_HUMAN, NR1H2_HUMAN, ZN581_HUMAN, CR3L1_HUMAN, EBPL_HUMAN, C2D1B_HUMAN, ANM7_HUMAN, RS6_HUMAN, BTF3_HUMAN, VAX1_HUMAN, KI21A_HUMAN, HMGN4_HUMAN, UNKL_HUMAN, SRRT_HUMAN, ZFYV9_HUMAN, PASK_HUMAN, K1H2_HUMAN, PLB1_HUMAN, PCF11_HUMAN, HMGB1_HUMAN, PRDM2_HUMAN, NFU1_HUMAN, SF3A2_HUMAN, RBCC1_HUMAN, FKBP8_HUMAN, NDUS1_HUMAN, NOA1_HUMAN, RM12_HUMAN, PDCD4_HUMAN, 2ABA_HUMAN, SOAT_HUMAN, CWC27_HUMAN, BBIP1_HUMAN, ZN442_HUMAN, UCHL5_HUMAN, BRX1_HUMAN, LMOD1_HUMAN, TEBP_HUMAN, RL37A_HUMAN, RL9_HUMAN, CHD6_HUMAN, IN35_HUMAN, SPT4H_HUMAN, RL23A_HUMAN, HTRA2_HUMAN, UFL1_HUMAN, SNAPN_HUMAN, OCAD1_HUMAN, RPAP2_HUMAN, PUR6_HUMAN, NEK4_HUMAN, CACL1_HUMAN, SNRPA_HUMAN, NR5A2_HUMAN, MVP_HUMAN, MEF2A_HUMAN, PKN3_HUMAN, TAF7_HUMAN, P4R3A_HUMAN, NUP98_HUMAN, AFF4_HUMAN, CALM1_HUMAN.CALM2_HUMAN.CALM3_HUMAN, SRPK1_HUMAN, DC1I2_HUMAN, MECP2_HUMAN, CATC_HUMAN, GDF15_HUMAN, TRRAP_HUMAN, WDR83_HUMAN, PTN3_HUMAN, PNPT1_HUMAN, GAS7_HUMAN, DESM_HUMAN, IKBB_HUMAN, LBR_HUMAN, SNX15_HUMAN, SP20H_HUMAN, RS8_HUMAN, SPZ1_HUMAN, PKHO1_HUMAN, PAX4_HUMAN, FACE1_HUMAN, PIWL4_HUMAN, RM40_HUMAN, WBP4_HUMAN, HS74L_HUMAN, SPA24_HUMAN, SYCP3_HUMAN, IF2M_HUMAN, RP1_HUMAN, EXO1_HUMAN, RL14_HUMAN, TTLL1_HUMAN, MYLIP_HUMAN, DOA_HUMAN, ZN451_HUMAN, OST48_HUMAN, PRGR_HUMAN, REV3L_HUMAN, TAF9_HUMAN, UPAR_HUMAN, CDT1_HUMAN, CRNL1_HUMAN, A0A0A6YY96_HUMAN.IREB2_HUMAN, MCM3_HUMAN, SRS11_HUMAN, ANK1_HUMAN, KLF3_HUMAN, ILK_HUMAN, CCL13_HUMAN, H2B1C_HUMAN, TBL1R_HUMAN, SMC1B_HUMAN, GUC1A_HUMAN, I20L2_HUMAN, RCC1_HUMAN, SETMR_HUMAN, NO40_HUMAN, SIM2_HUMAN, ARI1_HUMAN, HAUS3_HUMAN, KDM4D_HUMAN, DGKI_HUMAN, RPB2_HUMAN, SFPQ_HUMAN, INT1_HUMAN, HELQ_HUMAN, TFDP2_HUMAN, RPAB1_HUMAN, RPB11_HUMAN, URM1_HUMAN, KIF2A_HUMAN, COPB2_HUMAN, TAF10_HUMAN, AP2A1_HUMAN, DPOE1_HUMAN, INT12_HUMAN, ZBTB6_HUMAN, SMC2_HUMAN, RAD52_HUMAN, BRD4_HUMAN, C1TC_HUMAN, PRDX1_HUMAN, RPB4_HUMAN, APC15_HUMAN, DDX24_HUMAN, SPT6H_HUMAN, RPAB3_HUMAN, APC13_HUMAN, INT10_HUMAN, MED17_HUMAN, NELFB_HUMAN, NELFD_HUMAN, NELFE_HUMAN, TF2B_HUMAN, SRSF3_HUMAN, INT6_HUMAN, Q7Z3E4_HUMAN, CBPE_HUMAN, SNURF_HUMAN, ANM1_HUMAN, VTDB_HUMAN, SET_HUMAN, NP1L4_HUMAN, TF3C4_HUMAN, KAPCA_HUMAN, E2F3_HUMAN, PTMA_HUMAN, CNOT1_HUMAN, FURIN_HUMAN, STA5A_HUMAN, RRAGD_HUMAN, RRAGC_HUMAN, CSTF1_HUMAN, PK3CG_HUMAN, MFNG_HUMAN, LFNG_HUMAN, MYOD1_HUMAN, UBP2L_HUMAN, CPSF6_HUMAN, DMC1_HUMAN, MSH4_HUMAN, SND1_HUMAN, NOTC3_HUMAN, AP180_HUMAN, PAX6_HUMAN, NKX21_HUMAN, TDG_HUMAN, HDAC9_HUMAN, TRI63_HUMAN, MLH1_HUMAN, CCNE1_HUMAN, ARI3A_HUMAN, ATR_HUMAN, SRTD2_HUMAN, NTRK2_HUMAN, TF3B_HUMAN, TF2AA_HUMAN, T2AG_HUMAN, MED21_HUMAN, PABP1_HUMAN, RARG_HUMAN, PO3F4_HUMAN, SMC1A_HUMAN, TNPO1_HUMAN, UHRF1_HUMAN, CSN2_HUMAN, SMUF1_HUMAN, SMUF2_HUMAN, DPA1_HUMAN, ADA17_HUMAN, DLL4_HUMAN, H2AB2_HUMAN, CPSF2_HUMAN, RARB_HUMAN, ELL_HUMAN, TRIP4_HUMAN, DYRK2_HUMAN, MCAF1_HUMAN, MVD1_HUMAN, JUN_HUMAN, ASPP2_HUMAN, CCNE2_HUMAN, LAP2A_HUMAN.LAP2B_HUMAN, E2F6_HUMAN, HS71A_HUMAN.HS71B_HUMAN, GRP75_HUMAN, RRAGA_HUMAN, HMGN1_HUMAN, KPCA_HUMAN, KS6A3_HUMAN, HPIP_HUMAN, PRGC2_HUMAN, SRF_HUMAN, COT1_HUMAN, ZNF74_HUMAN, SPERI_HUMAN, TAF11_HUMAN, MTG8_HUMAN, GATA2_HUMAN, MCE1_HUMAN, MCES_HUMAN, PAEP_HUMAN, ALDH2_HUMAN, PIM1_HUMAN, HAP1_HUMAN, HXC10_HUMAN, FEZ1_HUMAN, BMPR2_HUMAN, AKTS1_HUMAN, DPOA2_HUMAN, ACL6A_HUMAN, LCK_HUMAN, CBL_HUMAN, FOXA1_HUMAN, PURA_HUMAN, SP4_HUMAN, BRD2_HUMAN, SP2_HUMAN, SP3_HUMAN, STA5B_HUMAN, DDX20_HUMAN, MTG8R_HUMAN, SAFB1_HUMAN, MED6_HUMAN, TAU_HUMAN, MSX1_HUMAN, HIP1_HUMAN, TMF1_HUMAN, FOXO1_HUMAN, NCOA7_HUMAN, MECR_HUMAN, NRIP2_HUMAN, KMT5C_HUMAN, CREG1_HUMAN, CTDS1_HUMAN, MPIP3_HUMAN, HIF3A_HUMAN, HAND2_HUMAN, PPBN_HUMAN, EDF1_HUMAN, CCNT1_HUMAN, TRAK2_HUMAN, CEBPB_HUMAN, TGFR1_HUMAN, KDM5A_HUMAN, NTRK1_HUMAN, CASP3_HUMAN, PRPF3_HUMAN, RU17_HUMAN, U2AF2_HUMAN, PSN1_HUMAN, CSH2_HUMAN, NR1I2_HUMAN, CHK1_HUMAN, NSG2_HUMAN, HSF1_HUMAN, SUFU_HUMAN, CEBPE_HUMAN, PDCD2_HUMAN, PSIP1_HUMAN, TAF4_HUMAN, TCP4_HUMAN, PSME1_HUMAN, COT2_HUMAN, NR1H4_HUMAN, NR1D1_HUMAN, CDK3_HUMAN, HPF1_HUMAN, RT31_HUMAN, UBP33_HUMAN, SEPT3_HUMAN, RL6_HUMAN, WFS1_HUMAN, FUND2_HUMAN, TRAF5_HUMAN, BTG1_HUMAN, RND1_HUMAN, PSN2_HUMAN, MEF2C_HUMAN, BL1S1_HUMAN, OFUT1_HUMAN, NUMBL_HUMAN, RPB7_HUMAN, KPCI_HUMAN, UBR5_HUMAN, APCL_HUMAN, TCFL5_HUMAN, ERCC6_HUMAN.ERPG3_HUMAN, HG2A_HUMAN, PPP5_HUMAN, STAU1_HUMAN, RBBP9_HUMAN, HDAC7_HUMAN, C1D_HUMAN, HDAC5_HUMAN, RPAB4_HUMAN, TAF12_HUMAN, TAF8_HUMAN, SOX6_HUMAN, SOX10_HUMAN, KS6A5_HUMAN, CHK2_HUMAN, TDT_HUMAN, CCNL2_HUMAN, PCIF1_HUMAN, PPIG_HUMAN, UBE2C_HUMAN, APBA1_HUMAN, IKZF1_HUMAN, P2R3A_HUMAN, CCND3_HUMAN, BRCA2_HUMAN, WDR12_HUMAN, DTX2_HUMAN, TCPA_HUMAN, NACAM_HUMAN.NACA_HUMAN, TGFI1_HUMAN, NR0B2_HUMAN, UBP4_HUMAN, FGFR1_HUMAN, FSBP_HUMAN.RA54B_HUMAN, RFXAP_HUMAN, SREK1_HUMAN, NMDZ1_HUMAN, YAP1_HUMAN, SPOP_HUMAN, KLF5_HUMAN, ZN689_HUMAN, STAT2_HUMAN, NOV_HUMAN, HTSF1_HUMAN, ACTG_HUMAN, FACD2_HUMAN, PTPRM_HUMAN, DEFB1_HUMAN, KSYK_HUMAN, NONO_HUMAN, CC14A_HUMAN, THA_HUMAN, TRI36_HUMAN, MTA1_HUMAN, ZMY11_HUMAN, POP7_HUMAN, RAP1A_HUMAN, CTCF_HUMAN, HDAC8_HUMAN, ELAV1_HUMAN, TIA1_HUMAN, TIAR_HUMAN, OFD1_HUMAN, ODPA_HUMAN, IRX4_HUMAN, NPAS2_HUMAN, CDAN1_HUMAN, IPO4_HUMAN, SSU72_HUMAN, SYMPK_HUMAN, KMT2E_HUMAN, MSH6_HUMAN, TBPL1_HUMAN, KDM6B_HUMAN, GTF2I_HUMAN, RHNO1_HUMAN, HEY2_HUMAN, ZEB2_HUMAN, TLE1_HUMAN, RAD50_HUMAN, TSPY1_HUMAN, ZN335_HUMAN, CABIN_HUMAN, UBN1_HUMAN, ZN143_HUMAN, MAGL2_HUMAN, XRCC3_HUMAN, ADT2_HUMAN, DDX56_HUMAN, RFC1_HUMAN, T2EA_HUMAN, MED9_HUMAN, MED29_HUMAN, MED19_HUMAN, MED28_HUMAN, PK3CA_HUMAN, DCP2_HUMAN, XRN1_HUMAN, EXOSX_HUMAN, EXOS2_HUMAN, EXOS4_HUMAN, PARN_HUMAN, CDN1C_HUMAN, H2A3_HUMAN, SPIB_HUMAN, MGAP_HUMAN, CTDS2_HUMAN, ASCL2_HUMAN, HSP7C_HUMAN, T2EB_HUMAN, TAF7L_HUMAN, ZMYM2_HUMAN, KLF1_HUMAN, ARI4A_HUMAN, AATF_HUMAN, ING1_HUMAN, ELP3_HUMAN, EIF3B_HUMAN, EIF3C_HUMAN, EIF3J_HUMAN, CKS1_HUMAN, SGO1_HUMAN, VDR_HUMAN, TAF1A_HUMAN, AN32A_HUMAN, NEDD4_HUMAN, UB2L3_HUMAN, PDC6I_HUMAN, SERPH_HUMAN, TTK_HUMAN, STK4_HUMAN, MED30_HUMAN, KDM6A_HUMAN, NSD2_HUMAN, PIAS1_HUMAN, CRKL_HUMAN, IF4B_HUMAN, MCM5_HUMAN, PPM1G_HUMAN, HLTF_HUMAN, SRP68_HUMAN, ZN207_HUMAN, TCAL1_HUMAN, AKAP1_HUMAN, RAE1L_HUMAN, UBP14_HUMAN, BABA2_HUMAN, KIF3A_HUMAN, ABRX2_HUMAN, DCAF4_HUMAN, BABA1_HUMAN, OTUD5_HUMAN, YLPM1_HUMAN, BRCC3_HUMAN, MCMBP_HUMAN, FBX38_HUMAN, PPIL4_HUMAN, DOCK7_HUMAN, GPN1_HUMAN, HNRH1_HUMAN, ZFR_HUMAN, RPC1_HUMAN, ILF3_HUMAN, RPC2_HUMAN, BAG6_HUMAN, KIF11_HUMAN, TAF13_HUMAN, KHDR2_HUMAN, DDX3Y_HUMAN, NUMA1_HUMAN, IPO9_HUMAN, SLN11_HUMAN, MCM10_HUMAN, SYTL2_HUMAN, ERBIN_HUMAN, CHFR_HUMAN, PRDM1_HUMAN, DNM3A_HUMAN, THAP1_HUMAN, AJUBA_HUMAN, LIMD1_HUMAN, WTIP_HUMAN, JUNB_HUMAN, LMNB1_HUMAN, MYCD_HUMAN, SKI_HUMAN, TRI25_HUMAN, FANCM_HUMAN, CLN3_HUMAN, ZBT7A_HUMAN, RPB9_HUMAN, NR4A2_HUMAN, IWS1_HUMAN, CREST_HUMAN, TAF1B_HUMAN, BAF_HUMAN, ADDA_HUMAN, CTCFL_HUMAN, NF2L1_HUMAN, HAIR_HUMAN, ZSCA1_HUMAN, RFWD2_HUMAN, WDR26_HUMAN, LIS1_HUMAN, NLE1_HUMAN, WDR61_HUMAN, ENL_HUMAN, AGO1_HUMAN, KDM4C_HUMAN, BPTF_HUMAN, SMCA1_HUMAN, CNOT2_HUMAN, KIBRA_HUMAN, SIR7_HUMAN, HSF4_HUMAN, OGA_HUMAN, SAP25_HUMAN, YES_HUMAN, MYEF2_HUMAN, P66A_HUMAN, P66B_HUMAN, SMRD2_HUMAN, KLF6_HUMAN, ESCO2_HUMAN, MS3L1_HUMAN, MGMT_HUMAN, USF1_HUMAN, PHF1_HUMAN, SRRM2_HUMAN, HNF4A_HUMAN, ZN516_HUMAN, ZMIZ2_HUMAN, NGN2_HUMAN, NDF1_HUMAN, SF01_HUMAN, PBX1_HUMAN, SYN1_HUMAN, PSMD3_HUMAN, PAR10_HUMAN, FOXP1_HUMAN, IKBE_HUMAN, SP130_HUMAN, RFC4_HUMAN, MRT4_HUMAN, HNF1B_HUMAN, UBE4B_HUMAN, PAX7_HUMAN, MEF2D_HUMAN, CENPS_HUMAN, RORA_HUMAN, ASH1L_HUMAN, ADNP_HUMAN, TOPRS_HUMAN, BACH2_HUMAN, PO5F1_HUMAN, DNM3L_HUMAN, MBD2_HUMAN, EMD_HUMAN, WAC_HUMAN, MKL1_HUMAN, MO4L1_HUMAN, MO4L2_HUMAN, DOT1L_HUMAN, ZEB1_HUMAN, KDM1B_HUMAN, ESCO1_HUMAN, SPI1_HUMAN, INT3_HUMAN, INT5_HUMAN, STN1_HUMAN, QKI_HUMAN, BCL3_HUMAN, TAD2A_HUMAN, SIAH2_HUMAN, IST1_HUMAN, PYGO2_HUMAN, IRF5_HUMAN, APLF_HUMAN, ATAD2_HUMAN, FBXW5_HUMAN, SPF30_HUMAN, GFI1_HUMAN, ICT1_HUMAN, RN168_HUMAN, DGCR8_HUMAN, MYPT1_HUMAN, RAG1_HUMAN, MTA3_HUMAN, RANB9_HUMAN, FAF1_HUMAN, UBXN7_HUMAN, NOP56_HUMAN, MED16_HUMAN, AFF1_HUMAN, MARK4_HUMAN, RNF4_HUMAN, KMT5A_HUMAN, SIR3_HUMAN, KC1A_HUMAN, EXOC1_HUMAN, ZBP1_HUMAN, IRF2_HUMAN, GTPB1_HUMAN, MOXD1_HUMAN, BRE1A_HUMAN, MSL2_HUMAN, CDR2_HUMAN, KITH_HUMAN, INT11_HUMAN, PAX3_HUMAN, PCKGC_HUMAN, TRI32_HUMAN, HDAC6_HUMAN, SMRCD_HUMAN, RSMB_HUMAN, TRI33_HUMAN, SOX2_HUMAN, CSR2B_HUMAN, RAD21_HUMAN, IRAK4_HUMAN, HDGF_HUMAN, BRPF1_HUMAN, RUNX3_HUMAN, JAK2_HUMAN, LIN37_HUMAN, JAK1_HUMAN, LIN9_HUMAN, LIN54_HUMAN, SMC3_HUMAN, APBB1_HUMAN, TWST1_HUMAN, IGF1_HUMAN, CDK5_HUMAN, UBE2A_HUMAN, ARRB1_HUMAN, ARRB2_HUMAN, HIPK2_HUMAN, KDM3B_HUMAN, MXI1_HUMAN, SRY_HUMAN, PSB9_HUMAN, SH3K1_HUMAN, TFE2_HUMAN, PCGF1_HUMAN, PCGF3_HUMAN, PCGF6_HUMAN, YAF2_HUMAN, BCL6B_HUMAN, TBX5_HUMAN, ABRX1_HUMAN, CUED2_HUMAN, FOXP3_HUMAN, PARD3_HUMAN, ERG_HUMAN, XPA_HUMAN, FBX25_HUMAN, ID1_HUMAN, NINL_HUMAN, SIX1_HUMAN, KDM2B_HUMAN, MPIP1_HUMAN, FOXM1_HUMAN, ERCC8_HUMAN, CSN1_HUMAN, ERCC1_HUMAN, EIF3F_HUMAN, SYUA_HUMAN, FBX2_HUMAN, EPN1_HUMAN, RNF34_HUMAN, CKAP2_HUMAN, TONSL_HUMAN, PSA2_HUMAN, PSA5_HUMAN, PSB6_HUMAN, PSB5_HUMAN, PSB8_HUMAN, PSB4_HUMAN, NFX1_HUMAN, MOAP1_HUMAN, SENP6_HUMAN, UBP37_HUMAN, CUL5_HUMAN, CSN5_HUMAN, DCNL1_HUMAN, CAND1_HUMAN, AT7L3_HUMAN, UBP22_HUMAN, PIAS3_HUMAN, TRI18_HUMAN, ISG15_HUMAN, PRAME_HUMAN, BRE1B_HUMAN, APRIO_HUMAN.PRIO_HUMAN, TEP1_HUMAN, IRAK1_HUMAN, CSTF2_HUMAN, CSTF3_HUMAN, DCAF1_HUMAN, YETS2_HUMAN, NC2B_HUMAN, LATS2_HUMAN, PSMD4_HUMAN, MAGAB_HUMAN, TOR1A_HUMAN, PHLA1_HUMAN, SPRTN_HUMAN, GRK5_HUMAN, SNAI2_HUMAN, CLP1_HUMAN, SHIP2_HUMAN, P85B_HUMAN, SHC1_HUMAN, CRK_HUMAN, EPS15_HUMAN, MYO6_HUMAN, TXN4B_HUMAN, KDM2A_HUMAN, RS4X_HUMAN, UB2D1_HUMAN, UB2D3_HUMAN, UBE2K_HUMAN, RFFL_HUMAN, PJA1_HUMAN, TRI55_HUMAN, ESPB1_HUMAN, TAF9B_HUMAN, RL10A_HUMAN, RL21_HUMAN, RS3A_HUMAN, RL7_HUMAN, RLA0_HUMAN, RS9_HUMAN, RL11_HUMAN, RL12_HUMAN, RL13_HUMAN, RL15_HUMAN, RL17_HUMAN, RL18A_HUMAN, RL18_HUMAN, RL24_HUMAN, RL8_HUMAN, RS11_HUMAN, RS15A_HUMAN, RS23_HUMAN, RS24_HUMAN, RS26_HUMAN, RS28_HUMAN, RS2_HUMAN, RS5_HUMAN, RS7_HUMAN, RL27A_HUMAN, RS13_HUMAN, RS25_HUMAN, RS14_HUMAN, RL31_HUMAN, RS12_HUMAN, RL30_HUMAN, RLA2_HUMAN, RL22_HUMAN, RU2A_HUMAN, ROA3_HUMAN, SMD1_HUMAN, RS17_HUMAN, RS15_HUMAN, SRSF7_HUMAN, RL32_HUMAN, RL29_HUMAN, RS27A_HUMAN, RS21_HUMAN, U2AF1_HUMAN.U2AF5_HUMAN, SF3A1_HUMAN, RS29_HUMAN, RL40_HUMAN, PRP4_HUMAN, RL1D1_HUMAN, FBRL_HUMAN, ILF2_HUMAN, TRA2B_HUMAN, NOP58_HUMAN, ROA0_HUMAN, RALY_HUMAN, SNUT1_HUMAN, RT05_HUMAN, SMU1_HUMAN, SNUT2_HUMAN, EBP2_HUMAN, LC7L3_HUMAN, RT22_HUMAN, MYH9_HUMAN, RT26_HUMAN, RM42_HUMAN, RT25_HUMAN, RS27L_HUMAN, TR150_HUMAN, TF3C1_HUMAN, RPAC2_HUMAN.RPC22_HUMAN, RT16_HUMAN, NDKB_HUMAN, RL10L_HUMAN, RLA0L_HUMAN, RRS1_HUMAN, LAMP2_HUMAN, RBM19_HUMAN, RM52_HUMAN, THIL_HUMAN, TOIP1_HUMAN, NFIA_HUMAN, UCRIL_HUMAN, PREP_HUMAN, RT34_HUMAN, DDX21_HUMAN, MK67I_HUMAN, DCTN2_HUMAN, MARCS_HUMAN, SAHH2_HUMAN, UT14A_HUMAN, SEPT7_HUMAN, LTOR3_HUMAN, SUCA_HUMAN, H2A1D_HUMAN, VAMP2_HUMAN, RPC7_HUMAN, NICA_HUMAN, XPOT_HUMAN, ZCHC8_HUMAN, RBM14_HUMAN, ODPAT_HUMAN, TRA2A_HUMAN, RM23_HUMAN, PERI_HUMAN, RT28_HUMAN, TIM50_HUMAN, TMED9_HUMAN, WDR74_HUMAN, ATPA_HUMAN, UBP1_HUMAN, MTCH1_HUMAN, METK2_HUMAN, KINH_HUMAN, MTCH2_HUMAN, XRCC4_HUMAN, SGTA_HUMAN, PGRC1_HUMAN, UBE3C_HUMAN, PPGB_HUMAN, WAP53_HUMAN, THTPA_HUMAN, CHRC1_HUMAN, VTNC_HUMAN, PRDX2_HUMAN, VATB2_HUMAN, RHOB_HUMAN, TF3C5_HUMAN, NADAP_HUMAN, SRSF5_HUMAN, RM48_HUMAN, ZCH18_HUMAN, PYR1_HUMAN, LPPRC_HUMAN, PTN1_HUMAN, RM51_HUMAN, LMAN1_HUMAN, UN45A_HUMAN, SAP_HUMAN, PUM1_HUMAN, PM34_HUMAN, SEPT2_HUMAN, VDAC2_HUMAN, K1C14_HUMAN, RM50_HUMAN, PUR9_HUMAN, ITA5_HUMAN, RM10_HUMAN, PPIL3_HUMAN, SDHF2_HUMAN, PALLD_HUMAN, HNRPM_HUMAN, SF3B6_HUMAN, XPO2_HUMAN, NHRF1_HUMAN, LS14A_HUMAN, NRDC_HUMAN, RS10L_HUMAN, S10A9_HUMAN, VATC1_HUMAN, RM13_HUMAN, PEX19_HUMAN, DIDO1_HUMAN, TPM1_HUMAN, MFTC_HUMAN, PRC1_HUMAN, RINT1_HUMAN, ECT2_HUMAN, AAPK1_HUMAN, LIMK2_HUMAN, ROCK1_HUMAN, HCLS1_HUMAN, RBP10_HUMAN, VAV_HUMAN, ARHG2_HUMAN, PP6R3_HUMAN, STK38_HUMAN, WDR6_HUMAN, PTBP3_HUMAN, CCZ1B_HUMAN.CCZ1_HUMAN, SCC4_HUMAN, SMHD1_HUMAN, WWTR1_HUMAN, DDX17_HUMAN, MED23_HUMAN, HTF4_HUMAN, PRP6_HUMAN, RBM10_HUMAN, DHX8_HUMAN, XPO5_HUMAN, NBEA_HUMAN, MDN1_HUMAN, IMB1_HUMAN, IPO5_HUMAN, TPPC9_HUMAN, TPC10_HUMAN, TCPG_HUMAN, TCPQ_HUMAN, VPS39_HUMAN, KLH15_HUMAN, C8AP2_HUMAN, KCC4_HUMAN, RHG32_HUMAN, REV1_HUMAN, HOIL1_HUMAN, TRIM8_HUMAN, EYA1_HUMAN, CFTR_HUMAN, ERAP1_HUMAN, JADE2_HUMAN, JADE3_HUMAN, TERA_HUMAN, FGF3_HUMAN, BTK_HUMAN, VCAM1_HUMAN, C1QBP_HUMAN, TBG1_HUMAN, IQCB1_HUMAN, VPS29_HUMAN, NOS2_HUMAN, TAF4B_HUMAN, MCAT_HUMAN, ING2_HUMAN, MLP3A_HUMAN, UBL4A_HUMAN, ITA4_HUMAN, INS_HUMAN, ZSWM7_HUMAN, NFYA_HUMAN, NFYB_HUMAN, PAK1_HUMAN, NSMF_HUMAN, UB2E1_HUMAN, PAN2_HUMAN, DTD1_HUMAN, PLMN_HUMAN, KPCZ_HUMAN, MMS22_HUMAN, TICRR_HUMAN, CD81_HUMAN, IGSF8_HUMAN, ICAM1_HUMAN, DPOLA_HUMAN, HDA11_HUMAN, DNM3B_HUMAN, RNF11_HUMAN, UBP49_HUMAN, NED4L_HUMAN, DAB2_HUMAN, HINT1_HUMAN, SMD3_HUMAN, DCPS_HUMAN, HEXI1_HUMAN, ZMYM5_HUMAN, ZHX1_HUMAN, TYDP2_HUMAN, CLK3_HUMAN, RM03_HUMAN, FBX6_HUMAN, TADBP_HUMAN, SMC4_HUMAN, MIB1_HUMAN, PWP1_HUMAN, HECW2_HUMAN, PRKN_HUMAN, MTF2_HUMAN, NDUA8_HUMAN, NFL_HUMAN, MYOME_HUMAN, ASNA_HUMAN, CDC37_HUMAN, COF1_HUMAN, COG3_HUMAN, CYHR1_HUMAN, SYRC_HUMAN, TFIP8_HUMAN, FKBP5_HUMAN, G3BP1_HUMAN, PSF3_HUMAN, HNRPR_HUMAN, DDX1_HUMAN, DIM1_HUMAN, EI2BB_HUMAN, EI2BG_HUMAN, EIF3D_HUMAN, FKBP3_HUMAN, IF2B3_HUMAN, RL35_HUMAN, ML12A_HUMAN.ML12B_HUMAN, ARP2_HUMAN, AGFG1_HUMAN, HEM2_HUMAN, DBNL_HUMAN, AMPL_HUMAN, LPP_HUMAN, WDR4_HUMAN, ZPR1_HUMAN, PA1B2_HUMAN, PP4R1_HUMAN, PPP6_HUMAN, BACH_HUMAN, GDIA_HUMAN, DYLT3_HUMAN, PNO1_HUMAN, RL28_HUMAN, RS18_HUMAN, PAIRB_HUMAN, PYM1_HUMAN, UBP48_HUMAN, VP26A_HUMAN, WDHD1_HUMAN, SEM1_HUMAN.SEML_HUMAN, SART3_HUMAN, ASB6_HUMAN, ZBTB1_HUMAN, UBS3B_HUMAN, RGAP1_HUMAN, LGR4_HUMAN, CSK22_HUMAN, KC1E_HUMAN, NOP53_HUMAN, NMD3_HUMAN, POP1_HUMAN, NOB1_HUMAN, H2A1_HUMAN, GRSF1_HUMAN, IRS4_HUMAN, NS1BP_HUMAN, PHF7_HUMAN, CHD1L_HUMAN, NFE4_HUMAN, MK03_HUMAN, LTOR5_HUMAN, TBA1A_HUMAN, TBB5_HUMAN, TBB4B_HUMAN, TCPE_HUMAN, TBB2A_HUMAN, TCPD_HUMAN, TBA1C_HUMAN, TCPH_HUMAN, RAVR1_HUMAN, EIF2A_HUMAN, CP250_HUMAN, CEP57_HUMAN, HAUS2_HUMAN, NEDD1_HUMAN, GCP3_HUMAN, GCP2_HUMAN, SAMH1_HUMAN, SENP7_HUMAN, GBB2_HUMAN, IRF7_HUMAN, PRDM6_HUMAN, TPP1_HUMAN, ELOA1_HUMAN, SENP5_HUMAN, CENPX_HUMAN, PCSK9_HUMAN, CD2AP_HUMAN, ERBB2_HUMAN, NIPA_HUMAN, PRS6A_HUMAN, KRT38_HUMAN, BCAS3_HUMAN, KLC3_HUMAN, FAN1_HUMAN, PHF6_HUMAN, PTF1A_HUMAN, HMGX4_HUMAN, PPIB_HUMAN, BAP18_HUMAN, SUPT3_HUMAN, TAF5L_HUMAN, TADA1_HUMAN, TAF6L_HUMAN, PHF12_HUMAN, CDYL2_HUMAN, CHAP1_HUMAN, LRWD1_HUMAN, ORC3_HUMAN, ORC4_HUMAN, ORC5_HUMAN, MIER1_HUMAN, ROAA_HUMAN, CUL7_HUMAN, CCDC8_HUMAN, LOXL2_HUMAN, DNM1L_HUMAN, ZBT21_HUMAN, TACC3_HUMAN, CASL_HUMAN, ANXA1_HUMAN, BAZ1A_HUMAN, SLX4_HUMAN, CTND1_HUMAN, CASP_HUMAN.CUX1_HUMAN, ENOA_HUMAN, EXOS9_HUMAN, KI67_HUMAN, MUS81_HUMAN, NOL9_HUMAN, PHF5A_HUMAN, TBA1B_HUMAN, TBB6_HUMAN, ZBTB2_HUMAN, ZBT25_HUMAN, ZMAT3_HUMAN, SIR6_HUMAN, SIK2_HUMAN, TYK2_HUMAN, LUZP4_HUMAN, PSF1_HUMAN, FP100_HUMAN, ABCE1_HUMAN, PPM1D_HUMAN, BHE41_HUMAN, AR6P4_HUMAN, NOL12_HUMAN, THAP2_HUMAN, PSME3_HUMAN, ECE2_HUMAN, AT5F1_HUMAN, RFA4_HUMAN, SPI2B_HUMAN, GA2L1_HUMAN, CCHL_HUMAN, CMTD1_HUMAN, BASI_HUMAN, SNX16_HUMAN, NUFP1_HUMAN, SEGN_HUMAN, DGUOK_HUMAN, GPN3_HUMAN, DDAH2_HUMAN, CEA21_HUMAN, NRG1_HUMAN, ZC3H3_HUMAN, FGF1_HUMAN, TN13B_HUMAN, NDUF5_HUMAN, PSMD7_HUMAN, GRAP2_HUMAN, TXD11_HUMAN, CCG4_HUMAN, BOD1_HUMAN, ZZZ3_HUMAN, PDPK1_HUMAN, SESN2_HUMAN, NU160_HUMAN, CAH14_HUMAN, S22AI_HUMAN, CIP2A_HUMAN, ERMP1_HUMAN, CATL2_HUMAN, CHSTA_HUMAN, RBM4B_HUMAN, RN146_HUMAN, MINY3_HUMAN, GL1AD_HUMAN.GRL1A_HUMAN.MYZAP_HUMAN, PNKD_HUMAN, ZN589_HUMAN, DCA16_HUMAN, ZN268_HUMAN, ZN707_HUMAN, DPOLB_HUMAN, EPN3_HUMAN, HLAE_HUMAN, LUC7L_HUMAN, AT1B4_HUMAN, SIA8A_HUMAN, SIAT9_HUMAN, CARD8_HUMAN, GNT2A_HUMAN, GLU2B_HUMAN, MKLN1_HUMAN, GID8_HUMAN, NFS1_HUMAN, ACTA_HUMAN, FAD1_HUMAN, KNG1_HUMAN, MICU2_HUMAN, ALG3_HUMAN, SGK1_HUMAN, DCR1C_HUMAN, ZBT44_HUMAN, AL3A2_HUMAN, PI51A_HUMAN, RBM24_HUMAN, PIFO_HUMAN, EMSA1_HUMAN, HELB_HUMAN, SCAPE_HUMAN, PMYT1_HUMAN, GSTM3_HUMAN, PALB2_HUMAN, SYDC_HUMAN, CE112_HUMAN, MYNN_HUMAN, CWC22_HUMAN, TNIP2_HUMAN, ZFP2_HUMAN, ZN394_HUMAN, ZN594_HUMAN, FBF1_HUMAN, DDX4_HUMAN, SP110_HUMAN, FA7_HUMAN, MYO3A_HUMAN, DREB_HUMAN, DYHC1_HUMAN, ZN169_HUMAN, AMOT_HUMAN, KS6B2_HUMAN, CHD5_HUMAN, A0A0B4J220_HUMAN.CK098_HUMAN, B4DXL2_HUMAN.RHG28_HUMAN, MYG1_HUMAN.Q86UA3_HUMAN, POLH_HUMAN, PHRF1_HUMAN, ABT1_HUMAN, ACTN3_HUMAN, SAHH_HUMAN, ALDOA_HUMAN, GDIR1_HUMAN, CHSP1_HUMAN, CEBPZ_HUMAN, CHM4A_HUMAN, CHM4B_HUMAN, CSN3_HUMAN, CSRP1_HUMAN, DDX27_HUMAN, DKC1_HUMAN, DUT_HUMAN, EF1B_HUMAN, IF2G_HUMAN, API5_HUMAN, CLH1_HUMAN, DX39A_HUMAN, RNZ2_HUMAN, MCFD2_HUMAN, NLRP1_HUMAN, PFD4_HUMAN, RL13A_HUMAN, TSNAX_HUMAN, EP400_HUMAN, SYFA_HUMAN, PUM3_HUMAN, PESC_HUMAN, LGUL_HUMAN, GLOD4_HUMAN, GUAA_HUMAN, GNL3L_HUMAN, SYHC_HUMAN, ALDOC_HUMAN, EF2_HUMAN, HMGN5_HUMAN, JUPI1_HUMAN, JUPI2_HUMAN, MATR3_HUMAN, PDCD6_HUMAN, RAB2A_HUMAN, P4R3B_HUMAN, ERP29_HUMAN, LASP1_HUMAN, NAMPT_HUMAN, SCOT1_HUMAN, SYSC_HUMAN, SDHA_HUMAN, IMPA1_HUMAN, IPO7_HUMAN, ITPA_HUMAN, MAK16_HUMAN, SYMC_HUMAN, MPP10_HUMAN, RT02_HUMAN, RT07_HUMAN, RT09_HUMAN, MOES_HUMAN, MY18A_HUMAN, DDX18_HUMAN, NSA2_HUMAN, NTAN1_HUMAN, SYFB_HUMAN, GIPC1_HUMAN, PDXK_HUMAN, SERB_HUMAN, OLA1_HUMAN, PDLI1_HUMAN, PELO_HUMAN, PNISR_HUMAN, RPAC1_HUMAN, EF1A2_HUMAN, SELB_HUMAN, TF3C3_HUMAN, PRDX6_HUMAN, SERC_HUMAN, PSA4_HUMAN, PRS7_HUMAN, RBM28_HUMAN, RBM34_HUMAN, BUD31_HUMAN, EIF2D_HUMAN, RL27_HUMAN, RL35A_HUMAN, RL37_HUMAN, RL38_HUMAN, RL39_HUMAN, RPN1_HUMAN, KRR1_HUMAN, ACOD_HUMAN, SC23A_HUMAN, SC23B_HUMAN, RPC3_HUMAN, SRSF2_HUMAN, STMN1_HUMAN, TBL3_HUMAN, TES_HUMAN, THOC6_HUMAN, TKT_HUMAN, UAP1_HUMAN, UBE2N_HUMAN, UGDH_HUMAN, HS105_HUMAN, IQGA1_HUMAN, SERA_HUMAN, HELLS_HUMAN, F8WC89_HUMAN.SAC31_HUMAN, ZYX_HUMAN, AN32B_HUMAN, FMR1_HUMAN, BEX1_HUMAN, BLID_HUMAN, ARY2_HUMAN, THRSP_HUMAN, SHPRH_HUMAN, KIF23_HUMAN, ZN512_HUMAN, KIFC1_HUMAN, DNLI3_HUMAN, ATAD5_HUMAN, CDCA2_HUMAN, UBN2_HUMAN, KI18B_HUMAN, RECQ1_HUMAN, RFX5_HUMAN, NUSAP_HUMAN, MORC3_HUMAN, NEUA_HUMAN, BRD3_HUMAN, ELF2_HUMAN, RLF_HUMAN, LCOR_HUMAN, UBP3_HUMAN, SMC6_HUMAN, ZMAT2_HUMAN, UNG_HUMAN, RSF1_HUMAN, HMGB3_HUMAN, ZN257_HUMAN, MED4_HUMAN, MED20_HUMAN, HERC2_HUMAN, B9D2_HUMAN, CE120_HUMAN, CE128_HUMAN, CP135_HUMAN, FTM_HUMAN, SCLT1_HUMAN, CEP19_HUMAN, DYLT1_HUMAN, STIL_HUMAN, TMM17_HUMAN, SSBP_HUMAN, PLD3A_HUMAN, STK36_HUMAN, TCOF_HUMAN, CHERP_HUMAN, CKAP4_HUMAN, SLAI2_HUMAN, SPTN1_HUMAN, FLNA_HUMAN, LIMA1_HUMAN, SPF45_HUMAN, SF3B1_HUMAN, SF3B5_HUMAN, RU1C_HUMAN, SR140_HUMAN, SMD2_HUMAN, BMS1_HUMAN, ST38L_HUMAN, PPM1B_HUMAN, RO52_HUMAN, E2F7_HUMAN, BCLF1_HUMAN, MYCBP_HUMAN, PCNP_HUMAN, G45IP_HUMAN, CYTB_HUMAN, RCL1_HUMAN, CCD86_HUMAN, CCAR1_HUMAN, KHDR1_HUMAN, ACINU_HUMAN, CWC15_HUMAN, NSRP1_HUMAN, ATP5J_HUMAN, BLMH_HUMAN, CA2D1_HUMAN, ZN526_HUMAN, KI20A_HUMAN, ZN687_HUMAN, EI2BA_HUMAN, ETV6_HUMAN, CARF_HUMAN, DHB4_HUMAN, STRN_HUMAN, SMBP2_HUMAN, PAR6B_HUMAN, SOSB2_HUMAN, ABCD3_HUMAN, P5CR1_HUMAN, RFC2_HUMAN, RFC3_HUMAN, RL36A_HUMAN, DPOG2_HUMAN, IBTK_HUMAN, RAB5C_HUMAN, VAPA_HUMAN, PAR6A_HUMAN, NEIL3_HUMAN, ATLA2_HUMAN, NU153_HUMAN, SORCN_HUMAN, SSRG_HUMAN, SURF6_HUMAN, KIFA3_HUMAN, TINF2_HUMAN, GAR1_HUMAN, TPD52_HUMAN, EMC2_HUMAN, SORT_HUMAN, ZFX_HUMAN, RET_HUMAN, KAD1_HUMAN, PABP4_HUMAN, GANP_HUMAN, EI2BD_HUMAN, SC16A_HUMAN, FBX22_HUMAN, RGMA_HUMAN, NU155_HUMAN, ESPL1_HUMAN, NPA1P_HUMAN, HNRDL_HUMAN, NPM3_HUMAN, RPP38_HUMAN, SDCG3_HUMAN, WDR3_HUMAN, B4GT7_HUMAN, DDX42_HUMAN, FAKD2_HUMAN, ZN609_HUMAN, MYH7B_HUMAN, FBX31_HUMAN, URP2_HUMAN, MAP11_HUMAN, RRP12_HUMAN, HAUS5_HUMAN, SPS2L_HUMAN, EDRF1_HUMAN, STAU2_HUMAN, REPI1_HUMAN, NOG2_HUMAN, P5CR2_HUMAN, CSN7A_HUMAN, FCF1_HUMAN, DDX47_HUMAN, RM27_HUMAN, VATD_HUMAN, RTCB_HUMAN, ESF1_HUMAN, DHX29_HUMAN, NAT10_HUMAN, NKRF_HUMAN, DHX33_HUMAN, REXO4_HUMAN, RTEL1_HUMAN, UBP36_HUMAN, BCORL_HUMAN, RT14_HUMAN, NOC3L_HUMAN, DDX31_HUMAN, ACSL4_HUMAN, EM55_HUMAN, VPS16_HUMAN, RM38_HUMAN, NOL6_HUMAN, RNF41_HUMAN, WAPL_HUMAN, SPAS2_HUMAN, DDX50_HUMAN, DDX54_HUMAN, CORO7_HUMAN, RIOX1_HUMAN, F192A_HUMAN, UTP23_HUMAN, RIOX2_HUMAN, OSBL5_HUMAN, CENPV_HUMAN, NCBP1_HUMAN, POC1B_HUMAN, DJC11_HUMAN, FOXK1_HUMAN, FOXK2_HUMAN, BIN1_HUMAN, GLI1_HUMAN, FNBP1_HUMAN, NKX61_HUMAN, JHD2C_HUMAN, HXA10_HUMAN, HXB9_HUMAN, DLX5_HUMAN, FBP1L_HUMAN, NKX25_HUMAN, SATB2_HUMAN, ZBT10_HUMAN, ALX4_HUMAN, HXC13_HUMAN, HXD13_HUMAN, MA7D3_HUMAN, TXND5_HUMAN, CAMP1_HUMAN, CGBP1_HUMAN, CREM_HUMAN, MYH7_HUMAN, NACC1_HUMAN, NFIC_HUMAN, NFIX_HUMAN, PATZ1_HUMAN, TPM2_HUMAN, SPCS_HUMAN, UBP47_HUMAN, DSRAD_HUMAN, ITF2_HUMAN, FOXB1_HUMAN, GLI2_HUMAN, GLI3_HUMAN, CEP55_HUMAN, CHM1B_HUMAN, LATS1_HUMAN, COR1C_HUMAN, DOC11_HUMAN, PAK4_HUMAN, FOXC2_HUMAN, FOXE1_HUMAN, FOXG1_HUMAN, FOXH1_HUMAN, FOXI2_HUMAN, UBP8_HUMAN, GAN_HUMAN, RND3_HUMAN, RPTOR_HUMAN, MTOR_HUMAN, RAD18_HUMAN, CRY1_HUMAN, CRY2_HUMAN, FOXL1_HUMAN, FOXL2_HUMAN, ALKB3_HUMAN, PSDE_HUMAN, MACD1_HUMAN, FOXQ1_HUMAN, FOXS1_HUMAN, ASXL2_HUMAN, RHOU_HUMAN, 2A5E_HUMAN, 2A5A_HUMAN, OTUB1_HUMAN, ERR2_HUMAN, DPPA4_HUMAN, NANOG_HUMAN, MYCN_HUMAN, RAB5A_HUMAN, RAB7A_HUMAN, LAMP1_HUMAN, ZMIZ1_HUMAN, PAF15_HUMAN, RDH14_HUMAN, COQ9_HUMAN, NDUF8_HUMAN, COQ2_HUMAN, COQ4_HUMAN, COQ5_HUMAN, ITAV_HUMAN, RC3H1_HUMAN, PSMD8_HUMAN, PPHLN_HUMAN, NFAC2_HUMAN, SLBP_HUMAN, ZN131_HUMAN, ELMO1_HUMAN, ELMO2_HUMAN, M3K1_HUMAN, IRS2_HUMAN, ZN746_HUMAN, PA24A_HUMAN, STYX_HUMAN, XRCC1_HUMAN, ZKSC4_HUMAN, ZN174_HUMAN, Z280C_HUMAN, ZN362_HUMAN, SRFB1_HUMAN, SDA1_HUMAN, NOP14_HUMAN, WIZ_HUMAN, MAZ_HUMAN, NOC4L_HUMAN, NUCKS_HUMAN, CATIN_HUMAN, PR38A_HUMAN, NOL10_HUMAN, EYA2_HUMAN, PTPRT_HUMAN, RT21_HUMAN, SRSF9_HUMAN, RT10_HUMAN, NUD16_HUMAN, RT11_HUMAN, RM19_HUMAN, RL36L_HUMAN, CIRBP_HUMAN, RT24_HUMAN, AROS_HUMAN, NMNA1_HUMAN, RM16_HUMAN, TFAM_HUMAN, NOP16_HUMAN, DUS11_HUMAN, DUS16_HUMAN, DUS5_HUMAN, DUS6_HUMAN, CETN1_HUMAN, TBL1Y_HUMAN, H2B1O_HUMAN, HBB_HUMAN, H2B1C_HUMAN.H2B1D_HUMAN, CAH1_HUMAN, PPBI_HUMAN, ARL4C_HUMAN, TALD3_HUMAN, YBOX2_HUMAN, KCC2D_HUMAN, ZN264_HUMAN, HBA_HUMAN, CE295_HUMAN, HBD_HUMAN, POTB3_HUMAN.POTEB_HUMAN, S38A7_HUMAN, PRDM5_HUMAN, PR20A_HUMAN.PR20B_HUMAN.PR20C_HUMAN.PR20D_HUMAN.PR20E_HUMAN, URB2_HUMAN, ZN223_HUMAN, TLR5_HUMAN, DHRS3_HUMAN, RBTN2_HUMAN, CE350_HUMAN, 4ET_HUMAN, ZN318_HUMAN, CTGF_HUMAN, IQCN_HUMAN, IZUM1_HUMAN, CE164_HUMAN, ANO6_HUMAN, ANKH1_HUMAN, SALL2_HUMAN, DDX51_HUMAN, ZN263_HUMAN, TTC8_HUMAN, I17RC_HUMAN, GIP_HUMAN, RECQ4_HUMAN, ALMS1_HUMAN, ZBTB5_HUMAN, ZN346_HUMAN, TRPS1_HUMAN, DOK2_HUMAN, TROAP_HUMAN, OPRM_HUMAN, DQX1_HUMAN, CRYL1_HUMAN, ZN644_HUMAN, KCNJ5_HUMAN, ZN408_HUMAN, ZN214_HUMAN, TULP3_HUMAN, MRAP2_HUMAN, RSBN1_HUMAN, PLCH1_HUMAN, CHM1A_HUMAN, E4F1_HUMAN, RIR2B_HUMAN, Z354C_HUMAN, LONP2_HUMAN, ZN669_HUMAN, ZN550_HUMAN, RICTR_HUMAN, MYL3_HUMAN, ZN311_HUMAN, P3C2A_HUMAN, Z354A_HUMAN, STRBP_HUMAN, AKIP_HUMAN, ZSA5A_HUMAN, APJ_HUMAN, APOA1_HUMAN, ZNF16_HUMAN, SODC_HUMAN, GLE1_HUMAN, FPPS_HUMAN, ZN184_HUMAN, ERF_HUMAN, ZN331_HUMAN, RT18C_HUMAN, ZN816_HUMAN, IL4RA_HUMAN, KAPCB_HUMAN, ZNF48_HUMAN, NKAP_HUMAN, KNOP1_HUMAN, PDGFB_HUMAN, MYO9A_HUMAN, 3BHS2_HUMAN, ZN544_HUMAN, SNX18_HUMAN, ZSC20_HUMAN, RBMS1_HUMAN, HOOK3_HUMAN, PVR_HUMAN, RBM4_HUMAN, TOE1_HUMAN, TRI37_HUMAN, 5HT2C_HUMAN, EVA1B_HUMAN, CEP97_HUMAN, SEN15_HUMAN, IF4E2_HUMAN, TCF25_HUMAN, CDO1_HUMAN, HAUS7_HUMAN, IKZF5_HUMAN, LOX5_HUMAN, RL26L_HUMAN, B3GL1_HUMAN, ZSC31_HUMAN, ZCRB1_HUMAN, GFAP_HUMAN, E9PAV9_HUMAN.GPTC4_HUMAN, SYFM_HUMAN, TSYL6_HUMAN, DD19B_HUMAN, ARHG6_HUMAN, ACADS_HUMAN, ZN281_HUMAN, KAP1_HUMAN, UB2E3_HUMAN, RRP8_HUMAN, SEN2_HUMAN, MKS1_HUMAN, GTSE1_HUMAN, BGAL_HUMAN, GPBP1_HUMAN, HAX1_HUMAN, ZNF2_HUMAN, ZN579_HUMAN, MET17_HUMAN, NF2L3_HUMAN, DHX35_HUMAN, FABD_HUMAN, ALX3_HUMAN, BCD1_HUMAN, PAK5_HUMAN, FXRD1_HUMAN, GLGB_HUMAN, RBM42_HUMAN, ZN517_HUMAN, MAD3_HUMAN, UXT_HUMAN, TBB8_HUMAN, HSP72_HUMAN, ZCCHV_HUMAN, ZN416_HUMAN, LONM_HUMAN, SNX21_HUMAN, BHA15_HUMAN, PK1IP_HUMAN, ISOC2_HUMAN, MIRO2_HUMAN, EAF6_HUMAN, ALBU_HUMAN, MLF1_HUMAN, EXT2_HUMAN, MED18_HUMAN, KAPCG_HUMAN, ZN574_HUMAN, CD11B_HUMAN, TRI35_HUMAN, PKHG5_HUMAN, IDE_HUMAN, UIF_HUMAN, DEFI6_HUMAN, ACM4_HUMAN, ZN668_HUMAN, ALG13_HUMAN, PTN2_HUMAN, PTN22_HUMAN, PTPRE_HUMAN, FANCC_HUMAN, FANCF_HUMAN, RBG10_HUMAN.RBG1L_HUMAN, MAGA1_HUMAN, IN80B_HUMAN, S7A6O_HUMAN, COX15_HUMAN, ODO2_HUMAN, HCD2_HUMAN, EDEM3_HUMAN, CCND2_HUMAN, PRAF3_HUMAN, B3GT4_HUMAN, EXT1_HUMAN, F185A_HUMAN, RHOA_HUMAN, GOPC_HUMAN, OBF1_HUMAN, TLE3_HUMAN, CENPW_HUMAN, MTF1_HUMAN, MK14_HUMAN, BACD3_HUMAN, DTX4_HUMAN, ADA10_HUMAN, HDGR3_HUMAN, MBD5_HUMAN, SRBP1_HUMAN, HHEX_HUMAN, TELO2_HUMAN, ARC_HUMAN, CDN2B_HUMAN, FGFR4_HUMAN, CENPT_HUMAN, CENPM_HUMAN, ACLY_HUMAN, MP2K3_HUMAN, M3K5_HUMAN, PGFRA_HUMAN, GLIS2_HUMAN, MP2K5_HUMAN, SOX4_HUMAN, FBX7_HUMAN, CYTA_HUMAN, KANL3_HUMAN, SSRD_HUMAN, ZEP2_HUMAN, CEP72_HUMAN, CYTSB_HUMAN, RM11_HUMAN, SIN1_HUMAN, PCGF5_HUMAN, ACON_HUMAN, DX39B_HUMAN, ACACA_HUMAN, ATD3A_HUMAN, CE170_HUMAN, USP9X_HUMAN, ATX2_HUMAN, CCDC6_HUMAN, IF4A1_HUMAN, TBK1_HUMAN, MYCB2_HUMAN, AMRA1_HUMAN, FAS_HUMAN, GEMI4_HUMAN, IQEC1_HUMAN, ATPG_HUMAN, AMER1_HUMAN, GWL_HUMAN, MTMR3_HUMAN, DNJC7_HUMAN, 1C01_HUMAN.1C02_HUMAN.1C03_HUMAN.1C04_HUMAN.1C05_HUMAN.1C06_HUMAN.1C07_HUMAN.1C08_HUMAN.1C12_HUMAN.1C14_HUMAN.1C15_HUMAN.1C16_HUMAN.1C17_HUMAN.1C18_HUMAN, ANR28_HUMAN, PATL1_HUMAN, SIK3_HUMAN, DJB11_HUMAN, ZN106_HUMAN, EDC3_HUMAN, BMP2K_HUMAN, ZN703_HUMAN, SC24B_HUMAN, GATA6_HUMAN, CPIN1_HUMAN, NFAC3_HUMAN, STK3_HUMAN, RANG_HUMAN, AIFM1_HUMAN, SDHB_HUMAN, RM37_HUMAN, SEBP2_HUMAN, F120B_HUMAN, TB182_HUMAN, ECHA_HUMAN, ERP44_HUMAN, ANR17_HUMAN, LIPA1_HUMAN, PRDX3_HUMAN, GCN1_HUMAN, AL1B1_HUMAN, NDUAD_HUMAN, PP6R1_HUMAN, ERRFI_HUMAN, CNOT3_HUMAN, HSP76_HUMAN, TATD2_HUMAN, SCO2_HUMAN, NUP93_HUMAN, ESS2_HUMAN, ZRAB2_HUMAN, ECHB_HUMAN, ISOC1_HUMAN, GNAI3_HUMAN, WRIP1_HUMAN, ELOC_HUMAN, CENPJ_HUMAN, ZN593_HUMAN, SAV1_HUMAN, NAA10_HUMAN, CITE2_HUMAN, CDC7_HUMAN, GFPT1_HUMAN, 1B07_HUMAN.1B08_HUMAN.1B13_HUMAN.1B14_HUMAN.1B15_HUMAN.1B18_HUMAN.1B27_HUMAN.1B35_HUMAN.1B37_HUMAN.1B38_HUMAN.1B39_HUMAN.1B40_HUMAN.1B41_HUMAN.1B42_HUMAN.1B44_HUMAN.1B45_HUMAN.1B46_HUMAN.1B47_HUMAN.1B48_HUMAN.1B49_HUMAN.1B50_HUMAN.1B51_HUMAN.1B52_HUMAN.1B53_HUMAN.1B54_HUMAN.1B55_HUMAN.1B56_HUMAN.1B57_HUMAN.1B58_HUMAN.1B59_HUMAN.1B67_HUMAN.1B73_HUMAN.1B78_HUMAN.1B81_HUMAN.1B82_HUMAN, NU205_HUMAN, SEH1_HUMAN, GCDH_HUMAN, ODPB_HUMAN, GSK3A_HUMAN, TGFB1_HUMAN, UGGG1_HUMAN, ANR11_HUMAN, FOXC1_HUMAN, DSN1_HUMAN, ZWINT_HUMAN, 1A01_HUMAN.1A02_HUMAN.1A03_HUMAN.1A11_HUMAN.1A23_HUMAN.1A24_HUMAN.1A25_HUMAN.1A26_HUMAN.1A29_HUMAN.1A30_HUMAN.1A31_HUMAN.1A32_HUMAN.1A33_HUMAN.1A34_HUMAN.1A36_HUMAN.1A43_HUMAN.1A66_HUMAN.1A68_HUMAN.1A69_HUMAN.1A74_HUMAN.1A80_HUMAN, THIO_HUMAN, ELOB_HUMAN, MAIP1_HUMAN, FAF2_HUMAN, TM10C_HUMAN, MCA3_HUMAN, H90B2_HUMAN, IPO8_HUMAN, MYL1_HUMAN, DCTN1_HUMAN, DNJB6_HUMAN, MIC13_HUMAN, BCR_HUMAN, ECD_HUMAN, UB2G2_HUMAN, TCPW_HUMAN, LSG1_HUMAN, PARG_HUMAN, RBM20_HUMAN, C1TM_HUMAN, CRTC3_HUMAN, P55G_HUMAN, AIP_HUMAN, N4BP2_HUMAN, MLF2_HUMAN, RAF1_HUMAN, MIS12_HUMAN, FAKD5_HUMAN, PEX1_HUMAN, NDUF4_HUMAN, MAEA_HUMAN, TF3C2_HUMAN, ANR54_HUMAN, SCAF8_HUMAN, CREB5_HUMAN, CNDD3_HUMAN, RNC_HUMAN, MCR_HUMAN, UMPS_HUMAN, GEMI2_HUMAN, RCN2_HUMAN, MSI1H_HUMAN, RBM27_HUMAN, NDUA9_HUMAN, LSM7_HUMAN, RPA2_HUMAN, NU107_HUMAN, KBL_HUMAN, HDHD5_HUMAN, EAPP_HUMAN, QTRT2_HUMAN, CLPX_HUMAN, LPIN1_HUMAN, THOC3_HUMAN, M4K4_HUMAN, GEMI6_HUMAN, NDUF3_HUMAN, IP3KC_HUMAN, M1IP1_HUMAN, NUBP2_HUMAN, MCCB_HUMAN, S11IP_HUMAN, RHG39_HUMAN, PARP4_HUMAN, FANCI_HUMAN, SPC24_HUMAN, ETAA1_HUMAN, NCOA4_HUMAN, SC24A_HUMAN, FLII_HUMAN, EYA4_HUMAN, HXK2_HUMAN, NAB1_HUMAN, CDK14_HUMAN, MKNK1_HUMAN, MEX3A_HUMAN, PTOV1_HUMAN, SLIRP_HUMAN, TGS1_HUMAN, ZIC2_HUMAN, NOSIP_HUMAN, MYCPP_HUMAN, IDH3B_HUMAN, 5NT3A_HUMAN, SYSM_HUMAN, DLGP5_HUMAN, PRI1_HUMAN, COQ8A_HUMAN, PITX1_HUMAN, DHC24_HUMAN, NU188_HUMAN, AKP13_HUMAN, DRG1_HUMAN, HSDL2_HUMAN, ALEX_HUMAN.GNAS1_HUMAN.GNAS2_HUMAN.GNAS3_HUMAN, MTMRE_HUMAN, PISD_HUMAN, RFOX2_HUMAN, FBX3_HUMAN, GPBL1_HUMAN, SYPM_HUMAN, TISB_HUMAN, STML2_HUMAN, PCM1_HUMAN, TOB2_HUMAN, PARK7_HUMAN, SYRM_HUMAN, PP6R2_HUMAN, GLYC_HUMAN, DDHD1_HUMAN, PDE12_HUMAN, NOM1_HUMAN, RO60_HUMAN, ELP2_HUMAN, INT13_HUMAN, WDR75_HUMAN, SELK_HUMAN, NIN_HUMAN, SUCB1_HUMAN, NUB1_HUMAN, PI4KA_HUMAN, ZN282_HUMAN, CEP85_HUMAN, COPG1_HUMAN, PANK4_HUMAN, FOXN4_HUMAN, PSMF1_HUMAN, FXRD2_HUMAN, DCTN4_HUMAN, GMPPA_HUMAN, INO1_HUMAN, MTMR5_HUMAN, PSD13_HUMAN, CE192_HUMAN, ABHDA_HUMAN, MPLKI_HUMAN, PDD2L_HUMAN, NIPS1_HUMAN, ACDSB_HUMAN, CNOT6_HUMAN, HBP1_HUMAN, TARB1_HUMAN, PIPSL_HUMAN, CNDG2_HUMAN, DPOE3_HUMAN, CEPT1_HUMAN, KIF14_HUMAN, CNO10_HUMAN, APT_HUMAN, ZN507_HUMAN, GAB1_HUMAN, CBSL_HUMAN.CBS_HUMAN, PDPR_HUMAN, PTH2_HUMAN, TIPRL_HUMAN, FEM1B_HUMAN, VGLL4_HUMAN, DNJB1_HUMAN, NUP43_HUMAN, PFD3_HUMAN, MAN1_HUMAN, DVL3_HUMAN, SCFD1_HUMAN, EYA3_HUMAN, SUCB2_HUMAN, TUT4_HUMAN, FOG2_HUMAN, LYPA2_HUMAN, CTF18_HUMAN, SRP54_HUMAN, CTNA1_HUMAN, SYEM_HUMAN, MGRN1_HUMAN, RB3GP_HUMAN, KLF16_HUMAN, STXB4_HUMAN, GLRX3_HUMAN, DUS9_HUMAN, VGLL3_HUMAN, SIVA_HUMAN, NPL4_HUMAN, ZGPAT_HUMAN, LST8_HUMAN, DVL2_HUMAN, MCL1_HUMAN, CENPF_HUMAN, FLCN_HUMAN, TAM41_HUMAN, FEM1A_HUMAN, NDC1_HUMAN, ARI5B_HUMAN, KTU_HUMAN, CND3_HUMAN, Q9H4D1_HUMAN.RIPK4_HUMAN, GLSK_HUMAN, 2ABB_HUMAN, PURA2_HUMAN, B2CL1_HUMAN, TRIB3_HUMAN, MP2K1_HUMAN, BRAF_HUMAN, COPE_HUMAN, GALE_HUMAN, IGF1R_HUMAN, RASK_HUMAN, SYLC_HUMAN, SIK1_HUMAN, IFIX_HUMAN, PTN11_HUMAN, MTG16_HUMAN, I2BP2_HUMAN, SOCS6_HUMAN, WDTC1_HUMAN, RNF31_HUMAN, TNFA_HUMAN, UB2R1_HUMAN, TCF19_HUMAN, SPDLY_HUMAN, INSM1_HUMAN, KMT5B_HUMAN, PADI4_HUMAN, HDGR2_HUMAN, SIR5_HUMAN, JARD2_HUMAN, BAZ2A_HUMAN, ALK_HUMAN, RORG_HUMAN, 1B40_HUMAN, B2MG_HUMAN, LMNB2_HUMAN, PGLT1_HUMAN, 1C07_HUMAN, PYGO1_HUMAN, BCL9_HUMAN, LIN52_HUMAN, TDRD1_HUMAN, H2AZ_HUMAN.H2B2E_HUMAN, AN32E_HUMAN, TRBC2_HUMAN, TCA_HUMAN, BCL9L_HUMAN.PYGO2_HUMAN, GT2D1_HUMAN, MEPCE_HUMAN, CCR5_HUMAN, KCND2_HUMAN, DBP_HUMAN, TLX1_HUMAN, ALG1_HUMAN, SLD5_HUMAN, HIC1_HUMAN, SLK_HUMAN, STX16_HUMAN, CSH1_HUMAN.CSH2_HUMAN, G3P_HUMAN, RET2_HUMAN, MTP_HUMAN, CTNL1_HUMAN, HMX3_HUMAN, RSMN_HUMAN.SNURF_HUMAN, THIK_HUMAN, TIGD6_HUMAN, PDLI5_HUMAN, KGP2_HUMAN, IFRD1_HUMAN, DAPK3_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P52789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hexokinase 2 [Source:HGNC Symbol;Acc:HGNC:4923]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXK2_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENOA_HUMAN, UBQL1_HUMAN, UBQL4_HUMAN, GTR4_HUMAN, PTGDS_HUMAN, KPCE_HUMAN, PRKN_HUMAN, FNTA_HUMAN, H2AV_HUMAN, HEXB_HUMAN, IPO5_HUMAN, NUBP1_HUMAN, PDLI1_HUMAN, PYGL_HUMAN, EGFR_HUMAN, CNBP_HUMAN, BUB3_HUMAN, HYOU1_HUMAN, SPEE_HUMAN, TBCB_HUMAN, TPP2_HUMAN, SYMC_HUMAN, SEP10_HUMAN, NTRK1_HUMAN, HS90A_HUMAN, RAD18_HUMAN, IRF3_HUMAN, FOXB1_HUMAN, FOXH1_HUMAN, FOXI2_HUMAN, FOXL1_HUMAN, FOXL2_HUMAN, COQ9_HUMAN, NDUA4_HUMAN, NMES1_HUMAN, HXK1_HUMAN, HXK3_HUMAN, EGLN3_HUMAN, FBXW7_HUMAN, CNOT2_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGF_HUMAN, FNTB_HUMAN, HEXA_HUMAN, SHC1_HUMAN, GRB2_HUMAN, SOS1_HUMAN, AP2C_HUMAN, RBX1_HUMAN, CUL1_HUMAN, SKP1_HUMAN, UBE2B_HUMAN, HBEGF_HUMAN, ERBB2_HUMAN, CDC37_HUMAN, ERBIN_HUMAN, IRF7_HUMAN, NOTC3_HUMAN, NC2A_HUMAN, NGF_HUMAN, NTRK1_HUMAN.TFG_HUMAN.TPR_HUMAN, P85A_HUMAN, GAB1_HUMAN, PLCG1_HUMAN, BUB1B_HUMAN, CDC20_HUMAN, MD2L1_HUMAN, STING_HUMAN, TBK1_HUMAN, NALP4_HUMAN, DTX4_HUMAN, ISG15_HUMAN, SNCAP_HUMAN, PIN1_HUMAN, CBL_HUMAN, FRS2_HUMAN, CRKL_HUMAN, RPGF1_HUMAN, KDIS_HUMAN, CRK_HUMAN, L1CAM_HUMAN, VEGFA_HUMAN, SRC_HUMAN, SHB_HUMAN, FAK1_HUMAN, VGFR2_HUMAN, ATX3_HUMAN, SUMO1_HUMAN, GPNMB_HUMAN, PINK1_HUMAN, FKBP6_HUMAN, NOS3_HUMAN, SMAD4_HUMAN, NKX25_HUMAN, SMAD2_HUMAN, RHG32_HUMAN, IQEC1_HUMAN, SDC3_HUMAN, TGFA_HUMAN, GNAI1_HUMAN, GNAI3_HUMAN, HDAC6_HUMAN, TERT_HUMAN, AKT1_HUMAN, KS6B1_HUMAN, MTOR_HUMAN, NED4L_HUMAN, GCR_HUMAN, FKBP5_HUMAN, ACAP1_HUMAN, CLH1_HUMAN, STK11_HUMAN, PAR6A_HUMAN, PAR3_HUMAN, PDPK1_HUMAN, PK3CB_HUMAN, NTF3_HUMAN, 1433S_HUMAN, RGS19_HUMAN, GIPC1_HUMAN, EREG_HUMAN, ERBB3_HUMAN, NRG4_HUMAN, ERBB4_HUMAN, HIF1A_HUMAN, MATK_HUMAN, ITB3_HUMAN, VTNC_HUMAN, ITAV_HUMAN, LCAP_HUMAN, VAMP2_HUMAN, BUB1_HUMAN, P73_HUMAN, TRPV1_HUMAN, AREG_HUMAN, BTC_HUMAN, ABL1_HUMAN, GBG2_HUMAN, GBB1_HUMAN, NRG1_HUMAN, PPP5_HUMAN, FAIM1_HUMAN, DCP1A_HUMAN, FBW1A_HUMAN, AIP_HUMAN, AHR_HUMAN, AKAP9_HUMAN, PKN1_HUMAN, 2A5D_HUMAN, KAP3_HUMAN, PP1A_HUMAN, UB2R1_HUMAN, ANDR_HUMAN, MUC1_HUMAN, STAT3_HUMAN, SHIP2_HUMAN, RGS16_HUMAN, PLEC_HUMAN, ARF4_HUMAN, K1C18_HUMAN, RASA1_HUMAN, PLD1_HUMAN, KPCA_HUMAN, NCK2_HUMAN, NCK1_HUMAN, RIPK1_HUMAN, MP2K1_HUMAN, P3C2B_HUMAN, I17RD_HUMAN, CSK_HUMAN, KAP0_HUMAN, PTK6_HUMAN, ERRFI_HUMAN, STABP_HUMAN, PTN1_HUMAN, HD_HUMAN, STA5A_HUMAN, C2D1A_HUMAN, GRB10_HUMAN, SOCS1_HUMAN, STAT1_HUMAN, PTN11_HUMAN, M3K14_HUMAN, PAK1_HUMAN, PTN6_HUMAN, STA5B_HUMAN, DOK2_HUMAN, VAV2_HUMAN, VAV_HUMAN, CBLB_HUMAN, CAV1_HUMAN, CBLC_HUMAN, PLS1_HUMAN, K1C17_HUMAN, K2C8_HUMAN, K2C7_HUMAN, SMD2_HUMAN, ATX2_HUMAN, SOCS3_HUMAN, MK01_HUMAN, TGFR1_HUMAN, M3K1_HUMAN, IKKE_HUMAN, M3K7_HUMAN, NFKB2_HUMAN, M3K3_HUMAN, IKKB_HUMAN, IKKA_HUMAN, MAVS_HUMAN, FOS_HUMAN, CAV2_HUMAN, MAFB_HUMAN, A4_HUMAN, TLR4_HUMAN, AT1A1_HUMAN, TIRAP_HUMAN, S10A7_HUMAN, CLCA_HUMAN, FKBP4_HUMAN, JAK2_HUMAN, EP300_HUMAN, PML_HUMAN, TOM70_HUMAN, JAK1_HUMAN, PO2F1_HUMAN, ARNT_HUMAN, RELB_HUMAN, ADAP1_HUMAN, FKBP8_HUMAN, HERC3_HUMAN, CBP_HUMAN, SUZ12_HUMAN, HERC5_HUMAN, IFIT1_HUMAN, IRF5_HUMAN, RING2_HUMAN, EGR1_HUMAN, TF2B_HUMAN, EZH2_HUMAN, NOD1_HUMAN, BMI1_HUMAN, IRAK1_HUMAN, CASP1_HUMAN, RAF1_HUMAN, CASP7_HUMAN, SMAD3_HUMAN, MYD88_HUMAN, TCAM1_HUMAN, NLRP3_HUMAN, PPIB_HUMAN, EGLN1_HUMAN, TMED7_HUMAN, G3P_HUMAN, MK08_HUMAN, SQSTM_HUMAN, ITB4_HUMAN, LEG3_HUMAN, LYN_HUMAN, RNZ2_HUMAN, EGLN2_HUMAN, 1433E_HUMAN, HOIL1_HUMAN, ADRB2_HUMAN, PP14A_HUMAN, EED_HUMAN, S10A9_HUMAN, MX1_HUMAN, EPAS1_HUMAN, DDX58_HUMAN, TANK_HUMAN, BAX_HUMAN, BAG1_HUMAN, AT1B1_HUMAN, UBC_HUMAN, PIAS4_HUMAN, RO52_HUMAN, SGTA_HUMAN, CHD8_HUMAN, MK09_HUMAN, XPO1_HUMAN, 1433Z_HUMAN, NEMO_HUMAN, HXC10_HUMAN, 4F2_HUMAN, ITBP2_HUMAN, KCNH2_HUMAN, SEC13_HUMAN, TLR2_HUMAN, CASP3_HUMAN, TBA1A_HUMAN, FAK2_HUMAN, UBB_HUMAN, NFAT5_HUMAN, HSP74_HUMAN, XIAP_HUMAN, BIRC5_HUMAN, ACSF2_HUMAN, ZFN2B_HUMAN, GOLM1_HUMAN, EXOC7_HUMAN, ACD_HUMAN, PYGM_HUMAN, RIPK2_HUMAN, PDCD5_HUMAN, HXK2_HUMAN, RIOK3_HUMAN, GAN_HUMAN, MET_HUMAN, 1A66_HUMAN, TERF1_HUMAN, REL_HUMAN, COQ8A_HUMAN, LNX1_HUMAN, MYC_HUMAN, SRC8_HUMAN, ZN746_HUMAN, BACH_HUMAN, NDK3_HUMAN, AFF4_HUMAN, ATD3B_HUMAN, CDK15_HUMAN, PLAK_HUMAN, HSPB2_HUMAN, AGR2_HUMAN, MIRO1_HUMAN, AF17_HUMAN, SLF1_HUMAN, ITA1_HUMAN, GCFC2_HUMAN, SLF2_HUMAN, GORS2_HUMAN, SYN1_HUMAN, PTPRG_HUMAN, SSXT_HUMAN, PSMD4_HUMAN, GSC2_HUMAN, SEPT7_HUMAN, TRI56_HUMAN, HSP13_HUMAN, TB182_HUMAN, ULK1_HUMAN, CRBA1_HUMAN, MLP3C_HUMAN, GBRL1_HUMAN, PPIC_HUMAN, ERCC1_HUMAN, HSP7C_HUMAN, PIWL1_HUMAN, SH3G2_HUMAN, CTAG2_HUMAN, ADRM1_HUMAN, BAKOR_HUMAN, PK3C3_HUMAN, RUBIC_HUMAN, BECN1_HUMAN, UVRAG_HUMAN, Q17RA0_HUMAN, KR196_HUMAN, SIL1_HUMAN, NOTC1_HUMAN, SNP25_HUMAN, MFN2_HUMAN, HEY1_HUMAN, HS71B_HUMAN.HSP77_HUMAN, PLCG2_HUMAN, SH2B1_HUMAN, SKP2_HUMAN, EDAD_HUMAN, TAB2_HUMAN, SLAP1_HUMAN, RL35A_HUMAN, ANF_HUMAN, NB5R1_HUMAN, PHOCN_HUMAN, MAST1_HUMAN, Q6PK50_HUMAN, IR3IP_HUMAN, AGO2_HUMAN, TXD12_HUMAN, TRI27_HUMAN, CRX_HUMAN, DPOLB_HUMAN, HS90B_HUMAN, MYLK2_HUMAN, FBX7_HUMAN, SH2B3_HUMAN, BEX1_HUMAN, NDOR1_HUMAN, THIO_HUMAN, RL31_HUMAN, SE6L1_HUMAN, UBC9_HUMAN, LIS1_HUMAN, NUDC2_HUMAN, TNR6B_HUMAN, TGFI1_HUMAN, TPC2A_HUMAN.TPC2B_HUMAN, ANXA2_HUMAN, KS6A2_HUMAN, PPIP1_HUMAN, CK001_HUMAN, K1C40_HUMAN, UBE3A_HUMAN, CCDC6_HUMAN.RET_HUMAN, GRAP2_HUMAN, KNL1_HUMAN, TEBP_HUMAN, ARF6_HUMAN, OS9_HUMAN, ZFHX3_HUMAN, TBA1A_HUMAN.TBA1B_HUMAN, ERP29_HUMAN, A0A075B738_HUMAN.PECA1_HUMAN, ZN503_HUMAN, ESR1_HUMAN, ANS1B_HUMAN, DNJB2_HUMAN, UBS3B_HUMAN, ROR1_HUMAN, KR123_HUMAN, BATF2_HUMAN, TELT_HUMAN, MOAP1_HUMAN, JSPR1_HUMAN, BIP_HUMAN, SRBS2_HUMAN, EP15R_HUMAN, ESR2_HUMAN, HRSL1_HUMAN, S10A4_HUMAN, GOGA2_HUMAN, ITB2_HUMAN, MATR3_HUMAN, ARI5A_HUMAN, EBP2_HUMAN, TRI23_HUMAN, UB2V2_HUMAN, UBE2N_HUMAN, HLTF_HUMAN, TNR6A_HUMAN, NAL12_HUMAN, RBP2_HUMAN, EXOC4_HUMAN, PEX19_HUMAN, SC61B_HUMAN, DLG1_HUMAN, 7B2_HUMAN, CHSS2_HUMAN, CAN7_HUMAN, IST1_HUMAN, PSN2_HUMAN, UBQL2_HUMAN, ACTN4_HUMAN, GRP75_HUMAN, EXOC6_HUMAN, RS27A_HUMAN.UBC_HUMAN, SH22A_HUMAN, NUMBL_HUMAN, CSK2B_HUMAN, STIP1_HUMAN, DJC13_HUMAN, RBNS5_HUMAN, SYQ_HUMAN, RIN1_HUMAN, CTG1B_HUMAN, HEXDC_HUMAN, SMAD1_HUMAN, COF1_HUMAN, ERP27_HUMAN, CRCM_HUMAN, APOC4_HUMAN, ATF4_HUMAN, TRAF2_HUMAN, TENS3_HUMAN, EXOC8_HUMAN, SRGN_HUMAN, UD17_HUMAN, PR15A_HUMAN, EXOC3_HUMAN, PSA7_HUMAN, UB2V1_HUMAN, CNOT1_HUMAN, 1433T_HUMAN, TAU_HUMAN, IP6K2_HUMAN, PHF5A_HUMAN, NXF1_HUMAN, JIP1_HUMAN, ORC2_HUMAN, PHAG1_HUMAN, KPCB_HUMAN, PIN4_HUMAN, RNF11_HUMAN, LSM1_HUMAN, FOXJ2_HUMAN, YES_HUMAN, MLP3A_HUMAN, HSDL2_HUMAN, NEDD4_HUMAN, TRI32_HUMAN, CNOT6_HUMAN, MITF_HUMAN, ZG16_HUMAN, ANS1A_HUMAN, RAGE_HUMAN, SFR19_HUMAN, STMN1_HUMAN, HDHD3_HUMAN, LAP4B_HUMAN, MAX_HUMAN, DICER_HUMAN, UBXN7_HUMAN, AURKA_HUMAN, ECHP_HUMAN.TBA8_HUMAN, RD23A_HUMAN, UBXN1_HUMAN, FZD7_HUMAN, GBRD_HUMAN, PURA_HUMAN, ATIF1_HUMAN, BAG6_HUMAN, TRAF6_HUMAN, MI4GD_HUMAN, NGLY1_HUMAN, PNMA1_HUMAN, RACK1_HUMAN, ABL2_HUMAN, P55G_HUMAN, LIGO1_HUMAN, LCP2_HUMAN, PCNA_HUMAN, CC136_HUMAN, MYDGF_HUMAN, FKBP2_HUMAN, P85B_HUMAN, CTBP2_HUMAN, RPN1_HUMAN, CBPC1_HUMAN, GKAP1_HUMAN, RL7_HUMAN, Q9BVE2_HUMAN, AR6P1_HUMAN, CASP8_HUMAN, DESM_HUMAN, CSTF2_HUMAN, IRS1_HUMAN, HNRL1_HUMAN, PCBP1_HUMAN, EF2_HUMAN, SPTB2_HUMAN, WEE1_HUMAN, HSPB1_HUMAN, PDC6I_HUMAN, SIAS_HUMAN, COPB_HUMAN, SC5A1_HUMAN, H2BFS_HUMAN, SPCS2_HUMAN, PP2AB_HUMAN, EKI1_HUMAN, RT29_HUMAN, A0A0A0MT22_HUMAN.PTPRC_HUMAN.X6R433_HUMAN, STAM2_HUMAN, KRA31_HUMAN, KR107_HUMAN, CNOT8_HUMAN, HTF4_HUMAN, ATPB_HUMAN, PTPRO_HUMAN, AKT3_HUMAN, EXOC2_HUMAN, MCM7_HUMAN, DHB12_HUMAN, ARBK1_HUMAN, MIF_HUMAN, SYEP_HUMAN, GBRAP_HUMAN, PTPRB_HUMAN, GHRL_HUMAN, ARRB2_HUMAN, D0VY79_HUMAN, GIT2_HUMAN, SH3K1_HUMAN, GPS2_HUMAN, DP13A_HUMAN, TM1L1_HUMAN, ZAP70_HUMAN, PR40A_HUMAN, IQGA1_HUMAN, BCL6_HUMAN, STAT2_HUMAN, CALM1_HUMAN.CALM2_HUMAN.CALM3_HUMAN, PABP3_HUMAN, FHL1_HUMAN, ACACA_HUMAN, ARBK2_HUMAN, Q5U5U6_HUMAN, MDM2_HUMAN, UFO_HUMAN, PSMD6_HUMAN, NUP58_HUMAN, UB2L6_HUMAN, RL3_HUMAN, JIP2_HUMAN, BRAF_HUMAN.K1549_HUMAN, SCMH1_HUMAN, KR108_HUMAN, FGR_HUMAN, PGPS1_HUMAN, BRX1_HUMAN, H2B2F_HUMAN, JUN_HUMAN, IMDH2_HUMAN, PTPRJ_HUMAN, ARL4C_HUMAN, LASP1_HUMAN, SET_HUMAN, PDCD2_HUMAN, GT252_HUMAN, TGFB1_HUMAN, RAB7A_HUMAN, CAVN1_HUMAN, KRA71_HUMAN, EHD4_HUMAN, CAV3_HUMAN, GDIA_HUMAN, LAT_HUMAN, PTN22_HUMAN, HNRPD_HUMAN, CSK21_HUMAN, MCA3_HUMAN, XPF_HUMAN, FAAA_HUMAN, PCH2_HUMAN, TFE2_HUMAN, MYOME_HUMAN, CALU_HUMAN, ITSN2_HUMAN, GFAP_HUMAN, CHIP_HUMAN, STAP2_HUMAN, IBP3_HUMAN, NDRG1_HUMAN, HSF4_HUMAN, WRP73_HUMAN, RNF4_HUMAN, ORML1_HUMAN, PSN1_HUMAN, VDAC1_HUMAN, TMOD1_HUMAN, HXA1_HUMAN, ANXA1_HUMAN.B5BU38_HUMAN, TM14C_HUMAN, APBB1_HUMAN, S10A6_HUMAN, TRIM8_HUMAN, PCGF6_HUMAN, HDAC3_HUMAN, AHSA1_HUMAN, WAC_HUMAN, BMP10_HUMAN, CNO6L_HUMAN, LAMB1_HUMAN, CCHCR_HUMAN, INHBB_HUMAN, CDIP1_HUMAN, JPH4_HUMAN, FRK_HUMAN, UBXN4_HUMAN, PA2G4_HUMAN, Q86WV8_HUMAN, RFA3_HUMAN, PA1B2_HUMAN, GRIP1_HUMAN, M3K12_HUMAN, AHNK_HUMAN, CYLC2_HUMAN, PRKDC_HUMAN, FINC_HUMAN, MMS22_HUMAN, USMG5_HUMAN, LRRK2_HUMAN, TEKT3_HUMAN, NFKB1_HUMAN, TCTP_HUMAN, K1H1_HUMAN, NMDE2_HUMAN, ATPG_HUMAN, CNDH2_HUMAN, RAB3A_HUMAN, 1A26_HUMAN, SCYL2_HUMAN, LRP1_HUMAN, VAPA_HUMAN, PDIA1_HUMAN, GLIS3_HUMAN, KDM2A_HUMAN, ROA1_HUMAN, CCNE1_HUMAN, EPS15_HUMAN, RABX5_HUMAN, CADH1_HUMAN, CBR1_HUMAN, SPAG8_HUMAN, FES_HUMAN, ITK_HUMAN, RET_HUMAN, RL1D1_HUMAN, PPM1F_HUMAN, KR133_HUMAN, CDK9_HUMAN, TRADD_HUMAN, SRSF6_HUMAN, SH21A_HUMAN, GELS_HUMAN, MAPK3_HUMAN, TRM2A_HUMAN, GSDMA_HUMAN, A2ML1_HUMAN, SPB3_HUMAN, RL24_HUMAN, MK06_HUMAN, MMP2_HUMAN, IF2P_HUMAN, 1B42_HUMAN, LCK_HUMAN, ADIPO_HUMAN, WASL_HUMAN, VHL_HUMAN, CNOT3_HUMAN, RHXF2_HUMAN, MPIP3_HUMAN, HRSL2_HUMAN, ZN510_HUMAN, RIPK3_HUMAN, PDIA5_HUMAN, IKBE_HUMAN, DYRK4_HUMAN, RASH_HUMAN, TEAD1_HUMAN, PAN3_HUMAN, TNR6C_HUMAN, RL40_HUMAN.UBC_HUMAN, ZIC1_HUMAN, IMA5_HUMAN, TF65_HUMAN, PI42B_HUMAN, DYH6_HUMAN, LDB2_HUMAN, HNRPR_HUMAN, RS27_HUMAN, PELI2_HUMAN, PIWL4_HUMAN, ATX1L_HUMAN, SRGEF_HUMAN, 5NT3A_HUMAN, RASF5_HUMAN, TRI25_HUMAN, FOG2_HUMAN, DYLT3_HUMAN, KSYK_HUMAN, CSTFT_HUMAN, RS3A_HUMAN, NS1BP_HUMAN, TAB1_HUMAN, TP4A3_HUMAN, HDAC7_HUMAN, OAZ1_HUMAN, RAP2A_HUMAN, MYCN_HUMAN, CSRP1_HUMAN, ZN655_HUMAN, SHC4_HUMAN, PBIP1_HUMAN, KPYM_HUMAN, ATF2_HUMAN, NPM_HUMAN.RARA_HUMAN, HGS_HUMAN, UCHL1_HUMAN, ENPL_HUMAN, PTN12_HUMAN, ATX1_HUMAN, KIF2C_HUMAN, GBRL2_HUMAN, CDK1_HUMAN, ARI1B_HUMAN, IKZF3_HUMAN, AP2A1_HUMAN, EEA1_HUMAN, KSR2_HUMAN, PIM1_HUMAN, CHK2_HUMAN, MED13_HUMAN, RAC1_HUMAN, KR197_HUMAN, SEMG1_HUMAN, SLAP2_HUMAN, AP4M1_HUMAN, MAGD1_HUMAN, GRAA_HUMAN, CKLF8_HUMAN, MK07_HUMAN, MLH1_HUMAN, CDK2_HUMAN, MLP3B_HUMAN, HMOX1_HUMAN, GALT2_HUMAN, SGCG_HUMAN, SORT_HUMAN, S10A2_HUMAN, PGTB1_HUMAN, CK049_HUMAN, ARPC5_HUMAN, H2A2B_HUMAN, PTPR2_HUMAN, SAFB2_HUMAN, UBP7_HUMAN, CERS2_HUMAN, EAPP_HUMAN, PDLI7_HUMAN, CC117_HUMAN, F10A1_HUMAN, TFP11_HUMAN, PKN2_HUMAN, H2B1H_HUMAN, CDK4_HUMAN, SGK1_HUMAN, PLCE1_HUMAN, TTC9C_HUMAN, UBP19_HUMAN, SMAD9_HUMAN, TRBP2_HUMAN, RGS2_HUMAN, CD59_HUMAN, TLX3_HUMAN, EF1G_HUMAN, DHX9_HUMAN, ARRB1_HUMAN, RGS4_HUMAN, IBP6_HUMAN, PAF1_HUMAN, PIWL2_HUMAN, HNRPQ_HUMAN, FLNC_HUMAN, CHIA_HUMAN, SPT4H_HUMAN, AP2M1_HUMAN, ADT1_HUMAN, MIC60_HUMAN, EF1A1_HUMAN, BMX_HUMAN, NCOA3_HUMAN, EIF3E_HUMAN, KPCZ_HUMAN, CREB3_HUMAN, RBL1_HUMAN, CTND1_HUMAN, CBX5_HUMAN, BLK_HUMAN, NOTO_HUMAN, AGAL_HUMAN, NKAP_HUMAN, CAMLG_HUMAN, HCK_HUMAN, FBXW2_HUMAN, PAI1_HUMAN, 1433B_HUMAN, DJB11_HUMAN, CCD39_HUMAN, TLN1_HUMAN, DAXX_HUMAN, TITIN_HUMAN, KR111_HUMAN, CALD1_HUMAN, SGT1_HUMAN, GLT12_HUMAN, SOCS6_HUMAN, PLCH1_HUMAN, PTN_HUMAN, PICK1_HUMAN, AKA12_HUMAN, PRDX1_HUMAN, AMHR2_HUMAN, AMPO_HUMAN, DTX2_HUMAN, PTCD3_HUMAN, A6NNN6_HUMAN.E7ETA6_HUMAN.PCM1_HUMAN.RET_HUMAN, SPICE_HUMAN, ITB1_HUMAN, F16P2_HUMAN, TPIS_HUMAN, TINF2_HUMAN, KAP1_HUMAN, DOK1_HUMAN, VIGLN_HUMAN, YYAP1_HUMAN, RXRA_HUMAN, TEKT5_HUMAN, APC4_HUMAN, NEK2_HUMAN, PYGB_HUMAN, IRS4_HUMAN, NECD_HUMAN, PHLA3_HUMAN, STX3_HUMAN, MD2BP_HUMAN, MK14_HUMAN, ZBT22_HUMAN, ATP23_HUMAN, VIME_HUMAN, RL37A_HUMAN, SNX9_HUMAN, ALDOA_HUMAN, RAPH1_HUMAN, TOM20_HUMAN, RNPS1_HUMAN, PTN18_HUMAN, PARP2_HUMAN, UBE2A_HUMAN, RAD51_HUMAN, RL26_HUMAN, FOXD2_HUMAN, KS6A5_HUMAN, NCBP1_HUMAN, CD99_HUMAN, PLPL2_HUMAN, B3KQG4_HUMAN, RBM10_HUMAN, LAMP1_HUMAN, CNTN2_HUMAN, TS101_HUMAN, CASP_HUMAN, SNX1_HUMAN, DCTN2_HUMAN, TRIB2_HUMAN, WBP4_HUMAN, DMPK_HUMAN, SNPC3_HUMAN, H15_HUMAN, SNF5_HUMAN, ELF5_HUMAN, THA_HUMAN, RETR1_HUMAN, RL23A_HUMAN, OAT_HUMAN, DAPK1_HUMAN, PR20D_HUMAN.PR20E_HUMAN, TRAF1_HUMAN, SALL2_HUMAN, FAS_HUMAN, SMC1A_HUMAN, WRIP1_HUMAN, HNRPC_HUMAN, VP33B_HUMAN, AAKB1_HUMAN, KPCD1_HUMAN, ZN207_HUMAN, PARVA_HUMAN, CHD5_HUMAN, STX17_HUMAN, CD37L_HUMAN, CO9A3_HUMAN, HSF2B_HUMAN, IKBB_HUMAN, PGFRA_HUMAN, RS16_HUMAN, DNJC4_HUMAN, SPY2_HUMAN, DYHC1_HUMAN, BRMS1_HUMAN, SYUA_HUMAN, SOS2_HUMAN, ROAA_HUMAN, NUMB_HUMAN, ENOG_HUMAN, P5CS_HUMAN, HEM4_HUMAN, ITSN1_HUMAN, M4K4_HUMAN, RBPMS_HUMAN, DVL1_HUMAN, FANCC_HUMAN, RB11A_HUMAN, NUP62_HUMAN, SH3L3_HUMAN, TFE3_HUMAN, THOC1_HUMAN, HLX_HUMAN, GCSAM_HUMAN, ANXA5_HUMAN, IF2B2_HUMAN, DESP_HUMAN, MSX2_HUMAN, Q96D37_HUMAN, RL36_HUMAN, H31_HUMAN, SHPRH_HUMAN, CNOT9_HUMAN, IF2B3_HUMAN, M3K8_HUMAN, UBS3A_HUMAN, CNO10_HUMAN, NOE1_HUMAN, TCAM2_HUMAN, SH3G3_HUMAN, ROA3_HUMAN, PIAS2_HUMAN, USH1C_HUMAN, DTBP1_HUMAN, CSN1_HUMAN, SUMF2_HUMAN, GSHB_HUMAN, MID49_HUMAN, TENS4_HUMAN, AP3D1_HUMAN, PDK3_HUMAN, EXT2_HUMAN, CPSF6_HUMAN, IF2B1_HUMAN, NCOR1_HUMAN, BCAS3_HUMAN.BCAS4_HUMAN, NPHP1_HUMAN, KRA33_HUMAN, P53_HUMAN, ARHG7_HUMAN, CCL21_HUMAN.Q6ICR7_HUMAN, B7Z2Q3_HUMAN.CCD14_HUMAN, RBCC1_HUMAN, SEPP1_HUMAN, EFHC1_HUMAN, COA7_HUMAN, CC150_HUMAN, UBA1_HUMAN, CAC1A_HUMAN, MDHC_HUMAN, A0A087X1W2_HUMAN.ANM1_HUMAN.H7C2I1_HUMAN, P3C2A_HUMAN, NTRK2_HUMAN, XPA_HUMAN, HEY2_HUMAN, RBMX_HUMAN, ACL6B_HUMAN, TNNT1_HUMAN, SF3A2_HUMAN, HEMGN_HUMAN, CTNA1_HUMAN, ACES_HUMAN, MCM5_HUMAN, MGN_HUMAN, KCTD9_HUMAN, AN32B_HUMAN, DYN2_HUMAN, TNR1A_HUMAN, UB2L3_HUMAN, BAIP2_HUMAN, WASF3_HUMAN, RL34_HUMAN, SYDC_HUMAN, BHE40_HUMAN, RS19_HUMAN, TNIK_HUMAN, RSF1_HUMAN, Q86WA0_HUMAN, RL35_HUMAN, GAB2_HUMAN, CAB39_HUMAN, UN45B_HUMAN, CNOT7_HUMAN, NUAK2_HUMAN, TP4A2_HUMAN, SRSF2_HUMAN, MTG8_HUMAN.RUNX1_HUMAN, AASD1_HUMAN, ZDHC3_HUMAN, CAC1G_HUMAN, 2A5E_HUMAN, U119A_HUMAN, EZRI_HUMAN, DGKI_HUMAN, SP20H_HUMAN, TNR16_HUMAN, PRGR_HUMAN, CH60_HUMAN, AGK_HUMAN, BRAF_HUMAN, Q9H836_HUMAN, IGLC1_HUMAN.IGLC3_HUMAN, FA2H_HUMAN, PTN2_HUMAN, ANXA1_HUMAN, Q59E96_HUMAN, QSOX1_HUMAN, CCD14_HUMAN, OPRD_HUMAN, CLAT_HUMAN, XRCC6_HUMAN, ARF3_HUMAN, FACR1_HUMAN, MAP1S_HUMAN, VDAC2_HUMAN, SMUF2_HUMAN, TBA4A_HUMAN, ICAM1_HUMAN, EIF2D_HUMAN, ERN1_HUMAN, E2AK3_HUMAN, GNA12_HUMAN, NR2C2_HUMAN, SIM2_HUMAN, MTG8_HUMAN, SCAM1_HUMAN, SCAM3_HUMAN, KCC2A_HUMAN, NOS1_HUMAN, FYN_HUMAN, TENA_HUMAN, CEBPB_HUMAN, ITB5_HUMAN, KCC2G_HUMAN, PLD2_HUMAN, NHRF1_HUMAN, E2AK1_HUMAN, CAC1B_HUMAN, PDLI5_HUMAN, SEPT4_HUMAN, GPR37_HUMAN, SEPT5_HUMAN, SYT11_HUMAN, CXA1_HUMAN, NPT2A_HUMAN, TNR6_HUMAN, GRB7_HUMAN, KAPCA_HUMAN, GRB14_HUMAN, KS6B2_HUMAN, ACTN1_HUMAN, TBB5_HUMAN, PPID_HUMAN, RL23_HUMAN, RL13_HUMAN, RAN_HUMAN, CLH2_HUMAN, GRM5_HUMAN, 41_HUMAN, NMDZ1_HUMAN, CD44_HUMAN, TOM34_HUMAN, NPAS2_HUMAN, AGTR1_HUMAN, K2C1_HUMAN, ACTS_HUMAN, PECA1_HUMAN, DYL1_HUMAN, DEGS1_HUMAN, GCYB1_HUMAN, CSK22_HUMAN, THYG_HUMAN, PDIA4_HUMAN, ARFP1_HUMAN, KLH41_HUMAN, HIF3A_HUMAN, RPGP1_HUMAN, PPARA_HUMAN, E2AK2_HUMAN, FCERB_HUMAN, UB2E1_HUMAN, UBE2C_HUMAN, UBE3C_HUMAN, BHLH9_HUMAN, PITX2_HUMAN, RAP1A_HUMAN, EHD2_HUMAN, AKT2_HUMAN, MK03_HUMAN, DNJA3_HUMAN, CATD_HUMAN, PSA2_HUMAN, PSA6_HUMAN, PSA1_HUMAN, APOB_HUMAN, FOXG1_HUMAN, FRS3_HUMAN, SHBG_HUMAN, VAV3_HUMAN, SNX6_HUMAN, SNX4_HUMAN, SNX2_HUMAN, CD82_HUMAN, HPGDS_HUMAN, BTK_HUMAN, SRFB1_HUMAN, HS71A_HUMAN.HS71B_HUMAN, DNJA1_HUMAN, HSF1_HUMAN, H10_HUMAN, NOTC4_HUMAN, MPIP1_HUMAN, ITA5_HUMAN, GNAI2_HUMAN, TIAM1_HUMAN, MYOD1_HUMAN, GNA13_HUMAN, CFTR_HUMAN, NMDE4_HUMAN, CNN1_HUMAN, CD47_HUMAN, RGRF1_HUMAN, NU214_HUMAN, CD166_HUMAN, CHK1_HUMAN, KSR1_HUMAN, MP2K2_HUMAN, ACOX1_HUMAN, CTNB1_HUMAN, MYH2_HUMAN, PF2R_HUMAN, HIPK2_HUMAN, PARP1_HUMAN, ZBP1_HUMAN, IDHP_HUMAN, PLMN_HUMAN, COPB2_HUMAN, AFAP1_HUMAN, DCE2_HUMAN, DCE1_HUMAN, POLH_HUMAN, REV1_HUMAN, MIS_HUMAN, ZO1_HUMAN, 1433F_HUMAN, CEAM1_HUMAN, MYB_HUMAN, RAG2_HUMAN, RL5_HUMAN, RS7_HUMAN, NU153_HUMAN, ACK1_HUMAN, BMAL1_HUMAN, SYT1_HUMAN, STK35_HUMAN, FER_HUMAN, PGFRB_HUMAN, SERPH_HUMAN, DLDH_HUMAN, BASI_HUMAN, STRN3_HUMAN, MVP_HUMAN, PDIA6_HUMAN, RL40_HUMAN, DNJC7_HUMAN, PPIL2_HUMAN, RNF12_HUMAN, WDR83_HUMAN, KPCD_HUMAN, MCR_HUMAN, F162A_HUMAN, PCBP2_HUMAN, GCYA1_HUMAN, CENPF_HUMAN, GBP1_HUMAN, RASK_HUMAN, RHOB_HUMAN, PAI2_HUMAN, PTPRS_HUMAN, SH2B2_HUMAN, NUP98_HUMAN, ZPR1_HUMAN, CSKP_HUMAN, ACTC_HUMAN, H31T_HUMAN, ELF3_HUMAN, EPHA2_HUMAN, HCDH_HUMAN, HDAC2_HUMAN, HDAC1_HUMAN, AIMP2_HUMAN, PGS2_HUMAN, APC_HUMAN, DPPA3_HUMAN, PRGC1_HUMAN, CXX1_HUMAN.RTL8C_HUMAN, FKB10_HUMAN, MTA1_HUMAN, MAPK2_HUMAN, DC1I2_HUMAN, IRS2_HUMAN, ACTN2_HUMAN, RGS3_HUMAN, GRN_HUMAN, CITE1_HUMAN, FKBPL_HUMAN, CDN1A_HUMAN, PTEN_HUMAN, Q3V639_HUMAN, TGIF1_HUMAN, NMNA2_HUMAN, CDCP1_HUMAN, ILK_HUMAN, SIA10_HUMAN, KTN1_HUMAN, PRR7_HUMAN, TERA_HUMAN, GSK3B_HUMAN, CDX2_HUMAN, PARK7_HUMAN, CALM3_HUMAN, CCAR2_HUMAN, TBCE_HUMAN, M3K11_HUMAN, CSF3R_HUMAN, BAG5_HUMAN, HS71A_HUMAN, FANCA_HUMAN, GRP3_HUMAN, STA13_HUMAN, BAG4_HUMAN, CTF18_HUMAN, HCFC1_HUMAN, CCNA1_HUMAN, RBP1_HUMAN, WASP_HUMAN, SRP19_HUMAN, DUS3_HUMAN, SIM1_HUMAN, DLG4_HUMAN, HOME1_HUMAN, APAF_HUMAN, FNIP1_HUMAN, IGF1R_HUMAN, MYH9_HUMAN, UB2J1_HUMAN, DNJB1_HUMAN, RNF41_HUMAN, VIP1_HUMAN, PRL_HUMAN, FKBP7_HUMAN, CATB_HUMAN, TGFR2_HUMAN, FLT3_HUMAN, HERP1_HUMAN, GCYA2_HUMAN, NCAM1_HUMAN, BACH1_HUMAN, TP53B_HUMAN, CDK5_HUMAN, LIMK1_HUMAN, BAP1_HUMAN, TAF1D_HUMAN, UBP11_HUMAN, PMS1_HUMAN, TPM1_HUMAN, RON_HUMAN, CCD50_HUMAN, POLK_HUMAN, TBG1_HUMAN, PSA4_HUMAN, HDAC4_HUMAN, ATGA1_HUMAN, NIPS2_HUMAN, RS3_HUMAN, RS6_HUMAN, SIN3A_HUMAN, UBP8_HUMAN, SRBP1_HUMAN, CSN3_HUMAN, MP2K5_HUMAN, DDB1_HUMAN, EWS_HUMAN, EPN1_HUMAN, SC6A3_HUMAN, LRIG1_HUMAN, CD11B_HUMAN, NCOR2_HUMAN, SRRM2_HUMAN, SP1_HUMAN, PRS8_HUMAN, FACD2_HUMAN, FANCI_HUMAN, SMYD2_HUMAN, ANM5_HUMAN, KLF5_HUMAN, MO4L1_HUMAN, MO4L2_HUMAN, MRGBP_HUMAN, CDC7_HUMAN, HTRA2_HUMAN, BCL2_HUMAN, HES1_HUMAN, DPOLN_HUMAN, SIAH2_HUMAN, CUL5_HUMAN, P4K2B_HUMAN, P4K2A_HUMAN, H2AX_HUMAN, AMRA1_HUMAN, CCNE2_HUMAN, H2A1A_HUMAN, FGFR3_HUMAN, RN185_HUMAN, NRAM2_HUMAN, MFN1_HUMAN, ERR2_HUMAN, CD5R1_HUMAN, UB2E2_HUMAN, ICT1_HUMAN, AAPK1_HUMAN, AGO4_HUMAN, PRP19_HUMAN, CD4_HUMAN, BCR_HUMAN, NFIP1_HUMAN, NFIP2_HUMAN, LEG1_HUMAN, DCR1C_HUMAN, HDAC5_HUMAN, MYCD_HUMAN, DNM1L_HUMAN, C1QBP_HUMAN, KPCI_HUMAN, ZWINT_HUMAN, LST2_HUMAN, INSI2_HUMAN, ACTA_HUMAN, NBN_HUMAN, NF2L1_HUMAN, DRA_HUMAN, 2B11_HUMAN.2B13_HUMAN.2B14_HUMAN.2B17_HUMAN.2B18_HUMAN.2B19_HUMAN.2B1A_HUMAN.2B1B_HUMAN.2B1C_HUMAN.2B1D_HUMAN.2B1E_HUMAN.2B1F_HUMAN.2B1G_HUMAN, DRB3_HUMAN, DRB4_HUMAN, DRB5_HUMAN, RBL2_HUMAN, PSA3_HUMAN, GLCM_HUMAN, SVIL_HUMAN, CDC27_HUMAN, OTU7B_HUMAN, F16P1_HUMAN, ATR_HUMAN, RAD21_HUMAN, HDGF_HUMAN, CDC73_HUMAN, SIR1_HUMAN, KAT5_HUMAN, UBP2_HUMAN, YAP1_HUMAN, PSMD2_HUMAN, SPRTN_HUMAN, SIR7_HUMAN, ARF5_HUMAN, SDF2L_HUMAN, NSF_HUMAN, PRS6A_HUMAN, SPRC_HUMAN, STMN3_HUMAN, TADBP_HUMAN, CD2AP_HUMAN, ALG2_HUMAN, MKKS_HUMAN, RCAN1_HUMAN, GBRB2_HUMAN, GBRA2_HUMAN, SRBS1_HUMAN, P2R3A_HUMAN, P63_HUMAN, FBX25_HUMAN, NALP2_HUMAN, ARI1_HUMAN, UBP28_HUMAN, TFR1_HUMAN, TOP2A_HUMAN, STRAA_HUMAN, LIMD1_HUMAN, AJUBA_HUMAN, WTIP_HUMAN, REST_HUMAN, H11_HUMAN, PRPS1_HUMAN, PPARD_HUMAN, KC1A_HUMAN, HOP_HUMAN, CUL3_HUMAN, CUL4A_HUMAN, CUL4B_HUMAN, CUL2_HUMAN, CSN5_HUMAN, CSN6_HUMAN, CAND1_HUMAN, NEDD8_HUMAN, GRK6_HUMAN, RFC2_HUMAN, UB2J2_HUMAN, 2AAA_HUMAN, TRI18_HUMAN, RICTR_HUMAN, HDAC8_HUMAN, ZMYM2_HUMAN, DSN1_HUMAN, NSL1_HUMAN, PMF1_HUMAN, MIS12_HUMAN, BLM_HUMAN, TERF2_HUMAN, NUDC_HUMAN, IBTK_HUMAN, TRAF3_HUMAN, MAGAB_HUMAN, RUXE_HUMAN, BTG1_HUMAN, EMD_HUMAN, MARK2_HUMAN, ACVL1_HUMAN, STK33_HUMAN, GRK5_HUMAN, TYPH_HUMAN, NOX5_HUMAN, HNRH1_HUMAN, BCLF1_HUMAN, DOCK4_HUMAN, MYCBP_HUMAN, UB2G2_HUMAN, FBX6_HUMAN, UB2D3_HUMAN, TOP1_HUMAN, VDAC3_HUMAN, CISD1_HUMAN, NDKB_HUMAN, UBC12_HUMAN, PACRG_HUMAN, TCPA_HUMAN, TCPB_HUMAN, MIRO2_HUMAN, SYIC_HUMAN, AIMP1_HUMAN, SYLC_HUMAN, SYK_HUMAN, SYRC_HUMAN, PRS7_HUMAN, PSA5_HUMAN, IMB1_HUMAN, PGK1_HUMAN, TNPO1_HUMAN, RS15A_HUMAN, IPO4_HUMAN, NUCL_HUMAN, ADT2_HUMAN, SAHH2_HUMAN, RL17_HUMAN, DFFB_HUMAN, H90B3_HUMAN, RD23B_HUMAN, ICLN_HUMAN, VP26A_HUMAN, VPS4B_HUMAN, VATB2_HUMAN, RL10A_HUMAN, EFTU_HUMAN, IGBP1_HUMAN, THIL_HUMAN, SSRG_HUMAN, TYSY_HUMAN, STAM1_HUMAN, RPAC1_HUMAN, UCHL3_HUMAN, UBE4B_HUMAN, USP9X_HUMAN, PRDX3_HUMAN, RL32_HUMAN, TCPG_HUMAN, UB2D1_HUMAN, PPIA_HUMAN, TXND5_HUMAN, PICAL_HUMAN, RU17_HUMAN, RS20_HUMAN, RBMS1_HUMAN, ITPA_HUMAN, PNPT1_HUMAN, ENOB_HUMAN, MARCS_HUMAN, HS905_HUMAN, SEPT2_HUMAN, H2A1D_HUMAN, MPV17_HUMAN, VATH_HUMAN, NUP37_HUMAN, WDFY1_HUMAN, RCCD1_HUMAN, H90B2_HUMAN, CD2B2_HUMAN, LMAN1_HUMAN, SPT5H_HUMAN, RL29_HUMAN, BRCA1_HUMAN, ECT2_HUMAN, DNLI4_HUMAN, MDC1_HUMAN, AURKB_HUMAN, MED12_HUMAN, MED1_HUMAN, MD13L_HUMAN, MED14_HUMAN, MED23_HUMAN, MED16_HUMAN, MED15_HUMAN, MED4_HUMAN, MED8_HUMAN, MED24_HUMAN, MED20_HUMAN, MED22_HUMAN, MED27_HUMAN, MED10_HUMAN, MED9_HUMAN, MED17_HUMAN, MED11_HUMAN, MED19_HUMAN, MED21_HUMAN, MED28_HUMAN, MED29_HUMAN, MED30_HUMAN, MED31_HUMAN, MED6_HUMAN, CCNC_HUMAN, CCDC6_HUMAN, CAH9_HUMAN, CFLAR_HUMAN, CTGF_HUMAN, MIPT3_HUMAN, LATS1_HUMAN, CD11A_HUMAN, U5S1_HUMAN, PRP8_HUMAN, FLII_HUMAN, UN45A_HUMAN, CYBP_HUMAN, CEP97_HUMAN, SCRIB_HUMAN, EDRF1_HUMAN, RPAB1_HUMAN, U520_HUMAN, RMP_HUMAN, HSP77_HUMAN, HSP76_HUMAN, HSP72_HUMAN, HS71L_HUMAN, KCNQ4_HUMAN, HS105_HUMAN, LDHA_HUMAN, C1TC_HUMAN, SERC_HUMAN, ACTG_HUMAN, TPM3_HUMAN, FLNA_HUMAN, SPTN1_HUMAN, NUMA1_HUMAN, PSMD1_HUMAN, PSB5_HUMAN, SYAC_HUMAN, EIF3H_HUMAN, RLA0_HUMAN, RS4X_HUMAN, MYG1_HUMAN.Q86UA3_HUMAN, SYIM_HUMAN, RSSA_HUMAN, VCAM1_HUMAN, ICK_HUMAN, MAST2_HUMAN, KAPCB_HUMAN, LIMK2_HUMAN, MERTK_HUMAN, TIE1_HUMAN, NPRL2_HUMAN, TNK1_HUMAN, EPHB6_HUMAN, CDK7_HUMAN, CSF1R_HUMAN, EPHB1_HUMAN, ACV1C_HUMAN, DDR2_HUMAN, FASTK_HUMAN, BMR1A_HUMAN, GSK3A_HUMAN, INSRR_HUMAN, GRK4_HUMAN, TSSK2_HUMAN, FGFR1_HUMAN, CLK3_HUMAN, NTRK3_HUMAN, VGFR3_HUMAN, ACV1B_HUMAN, AVR2B_HUMAN, M3K2_HUMAN, TYK2_HUMAN, KKCC1_HUMAN, WNK4_HUMAN, SRPK1_HUMAN, KGP2_HUMAN, MP2K7_HUMAN, FBXL3_HUMAN, FBW1B_HUMAN, FBXL2_HUMAN, FXL12_HUMAN, ENC1_HUMAN, KLH25_HUMAN, FXL14_HUMAN, FBX9_HUMAN, RAPSN_HUMAN, FBH1_HUMAN, FXL15_HUMAN, KLH10_HUMAN, FXL18_HUMAN.Q96D16_HUMAN, DET1_HUMAN, KLH14_HUMAN, VPS18_HUMAN, FBX17_HUMAN, FBX27_HUMAN, NHLC1_HUMAN, FBX3_HUMAN, RB40A_HUMAN, ANC2_HUMAN, AREL1_HUMAN, WWP1_HUMAN, HECD3_HUMAN, TRI10_HUMAN, TRIM2_HUMAN, KLH13_HUMAN, HERC6_HUMAN, RHBT1_HUMAN, FBX40_HUMAN, FBXW5_HUMAN, KCNG1_HUMAN, TRI36_HUMAN, ZBT17_HUMAN, ASB6_HUMAN, MARH9_HUMAN, LRSM1_HUMAN, FBX4_HUMAN, TNAP3_HUMAN, VPS41_HUMAN, KCNA5_HUMAN, KCNS3_HUMAN, SPSB1_HUMAN, KCNA6_HUMAN, HERC4_HUMAN, TRI41_HUMAN, G2E3_HUMAN, RN111_HUMAN, BRE1B_HUMAN, MDM4_HUMAN, TRI37_HUMAN, RGS11_HUMAN, RGS6_HUMAN, PREB_HUMAN, RAG1_HUMAN, NR1H3_HUMAN, RGS7_HUMAN, PRDM1_HUMAN, DLX6_HUMAN, NR1I3_HUMAN, IRF2_HUMAN, NR1I2_HUMAN, HMGA1_HUMAN, TBX22_HUMAN, BBX_HUMAN, DMRTA_HUMAN, SETB1_HUMAN, SLN11_HUMAN, TCF25_HUMAN, ISX_HUMAN, CEBPE_HUMAN, MKX_HUMAN, FOXM1_HUMAN, MAFG_HUMAN, HIPK4_HUMAN, MK04_HUMAN, IRAK2_HUMAN, STK38_HUMAN, TSSK1_HUMAN, PDK1L_HUMAN, KPCT_HUMAN, TYRO3_HUMAN, RPKL1_HUMAN, DDR1_HUMAN, GRK7_HUMAN, EPHA1_HUMAN, KPCG_HUMAN, PIM3_HUMAN, TESK1_HUMAN, KPCL_HUMAN, MYLK3_HUMAN, CDK6_HUMAN, ALK_HUMAN, KS6C1_HUMAN, AAPK2_HUMAN, M3K5_HUMAN, ST38L_HUMAN, KS6A6_HUMAN, KS6A3_HUMAN, EPHA4_HUMAN, IRAK3_HUMAN, CAMKV_HUMAN, KCC1G_HUMAN, TAOK3_HUMAN, ROR2_HUMAN, PASK_HUMAN, CDK14_HUMAN, M4K2_HUMAN, MINK1_HUMAN, NEK9_HUMAN, DAPK3_HUMAN, KKCC2_HUMAN, PAK6_HUMAN, KCC4_HUMAN, KPCD2_HUMAN, KS6A1_HUMAN, KCC2B_HUMAN, KCC2D_HUMAN, IQCB1_HUMAN, TBB2B_HUMAN, SSBP_HUMAN, TBB4B_HUMAN, PDRG1_HUMAN, DNJA2_HUMAN, NOS2_HUMAN, AGO1_HUMAN, ELAV1_HUMAN, MET18_HUMAN, CMKMT_HUMAN, UBL4A_HUMAN, ITA4_HUMAN, LAS1L_HUMAN, PELP1_HUMAN, ACSL1_HUMAN, ACSL4_HUMAN, MDHM_HUMAN, CPT1A_HUMAN, NB5R3_HUMAN, MARC1_HUMAN, TOM22_HUMAN, FIS1_HUMAN, MARH5_HUMAN, TBC15_HUMAN, TOM1_HUMAN, MYO6_HUMAN, TAXB1_HUMAN, CACO2_HUMAN, PSB1_HUMAN, PSB2_HUMAN, PSB3_HUMAN, PSB4_HUMAN, PSB6_HUMAN, PSB7_HUMAN, PRS4_HUMAN, PRS6B_HUMAN, PRS10_HUMAN, PAAF1_HUMAN, PSMD3_HUMAN, PSMD5_HUMAN, PSMD7_HUMAN, PSMD8_HUMAN, PSMD9_HUMAN, PSD10_HUMAN, PSD11_HUMAN, PSD12_HUMAN, PSD13_HUMAN, PSDE_HUMAN, PSME1_HUMAN, PSME2_HUMAN, PSME3_HUMAN, KLF2_HUMAN, PTN23_HUMAN, CHM4A_HUMAN, FOXO1_HUMAN, DTL_HUMAN, S12A3_HUMAN, PAN2_HUMAN, NPM_HUMAN, SMG1_HUMAN, SOX2_HUMAN, RAD52_HUMAN, IRF1_HUMAN, BAG3_HUMAN, DEAF1_HUMAN, IGKC_HUMAN.KVD16_HUMAN, TBB4A_HUMAN, TBB2A_HUMAN, TBB3_HUMAN, TBB6_HUMAN, HBA_HUMAN, XPO2_HUMAN, KRT86_HUMAN, AP1S1_HUMAN, ATX10_HUMAN, SMD1_HUMAN, CIP2A_HUMAN, AP1M2_HUMAN, IPO7_HUMAN, XPOT_HUMAN, SGPL1_HUMAN, 2ABA_HUMAN, GCN1_HUMAN, EI2BB_HUMAN, SERA_HUMAN, LANC2_HUMAN, SAAL1_HUMAN, SPTC1_HUMAN, GEMI6_HUMAN, HOOK2_HUMAN, RANG_HUMAN, ARL1_HUMAN, PPP6_HUMAN, AP1G2_HUMAN, AP2B1_HUMAN, S61A1_HUMAN, TPPC3_HUMAN, PDIA3_HUMAN, COG7_HUMAN, IQGA3_HUMAN, MMS19_HUMAN, STRAP_HUMAN, MON2_HUMAN, EI2BG_HUMAN, COG5_HUMAN, RCN2_HUMAN, COG6_HUMAN, THEM6_HUMAN, S39AB_HUMAN, COG4_HUMAN, PFKAP_HUMAN, TECR_HUMAN, TIM50_HUMAN, AP1M1_HUMAN, XPO7_HUMAN, PP6R1_HUMAN, SE1L1_HUMAN, PFKAL_HUMAN, XPO5_HUMAN, AP2A2_HUMAN, ITIH2_HUMAN, PHLA1_HUMAN, DDX20_HUMAN, LEG8_HUMAN, TPP1_HUMAN, EXC6B_HUMAN, FAKD4_HUMAN, ZW10_HUMAN, ARHG5_HUMAN, AP1G1_HUMAN, IPO8_HUMAN, COG1_HUMAN, AT2A2_HUMAN, NUP85_HUMAN, XPO6_HUMAN, GEMI4_HUMAN, AL3A2_HUMAN, NUP93_HUMAN, RAGP1_HUMAN, BIG1_HUMAN, TELO2_HUMAN, EI2BE_HUMAN, BIG3_HUMAN, DOP2_HUMAN, CNDG2_HUMAN, GBF1_HUMAN, SMC2_HUMAN, RN213_HUMAN, NBEL2_HUMAN, FDFT_HUMAN, ACOT9_HUMAN, VAC14_HUMAN, FA8_HUMAN, TGM2_HUMAN, ORC5_HUMAN, BCAT2_HUMAN, RL13A_HUMAN, LSM8_HUMAN, YTDC1_HUMAN, TOM40_HUMAN, HEXI1_HUMAN, BIRC3_HUMAN, BIRC2_HUMAN, RENT2_HUMAN, DYR1A_HUMAN, NLK_HUMAN, RPB1_HUMAN, KTNA1_HUMAN, LPPRC_HUMAN, ROA2_HUMAN, CLPX_HUMAN, CBX1_HUMAN, ACTB_HUMAN, CASPE_HUMAN, GLU2B_HUMAN, TBA1C_HUMAN, AIFM1_HUMAN, ALBU_HUMAN, RBM8A_HUMAN, RT31_HUMAN, MPCP_HUMAN, ATPA_HUMAN, ECHB_HUMAN, NFL_HUMAN, CMC2_HUMAN, ATPO_HUMAN, RT07_HUMAN, OPA1_HUMAN, NFM_HUMAN, CBX3_HUMAN, IF4B_HUMAN, SNUT1_HUMAN, ATPK_HUMAN, ML12A_HUMAN.ML12B_HUMAN, RL6_HUMAN, HNRPF_HUMAN, TPM4_HUMAN, NDUS4_HUMAN, AINX_HUMAN, CIRBP_HUMAN, YBOX3_HUMAN, LMNB1_HUMAN, CALR_HUMAN, RM12_HUMAN, SFPQ_HUMAN, RFC4_HUMAN, FUS_HUMAN, NDUS2_HUMAN, RUVB1_HUMAN, LMNA_HUMAN, RUVB2_HUMAN, VGF_HUMAN, ZC3HF_HUMAN, GPDM_HUMAN, CMGA_HUMAN, GNT2A_HUMAN, ADAS_HUMAN, SCG1_HUMAN, ABCE1_HUMAN, RT28_HUMAN, RT18B_HUMAN, RL26L_HUMAN, STML2_HUMAN, ODB2_HUMAN, NACAM_HUMAN.NACA_HUMAN, MIC19_HUMAN, NDUAA_HUMAN, AMOT_HUMAN, HNRH3_HUMAN, RT23_HUMAN, TBB1_HUMAN, NIPS1_HUMAN, PCCA_HUMAN, PCCB_HUMAN, MCCB_HUMAN, HNRC1_HUMAN, HNRDL_HUMAN, NDUS3_HUMAN, CKAP4_HUMAN, RL22_HUMAN, RS27A_HUMAN, TXTP_HUMAN, EF1A2_HUMAN, ATD3A_HUMAN, RL8_HUMAN, PGAM5_HUMAN, SRSF1_HUMAN, RALY_HUMAN, RS2_HUMAN, H12_HUMAN, RT15_HUMAN, HNRPM_HUMAN, RT27_HUMAN, PAIRB_HUMAN, PRP6_HUMAN, RS8_HUMAN, RS25_HUMAN, RS14_HUMAN, DDX17_HUMAN, RL12_HUMAN, RL4_HUMAN, RT22_HUMAN, RL7A_HUMAN, DDX5_HUMAN, HNRPK_HUMAN, HNRPU_HUMAN, DDX3X_HUMAN, EF1A3_HUMAN, SCMC1_HUMAN, DBF4A_HUMAN, NACC1_HUMAN, KEAP1_HUMAN, ARF_HUMAN.CDN2A_HUMAN, CKS1_HUMAN, SAHH_HUMAN, ARI2_HUMAN, ARLY_HUMAN, BIN1_HUMAN, BNIP2_HUMAN, TLS1_HUMAN, CAN2_HUMAN, KCRB_HUMAN, CLIP1_HUMAN, DFFA_HUMAN, IF6_HUMAN, FERM2_HUMAN, PUR4_HUMAN, DCTP1_HUMAN, FUMH_HUMAN, GNPI1_HUMAN, TF3C4_HUMAN, AL1B1_HUMAN, TATD1_HUMAN, ARFG1_HUMAN, FKBP9_HUMAN, PDC10_HUMAN, PLPHP_HUMAN, WDR61_HUMAN, CAP1_HUMAN, MCM3_HUMAN, PP6R3_HUMAN, GANAB_HUMAN, PUR9_HUMAN, MCTS1_HUMAN, TFIP8_HUMAN, TRXR1_HUMAN, ISOC1_HUMAN, KI13A_HUMAN, MARE1_HUMAN, IF2A_HUMAN, RL27A_HUMAN, MSHR_HUMAN, MCM2_HUMAN, MSH6_HUMAN, NOL3_HUMAN, NSF1C_HUMAN, EHD1_HUMAN, STK39_HUMAN, NUBP2_HUMAN, PSME4_HUMAN, RUXF_HUMAN, STK24_HUMAN, IF5_HUMAN, ERP44_HUMAN, STK26_HUMAN, MYO1E_HUMAN, PTMA_HUMAN, TWF2_HUMAN, TRI47_HUMAN, TRNT1_HUMAN, UBA5_HUMAN, VINC_HUMAN, PYM1_HUMAN, XPP1_HUMAN, XRCC5_HUMAN, RFA2_HUMAN, RFA1_HUMAN, WWOX_HUMAN, UBP5_HUMAN, RHBT2_HUMAN, EYA1_HUMAN, SEM1_HUMAN.SEML_HUMAN, PANK4_HUMAN, HUWE1_HUMAN, AAKG1_HUMAN, PLK1_HUMAN, F263_HUMAN, SAE2_HUMAN, MP2K4_HUMAN, UBR4_HUMAN, S12A2_HUMAN, MP2K3_HUMAN, ATP5L_HUMAN, PTPRF_HUMAN, RHG01_HUMAN, ITCH_HUMAN, PDK1_HUMAN, PLD3_HUMAN, 2A5G_HUMAN, AP3M1_HUMAN, PFKAM_HUMAN, AP1S2_HUMAN, AP1B1_HUMAN, PPAC_HUMAN, AP2S1_HUMAN, UBE2S_HUMAN, AP3S1_HUMAN, VRK1_HUMAN, CLUS_HUMAN, STAU1_HUMAN, DERL1_HUMAN, NDE1_HUMAN, DLX2_HUMAN, ITF2_HUMAN, DAB2P_HUMAN, CP250_HUMAN, CEP57_HUMAN, CEP76_HUMAN, DDIT4_HUMAN, SIVA_HUMAN, DCBD2_HUMAN, B2CL1_HUMAN, MCL1_HUMAN, PD2R_HUMAN, ZBT16_HUMAN, OPTN_HUMAN, ECHP_HUMAN, IL6RB_HUMAN, KR103_HUMAN, MID51_HUMAN.MIDUO_HUMAN, XPO4_HUMAN, NANOG_HUMAN, RHNO1_HUMAN, SNX17_HUMAN, SNX27_HUMAN, CUL7_HUMAN, OBSL1_HUMAN, CCDC8_HUMAN, TREX1_HUMAN, DSG2_HUMAN, MYO1B_HUMAN, CALX_HUMAN, DPM1_HUMAN, HCD2_HUMAN, DC1L1_HUMAN, FAF2_HUMAN, SYYC_HUMAN, ECM29_HUMAN, ST1A1_HUMAN, SRPRA_HUMAN, MRT4_HUMAN, EIF3M_HUMAN, TIM23_HUMAN, SSRD_HUMAN, RPR1A_HUMAN, MYO1D_HUMAN, FBRL_HUMAN, AFG32_HUMAN, SMC3_HUMAN, NDUA9_HUMAN, LONM_HUMAN, RL38_HUMAN, RU2A_HUMAN, COPA_HUMAN, ATAD1_HUMAN, PDIP2_HUMAN, WDR6_HUMAN, SCFD1_HUMAN, NDUS1_HUMAN, MGST1_HUMAN, CN37_HUMAN, EI2BD_HUMAN, TRUA_HUMAN, ARP2_HUMAN, EI2BA_HUMAN, 1A01_HUMAN.1A02_HUMAN.1A03_HUMAN.1A11_HUMAN.1A23_HUMAN.1A24_HUMAN.1A25_HUMAN.1A26_HUMAN.1A29_HUMAN.1A30_HUMAN.1A31_HUMAN.1A32_HUMAN.1A33_HUMAN.1A34_HUMAN.1A36_HUMAN.1A43_HUMAN.1A66_HUMAN.1A68_HUMAN.1A69_HUMAN.1A74_HUMAN.1A80_HUMAN, P5CR2_HUMAN, MYO1C_HUMAN, DRS7B_HUMAN, RFC5_HUMAN, OSBP1_HUMAN, YBEY_HUMAN, EF1B_HUMAN, GSH0_HUMAN, MIC10_HUMAN, PELO_HUMAN, RM10_HUMAN, CTBP1_HUMAN, ABCF2_HUMAN, MPC2_HUMAN, LIMA1_HUMAN, CND3_HUMAN, EIF3K_HUMAN, PUM1_HUMAN, TOIP1_HUMAN, ALEX_HUMAN.GNAS1_HUMAN.GNAS2_HUMAN.GNAS3_HUMAN, EIF3F_HUMAN, SGMR2_HUMAN, CND2_HUMAN, RFC3_HUMAN, STT3A_HUMAN, GCP2_HUMAN, PON2_HUMAN, ABCD3_HUMAN, CDIPT_HUMAN, SDF2_HUMAN, DIM1_HUMAN, BCCIP_HUMAN, PYC_HUMAN, SRPRB_HUMAN, UTP15_HUMAN, GBB2_HUMAN, RER1_HUMAN, LRWD1_HUMAN, CF120_HUMAN, BZW1_HUMAN, AAAT_HUMAN, NSUN2_HUMAN, SFXN3_HUMAN, UFL1_HUMAN, ELP1_HUMAN, PDS5A_HUMAN, TR10B_HUMAN, AT5F1_HUMAN, FLOT2_HUMAN, NTPCR_HUMAN, ACOD_HUMAN, QCR2_HUMAN, AT2B1_HUMAN, IF4G2_HUMAN, SAM50_HUMAN, DJC11_HUMAN, NCLN_HUMAN, SKIV2_HUMAN, RRP44_HUMAN, LSR_HUMAN, PRI1_HUMAN, MRM3_HUMAN, AAMP_HUMAN, RAB18_HUMAN, AAAS_HUMAN, KIF1A_HUMAN, TPPC5_HUMAN, TBL3_HUMAN, ARHG2_HUMAN, DHC24_HUMAN, FADS2_HUMAN, CKAP2_HUMAN, CEBPZ_HUMAN, DSRAD_HUMAN, STOM_HUMAN, LANC1_HUMAN, TAF4_HUMAN, PSPC1_HUMAN, AAMDC_HUMAN, CAP2_HUMAN, PLST_HUMAN, H1X_HUMAN, RM09_HUMAN, CADH5_HUMAN, MCF2_HUMAN, AFAD_HUMAN, SUMO2_HUMAN, BAD_HUMAN, LUZP4_HUMAN, CD3D_HUMAN, UBP36_HUMAN, SC22C_HUMAN, ZN501_HUMAN, SDCB1_HUMAN, TCPH_HUMAN, BTBDA_HUMAN, KCD20_HUMAN, APC16_HUMAN, AGO3_HUMAN, CAZA2_HUMAN, HEYL_HUMAN, ACTN3_HUMAN, NUD12_HUMAN, MOG1_HUMAN, SEP12_HUMAN, BORG4_HUMAN, SEPT3_HUMAN, TMM25_HUMAN, NP1L1_HUMAN, PTC1_HUMAN, PTPRK_HUMAN, SEPT1_HUMAN, CP1A1_HUMAN, ZFP41_HUMAN, CDKL2_HUMAN, CDKL4_HUMAN, CDK13_HUMAN, SOX4_HUMAN, CRY2_HUMAN, GATA3_HUMAN, UBR5_HUMAN, AKTIP_HUMAN, PK3CA_HUMAN, ARH40_HUMAN, AMFR_HUMAN, TRIO_HUMAN, LGR5_HUMAN, RABE1_HUMAN, GAK_HUMAN, PCDGK_HUMAN, LRRN3_HUMAN, MIB1_HUMAN, OFD1_HUMAN, PIBF1_HUMAN, CATA_HUMAN, DSG1_HUMAN, TGM1_HUMAN, PROF1_HUMAN, H2B1L_HUMAN, TGM3_HUMAN, DSC1_HUMAN, D3DNK7_HUMAN.LEKR1_HUMAN, BT1A1_HUMAN, GSTP1_HUMAN, ABCB7_HUMAN, HP1B3_HUMAN, KI26B_HUMAN, SYT4_HUMAN, RHBT3_HUMAN, RB15B_HUMAN, RRP5_HUMAN, RFOX2_HUMAN, RBM14_HUMAN, RNF31_HUMAN, UBP4_HUMAN, LIPB1_HUMAN, INT6_HUMAN, ARHGB_HUMAN, NSMA3_HUMAN, SYNP2_HUMAN, S27A4_HUMAN, DDX41_HUMAN, ASAP1_HUMAN, RRBP1_HUMAN, UNC5B_HUMAN, AUP1_HUMAN, XPR1_HUMAN, RP9_HUMAN, REPS1_HUMAN, SMCA4_HUMAN, DDX21_HUMAN, CO7_HUMAN, MSTO1_HUMAN, ASAP2_HUMAN, PRP4B_HUMAN, SMCA1_HUMAN, FIP1_HUMAN, DLGP5_HUMAN, TRA2A_HUMAN, ACINU_HUMAN, SMCA5_HUMAN, RABE2_HUMAN, SRS10_HUMAN, TRA2B_HUMAN, PLPL6_HUMAN, TAF6L_HUMAN, ARAP3_HUMAN, DDX18_HUMAN, KHDR1_HUMAN, CERK1_HUMAN, SRSF7_HUMAN, SPTC2_HUMAN, PLRG1_HUMAN, FMR1_HUMAN, HIP1R_HUMAN, VIR_HUMAN, CDC5L_HUMAN, ARAP1_HUMAN, SMRC2_HUMAN, VANG2_HUMAN, UNC5C_HUMAN, MOT1_HUMAN, RFC1_HUMAN, PTK7_HUMAN, SMRD2_HUMAN, AP3B1_HUMAN, RL15_HUMAN, DDX27_HUMAN, MTCH2_HUMAN, SMRC1_HUMAN, LBR_HUMAN, CNDD3_HUMAN, QKI_HUMAN, PCAT2_HUMAN, M4K5_HUMAN, CP110_HUMAN, ZCH18_HUMAN, CWC22_HUMAN, F1711_HUMAN, SRSF9_HUMAN, NKRF_HUMAN, FMNL3_HUMAN, PIGT_HUMAN, RBM15_HUMAN, EDC3_HUMAN, WDR5_HUMAN, NOP2_HUMAN, NOG2_HUMAN, M2OM_HUMAN, RRP1B_HUMAN, INT5_HUMAN, AAK1_HUMAN, CCNT1_HUMAN, RM28_HUMAN, WWP2_HUMAN, SC24B_HUMAN, FXR2_HUMAN, DHX15_HUMAN, GHC1_HUMAN, SSRA_HUMAN, PLXB2_HUMAN, TEX10_HUMAN, SPB1_HUMAN, TMM59_HUMAN, TF3C2_HUMAN, CPSF1_HUMAN, TMX3_HUMAN, NOP58_HUMAN, RPRD2_HUMAN, FARP1_HUMAN, ADT3_HUMAN, ERLN2_HUMAN, SMRD1_HUMAN, DVL3_HUMAN, DNJB6_HUMAN, NOG1_HUMAN, ROA0_HUMAN, PLXA4_HUMAN, NAT10_HUMAN, DDX28_HUMAN, SNW1_HUMAN, RM24_HUMAN, PRRT4_HUMAN, TRIP4_HUMAN, RBM28_HUMAN, RPOM_HUMAN, PCDB3_HUMAN, XRN1_HUMAN, DKC1_HUMAN, DHX30_HUMAN, SENP3_HUMAN, AGRL2_HUMAN, E9PAV9_HUMAN.GPTC4_HUMAN, RASL2_HUMAN, MCCA_HUMAN, DDX24_HUMAN, RL14_HUMAN, KIF14_HUMAN, MOV10_HUMAN, FXR1_HUMAN, RT35_HUMAN, MARK3_HUMAN, DECR_HUMAN, GRDN_HUMAN, ANKL2_HUMAN, PRP31_HUMAN, LARP7_HUMAN, RL10_HUMAN, PACS1_HUMAN, F120A_HUMAN, KC1E_HUMAN, MAN1_HUMAN, NOL9_HUMAN, IF122_HUMAN, S11IP_HUMAN, P66B_HUMAN, CHERP_HUMAN, HNRL2_HUMAN, ESYT2_HUMAN, MYH10_HUMAN, HAX1_HUMAN, HELLS_HUMAN, GCP6_HUMAN, RT09_HUMAN, RM03_HUMAN, RSBNL_HUMAN, SAFB1_HUMAN, ARHGC_HUMAN, LAP2A_HUMAN.LAP2B_HUMAN, POP1_HUMAN, RS9_HUMAN, ILF3_HUMAN, MDR1_HUMAN, TF3C5_HUMAN, YBOX1_HUMAN, RBM4_HUMAN, PTN9_HUMAN, BRD3_HUMAN, TIF1A_HUMAN, CLAP2_HUMAN, MADD_HUMAN, TSC2_HUMAN, DDX23_HUMAN, RRP12_HUMAN, EDC4_HUMAN, PTPRR_HUMAN, ATP7A_HUMAN, HIP1_HUMAN, IGSF3_HUMAN, SPA5L_HUMAN, GCP5_HUMAN, GIT1_HUMAN, PATL1_HUMAN, NU160_HUMAN, PDE4B_HUMAN, SUN2_HUMAN, PP1RA_HUMAN, SRP72_HUMAN, NOM1_HUMAN, RL18_HUMAN, CE170_HUMAN, TR150_HUMAN, PDPR_HUMAN, DREB_HUMAN, STT3B_HUMAN, COPE_HUMAN, CAPR1_HUMAN, PHB2_HUMAN, SR140_HUMAN, LIPA1_HUMAN, GNL3_HUMAN, MTA2_HUMAN, ALDR_HUMAN, ANXA6_HUMAN, ASNS_HUMAN, ATP5J_HUMAN, APEX1_HUMAN, NMD3_HUMAN, CAPZB_HUMAN, COR1C_HUMAN, D2HDH_HUMAN, DCA13_HUMAN, OST48_HUMAN, DDX56_HUMAN, DUT_HUMAN, GABT_HUMAN, THIM_HUMAN, AL4A1_HUMAN, GPX4_HUMAN, HINT1_HUMAN, LDHB_HUMAN, MOES_HUMAN, PIMT_HUMAN, PGK2_HUMAN, PGM1_HUMAN, RCN1_HUMAN, RADI_HUMAN, SODC_HUMAN, TAGL_HUMAN, TAGL2_HUMAN, TKT_HUMAN, WDR1_HUMAN, ERF1_HUMAN, FABP5_HUMAN, FKB1A_HUMAN, FKB1B_HUMAN, SYDM_HUMAN, GARS_HUMAN, GLGB_HUMAN, GFPT1_HUMAN, G6PI_HUMAN, SYHC_HUMAN, CH10_HUMAN, DNJB4_HUMAN, DNJB5_HUMAN, DNJC2_HUMAN, DNJC3_HUMAN, DNJC8_HUMAN, SNAA_HUMAN, IMA7_HUMAN, IPO9_HUMAN, IMA6_HUMAN, CPIN1_HUMAN, RCC2_HUMAN, NMT1_HUMAN, NU205_HUMAN, PABP4_HUMAN, PDCD6_HUMAN, PEF1_HUMAN, PGAM1_HUMAN, PIGS_HUMAN, PLBL2_HUMAN, MYP2_HUMAN, PP14B_HUMAN, GT251_HUMAN, RPN2_HUMAN, SEPT8_HUMAN, SORCN_HUMAN, GOLP3_HUMAN, STIM1_HUMAN, STIM2_HUMAN, TALDO_HUMAN, TIPRL_HUMAN, MSH2_HUMAN, TRIA1_HUMAN, TRM6_HUMAN, TRM61_HUMAN, SYVC_HUMAN, ZMYM3_HUMAN, CPSF2_HUMAN, AP3B2_HUMAN, VIP2_HUMAN, FMNL2_HUMAN, MBB1A_HUMAN, SRPK2_HUMAN, SRP68_HUMAN, RL19_HUMAN, LSG1_HUMAN, NOC3L_HUMAN, TF3C3_HUMAN, GCP3_HUMAN, TM10C_HUMAN, XRN2_HUMAN, MSH3_HUMAN, MTMRD_HUMAN, DHTK1_HUMAN, NAA16_HUMAN, KIFA3_HUMAN, TMM33_HUMAN, WASF2_HUMAN, DPOE1_HUMAN, ELOA1_HUMAN, PRP16_HUMAN, PHF6_HUMAN, CTR9_HUMAN, ANM3_HUMAN, SCAF8_HUMAN, ILF2_HUMAN, TONSL_HUMAN, MYPT1_HUMAN, SRSF5_HUMAN, PUM3_HUMAN, PTBP1_HUMAN, PYR1_HUMAN, ACSL3_HUMAN, CHD1L_HUMAN, RM38_HUMAN, DVL2_HUMAN, RT05_HUMAN, RT34_HUMAN, PESC_HUMAN, STXB3_HUMAN, VPS39_HUMAN, SART3_HUMAN, PRPF3_HUMAN, SYEM_HUMAN, EMC1_HUMAN, OGT1_HUMAN, AT12A_HUMAN, S4A7_HUMAN, RBM25_HUMAN, ATLA3_HUMAN, EXOSX_HUMAN, TF3C1_HUMAN, TPPC9_HUMAN, SRRM1_HUMAN, INT1_HUMAN, SF3B2_HUMAN, MYO9B_HUMAN, WDR11_HUMAN, SMAL1_HUMAN, PI4KA_HUMAN, NU107_HUMAN, EMC2_HUMAN, SYNE1_HUMAN, TBL1R_HUMAN, DJC10_HUMAN, SC16A_HUMAN, MRCKB_HUMAN, CLCN5_HUMAN, THOC4_HUMAN, RPC1_HUMAN, WDR48_HUMAN, DOCK1_HUMAN, CY1_HUMAN, TLE3_HUMAN, THOC2_HUMAN, IF2G_HUMAN, MYO5A_HUMAN, NP1L4_HUMAN, PABP1_HUMAN, UBF1_HUMAN, PHB_HUMAN, PLPP_HUMAN, L2GL1_HUMAN, PLOD1_HUMAN, ERGI1_HUMAN, CYFP1_HUMAN, DYN1_HUMAN, SUCB1_HUMAN, LYRIC_HUMAN, CAN1_HUMAN, EDEM3_HUMAN, PLOD3_HUMAN, CLAP1_HUMAN, NONO_HUMAN, EPMIP_HUMAN, RPTOR_HUMAN, RM37_HUMAN, ELMO1_HUMAN, TPPC8_HUMAN, APC1_HUMAN, PI3R4_HUMAN, DPOD1_HUMAN, DIEXF_HUMAN, HAT1_HUMAN, SMC4_HUMAN, MCE1_HUMAN, ZN598_HUMAN, MTREX_HUMAN, DIP2B_HUMAN, IDH3B_HUMAN, LS14A_HUMAN, DP13B_HUMAN, RPB2_HUMAN, RM15_HUMAN, GNPAT_HUMAN, KDM1A_HUMAN, RDH11_HUMAN, SRGP2_HUMAN, CRNL1_HUMAN, PHX2A_HUMAN, HAUS5_HUMAN, EPN4_HUMAN, UGDH_HUMAN, KPBB_HUMAN, UBP10_HUMAN, PCF11_HUMAN, NU133_HUMAN, CPSF3_HUMAN, ANR28_HUMAN, PININ_HUMAN, ABCF1_HUMAN, ATLA1_HUMAN, TAF6_HUMAN, UHRF1_HUMAN, SDHA_HUMAN, PCAT1_HUMAN, RM39_HUMAN, WASF1_HUMAN, HNRPL_HUMAN, CPSF7_HUMAN, ECHA_HUMAN, PDE12_HUMAN, DCX_HUMAN, ELP3_HUMAN, MICA1_HUMAN, NEST_HUMAN, HSDL1_HUMAN, GPSM1_HUMAN, HPF1_HUMAN, I2BPL_HUMAN, KLC2_HUMAN, QCR1_HUMAN, PCKGM_HUMAN, SAC1_HUMAN, CHD4_HUMAN, KIF2A_HUMAN, TACC3_HUMAN, BTAF1_HUMAN, SYRM_HUMAN, NCKP1_HUMAN, EIF3D_HUMAN, YMEL1_HUMAN, IF4A3_HUMAN, HAUS6_HUMAN, G3BP2_HUMAN, WDHD1_HUMAN, SDA1_HUMAN, DNMT1_HUMAN, TANC1_HUMAN, CDC45_HUMAN, CIC_HUMAN, ABCD2_HUMAN, GTPB1_HUMAN, PRP4_HUMAN, ACL6A_HUMAN, CCAR1_HUMAN, WASC4_HUMAN, TPC12_HUMAN, FAKD5_HUMAN, PGRC2_HUMAN, OCRL_HUMAN, SYSM_HUMAN, EXOC1_HUMAN, ZCHC8_HUMAN, CARM1_HUMAN, MRP1_HUMAN, LEO1_HUMAN, LMNB2_HUMAN, GYS1_HUMAN, ACPH_HUMAN, AKAP1_HUMAN, MOGS_HUMAN, TIF1B_HUMAN, LC7L3_HUMAN, ANFY1_HUMAN, G3BP1_HUMAN, INT3_HUMAN, SYF1_HUMAN, LYAG_HUMAN, DHX8_HUMAN, RINI_HUMAN, ABI2_HUMAN, AQR_HUMAN, PPCE_HUMAN, COG2_HUMAN, SEPT9_HUMAN, INT4_HUMAN, ERLN1_HUMAN, RPAP1_HUMAN, CASP_HUMAN.CUX1_HUMAN, RM19_HUMAN, ABCD1_HUMAN, PDS5B_HUMAN, KIF4A_HUMAN, I2BP1_HUMAN, BRE1A_HUMAN, NOC2L_HUMAN, ODP2_HUMAN, NAA35_HUMAN, PUM2_HUMAN, PO210_HUMAN, RANB9_HUMAN, WRN_HUMAN, MD1L1_HUMAN, MRE11_HUMAN, ATG7_HUMAN, CP131_HUMAN, TRI33_HUMAN, DIC_HUMAN, GEMI5_HUMAN, MAP2_HUMAN, PP1B_HUMAN, NICA_HUMAN, SYNC_HUMAN, IF4E_HUMAN, TFB2M_HUMAN, ARGL1_HUMAN, TTK_HUMAN, RAD50_HUMAN, GOGA3_HUMAN, TPC11_HUMAN, IFT81_HUMAN, SMRCD_HUMAN, WDR35_HUMAN, PRI2_HUMAN, NAMPT_HUMAN, SOGA3_HUMAN, SFXN1_HUMAN, COPD_HUMAN, ODO1_HUMAN, FPPS_HUMAN, INSR_HUMAN, I2BP2_HUMAN, ATX2L_HUMAN, IF2B_HUMAN, MAP4_HUMAN, BRAT1_HUMAN, SMC6_HUMAN, RSMN_HUMAN, RIC8A_HUMAN, IF4A1_HUMAN, KIF15_HUMAN, CLP1L_HUMAN, VPS16_HUMAN, VP26B_HUMAN, AMPB_HUMAN, RBM39_HUMAN, NU155_HUMAN, KI21A_HUMAN, GAPD1_HUMAN, WAPL_HUMAN, RS13_HUMAN, ARHG1_HUMAN, ACTZ_HUMAN, KLC4_HUMAN, ISLR2_HUMAN, LRC8A_HUMAN, BOP1_HUMAN, AFTIN_HUMAN, ORC3_HUMAN, FOXK1_HUMAN, ODPA_HUMAN, WASC5_HUMAN, MEP50_HUMAN, DDX1_HUMAN, CAMP1_HUMAN, RABL6_HUMAN, SRRT_HUMAN, STXB1_HUMAN, OTUB1_HUMAN, UBP2L_HUMAN, EXOC5_HUMAN, LRC59_HUMAN, COPG2_HUMAN, TIM44_HUMAN, MTMR5_HUMAN, ARC1B_HUMAN, VPS52_HUMAN, IF4G3_HUMAN, RPA2_HUMAN, SFSWA_HUMAN, VP33A_HUMAN, MCM10_HUMAN, AVL9_HUMAN, RINT1_HUMAN, AT2C1_HUMAN, ERCC2_HUMAN, WDR82_HUMAN, TGO1_HUMAN, SC23B_HUMAN, RPC2_HUMAN, FYV1_HUMAN, MPP6_HUMAN, RBGPR_HUMAN, CND1_HUMAN, UGGG1_HUMAN, KDM3B_HUMAN, FEN1_HUMAN, ECH1_HUMAN, KINH_HUMAN, SYMPK_HUMAN, NDC80_HUMAN, VPS11_HUMAN, STRN_HUMAN, SCYL1_HUMAN, DD19A_HUMAN, SC23A_HUMAN, DCAF1_HUMAN, ODPB_HUMAN, SC24D_HUMAN, ACADM_HUMAN, ERC6L_HUMAN, RHG17_HUMAN, DDX6_HUMAN, JIP3_HUMAN, PALLD_HUMAN, KIF11_HUMAN, GET4_HUMAN, MCM6_HUMAN, CSDE1_HUMAN, DHX16_HUMAN, RBGP1_HUMAN, DCTN1_HUMAN, GCP60_HUMAN, COPG1_HUMAN, GRIN1_HUMAN, EIF3C_HUMAN, RTRAF_HUMAN, RTL1_HUMAN, RT02_HUMAN, IF4G1_HUMAN, EXOS4_HUMAN, MCM4_HUMAN, SEC63_HUMAN, DPYL1_HUMAN, MCES_HUMAN, ARVC_HUMAN, CKAP5_HUMAN, NU188_HUMAN, PCM1_HUMAN, KNTC1_HUMAN, LPIN1_HUMAN, TIA1_HUMAN, NUP54_HUMAN, KIF3A_HUMAN, CLIC4_HUMAN, GSLG1_HUMAN, P4R3A_HUMAN, RTF1_HUMAN, ROCK1_HUMAN, IMA4_HUMAN, VCIP1_HUMAN, SC24A_HUMAN, SPSY_HUMAN, FUBP2_HUMAN, CLGN_HUMAN, FOCAD_HUMAN, S23IP_HUMAN, RB3GP_HUMAN, SCOT1_HUMAN, ARP3_HUMAN, PYRG2_HUMAN, TMM43_HUMAN, WAC2A_HUMAN, VAPB_HUMAN, STRN4_HUMAN, ULA1_HUMAN, SREK1_HUMAN, TFG_HUMAN, SF3A1_HUMAN, GEPH_HUMAN, PDCD4_HUMAN, U2AF2_HUMAN, VPS35_HUMAN, NAA15_HUMAN, TOP2B_HUMAN, ACON_HUMAN, AGAP3_HUMAN, ROCK2_HUMAN, CPSF5_HUMAN, PSA_HUMAN, ADDA_HUMAN, RS5_HUMAN, IDHC_HUMAN, SC24C_HUMAN, KIF3B_HUMAN, CBPD_HUMAN, EF1D_HUMAN, ETFB_HUMAN, MCMBP_HUMAN, RBM12_HUMAN, RENT1_HUMAN, USO1_HUMAN, COG3_HUMAN, CLPT1_HUMAN, TLK2_HUMAN, PRUN1_HUMAN, P5CR1_HUMAN, TCRG1_HUMAN, ARPC2_HUMAN, DBR1_HUMAN, ETFA_HUMAN, BICD1_HUMAN, KLC1_HUMAN, DPYL4_HUMAN, SV2A_HUMAN, P4R3B_HUMAN, NCPR_HUMAN, FKBP3_HUMAN, UBP48_HUMAN, NUP88_HUMAN, NNTM_HUMAN, TAOK1_HUMAN, PPWD1_HUMAN, PABP2_HUMAN, DPOLA_HUMAN, CP062_HUMAN, DHSO_HUMAN, PP2AA_HUMAN, CATIN_HUMAN, VPS51_HUMAN, RBBP4_HUMAN, CAZA1_HUMAN, FAF1_HUMAN, GSTO1_HUMAN, SNRPA_HUMAN, TXLNG_HUMAN, NELFE_HUMAN, MUTA_HUMAN, DC1L2_HUMAN, TIM_HUMAN, CBSL_HUMAN.CBS_HUMAN, ESYT1_HUMAN, PPIL4_HUMAN, SLK_HUMAN, PNKP_HUMAN, ACLY_HUMAN, VPP1_HUMAN, VTA1_HUMAN, HOOK3_HUMAN, SCRB2_HUMAN, G6PD_HUMAN, SF3B1_HUMAN, TSR1_HUMAN, UCHL5_HUMAN, PUF60_HUMAN, SYLM_HUMAN, 1433G_HUMAN, SUV3_HUMAN, JIP4_HUMAN, IMDH1_HUMAN, T2FA_HUMAN, EXOS9_HUMAN, RHG35_HUMAN, KIF5C_HUMAN, ATLA2_HUMAN, SF3B3_HUMAN, DIAP1_HUMAN, DOPO_HUMAN, ELP2_HUMAN, GRPE1_HUMAN, TWF1_HUMAN, WBP11_HUMAN, EMAL4_HUMAN, ANM1_HUMAN, CORO7_HUMAN, API5_HUMAN, SP16H_HUMAN, RUFY1_HUMAN, KBP_HUMAN, SF3A3_HUMAN, DCTN4_HUMAN, SYWC_HUMAN, NELFB_HUMAN, GLYM_HUMAN, ENAH_HUMAN, DNLI1_HUMAN, STRA6_HUMAN, SSRP1_HUMAN, HDGR2_HUMAN, EIF3G_HUMAN, TBCD_HUMAN, RALA_HUMAN, EIF3A_HUMAN, U2AF1_HUMAN.U2AF5_HUMAN, NUF2_HUMAN, GDAP1_HUMAN, CADH2_HUMAN, CISY_HUMAN, EIF3B_HUMAN, DPYL2_HUMAN, RTN4_HUMAN, DHB4_HUMAN, GOLI4_HUMAN, EIF3I_HUMAN, SF01_HUMAN, ACADV_HUMAN, STAG2_HUMAN, DPP9_HUMAN, EIF2A_HUMAN, TCOF_HUMAN, RAB5C_HUMAN, DBNL_HUMAN, INO1_HUMAN, CTNA2_HUMAN, PAK4_HUMAN, NELFD_HUMAN, MAP1A_HUMAN, CSN4_HUMAN, IMA1_HUMAN, DX39A_HUMAN, APMAP_HUMAN, SC31A_HUMAN, AT1A3_HUMAN, RIR2_HUMAN, DCPS_HUMAN, NAA25_HUMAN, RL9_HUMAN, NPL4_HUMAN, ERG7_HUMAN, PAPOA_HUMAN, SRS11_HUMAN, ALDH2_HUMAN, KCRU_HUMAN, GNAO_HUMAN, LUC7L_HUMAN, RIR1_HUMAN, DPP3_HUMAN, NUP50_HUMAN, SYSC_HUMAN, SE6L2_HUMAN, T2FB_HUMAN, PUR2_HUMAN, ALDOC_HUMAN, NELFA_HUMAN, SYCC_HUMAN, TCPD_HUMAN, TCPE_HUMAN, PAPS1_HUMAN, SAE1_HUMAN, VATA_HUMAN, LMAN2_HUMAN, SRP54_HUMAN, IDE_HUMAN, SND1_HUMAN, MRP_HUMAN, GLRX3_HUMAN, LETM1_HUMAN, DDX42_HUMAN, BAP31_HUMAN, ANX11_HUMAN, TCPZ_HUMAN, EIF3L_HUMAN, FUBP1_HUMAN, CLIC1_HUMAN, ECHM_HUMAN, LKHA4_HUMAN, UBP14_HUMAN, TCPQ_HUMAN, ANK2_HUMAN, TPR_HUMAN, NRCAM_HUMAN, METK2_HUMAN, HTSF1_HUMAN, KAD2_HUMAN, IF4H_HUMAN, DHE3_HUMAN, TXNL1_HUMAN, HMGB2_HUMAN, RSRC1_HUMAN, PRDX6_HUMAN, EIF3J_HUMAN, SYTC_HUMAN, ERO1A_HUMAN, MAOM_HUMAN, ESTD_HUMAN, PUR8_HUMAN, AATM_HUMAN, GCSP_HUMAN, PAK2_HUMAN, UBA6_HUMAN, MAP1B_HUMAN, VAT1_HUMAN, PA1B3_HUMAN, OLA1_HUMAN, GDIR1_HUMAN, DDX46_HUMAN, THIC_HUMAN, ASNA_HUMAN, AN32A_HUMAN, PUR6_HUMAN, IPYR_HUMAN, DX39B_HUMAN, BCAS3_HUMAN, H2B1C_HUMAN, CLK1_HUMAN, CE162_HUMAN, LCA5_HUMAN, CNTRL_HUMAN, FBF1_HUMAN, NPHP4_HUMAN, FTM_HUMAN, SCLT1_HUMAN, RPGR1_HUMAN, TECT1_HUMAN, NDUAC_HUMAN, CREM_HUMAN, DDX11_HUMAN, FHL2_HUMAN, TSNAX_HUMAN, RT12_HUMAN, FBX31_HUMAN, GOT1B_HUMAN, RFWD3_HUMAN, TNPO3_HUMAN, INT7_HUMAN, RAIN_HUMAN, KANL3_HUMAN, AKIP1_HUMAN, ATPF1_HUMAN, ZMYM1_HUMAN, WDR26_HUMAN, LCOR_HUMAN, ANLN_HUMAN, TGS1_HUMAN, GATA2_HUMAN, NF2L3_HUMAN, GRIK2_HUMAN, COMD1_HUMAN, SLMAP_HUMAN, TBB8_HUMAN, KIT_HUMAN, SNG3_HUMAN, TROP_HUMAN, ARI3A_HUMAN, HEAT1_HUMAN, SATB2_HUMAN, ARI3B_HUMAN, G45IP_HUMAN, HIC2_HUMAN, A0A087WU62_HUMAN.RM45_HUMAN, KAISO_HUMAN, HXA10_HUMAN, NOVA1_HUMAN, RCC1_HUMAN, SATB1_HUMAN, SUGP2_HUMAN, ZFHX4_HUMAN, FUBP3_HUMAN, HXD13_HUMAN, RM20_HUMAN, NOVA2_HUMAN, TYY1_HUMAN, DUS9_HUMAN, E4F1_HUMAN, MEN1_HUMAN, RM18_HUMAN, RM27_HUMAN, RM50_HUMAN, RM51_HUMAN, RT30_HUMAN, NDUV2_HUMAN, RIF1_HUMAN, SALL1_HUMAN, SIX5_HUMAN, AP2A_HUMAN, TLE1_HUMAN, TLE4_HUMAN, UBE4A_HUMAN, ZBT40_HUMAN, ZFR_HUMAN, ZN131_HUMAN, NHEJ1_HUMAN, DNLI3_HUMAN, H2AY_HUMAN, XRCC1_HUMAN, PPARG_HUMAN, RUNX2_HUMAN, CX7A2_HUMAN, MYEF2_HUMAN, FOXI1_HUMAN, RECQ1_HUMAN, HXC13_HUMAN, DLX5_HUMAN, MECP2_HUMAN, PBX2_HUMAN, PKP1_HUMAN, TIM8B_HUMAN, SORL_HUMAN, CGL_HUMAN, PAPD1_HUMAN, FA83D_HUMAN, CXA5_HUMAN, CXG1_HUMAN, CXB1_HUMAN, RND3_HUMAN, CRY1_HUMAN, MDN1_HUMAN, COT1_HUMAN, TAF9_HUMAN, KIF22_HUMAN, ORC4_HUMAN, RMD3_HUMAN, UTP20_HUMAN, BAZ1A_HUMAN, CENPB_HUMAN, HSP7E_HUMAN, IRF9_HUMAN, STAG1_HUMAN, UTP6_HUMAN, IFRD1_HUMAN, DDX52_HUMAN, MA7D1_HUMAN, NFXL1_HUMAN, STRBP_HUMAN, TOP3B_HUMAN, MYCB2_HUMAN, RAE1L_HUMAN, SEN34_HUMAN, SPF27_HUMAN, RL10L_HUMAN, CDK8_HUMAN, EP400_HUMAN, NAA10_HUMAN, RCOR1_HUMAN, H14_HUMAN, CR3L2_HUMAN, KC1AL_HUMAN, SMU1_HUMAN, GFPT2_HUMAN, A16L2_HUMAN, TMOD3_HUMAN, PERI_HUMAN, SNX8_HUMAN, P4HA1_HUMAN, SIX1_HUMAN, TAP26_HUMAN, RM21_HUMAN, RT18A_HUMAN, GLYR1_HUMAN, NSUN4_HUMAN, RECQ4_HUMAN, RTCA_HUMAN, TTF1_HUMAN, TTF2_HUMAN, CCNB1_HUMAN, FZR1_HUMAN, PTTG1_HUMAN, MAGC2_HUMAN, GLI1_HUMAN, DTX3L_HUMAN, NELL1_HUMAN, CYTA_HUMAN, ANO5_HUMAN, COHA1_HUMAN, RS15_HUMAN, SPR1A_HUMAN, SRAC1_HUMAN, PTPRD_HUMAN, GSTT1_HUMAN, LAT1_HUMAN, AT2B4_HUMAN, OSMR_HUMAN, PO5F1_HUMAN, XRCC4_HUMAN, SOX10_HUMAN, COQ5_HUMAN, COQ7_HUMAN, COQ3_HUMAN, COQ4_HUMAN, COQ6_HUMAN, L2HDH_HUMAN, SPART_HUMAN, SYJ2B_HUMAN, RT4I1_HUMAN, RAB32_HUMAN, PTPM1_HUMAN, DCAKD_HUMAN, PPOX_HUMAN, BCS1_HUMAN, MIC27_HUMAN, HINT3_HUMAN, TAM41_HUMAN, COXM2_HUMAN, RDH14_HUMAN, PPM1K_HUMAN, COX7C_HUMAN, CISD2_HUMAN, AOFA_HUMAN, COX11_HUMAN, RAB35_HUMAN, PX11B_HUMAN, NCEH1_HUMAN, FUND2_HUMAN, PRLD1_HUMAN, NDUF4_HUMAN, COX19_HUMAN, LYRM7_HUMAN, TIM21_HUMAN, UQCC2_HUMAN, PGES2_HUMAN, CCD51_HUMAN, TMM70_HUMAN, NDUF3_HUMAN, COX8A_HUMAN, TIDC1_HUMAN, TMM11_HUMAN, T126A_HUMAN, COX20_HUMAN, NDUB5_HUMAN, CHDH_HUMAN, SCPDL_HUMAN, NFS1_HUMAN, NDUS8_HUMAN, RDH13_HUMAN, COX7R_HUMAN, SNP29_HUMAN, QCR8_HUMAN, KGUA_HUMAN, PTH2_HUMAN, CPT2_HUMAN, NDUF2_HUMAN, MTX1_HUMAN, CX6A1_HUMAN, ACAD9_HUMAN, NDUB4_HUMAN, MAIP1_HUMAN, SFXN4_HUMAN, COX6C_HUMAN, NDUS6_HUMAN, NDUA7_HUMAN, MRPP3_HUMAN, NDUBB_HUMAN, NDUBA_HUMAN, NDUS5_HUMAN, COA3_HUMAN, GLSK_HUMAN, NDUA6_HUMAN, CHCH2_HUMAN, SCO2_HUMAN, NDUS7_HUMAN, NDUB3_HUMAN, UQCC1_HUMAN, CMTD1_HUMAN, ROMO1_HUMAN, OXA1L_HUMAN, TIM14_HUMAN, HEBP1_HUMAN, COQ8B_HUMAN, RMND1_HUMAN, OCAD1_HUMAN, NDUA5_HUMAN, CMC1_HUMAN, CCHL_HUMAN, SQOR_HUMAN, MTX2_HUMAN, NDUAD_HUMAN, NDUB8_HUMAN, TM177_HUMAN, HEMH_HUMAN, NDUB7_HUMAN, TM205_HUMAN, NDUV1_HUMAN, NDUB1_HUMAN, ETFD_HUMAN, MPPA_HUMAN, MPPB_HUMAN, ATP5I_HUMAN, UCRI_HUMAN, ATP5H_HUMAN, NDUA2_HUMAN, NDUAB_HUMAN, ECI2_HUMAN, MCU_HUMAN, QCR7_HUMAN, QCR9_HUMAN, ATP5E_HUMAN, TMM65_HUMAN, ERAL1_HUMAN, TIM16_HUMAN, GHITM_HUMAN, GSTK1_HUMAN, GLRX5_HUMAN, THIK_HUMAN, CYB5B_HUMAN, AIFM2_HUMAN, PREP_HUMAN, ACSL5_HUMAN, FXRD1_HUMAN, COX5A_HUMAN, NDUB9_HUMAN, NDUA8_HUMAN, BDH_HUMAN, F213A_HUMAN, HTAI2_HUMAN, SCO1_HUMAN, RM14_HUMAN, COMT_HUMAN, MTCH1_HUMAN, SDHB_HUMAN, COX15_HUMAN, DHSD_HUMAN, MICU1_HUMAN, RAB24_HUMAN, ARM10_HUMAN, RC3H1_HUMAN, CXXC4_HUMAN.J9JIF5_HUMAN, CXXC5_HUMAN, GMEB1_HUMAN, NR2C1_HUMAN, SP100_HUMAN, RLA1_HUMAN, BAF_HUMAN, PTPRU_HUMAN, LRIG2_HUMAN, BBC3B_HUMAN.BBC3_HUMAN, RAD_HUMAN, BABA2_HUMAN, ATOH1_HUMAN, CRBN_HUMAN, LTK_HUMAN, SOX9_HUMAN, IBP2_HUMAN, FLCN_HUMAN, FNIP2_HUMAN, PDP1_HUMAN, PTN7_HUMAN, PTPRA_HUMAN, PTPRH_HUMAN, PTPRT_HUMAN, PPM1A_HUMAN, MPZL2_HUMAN, SSH1_HUMAN, SRRM4_HUMAN, CLM7_HUMAN, E9PPJ3_HUMAN.SMTL1_HUMAN, KR161_HUMAN, MYO9A_HUMAN, IGLL5_HUMAN, RAS4B_HUMAN, PGRC1_HUMAN, ACACB_HUMAN, IF1AY_HUMAN, E41L2_HUMAN, FOXO3_HUMAN, DYRK3_HUMAN, SPAG7_HUMAN, OR2F2_HUMAN, ABCA1_HUMAN, HERC2_HUMAN, 1B07_HUMAN.1B08_HUMAN.1B13_HUMAN.1B14_HUMAN.1B15_HUMAN.1B18_HUMAN.1B27_HUMAN.1B35_HUMAN.1B37_HUMAN.1B38_HUMAN.1B39_HUMAN.1B40_HUMAN.1B41_HUMAN.1B42_HUMAN.1B44_HUMAN.1B45_HUMAN.1B46_HUMAN.1B47_HUMAN.1B48_HUMAN.1B49_HUMAN.1B50_HUMAN.1B51_HUMAN.1B52_HUMAN.1B53_HUMAN.1B54_HUMAN.1B55_HUMAN.1B56_HUMAN.1B57_HUMAN.1B58_HUMAN.1B59_HUMAN.1B67_HUMAN.1B73_HUMAN.1B78_HUMAN.1B81_HUMAN.1B82_HUMAN, CO1A1_HUMAN, FETUA_HUMAN, MAS_HUMAN, HMGN2_HUMAN, RLA2_HUMAN, LA_HUMAN, CO1A2_HUMAN, K1C16_HUMAN, HMGB1_HUMAN, DRD2_HUMAN, GLNA_HUMAN, LFA3_HUMAN, NF1_HUMAN, CNTF_HUMAN, DPP4_HUMAN, DHI1_HUMAN, GBRA3_HUMAN, K1C9_HUMAN, GRIK4_HUMAN, IDH3G_HUMAN, KCNQ1_HUMAN, TCP4_HUMAN, SESN2_HUMAN, KR109_HUMAN, S10AA_HUMAN, RAB1A_HUMAN, NTH_HUMAN, AK17A_HUMAN, SLC31_HUMAN, BPTF_HUMAN, CSTF3_HUMAN, VPP3_HUMAN, LRP8_HUMAN, PDE1C_HUMAN, DIP2A_HUMAN, CBX2_HUMAN, GRM4_HUMAN, STIL_HUMAN, DIXC1_HUMAN, HERC1_HUMAN, E2F4_HUMAN, MICB_HUMAN, KR151_HUMAN, RHG29_HUMAN, DOP1_HUMAN, EYS_HUMAN, SKT_HUMAN, MCAF2_HUMAN, EST4A_HUMAN, NADE_HUMAN, PKHA7_HUMAN, EMAL6_HUMAN, ZCCHV_HUMAN, PCLI1_HUMAN, SETX_HUMAN, OR2W3_HUMAN, PRS42_HUMAN, ZN573_HUMAN, S13A5_HUMAN, ZZZ3_HUMAN, CENPL_HUMAN, MIER1_HUMAN, RM43_HUMAN, ZN114_HUMAN, MK15_HUMAN, CHD6_HUMAN, MUC16_HUMAN, DYH7_HUMAN, ROBO4_HUMAN, S39A7_HUMAN, EDEM1_HUMAN, LFG3_HUMAN, ELP4_HUMAN, MTMR8_HUMAN, DYH8_HUMAN, PRIC1_HUMAN, SPB12_HUMAN, MINT_HUMAN, SOSB1_HUMAN, ZFY21_HUMAN, SYT17_HUMAN, CNPY3_HUMAN, ASHWN_HUMAN, PLVAP_HUMAN, NXF2_HUMAN, KTBL1_HUMAN, NUCKS_HUMAN, REEP4_HUMAN, NOL6_HUMAN, RPF1_HUMAN, IRPL2_HUMAN, MLXPL_HUMAN, INCE_HUMAN, EXOS3_HUMAN, TEKT2_HUMAN, SO3A1_HUMAN, JUPI1_HUMAN, TRHDE_HUMAN, GRID1_HUMAN, S45A2_HUMAN, ING4_HUMAN, NOSIP_HUMAN, CBY1_HUMAN, WIPI2_HUMAN, PCDG3_HUMAN, K2C3_HUMAN, K1C10_HUMAN, K22E_HUMAN, K2C5_HUMAN, GOGB1_HUMAN, GP149_HUMAN, MERL_HUMAN, PPM1E_HUMAN, STYX_HUMAN, DUS12_HUMAN, DUS19_HUMAN, DUS6_HUMAN, MTMR3_HUMAN, HKDC1_HUMAN, NANO2_HUMAN, CR3L1_HUMAN, ZN692_HUMAN, RM34_HUMAN, SEP14_HUMAN, NPC2_HUMAN, LOX5_HUMAN, GA45B_HUMAN, JUNB_HUMAN, TXNIP_HUMAN, NLE1_HUMAN, T2EB_HUMAN, MSRA_HUMAN, TCPW_HUMAN, GPBL1_HUMAN, GLMN_HUMAN, ZN263_HUMAN, TEAN2_HUMAN, A6NFS0_HUMAN.ZN275_HUMAN, CENPR_HUMAN, SEP11_HUMAN, KLDC3_HUMAN, RPF2_HUMAN, DDX31_HUMAN, BODG_HUMAN, RL27_HUMAN, RL18A_HUMAN, ZN689_HUMAN, CDC23_HUMAN, CENPN_HUMAN, PK1IP_HUMAN, RRS1_HUMAN, CENPU_HUMAN, ZN184_HUMAN, NSD2_HUMAN, ZN800_HUMAN, TPC2_HUMAN, A1AG1_HUMAN, TSKS_HUMAN, RLP24_HUMAN, SG1D4_HUMAN, SRP09_HUMAN, RRP8_HUMAN, DEF1_HUMAN, GBP2_HUMAN, ZFP62_HUMAN, E41L5_HUMAN, ZN512_HUMAN, ACTBL_HUMAN, ERD21_HUMAN, NOL7_HUMAN, DOCK7_HUMAN, REPI1_HUMAN, ZNF48_HUMAN, RL30_HUMAN, NSA2_HUMAN, RBM34_HUMAN, ZSC25_HUMAN, RM35_HUMAN, BATF3_HUMAN, SURF6_HUMAN, SIA8D_HUMAN, 5HT3A_HUMAN, PCDBB_HUMAN, NIP7_HUMAN, RL11_HUMAN, ARNT2_HUMAN, NOL12_HUMAN, NOP56_HUMAN, ZN414_HUMAN, FCF1_HUMAN, MAK16_HUMAN, RL7L_HUMAN, ABT1_HUMAN, ZN771_HUMAN, NOP53_HUMAN, PTPRE_HUMAN, RAB31_HUMAN, PP2BB_HUMAN, PPM1B_HUMAN, TPTE_HUMAN, SL9A1_HUMAN, CYLD_HUMAN, MAGA1_HUMAN, COQ2_HUMAN, ODO2_HUMAN, BNIP3_HUMAN, CCND2_HUMAN, EXT1_HUMAN, T22D4_HUMAN, MCPH1_HUMAN, PLK2_HUMAN, TES_HUMAN, APRIO_HUMAN.PRIO_HUMAN, HEPS_HUMAN, DISC1_HUMAN, UBP30_HUMAN, CCND1_HUMAN, CCND3_HUMAN, CRYAB_HUMAN, AT5G1_HUMAN, MTG16_HUMAN, CEBPD_HUMAN, UB2E3_HUMAN, UBE2K_HUMAN, UBE2T_HUMAN, UBE2Z_HUMAN, HIF1N_HUMAN, TBA1B_HUMAN, HELZ_HUMAN, GLI3_HUMAN, LTV1_HUMAN, AKP8L_HUMAN, BCOR_HUMAN, SDCG3_HUMAN, RBBP7_HUMAN, AMER1_HUMAN, GWL_HUMAN, 1C01_HUMAN.1C02_HUMAN.1C03_HUMAN.1C04_HUMAN.1C05_HUMAN.1C06_HUMAN.1C07_HUMAN.1C08_HUMAN.1C12_HUMAN.1C14_HUMAN.1C15_HUMAN.1C16_HUMAN.1C17_HUMAN.1C18_HUMAN, ZN281_HUMAN, SMN_HUMAN, NOB1_HUMAN, SIK3_HUMAN, ZN318_HUMAN, ZN106_HUMAN, ARIP4_HUMAN, BMP2K_HUMAN, MA7D3_HUMAN, AXIN1_HUMAN, CHD1_HUMAN, OTUD5_HUMAN, NOTC2_HUMAN, ZN703_HUMAN, BRCA2_HUMAN, GATA6_HUMAN, NFAC3_HUMAN, STK3_HUMAN, ETV6_HUMAN, PPM1G_HUMAN, ZBT10_HUMAN, SEBP2_HUMAN, F120B_HUMAN, ANR17_HUMAN, CLSPN_HUMAN, NASP_HUMAN, PRDX2_HUMAN, CRTC2_HUMAN, GTF2I_HUMAN, TROAP_HUMAN, TATD2_HUMAN, ALG13_HUMAN, MOFA1_HUMAN, ESS2_HUMAN, ZRAB2_HUMAN, PNO1_HUMAN, ELOC_HUMAN, CENPJ_HUMAN, ZN593_HUMAN, SAV1_HUMAN, NFAC1_HUMAN, ZNF24_HUMAN, CITE2_HUMAN, 4ET_HUMAN, SEH1_HUMAN, GCDH_HUMAN, ANR11_HUMAN, FOXC1_HUMAN, ELOB_HUMAN, SUFU_HUMAN, MYL1_HUMAN, MIC13_HUMAN, RPAB3_HUMAN, PJA1_HUMAN, SIN1_HUMAN, ECD_HUMAN, PARG_HUMAN, MIP18_HUMAN, RBM20_HUMAN, GLI2_HUMAN, C1TM_HUMAN, CRTC3_HUMAN, RPAB5_HUMAN, PP1G_HUMAN, TBL1X_HUMAN, ZBTB1_HUMAN, N4BP2_HUMAN, MLF2_HUMAN, ANKH1_HUMAN, RPB3_HUMAN, SAMH1_HUMAN, SMG7_HUMAN, GPN1_HUMAN, PEX1_HUMAN, MAEA_HUMAN, HAUS7_HUMAN, ANR54_HUMAN, GID8_HUMAN, NOC4L_HUMAN, CREB5_HUMAN, RNC_HUMAN, UMPS_HUMAN, RMI1_HUMAN, GEMI2_HUMAN, GTSE1_HUMAN, PNKD_HUMAN, MSI1H_HUMAN, RBM27_HUMAN, SGO2_HUMAN, SIK2_HUMAN, LSM7_HUMAN, RPAP2_HUMAN, KBL_HUMAN, SMG5_HUMAN, HDHD5_HUMAN, QTRT2_HUMAN, THOC3_HUMAN, IP3KC_HUMAN, M1IP1_HUMAN, RHG39_HUMAN, RING1_HUMAN, WDR62_HUMAN, TICRR_HUMAN, PARP4_HUMAN, HJURP_HUMAN, NCOA2_HUMAN, HAUS2_HUMAN, SPC24_HUMAN, ETAA1_HUMAN, NCOA4_HUMAN, RBP10_HUMAN, TCAL1_HUMAN, PFD2_HUMAN, EYA4_HUMAN, NAB1_HUMAN, MKNK1_HUMAN, TALD3_HUMAN, MEX3A_HUMAN, PTOV1_HUMAN, SLIRP_HUMAN, IF4E2_HUMAN, ZIC2_HUMAN, SUCA_HUMAN, ERCC3_HUMAN, CDC42_HUMAN, STK4_HUMAN, MKLN1_HUMAN, IN80B_HUMAN, MYCPP_HUMAN, CSN2_HUMAN, PITX1_HUMAN, BRCC3_HUMAN, LEF1_HUMAN, AKP13_HUMAN, DRG1_HUMAN, MTMRE_HUMAN, PISD_HUMAN, CDK12_HUMAN, RPAC2_HUMAN.RPC22_HUMAN, SYPM_HUMAN, TISB_HUMAN, RAVR1_HUMAN, TOB2_HUMAN, PP6R2_HUMAN, TOP3A_HUMAN, SENP1_HUMAN, GLYC_HUMAN, PFD6_HUMAN, DDHD1_HUMAN, RNF10_HUMAN, RO60_HUMAN, PCGF1_HUMAN, INT13_HUMAN, WDR75_HUMAN, CE350_HUMAN, SELK_HUMAN, PHF8_HUMAN, NIN_HUMAN, NUB1_HUMAN, ASPM_HUMAN, TOPB1_HUMAN, ZN282_HUMAN, CEP85_HUMAN, TCAL4_HUMAN, ZN644_HUMAN, FOXN4_HUMAN, PSMF1_HUMAN, FXRD2_HUMAN, GMPPA_HUMAN, CE192_HUMAN, ABHDA_HUMAN, MPLKI_HUMAN, PDD2L_HUMAN, ACDSB_HUMAN, APC7_HUMAN, TARB1_HUMAN, PIPSL_HUMAN, APC5_HUMAN, MYBB_HUMAN, EXO1_HUMAN, DPOE3_HUMAN, CEPT1_HUMAN, RHOA_HUMAN, COPRS_HUMAN, APT_HUMAN, ZBTB5_HUMAN, ZN507_HUMAN, IKBA_HUMAN, FEM1B_HUMAN, VGLL4_HUMAN, FSBP_HUMAN.RA54B_HUMAN, CYC_HUMAN, TPX2_HUMAN, NUP43_HUMAN, PFD3_HUMAN, MAT1_HUMAN, PFD1_HUMAN, PAX3_HUMAN, EYA3_HUMAN, SUCB2_HUMAN, MAML1_HUMAN, RGAP1_HUMAN, SLX4_HUMAN, TUT4_HUMAN, LYPA2_HUMAN, HXB9_HUMAN, MGRN1_HUMAN, KLF16_HUMAN, STXB4_HUMAN, JHD2C_HUMAN, CD123_HUMAN, IFT74_HUMAN, VGLL3_HUMAN, ZGPAT_HUMAN, LST8_HUMAN, ENL_HUMAN, MGAP_HUMAN, FEM1A_HUMAN, NDC1_HUMAN, DCP2_HUMAN, ARI5B_HUMAN, GPBP1_HUMAN, KTU_HUMAN, Q9H4D1_HUMAN.RIPK4_HUMAN, TCHP_HUMAN, GALE_HUMAN, PPIE_HUMAN, H2AZ_HUMAN, GGA1_HUMAN, GGA2_HUMAN, GGA3_HUMAN, NEB2_HUMAN, UPAR_HUMAN, GBG12_HUMAN, AMPN_HUMAN, LMO7_HUMAN, FLOT1_HUMAN, UTRO_HUMAN, ML12B_HUMAN, PIHD1_HUMAN, TNIP2_HUMAN, NKX21_HUMAN, CHD3_HUMAN, TNFA_HUMAN, DOLK_HUMAN, MKS3_HUMAN, ZC12A_HUMAN, SPDLY_HUMAN, TPC2B_HUMAN, PAXI_HUMAN, SRBP2_HUMAN, EPGN_HUMAN, 2B14_HUMAN, OCTC_HUMAN, TAF9B_HUMAN, TSPOB_HUMAN.TSPO_HUMAN, PKP2_HUMAN, CCR5_HUMAN, SRA1_HUMAN, CAMP2_HUMAN, TE2IP_HUMAN, KRIT1_HUMAN, S10AB_HUMAN, PDIA2_HUMAN, H2B1N_HUMAN, EFNB1_HUMAN, STF1_HUMAN, BCAR1_HUMAN, K1C14_HUMAN, SIX3_HUMAN, K2C6A_HUMAN, KCNA1_HUMAN, RA51C_HUMAN, PTPRC_HUMAN, EPHB4_HUMAN, NOMO2_HUMAN, MPRIP_HUMAN, S14L2_HUMAN, H2B1C_HUMAN.H2B1D_HUMAN, PGH2_HUMAN, RPGF4_HUMAN, PP4P1_HUMAN, PIAS1_HUMAN, AP180_HUMAN, TNNI3_HUMAN, MYL9_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P21796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage dependent anion channel 1 [Source:HGNC Symbol;Acc:HGNC:12669]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDAC1_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTEF3_HUMAN, SQSTM_HUMAN, MFN2_HUMAN, MFN1_HUMAN, VDAC2_HUMAN, NOS3_HUMAN, CDK2_HUMAN, BCL2_HUMAN, VDAC3_HUMAN, AATM_HUMAN, DOC2A_HUMAN, 1433E_HUMAN, BAK_HUMAN, NDUV1_HUMAN, IF6_HUMAN, HXK1_HUMAN, ITPR1_HUMAN, TRAF6_HUMAN, CRCM_HUMAN, GBRL2_HUMAN, KINH_HUMAN, GRP75_HUMAN, ATF2_HUMAN, PRDX6_HUMAN, FLRT2_HUMAN, GELS_HUMAN, TRAF2_HUMAN, SF3A1_HUMAN, THIC_HUMAN, GSTK1_HUMAN, RAI14_HUMAN, TM11F_HUMAN, SPTB2_HUMAN, SYUA_HUMAN, CBR1_HUMAN, TITIN_HUMAN, ADT3_HUMAN, MTOR_HUMAN, B2CL1_HUMAN, NUDC_HUMAN, RIF1_HUMAN, IKKE_HUMAN, GANAB_HUMAN, TMX1_HUMAN, CALX_HUMAN, 1B42_HUMAN, FSCN1_HUMAN, TPM3_HUMAN, NOL7_HUMAN, RIPK2_HUMAN, PANK2_HUMAN, CDK1_HUMAN, PCSK6_HUMAN, LRRK2_HUMAN, CSK2B_HUMAN, STOM_HUMAN, TOM20_HUMAN, KCRU_HUMAN, MCL1_HUMAN, B2L11_HUMAN, DYLT3_HUMAN, BAX_HUMAN, RAF1_HUMAN, DYLT1_HUMAN, PPIF_HUMAN, TBA4A_HUMAN, KPCE_HUMAN, TOM22_HUMAN, TOM70_HUMAN, TOM40_HUMAN, HSP7C_HUMAN, A4_HUMAN, SPG7_HUMAN, CAV1_HUMAN, ESR1_HUMAN, CYC_HUMAN, UBC_HUMAN, ICT1_HUMAN, CD4_HUMAN, HDAC5_HUMAN, MK03_HUMAN, MK01_HUMAN, SIR7_HUMAN, PRKN_HUMAN, RL40_HUMAN, SF01_HUMAN, VAPA_HUMAN, SFXN3_HUMAN, TIAR_HUMAN, SUGP1_HUMAN, FACE1_HUMAN, THIM_HUMAN, FLOT2_HUMAN, ACAD9_HUMAN, MGT4B_HUMAN, SSDH_HUMAN, TBA1B_HUMAN, MDC1_HUMAN, VCAM1_HUMAN, BAG3_HUMAN, ADRB2_HUMAN, SPRTN_HUMAN, FXRD2_HUMAN, UBAC2_HUMAN, APOE_HUMAN, PLIN3_HUMAN, ATPA_HUMAN, ATPB_HUMAN, ATPD_HUMAN, ATP5I_HUMAN, ATPO_HUMAN, VA0D1_HUMAN, BAP29_HUMAN, BAP31_HUMAN, CISD1_HUMAN, CISD2_HUMAN, CLH1_HUMAN, OST48_HUMAN, GPX4_HUMAN, MAGT1_HUMAN, NDUA8_HUMAN, NDUA9_HUMAN, PHB_HUMAN, PHB2_HUMAN, RPN1_HUMAN, SGPL1_HUMAN, SSRG_HUMAN, STX12_HUMAN, TSPOB_HUMAN.TSPO_HUMAN, MRP1_HUMAN, MRP3_HUMAN, ACADM_HUMAN, AQP9_HUMAN, AT1A1_HUMAN, AT1A2_HUMAN, AT1A3_HUMAN, AT1B1_HUMAN, AT1B3_HUMAN, ATPG_HUMAN, AT5F1_HUMAN, VATA_HUMAN, COX41_HUMAN, CY1_HUMAN, MIC60_HUMAN, MTCH1_HUMAN, MTCH2_HUMAN, NDUB4_HUMAN, NDUS4_HUMAN, M2OM_HUMAN, TECR_HUMAN, QCR7_HUMAN, QCR2_HUMAN, NTRK1_HUMAN, MED20_HUMAN, EWS_HUMAN, RAB2A_HUMAN, RAB5C_HUMAN, RAB7A_HUMAN, FGOP2_HUMAN, GOT1B_HUMAN, MYO19_HUMAN, MMGT1_HUMAN, U2AF2_HUMAN, COX15_HUMAN, SOAT1_HUMAN, PPM1B_HUMAN, XRCC6_HUMAN, ML12A_HUMAN.ML12B_HUMAN, THIO_HUMAN, CHM4B_HUMAN, ADT1_HUMAN, TPM1_HUMAN, MIC19_HUMAN, SFXN1_HUMAN, NDUA5_HUMAN, ADT2_HUMAN, CX7A2_HUMAN, BAF_HUMAN, PPM1A_HUMAN, PPIA_HUMAN, H1X_HUMAN, SCYL2_HUMAN, ARF1_HUMAN, PGRC1_HUMAN, SAP18_HUMAN, RL36_HUMAN, LMNB1_HUMAN, ATP5H_HUMAN, MOB2_HUMAN, RL27_HUMAN, XRCC5_HUMAN, D19L1_HUMAN, STML2_HUMAN, ODPB_HUMAN, RL12_HUMAN, RL35_HUMAN, EMD_HUMAN, H10_HUMAN, RMXL2_HUMAN, ILF2_HUMAN, RL28_HUMAN, COX5A_HUMAN, MPCP_HUMAN, RL30_HUMAN, DKC1_HUMAN, FBRL_HUMAN, ELAV1_HUMAN, RNPS1_HUMAN, SERPH_HUMAN, PRDX3_HUMAN, SSRD_HUMAN, ATD3A_HUMAN, ATPK_HUMAN, NDUS1_HUMAN, PI51C_HUMAN, NOP56_HUMAN, SSBP_HUMAN, RCN2_HUMAN, QCR1_HUMAN, PABP1_HUMAN, 1433Z_HUMAN, NOP58_HUMAN, ECHB_HUMAN, RUVB1_HUMAN, SPIN1_HUMAN, MCA3_HUMAN, SURF6_HUMAN, HNRDL_HUMAN, ENPL_HUMAN, NDUV2_HUMAN, SF3B6_HUMAN, H2AV_HUMAN, NDUS3_HUMAN, CLCC1_HUMAN, SYDC_HUMAN, ETFA_HUMAN, ODPA_HUMAN, H2AY_HUMAN, AIFM1_HUMAN, SSRP1_HUMAN, TKT_HUMAN, CBX3_HUMAN, ERLN2_HUMAN, 4F2_HUMAN, KCRB_HUMAN, ERLN1_HUMAN, BASI_HUMAN, NP1L1_HUMAN, RL1D1_HUMAN, AAAT_HUMAN, LA_HUMAN, RPN2_HUMAN, TR150_HUMAN, CBX1_HUMAN, DDX21_HUMAN, RM12_HUMAN, SAFB1_HUMAN, SP16H_HUMAN, EF1G_HUMAN, CMC2_HUMAN, ECHA_HUMAN, LMNB2_HUMAN, PERI_HUMAN, HORN_HUMAN, HP1B3_HUMAN, COPE_HUMAN, SYEP_HUMAN, RTCB_HUMAN, EF2_HUMAN, SYIC_HUMAN, TOP2A_HUMAN, TCPQ_HUMAN, SYLC_HUMAN, MYH11_HUMAN, IMB1_HUMAN, TOP1_HUMAN, H2A1B_HUMAN, H2B1C_HUMAN.H2B1D_HUMAN, H2B1C_HUMAN, RNF31_HUMAN, TADBP_HUMAN, FGFR1_HUMAN, PIHD1_HUMAN, CHD3_HUMAN, CHD4_HUMAN, F162A_HUMAN, CI163_HUMAN.YI001_HUMAN, 1B07_HUMAN.1B08_HUMAN.1B13_HUMAN.1B14_HUMAN.1B15_HUMAN.1B18_HUMAN.1B27_HUMAN.1B35_HUMAN.1B37_HUMAN.1B38_HUMAN.1B39_HUMAN.1B40_HUMAN.1B41_HUMAN.1B42_HUMAN.1B44_HUMAN.1B45_HUMAN.1B46_HUMAN.1B47_HUMAN.1B48_HUMAN.1B49_HUMAN.1B50_HUMAN.1B51_HUMAN.1B52_HUMAN.1B53_HUMAN.1B54_HUMAN.1B55_HUMAN.1B56_HUMAN.1B57_HUMAN.1B58_HUMAN.1B59_HUMAN.1B67_HUMAN.1B73_HUMAN.1B78_HUMAN.1B81_HUMAN.1B82_HUMAN, DHRS2_HUMAN, ACTB_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPLA_HUMAN, SUMO2_HUMAN, CCNB1_HUMAN, 1433S_HUMAN, JUN_HUMAN, LST8_HUMAN, PRR5_HUMAN.RHG08_HUMAN, SIN1_HUMAN, RICTR_HUMAN, P53_HUMAN, PO4F2_HUMAN, AP2A_HUMAN, DEK_HUMAN, ATAD2_HUMAN, CTLA4_HUMAN, RUNX1_HUMAN, PEBB_HUMAN, FOXP3_HUMAN, RUNX3_HUMAN, SMAD3_HUMAN, FOXO3_HUMAN, SMAD4_HUMAN, PRI1_HUMAN, PRI2_HUMAN, DPOLA_HUMAN, DPOA2_HUMAN, HOIL1_HUMAN, SHRPN_HUMAN, TRADD_HUMAN, RIPK1_HUMAN, FADD_HUMAN, CASP8_HUMAN, OTUL_HUMAN, NGF_HUMAN, TNR16_HUMAN, CENPR_HUMAN, BEX3_HUMAN, MYD88_HUMAN, IRAK1_HUMAN, KPCI_HUMAN, IKKB_HUMAN, NFKB1_HUMAN, TF65_HUMAN, GLU2B_HUMAN, CALR_HUMAN, CABL1_HUMAN, WEE1_HUMAN, CFLAR_HUMAN, BID_HUMAN, BAD_HUMAN, APAF_HUMAN, CASP9_HUMAN, IMA5_HUMAN, DFFA_HUMAN, DFFB_HUMAN, M3K1_HUMAN, IKKA_HUMAN, NEMO_HUMAN, IRAK2_HUMAN, MYO1C_HUMAN, NANOG_HUMAN, PO5F1_HUMAN, DPPA4_HUMAN, SOX2_HUMAN, CCNB2_HUMAN, MRVI1_HUMAN, TXNIP_HUMAN, NRF1_HUMAN, PRGC2_HUMAN, CNGA4_HUMAN, CNGA2_HUMAN, CNGB1_HUMAN, ST1A3_HUMAN.ST1A4_HUMAN, ST1A4_HUMAN, GSTA4_HUMAN, OPLA_HUMAN, ACHB2_HUMAN, ACHA4_HUMAN, CBY1_HUMAN, CTNB1_HUMAN, XPO1_HUMAN, LCK_HUMAN, IL27B_HUMAN, EF1B_HUMAN, EF1D_HUMAN, ACHA6_HUMAN, ACHB3_HUMAN, CO4A5_HUMAN, CO4A4_HUMAN, CO4A3_HUMAN, M3K3_HUMAN, UBE2N_HUMAN, UB2V1_HUMAN, RPTOR_HUMAN, ASHWN_HUMAN, DDX1_HUMAN, FA98B_HUMAN, RTRAF_HUMAN, ARCH_HUMAN, NTRK1_HUMAN.TFG_HUMAN.TPR_HUMAN, KCRM_HUMAN, GSTP1_HUMAN, AKTS1_HUMAN, HSF1_HUMAN, M3K5_HUMAN, DNJA4_HUMAN, CCNE1_HUMAN, RFA4_HUMAN, RFA3_HUMAN, RFA2_HUMAN, RFA1_HUMAN, CCNA1_HUMAN, CCNA2_HUMAN, KALM_HUMAN, LAMA4_HUMAN, LAMC1_HUMAN, LAMB1_HUMAN, LAMB2_HUMAN, LAMC3_HUMAN, SRC_HUMAN, ITB1_HUMAN, ITA4_HUMAN, JAM3_HUMAN, JAM2_HUMAN, PPIL2_HUMAN, LEUK_HUMAN, AT1B2_HUMAN, YLAT1_HUMAN, LAT2_HUMAN, BAT1_HUMAN, XCT_HUMAN, LAT1_HUMAN, AAA1_HUMAN, YLAT2_HUMAN, ISG15_HUMAN, SMCA4_HUMAN, BRWD1_HUMAN, IL16_HUMAN, TNR14_HUMAN, BTLA_HUMAN, GRB2_HUMAN, CLCA_HUMAN, ITB7_HUMAN, MADCA_HUMAN, SNCAP_HUMAN, UB2L6_HUMAN, SIAH1_HUMAN, USP9X_HUMAN, SORL_HUMAN, 1433B_HUMAN, BRAF_HUMAN.K1549_HUMAN, FRS2_HUMAN, PLCG1_HUMAN, CRKL_HUMAN, RPGF1_HUMAN, KDIS_HUMAN, CRK_HUMAN, L1CAM_HUMAN, MP2K1_HUMAN, MP2K2_HUMAN, OSTP_HUMAN, ITA9_HUMAN, T126B_HUMAN, CIA30_HUMAN, ECSIT_HUMAN, TSPO_HUMAN, RIMB1_HUMAN, ATX3_HUMAN, GOGA4_HUMAN, AUXI_HUMAN, AP4E1_HUMAN, AP4M1_HUMAN, AP4B1_HUMAN, AP4S1_HUMAN, SUMO1_HUMAN, PINK1_HUMAN, VDAC1_HUMAN, PTEN_HUMAN, TLN1_HUMAN, FARP2_HUMAN, NCAM1_HUMAN, EPHB2_HUMAN, GFRA4_HUMAN, RET_HUMAN, PSPN_HUMAN, WWTR1_HUMAN, MPIP3_HUMAN, MOT4_HUMAN, MOT3_HUMAN, MOT1_HUMAN, DUS2L_HUMAN, SF3A2_HUMAN, SF3A3_HUMAN, ATP5E_HUMAN, AXIN1_HUMAN, LRP6_HUMAN, WNT3A_HUMAN, GSK3B_HUMAN, FZD5_HUMAN, VA0D2_HUMAN, PRKDC_HUMAN, SSRA_HUMAN, SSRB_HUMAN, FUBP2_HUMAN, PESC_HUMAN, EBP2_HUMAN, GNL3_HUMAN, UBP37_HUMAN, PRS8_HUMAN, COPB2_HUMAN, COPA_HUMAN, IL27A_HUMAN, IL12A_HUMAN, NPM_HUMAN.RARA_HUMAN, RBBP7_HUMAN, HJURP_HUMAN, RBBP4_HUMAN, VA0E1_HUMAN, VATL_HUMAN, VATO_HUMAN, VPP1_HUMAN, ODPAT_HUMAN, ACY1_HUMAN, FOS_HUMAN, KAPCA_HUMAN, PTN11_HUMAN, GAB1_HUMAN, DPOLL_HUMAN, DCR1C_HUMAN, STK11_HUMAN, HS90A_HUMAN, TNR5_HUMAN, CD40L_HUMAN, HDAC4_HUMAN, GPC1_HUMAN, FGF2_HUMAN, NCOR1_HUMAN, BIRC3_HUMAN, BIRC2_HUMAN, P63_HUMAN, AKT1_HUMAN, M3K7_HUMAN, TAB2_HUMAN, TAB1_HUMAN, SNF5_HUMAN, SMCE1_HUMAN, ESR2_HUMAN, ZNF14_HUMAN, SDC1_HUMAN, TGFR2_HUMAN, TGFR1_HUMAN, TGFB1_HUMAN, ACVL1_HUMAN, EGLN_HUMAN, IMA1_HUMAN, PO2F1_HUMAN, BRCA1_HUMAN, NF1_HUMAN, ARHGF_HUMAN, EPHA4_HUMAN, EFNA1_HUMAN, FINC_HUMAN, CSPG4_HUMAN, CSF2_HUMAN, SHC1_HUMAN, IL3RB_HUMAN, CSF2R_HUMAN, JAK2_HUMAN, PRR5_HUMAN, DPTOR_HUMAN, PARK7_HUMAN, RHG32_HUMAN, ZN274_HUMAN, BDNF_HUMAN, SORT_HUMAN, TDT_HUMAN, FGF1_HUMAN, FGF4_HUMAN, TP4A1_HUMAN, BRAF_HUMAN, PLD2_HUMAN, PDPK1_HUMAN, CAR11_HUMAN, MALT1_HUMAN, BCL10_HUMAN, TNR1A_HUMAN, TNFA_HUMAN, TRAF1_HUMAN, GBB1_HUMAN, GBG2_HUMAN, CBLB_HUMAN, TSP2_HUMAN, ABI1_HUMAN, BARD1_HUMAN, TERT_HUMAN, KS6B1_HUMAN, NED4L_HUMAN, TBB2A_HUMAN, HDAC6_HUMAN, PAXI_HUMAN, TNAP3_HUMAN, TOR1A_HUMAN, GTR4_HUMAN, ACAP1_HUMAN, PAR6A_HUMAN, PAR3_HUMAN, SC6A3_HUMAN, NOD2_HUMAN, IGSF8_HUMAN, CDN1B_HUMAN, NTF3_HUMAN, CITE1_HUMAN, TR10B_HUMAN, TNF10_HUMAN, TNR1B_HUMAN, PLD1_HUMAN, RGS19_HUMAN, GIPC1_HUMAN, MRE11_HUMAN, NBN_HUMAN, ATM_HUMAN, RAD50_HUMAN, ADA28_HUMAN, SIR1_HUMAN, HS90B_HUMAN, TGM2_HUMAN, FKBP8_HUMAN, JUNB_HUMAN, TYY1_HUMAN, PRGC1_HUMAN, NFAC1_HUMAN, ITA3_HUMAN, KPCD_HUMAN, TRAF3_HUMAN, EP300_HUMAN, IL3RA_HUMAN, IL3_HUMAN, MK_HUMAN, MATK_HUMAN, LMO4_HUMAN, HDAC1_HUMAN, MTA1_HUMAN, JUND_HUMAN, SET_HUMAN, RUVB2_HUMAN, TSP1_HUMAN, ITA6_HUMAN, EIF2A_HUMAN, GATA4_HUMAN, HEY1_HUMAN, BMPR2_HUMAN, GDF2_HUMAN, H2AX_HUMAN, PLCB2_HUMAN, CREB1_HUMAN, ITB2_HUMAN, ITAD_HUMAN, FKB1A_HUMAN, NTF4_HUMAN, NDEL1_HUMAN, BCOR_HUMAN, BCL6_HUMAN, DPOLM_HUMAN, CDN1A_HUMAN, TRPV1_HUMAN, NCOR2_HUMAN, GATA1_HUMAN, RFXK_HUMAN, CD81_HUMAN, EFNA5_HUMAN, PDCD4_HUMAN, IF4A1_HUMAN, MYH2_HUMAN, AP1M1_HUMAN, ITA7_HUMAN, ABL1_HUMAN, CD14_HUMAN, CEBPA_HUMAN, SIR2_HUMAN, GATA2_HUMAN, HEY2_HUMAN, STA5A_HUMAN, ITAV_HUMAN, ITB3_HUMAN, NR0B2_HUMAN, JDP2_HUMAN, TR10A_HUMAN, F13A_HUMAN, PML_HUMAN, FAIM1_HUMAN, VGFR3_HUMAN, VEGFD_HUMAN, TP4A3_HUMAN, SIN3B_HUMAN, SAP30_HUMAN, SIN3A_HUMAN, AN32A_HUMAN, LIS1_HUMAN, KTNA1_HUMAN, DYHC1_HUMAN, PEBP1_HUMAN, ANRA2_HUMAN, SMRC1_HUMAN, SMRD1_HUMAN, SMRC2_HUMAN, HSPB1_HUMAN, PTC1_HUMAN, BIK_HUMAN, PCNA_HUMAN, CO4A2_HUMAN, CO4A6_HUMAN, CO4A1_HUMAN, IL1R1_HUMAN, IL1A_HUMAN, CARM1_HUMAN, GRIP1_HUMAN, GBRA6_HUMAN, GBRA1_HUMAN, GBRA5_HUMAN, GBRA4_HUMAN, GBRA3_HUMAN, GBRA2_HUMAN, IF4E_HUMAN, IF4G1_HUMAN, LMNA_HUMAN, ALEX_HUMAN.GNAS1_HUMAN.GNAS2_HUMAN.GNAS3_HUMAN, ADCY1_HUMAN, NKX25_HUMAN, MEF2C_HUMAN, TRAF5_HUMAN, TNR17_HUMAN, TNF13_HUMAN, CD80_HUMAN, TN13B_HUMAN, TNR9_HUMAN, TNFL9_HUMAN, TR13B_HUMAN, 1433F_HUMAN, CD86_HUMAN, NUMA1_HUMAN, TPX2_HUMAN, ITA1_HUMAN, FYN_HUMAN, SRF_HUMAN, CXCR4_HUMAN, AKAP9_HUMAN, PKN1_HUMAN, 2A5D_HUMAN, KAP3_HUMAN, PP1A_HUMAN, TLR4_HUMAN, TANK_HUMAN, RON_HUMAN, ITB4_HUMAN, GLI1_HUMAN, GLI3_HUMAN, P85A_HUMAN, LCP2_HUMAN, P85B_HUMAN, ZAP70_HUMAN, VAV_HUMAN, U119A_HUMAN, JAK1_HUMAN, RASH_HUMAN, ARRB2_HUMAN, ARRB1_HUMAN, BTK_HUMAN, CD19_HUMAN, CD79B_HUMAN, CD79A_HUMAN, FCG2B_HUMAN, IRAK4_HUMAN, TAB3_HUMAN, CCND1_HUMAN, LYN_HUMAN, IL2RB_HUMAN, ITM2B_HUMAN, STAT6_HUMAN, STAT3_HUMAN, ANDR_HUMAN, RBAK_HUMAN, NCOA4_HUMAN, CYLD_HUMAN, VATE1_HUMAN, TNR11_HUMAN, TSHR_HUMAN, TNR12_HUMAN, FLOT1_HUMAN, KS6A1_HUMAN, KS6A2_HUMAN, MK14_HUMAN, MP2K3_HUMAN, ELK1_HUMAN, GRB7_HUMAN, FRS3_HUMAN, CADH1_HUMAN, DYN1_HUMAN, EGFR_HUMAN, TNIP1_HUMAN, PRLR_HUMAN, SMAD2_HUMAN, STRAP_HUMAN, PJA1_HUMAN, PRS7_HUMAN, IMA4_HUMAN, TBK1_HUMAN, PSB5_HUMAN, PRS4_HUMAN, KCNQ1_HUMAN, PSMD1_HUMAN, CDC37_HUMAN, PSD12_HUMAN, PSMD6_HUMAN, M3K14_HUMAN, PSD13_HUMAN, RELB_HUMAN, PSMD3_HUMAN, FKBP5_HUMAN, TNR8_HUMAN, TP4AP_HUMAN, KTN1_HUMAN, ROMO1_HUMAN, PSMD7_HUMAN, PRS6A_HUMAN, FLNA_HUMAN, IKBB_HUMAN, NFKB2_HUMAN, NCF1_HUMAN, ITPR1_HUMAN.ITPR3_HUMAN, FGF10_HUMAN.FGF11_HUMAN.FGF13_HUMAN.FGF14_HUMAN.FGF16_HUMAN.FGF17_HUMAN.FGF18_HUMAN.FGF19_HUMAN.FGF1_HUMAN.FGF20_HUMAN.FGF21_HUMAN.FGF22_HUMAN.FGF23_HUMAN.FGF2_HUMAN.FGF3_HUMAN.FGF4_HUMAN.FGF5_HUMAN.FGF6_HUMAN.FGF7_HUMAN.FGF8_HUMAN.FGF9_HUMAN, FGFR1_HUMAN.FGFR2_HUMAN.FGFR3_HUMAN.FGFR4_HUMAN, DUS6_HUMAN, MK01_HUMAN.MK03_HUMAN, 1433B_HUMAN.1433E_HUMAN.1433F_HUMAN.1433G_HUMAN.1433S_HUMAN.1433T_HUMAN.1433Z_HUMAN, ACBP_HUMAN.ANF_HUMAN.ANGT_HUMAN.AREG_HUMAN.BDNF_HUMAN.BMP10_HUMAN.BMP15_HUMAN.BMP2_HUMAN.BMP3_HUMAN.BMP4_HUMAN.BMP5_HUMAN.BMP6_HUMAN.BMP7_HUMAN.BMP8B_HUMAN.BTC_HUMAN.CALCA_HUMAN.CALCB_HUMAN.CALC_HUMAN.CCKN_HUMAN.CD40L_HUMAN.CD80_HUMAN.CD86_HUMAN.CGB7_HUMAN.COLI_HUMAN.CRF_HUMAN.CSF2_HUMAN.CSF3_HUMAN.CSH2_HUMAN.DHH_HUMAN.DLL1_HUMAN.DLL3_HUMAN.DLL4_HUMAN.EDN1_HUMAN.EDN2_HUMAN.EDN3_HUMAN.EGF_HUMAN.EPO_HUMAN.EREG_HUMAN.FGF10_HUMAN.FGF11_HUMAN.FGF13_HUMAN.FGF14_HUMAN.FGF16_HUMAN.FGF17_HUMAN.FGF18_HUMAN.FGF19_HUMAN.FGF1_HUMAN.FGF20_HUMAN.FGF21_HUMAN.FGF22_HUMAN.FGF23_HUMAN.FGF2_HUMAN.FGF3_HUMAN.FGF4_HUMAN.FGF5_HUMAN.FGF6_HUMAN.FGF7_HUMAN.FGF8_HUMAN.FGF9_HUMAN.FSHB_HUMAN.GALA_HUMAN.GAST_HUMAN.GDF10_HUMAN.GDF11_HUMAN.GDF2_HUMAN.GDF3_HUMAN.GDF5_HUMAN.GDF6_HUMAN.GDF7_HUMAN.GDF8_HUMAN.GDF9_HUMAN.GDNF_HUMAN.GIP_HUMAN.GLHA_HUMAN.GLUC_HUMAN.GON1_HUMAN.GRP_HUMAN.HBEGF_HUMAN.HGF_HUMAN.IFN10_HUMAN.IFN14_HUMAN.IFN16_HUMAN.IFN17_HUMAN.IFN21_HUMAN.IFNA1_HUMAN.IFNA2_HUMAN.IFNA4_HUMAN.IFNA5_HUMAN.IFNA6_HUMAN.IFNA7_HUMAN.IFNA8_HUMAN.IFNB_HUMAN.IFNG_HUMAN.IFNW1_HUMAN.IGF1_HUMAN.IGF2_HUMAN.IHH_HUMAN.IL10_HUMAN.IL11_HUMAN.IL12A_HUMAN.IL12B_HUMAN.IL13_HUMAN.IL15_HUMAN.IL16_HUMAN.IL17_HUMAN.IL18_HUMAN.IL1A_HUMAN.IL1B_HUMAN.IL3_HUMAN.IL4_HUMAN.IL5_HUMAN.IL6_HUMAN.IL7_HUMAN.IL8_HUMAN.IL9_HUMAN.INHA_HUMAN.INHBA_HUMAN.INHBB_HUMAN.INHBC_HUMAN.INHBE_HUMAN.INS_HUMAN.JAG1_HUMAN.JAG2_HUMAN.KNG1_HUMAN.LEP_HUMAN.LIF_HUMAN.LSHB_HUMAN.MOTI_HUMAN.NDP_HUMAN.NEU1_HUMAN.NEU2_HUMAN.NGF_HUMAN.NODAL_HUMAN.NPY_HUMAN.NRG1_HUMAN.NRG2_HUMAN.NRG3_HUMAN.NRG4_HUMAN.NTF3_HUMAN.NTF4_HUMAN.PAHO_HUMAN.PDGFA_HUMAN.PDGFB_HUMAN.PRL_HUMAN.PRRP_HUMAN.PYY_HUMAN.SCF_HUMAN.SECR_HUMAN.SHH_HUMAN.SLIB_HUMAN.SMS_HUMAN.SOMA_HUMAN.TGFA_HUMAN.TGFB1_HUMAN.TGFB2_HUMAN.TGFB3_HUMAN.TKN1_HUMAN.TKNK_HUMAN.TNF10_HUMAN.TNFA_HUMAN.TNFB_HUMAN.TNFL6_HUMAN.TPO_HUMAN.TRH_HUMAN.TSHB_HUMAN.TXLNA_HUMAN.VEGFA_HUMAN.VEGFB_HUMAN.VEGFC_HUMAN.VEGFD_HUMAN.VIP_HUMAN.WN10A_HUMAN.WN10B_HUMAN.WNT11_HUMAN.WNT16_HUMAN.WNT1_HUMAN.WNT2B_HUMAN.WNT2_HUMAN.WNT3A_HUMAN.WNT3_HUMAN.WNT4_HUMAN.WNT5A_HUMAN.WNT5B_HUMAN.WNT6_HUMAN.WNT7A_HUMAN.WNT7B_HUMAN.WNT8A_HUMAN.WNT8B_HUMAN.WNT9A_HUMAN.WNT9B_HUMAN, AA1R_HUMAN.AA2AR_HUMAN.AA2BR_HUMAN.AGTR1_HUMAN.AGTR2_HUMAN.CXCR1_HUMAN.CXCR2_HUMAN.DRD1_HUMAN.DRD2_HUMAN.DRD3_HUMAN.DRD4_HUMAN.DRD5_HUMAN.FZD10_HUMAN.FZD1_HUMAN.FZD2_HUMAN.FZD3_HUMAN.FZD4_HUMAN.FZD5_HUMAN.FZD6_HUMAN.FZD7_HUMAN.FZD8_HUMAN.FZD9_HUMAN.GRM1_HUMAN.GRM2_HUMAN.GRM3_HUMAN.GRM4_HUMAN.GRM5_HUMAN.GRM6_HUMAN.GRM7_HUMAN.GRM8_HUMAN.SMO_HUMAN.TMIG3_HUMAN, ITA10_HUMAN.ITA11_HUMAN.ITA1_HUMAN.ITA2B_HUMAN.ITA2_HUMAN.ITA3_HUMAN.ITA4_HUMAN.ITA5_HUMAN.ITA6_HUMAN.ITA7_HUMAN.ITA8_HUMAN.ITA9_HUMAN.ITAD_HUMAN.ITAE_HUMAN.ITAL_HUMAN.ITAM_HUMAN.ITAV_HUMAN.ITAX_HUMAN, ITB1_HUMAN.ITB2_HUMAN.ITB3_HUMAN.ITB4_HUMAN.ITB5_HUMAN.ITB6_HUMAN.ITB7_HUMAN.ITB8_HUMAN, RIPK1_HUMAN.RIPK2_HUMAN.RIPK3_HUMAN, GNAI3_HUMAN, TIF1B_HUMAN, ACON_HUMAN, SUZ12_HUMAN, RING2_HUMAN, EED_HUMAN, PBX1_HUMAN, MYH10_HUMAN, DHX58_HUMAN, PHF7_HUMAN, ADA17_HUMAN, BZW1_HUMAN, SYUG_HUMAN, BST2_HUMAN, LIRA4_HUMAN, EGR1_HUMAN, EXOC2_HUMAN, RALA_HUMAN, RRAGC_HUMAN, ACTN3_HUMAN, RM01_HUMAN, SMRD3_HUMAN, PYC_HUMAN, FOXM1_HUMAN, TPH1_HUMAN, ERMIN_HUMAN, TBB5_HUMAN, EFTU_HUMAN, TERA_HUMAN, G3BP1_HUMAN, MK10_HUMAN, CASP3_HUMAN, A16L1_HUMAN, STING_HUMAN, ASC_HUMAN, PADI2_HUMAN, FILA_HUMAN, SRSF1_HUMAN, RS20_HUMAN, S61A1_HUMAN, EIF3G_HUMAN, TSC2_HUMAN, PSMD4_HUMAN, BMI1_HUMAN, NSF1C_HUMAN, GRAB_HUMAN, RXRA_HUMAN, KAT5_HUMAN, B2LA1_HUMAN, RL6_HUMAN, MK08_HUMAN, MK13_HUMAN, AT2B4_HUMAN, AZI2_HUMAN, RGS14_HUMAN, ROA2_HUMAN, ERCC2_HUMAN, CCNB3_HUMAN, DBLOH_HUMAN, TNF14_HUMAN, TNR3_HUMAN, TBL1R_HUMAN, SHIP1_HUMAN, XIAP_HUMAN, TRIP6_HUMAN, MK07_HUMAN, IRF4_HUMAN, HINT1_HUMAN, CDC20_HUMAN, BMX_HUMAN, RL23_HUMAN, AL3A2_HUMAN, ACTN4_HUMAN, UBXN1_HUMAN, DYH1_HUMAN, PTN7_HUMAN, IL4_HUMAN, CEBPD_HUMAN, RBP2_HUMAN, HDX_HUMAN, TELO2_HUMAN, AES_HUMAN, TFPT_HUMAN, MO4L1_HUMAN, CEP70_HUMAN, DDX58_HUMAN, TCTP_HUMAN, CAN2_HUMAN, EZH2_HUMAN, CTNA1_HUMAN, DEMA_HUMAN, ETV3_HUMAN, KPCZ_HUMAN, IKBA_HUMAN, ARL4D_HUMAN, PLPL9_HUMAN, TLE3_HUMAN, TCAM1_HUMAN, CCD50_HUMAN, TRIM1_HUMAN, TOLIP_HUMAN, RASLC_HUMAN, M3K13_HUMAN, SYC2L_HUMAN, ACTS_HUMAN, PAPS2_HUMAN, INSR_HUMAN, FMNL1_HUMAN, PELI3_HUMAN, HS3S1_HUMAN, KEAP1_HUMAN, STAT1_HUMAN, S39AE_HUMAN, GORAB_HUMAN, EF2K_HUMAN, STAB2_HUMAN, 3HIDH_HUMAN, DIRA1_HUMAN, PELI1_HUMAN, RUSC1_HUMAN, IRF3_HUMAN, 1C01_HUMAN.1C02_HUMAN.1C03_HUMAN.1C04_HUMAN.1C05_HUMAN.1C06_HUMAN.1C07_HUMAN.1C08_HUMAN.1C12_HUMAN.1C14_HUMAN.1C15_HUMAN.1C16_HUMAN.1C17_HUMAN.1C18_HUMAN, SMCA5_HUMAN, CATA_HUMAN, ANKS6_HUMAN, PDE4D_HUMAN, INAR1_HUMAN, SMC3_HUMAN, ADAP1_HUMAN, IF4E2_HUMAN, STPAP_HUMAN, CIKS_HUMAN, I2BP1_HUMAN, I17RA_HUMAN, UBB_HUMAN, LEG3_HUMAN, E2F1_HUMAN, HSF4_HUMAN, PKHG2_HUMAN, QPCTL_HUMAN, TAXB1_HUMAN, RACK1_HUMAN, ERCC3_HUMAN, CC106_HUMAN, SOCS3_HUMAN, HERP1_HUMAN, DD19B_HUMAN, PDIA6_HUMAN, HOME2_HUMAN, IRAK3_HUMAN, IRF1_HUMAN, SPHK1_HUMAN, PUF60_HUMAN, ING3_HUMAN, SIGIR_HUMAN, GATA3_HUMAN, WDR5_HUMAN, NSF_HUMAN, BBX_HUMAN, FUT7_HUMAN, K1H1_HUMAN, AQP1_HUMAN, BECN1_HUMAN, CAR16_HUMAN, ADAP2_HUMAN, BL1S1_HUMAN, ZC3H3_HUMAN, ACTN2_HUMAN, FHL1_HUMAN, PK3CA_HUMAN, AJUBA_HUMAN, RB40B_HUMAN, SNUT1_HUMAN, HNF1A_HUMAN, TRI63_HUMAN, PIN1_HUMAN, CPLX3_HUMAN, HSP74_HUMAN, C2TA_HUMAN, PP14A_HUMAN, PSA1_HUMAN, BRD3_HUMAN, IRS1_HUMAN, ARL4C_HUMAN, FA53A_HUMAN, KSR2_HUMAN, ACSL4_HUMAN, C1QBP_HUMAN, PAWR_HUMAN, SERA_HUMAN, CACO2_HUMAN, SGK1_HUMAN, KCC2B_HUMAN, RAP1B_HUMAN, GORS2_HUMAN, KLC4_HUMAN, TEKT4_HUMAN, RBM8A_HUMAN, PSN1_HUMAN, ATG4A_HUMAN, LRC59_HUMAN, SNX6_HUMAN, SPOP_HUMAN, MDHM_HUMAN, ASXL2_HUMAN, TTC3_HUMAN, NDUA4_HUMAN, OTX2_HUMAN, LIMA1_HUMAN, RD23A_HUMAN, CASPA_HUMAN, GLYM_HUMAN, CUED2_HUMAN, TBP_HUMAN, MK11_HUMAN, EPN2_HUMAN, PP1G_HUMAN, JIP1_HUMAN, CCD15_HUMAN, MAVS_HUMAN, TBA3E_HUMAN, KCNH2_HUMAN, G3P_HUMAN, NOD1_HUMAN, CASL_HUMAN, PRPS1_HUMAN, PSD11_HUMAN, TNIP2_HUMAN, PCAT1_HUMAN, TRBP2_HUMAN, MAP9_HUMAN, SEPT9_HUMAN, LAP2A_HUMAN.LAP2B_HUMAN, NOLC1_HUMAN, GRAM_HUMAN, CXB1_HUMAN, PEA15_HUMAN, RM35_HUMAN, TRI25_HUMAN, ADH4_HUMAN, HNRPF_HUMAN, PLCC_HUMAN, RLA1_HUMAN, TCAM2_HUMAN, ECHD2_HUMAN, PLK1_HUMAN, RSLBB_HUMAN, PAK1_HUMAN, ACTY_HUMAN, HGS_HUMAN, AIMP1_HUMAN, AGO1_HUMAN, MEX3C_HUMAN, USE1_HUMAN, SMC1A_HUMAN, PADI1_HUMAN, PHF11_HUMAN, CH60_HUMAN, CRIP2_HUMAN, ATF3_HUMAN, APT_HUMAN, TNIK_HUMAN, DAPK1_HUMAN, ADRM1_HUMAN, GASP1_HUMAN, 4EBP1_HUMAN, COPRS_HUMAN, KIF3B_HUMAN, NEK2_HUMAN, CTND1_HUMAN, TBCD4_HUMAN, PAIRB_HUMAN, TNR18_HUMAN, ABCF1_HUMAN, CSN5_HUMAN, I17RD_HUMAN, KS6A4_HUMAN, CEP57_HUMAN, OAT_HUMAN, ZFYV1_HUMAN, SPTC1_HUMAN, HEP2_HUMAN, NBR1_HUMAN, TYDP2_HUMAN, RS8_HUMAN, PGAM1_HUMAN, RS19_HUMAN, IF1AX_HUMAN, UBP4_HUMAN, KIF3A_HUMAN, KS6A3_HUMAN, PON2_HUMAN, TETN_HUMAN, EIF1_HUMAN, T53I2_HUMAN, CC85B_HUMAN, RT18A_HUMAN, STRAB_HUMAN, KIF2C_HUMAN, ITAM_HUMAN, ZMYM3_HUMAN, PTPA_HUMAN, ARFP2_HUMAN, RM10_HUMAN, ELK4_HUMAN, R51A1_HUMAN, STAU1_HUMAN, DDX17_HUMAN, PTBP1_HUMAN, MLP3A_HUMAN, NUSAP_HUMAN, DDX3X_HUMAN, REL_HUMAN, UBAP1_HUMAN, TNR27_HUMAN, NFAT5_HUMAN, S10A4_HUMAN, FND3A_HUMAN, ADDB_HUMAN, KPRB_HUMAN, GOSR2_HUMAN, UCHL1_HUMAN, NBPF3_HUMAN, TLR2_HUMAN, NONO_HUMAN, DAD1_HUMAN, EI2BE_HUMAN, SAHH_HUMAN, GIMA4_HUMAN, CADH2_HUMAN, PPBT_HUMAN, KPCA_HUMAN, SREK1_HUMAN, BIP_HUMAN, PAHX_HUMAN, APBA3_HUMAN, TSC1_HUMAN, KPCD1_HUMAN, PCBP2_HUMAN, EIF3E_HUMAN, NSD2_HUMAN, NF2L2_HUMAN, AGTR1_HUMAN, NFL_HUMAN, AT2C1_HUMAN, K1C15_HUMAN, HMGB1_HUMAN, ODP2_HUMAN, MTAP2_HUMAN, CHK2_HUMAN, MATR3_HUMAN, AT2A2_HUMAN, WDFY3_HUMAN, GBRL1_HUMAN, KCC2D_HUMAN, SMUF1_HUMAN, MPP3_HUMAN, MP2K6_HUMAN, CLIP1_HUMAN, CASP1_HUMAN, NOTC1_HUMAN, IF5_HUMAN, NHRF1_HUMAN, LMO7_HUMAN, UBE2S_HUMAN, MTUS2_HUMAN, FEN1_HUMAN, AP2B1_HUMAN, SMC4_HUMAN, CEBPB_HUMAN, PRAF1_HUMAN, RHEB_HUMAN, LY96_HUMAN, S10A9_HUMAN, TIPIN_HUMAN, KCNJ3_HUMAN, RAGE_HUMAN, HNRPC_HUMAN, KCC2G_HUMAN, ANXA9_HUMAN, TCP10_HUMAN, PIMRE_HUMAN, BC11B_HUMAN, MSH2_HUMAN, CACB1_HUMAN, RL31_HUMAN, GGA1_HUMAN, SFPQ_HUMAN, RP9_HUMAN, NDC80_HUMAN, ZN622_HUMAN, SPTN1_HUMAN, SCYL1_HUMAN, MSRE_HUMAN, KS6A5_HUMAN, TRAF4_HUMAN, HDAC3_HUMAN, RCAN1_HUMAN, SPY2_HUMAN, GRB10_HUMAN, ATP5L_HUMAN, PREX1_HUMAN, MLP3C_HUMAN, COMT_HUMAN, ACTG_HUMAN, EF1A1_HUMAN, BYST_HUMAN, RS10_HUMAN, TMED7_HUMAN, PTN2_HUMAN, RRAGB_HUMAN, SDHA_HUMAN, ECHD1_HUMAN, LEF1_HUMAN, DUS16_HUMAN, RASK_HUMAN, MXI1_HUMAN, CASP6_HUMAN, RMXL1_HUMAN, GFAP_HUMAN, RM28_HUMAN, MKNK2_HUMAN, BUD31_HUMAN, TFP11_HUMAN, ICLN_HUMAN, SHLB1_HUMAN, ANXA4_HUMAN, PADI4_HUMAN, TTLL7_HUMAN, KLC2_HUMAN, HNRPU_HUMAN, IRF7_HUMAN, RHG21_HUMAN, EDAD_HUMAN, UBQL1_HUMAN, SENP2_HUMAN, EF1A2_HUMAN, NPM_HUMAN, HMGB2_HUMAN, IF4B_HUMAN, BAG1_HUMAN, M3K10_HUMAN, IGBP1_HUMAN, PRS23_HUMAN, H2B1M_HUMAN, CNNM3_HUMAN, RM49_HUMAN, TISB_HUMAN, LNX1_HUMAN, ATF1_HUMAN, FHL2_HUMAN, RIPK4_HUMAN, XAF1_HUMAN, NECP1_HUMAN, PCBP1_HUMAN, NCOA6_HUMAN, HNRH1_HUMAN, GABPA_HUMAN, ERCC5_HUMAN, RAN_HUMAN, TCPE_HUMAN, SRBP2_HUMAN, SLAI2_HUMAN, GCKR_HUMAN, ATF6A_HUMAN, TAU_HUMAN, MX1_HUMAN, UBP7_HUMAN, ZMY11_HUMAN, SIAH2_HUMAN, UB2D2_HUMAN, ITPR3_HUMAN, RTF1_HUMAN, KCNJ6_HUMAN, AKT2_HUMAN, FATE1_HUMAN, MND1_HUMAN, DAB2_HUMAN, UCHL5_HUMAN, LMTD1_HUMAN, IFIH1_HUMAN, SH3K1_HUMAN, E41L2_HUMAN, HAUS6_HUMAN, NLRX1_HUMAN, SPNS1_HUMAN, CDIPT_HUMAN, FAKD5_HUMAN, TALAN_HUMAN.ZN365_HUMAN, DLRB2_HUMAN, APEX1_HUMAN, PELI2_HUMAN, DHB4_HUMAN, TMOD3_HUMAN, EPN1_HUMAN, UB2E2_HUMAN, KPRA_HUMAN, SC22B_HUMAN, TOX2_HUMAN, AMOT_HUMAN, PTN12_HUMAN, FOXO4_HUMAN, BOD1_HUMAN, WASP_HUMAN, KC1D_HUMAN, DIC_HUMAN, BTF3_HUMAN, SMUG1_HUMAN, ADAS_HUMAN, ATG4B_HUMAN, LACRT_HUMAN, M3K11_HUMAN, MEIS2_HUMAN, KCNA4_HUMAN, ERBIN_HUMAN, RS16_HUMAN, NMRL1_HUMAN, PLS1_HUMAN, ST38L_HUMAN, IF2B_HUMAN, RAD18_HUMAN, DAB2P_HUMAN, STXB1_HUMAN, T2EB_HUMAN, SIKE1_HUMAN, SEPT5_HUMAN, ZFY27_HUMAN, CUL3_HUMAN, IKIP_HUMAN, HCDH_HUMAN, KAP0_HUMAN, CASPE_HUMAN, RM43_HUMAN, PACRG_HUMAN, CPLX2_HUMAN, AT2B2_HUMAN, ROA3_HUMAN, SMAP1_HUMAN, TBCD7_HUMAN, GRAA_HUMAN, CSK21_HUMAN, MK09_HUMAN, RGS10_HUMAN, TRI27_HUMAN, ZNF22_HUMAN, TRI37_HUMAN, SETBP_HUMAN, AT2B1_HUMAN, ULK2_HUMAN, DYR1B_HUMAN, FKB14_HUMAN, K2C8_HUMAN, ROP1L_HUMAN, DMAP1_HUMAN, BATF2_HUMAN, SCEL_HUMAN, RS3_HUMAN, MYEF2_HUMAN, RLA0_HUMAN, BAIP2_HUMAN, ADA15_HUMAN, IRF9_HUMAN, HINT2_HUMAN, DYN2_HUMAN, YAP1_HUMAN, SMAD1_HUMAN, APOD_HUMAN, LEG1_HUMAN, MYL5_HUMAN, RM34_HUMAN, MAPK2_HUMAN, ZMYM5_HUMAN, RBL1_HUMAN, GLI2_HUMAN, IPO8_HUMAN, CUL1_HUMAN, MP2K4_HUMAN, MAFB_HUMAN, RAD21_HUMAN, SCG1_HUMAN, SHOC2_HUMAN, DCTN6_HUMAN, DCX_HUMAN, KSYK_HUMAN, KLF4_HUMAN, ATX1_HUMAN, VATG1_HUMAN, MYB_HUMAN, TFR1_HUMAN, TCAL2_HUMAN, ARFG1_HUMAN, SF3B1_HUMAN, PARP1_HUMAN, DHB12_HUMAN, NDUB6_HUMAN, FA32A_HUMAN, NMI_HUMAN, LTOR3_HUMAN, CX6A2_HUMAN, GBA2_HUMAN, IQGA1_HUMAN, RS27A_HUMAN, MYO1E_HUMAN, MEX3B_HUMAN, LYRM7_HUMAN, PSRC1_HUMAN, RHG24_HUMAN, AKAP5_HUMAN, TAF9B_HUMAN, RGS5_HUMAN, CAC1A_HUMAN, RL4_HUMAN, NHRF2_HUMAN, ATG7_HUMAN, H2B1A_HUMAN, RSLAB_HUMAN, TLR1_HUMAN, PRRC1_HUMAN, RM19_HUMAN, TCF19_HUMAN, RL13A_HUMAN, HNRPQ_HUMAN, RS12_HUMAN, ITB6_HUMAN, FUBP1_HUMAN, LZTS2_HUMAN, GAK_HUMAN, DYL1_HUMAN, KCC2A_HUMAN, AKND1_HUMAN, GRP3_HUMAN, RT24_HUMAN, IFIT1_HUMAN, AURKA_HUMAN, RGS3_HUMAN, TACO1_HUMAN, M3K20_HUMAN, AF1L2_HUMAN, DNJB1_HUMAN, FHL3_HUMAN, SERP1_HUMAN, HERC3_HUMAN, RBL2_HUMAN, RL41_HUMAN, TPC2L_HUMAN, CSN7B_HUMAN, NOB1_HUMAN, PDE4A_HUMAN, NUP93_HUMAN, MAGH1_HUMAN, EI2BA_HUMAN, RM11_HUMAN, RS9_HUMAN, CADH5_HUMAN, IGF1R_HUMAN, LMCD1_HUMAN, PCKGC_HUMAN, SPY4_HUMAN, ZW10_HUMAN, TRI23_HUMAN, ULK1_HUMAN, CDKL3_HUMAN, CARD6_HUMAN, IL15_HUMAN, AMFR_HUMAN, 1433G_HUMAN, RAB18_HUMAN, RASA1_HUMAN, NU155_HUMAN, TWF1_HUMAN, TBCC_HUMAN, COG7_HUMAN, COG5_HUMAN, P5CR2_HUMAN, RBM10_HUMAN, KIFC3_HUMAN, IDH3G_HUMAN, CC136_HUMAN, MYT1_HUMAN, PTN1_HUMAN, NMT2_HUMAN, SYJ2B_HUMAN, DUS26_HUMAN, LPPRC_HUMAN, KC1E_HUMAN, SH3G2_HUMAN, RS11_HUMAN, DEDD_HUMAN, N4BP1_HUMAN, TLR3_HUMAN, TIRAP_HUMAN, BL1S2_HUMAN, IRF8_HUMAN, KCNJ5_HUMAN, AP2M1_HUMAN, CBL_HUMAN, LYL1_HUMAN, TBA1A_HUMAN, OPTN_HUMAN, MYH9_HUMAN, RNF41_HUMAN, SPYA_HUMAN, ADH1B_HUMAN, BL1S5_HUMAN, NPL4_HUMAN, MK12_HUMAN, NDUS2_HUMAN, DNJC8_HUMAN, TCP1L_HUMAN, ASB3_HUMAN, TAP26_HUMAN, NCBP1_HUMAN, RENT1_HUMAN, NAL12_HUMAN, CARD9_HUMAN, OPRD_HUMAN, APBB1_HUMAN, KLF11_HUMAN, FBW1A_HUMAN, GPS2_HUMAN, LIMD1_HUMAN, RRAS2_HUMAN, UBP5_HUMAN, BIN1_HUMAN, TEANC_HUMAN, PTAFR_HUMAN, RS5_HUMAN, ALDOB_HUMAN, TMM33_HUMAN, RPAB4_HUMAN, ATG13_HUMAN, DUS4_HUMAN, NEUA_HUMAN, PPID_HUMAN, WRIP1_HUMAN, TIM50_HUMAN, MRM3_HUMAN, DPOD3_HUMAN, PRR5L_HUMAN, ANM1_HUMAN, TNR4_HUMAN, CR3L1_HUMAN, HS71B_HUMAN, PA24D_HUMAN, SRPRB_HUMAN, NDK3_HUMAN, SPRE2_HUMAN, LEG9_HUMAN, HNRPK_HUMAN, FOXO1_HUMAN, 1433T_HUMAN, PPARG_HUMAN, AF17_HUMAN, GCC1_HUMAN, VP33B_HUMAN, ENOB_HUMAN, DX39A_HUMAN, PO210_HUMAN, RIPP1_HUMAN, ARC1B_HUMAN, EIF3B_HUMAN, 5NTC_HUMAN, HMGA1_HUMAN, LATS1_HUMAN, EPAS1_HUMAN, ARMC1_HUMAN, TBB4B_HUMAN, ACD10_HUMAN, IF16_HUMAN, SNX1_HUMAN, NOXA1_HUMAN, K2C1_HUMAN, ODFP2_HUMAN, E41L5_HUMAN, PSA4_HUMAN, CBP_HUMAN, WDR34_HUMAN, ECI2_HUMAN, CD003_HUMAN, HS105_HUMAN, MLP3B_HUMAN, MAP2_HUMAN, PRIO_HUMAN, STIP1_HUMAN, RRAGD_HUMAN, OPRK_HUMAN, NEK1_HUMAN, SPAT7_HUMAN, CU002_HUMAN, FTM_HUMAN, ERBB2_HUMAN, TFDP3_HUMAN, NB5R3_HUMAN, DHX9_HUMAN, HIRP3_HUMAN, PLST_HUMAN, RL18A_HUMAN, ZSCA4_HUMAN, SMAD9_HUMAN, GMCL2_HUMAN, ANXA2_HUMAN, DDX5_HUMAN, NEAS1_HUMAN, RL40_HUMAN.UBC_HUMAN, ECHP_HUMAN.TBA8_HUMAN, PSME1_HUMAN, SSXT_HUMAN, CCNL2_HUMAN, SMN_HUMAN, CCNE2_HUMAN, KDM6B_HUMAN, IDE_HUMAN, EIF3A_HUMAN, PNKD_HUMAN, DGKI_HUMAN, RMD3_HUMAN, FIGLA_HUMAN, LHX3_HUMAN, ARBK1_HUMAN, NCPR_HUMAN, PEX5_HUMAN, GCM2_HUMAN, MAX_HUMAN, VIME_HUMAN, FBX4_HUMAN, TOP2B_HUMAN, SRPK1_HUMAN, LXN_HUMAN, A0A0A0MQR8_HUMAN.A0A0A0MST9_HUMAN.A0A0A0MT23_HUMAN.MARK3_HUMAN, SIK1_HUMAN, H0Y494_HUMAN.J3KPC8_HUMAN.SIK3_HUMAN, TM242_HUMAN, KRT35_HUMAN, PMYT1_HUMAN, ATLA3_HUMAN, APC_HUMAN, HXB7_HUMAN, RU2B_HUMAN, FSD1_HUMAN, MCAF1_HUMAN, RPAB1_HUMAN, SRRT_HUMAN, BPTF_HUMAN, NMNA1_HUMAN, TF7L2_HUMAN, CAMP1_HUMAN, OCRL_HUMAN, EPN4_HUMAN, MPRI_HUMAN, P3C2A_HUMAN, CD33_HUMAN, RPC3_HUMAN, DDT4L_HUMAN, LRP8_HUMAN, UBS3A_HUMAN, UBQL2_HUMAN, PTPRJ_HUMAN, GTR1_HUMAN, B3AT_HUMAN, ARI1A_HUMAN, UN45A_HUMAN, ZF64B_HUMAN, KCD16_HUMAN, PSA_HUMAN, RAB13_HUMAN, PSA3_HUMAN, DLX3_HUMAN, CTBP1_HUMAN, MARF1_HUMAN, BROX_HUMAN, MYC_HUMAN, SNW1_HUMAN, DNM1L_HUMAN, TBA1A_HUMAN.TBA1B_HUMAN, LEPR_HUMAN, KRA92_HUMAN, VPS35_HUMAN, RFOX2_HUMAN, KAT6B_HUMAN, SMUF2_HUMAN, ARI1B_HUMAN, SPF45_HUMAN, CP4F2_HUMAN, PKHO1_HUMAN, SAFB2_HUMAN, KSR1_HUMAN, VRK2_HUMAN, K1C27_HUMAN, RS27A_HUMAN.UBC_HUMAN, PRGR_HUMAN, NREP_HUMAN, UBE3A_HUMAN, MOES_HUMAN, GLIS2_HUMAN, U2AF5_HUMAN, ZNF76_HUMAN, NUCL_HUMAN, WBP11_HUMAN, RBM28_HUMAN, B2CL2_HUMAN, MAP4_HUMAN, AMPL_HUMAN, GO45_HUMAN, SNAI1_HUMAN, CPSF6_HUMAN, ARL1_HUMAN, AKP13_HUMAN, PSA7_HUMAN, PSDE_HUMAN, EAA3_HUMAN, DPYL1_HUMAN, PIAS2_HUMAN, PLP2_HUMAN, DDIT4_HUMAN, H2A1_HUMAN, CDKN3_HUMAN, T176A_HUMAN, BGAL_HUMAN, KITH_HUMAN, Q6FG41_HUMAN, S13A4_HUMAN, BAZ2B_HUMAN, PDIA4_HUMAN, IKZF1_HUMAN, CRBN_HUMAN, ERP44_HUMAN, MARE3_HUMAN, AIF1_HUMAN, AGRIN_HUMAN, GSTA1_HUMAN, ZN746_HUMAN, PDZ1I_HUMAN, SPIB_HUMAN, T2R19_HUMAN, MIP_HUMAN, ICA69_HUMAN, KRA62_HUMAN, PDK1_HUMAN, CHERP_HUMAN, AFF4_HUMAN, ATD3B_HUMAN, CDK15_HUMAN, PLAK_HUMAN, MUC7_HUMAN, NGAP_HUMAN, MACF1_HUMAN, UBB_HUMAN.UBC_HUMAN, DAZP2_HUMAN, FKBP7_HUMAN, ATF4_HUMAN, JMJD6_HUMAN, ASPP2_HUMAN, NUP54_HUMAN, MAL2_HUMAN, DAPP1_HUMAN, FOXR1_HUMAN, TM218_HUMAN, FLRT3_HUMAN, G137B_HUMAN, NLRP1_HUMAN, ZRAN1_HUMAN, KI2L3_HUMAN, SPG21_HUMAN, DALD3_HUMAN, APBP2_HUMAN, XRCC4_HUMAN, NHEJ1_HUMAN, STAR3_HUMAN, ARI5A_HUMAN, KIF6_HUMAN, AMRA1_HUMAN, NOG1_HUMAN, S4A4_HUMAN, CAH4_HUMAN, APEX2_HUMAN, MIRO1_HUMAN, NOSTN_HUMAN, KC1A_HUMAN, MTA2_HUMAN, CAN3_HUMAN, UB2R1_HUMAN, SFSWA_HUMAN, MAST2_HUMAN, RAB8A_HUMAN, Q8IXN4_HUMAN, PRDX2_HUMAN, PTPM1_HUMAN, TM14C_HUMAN, ACTC_HUMAN, RBTN2_HUMAN, TNPO2_HUMAN, FMR1_HUMAN, FXR2_HUMAN, PCGF5_HUMAN, SFT2A_HUMAN, PRP19_HUMAN, ARID2_HUMAN, CSN3_HUMAN, CYH2_HUMAN, SCML2_HUMAN, SMG9_HUMAN, DYSF_HUMAN, CSK22_HUMAN, KIF5C_HUMAN, IF4A2_HUMAN, LYAR_HUMAN, WRN_HUMAN, EFHD1_HUMAN, APOH_HUMAN, PLF4_HUMAN, CXA4_HUMAN, Q96FB2_HUMAN, PSN2_HUMAN, DISC1_HUMAN, B2L10_HUMAN, CDC42_HUMAN, ARHG7_HUMAN, ATRAP_HUMAN, ZHX1_HUMAN, AIRE_HUMAN, RIPK3_HUMAN, PTN9_HUMAN, RB33B_HUMAN, LTOR5_HUMAN, AQP6_HUMAN, MDM2_HUMAN, DNMT1_HUMAN, RTN3_HUMAN, BMF_HUMAN, S35B4_HUMAN, FA50B_HUMAN, TMM43_HUMAN, NEDD8_HUMAN, MPIP2_HUMAN, ARHG2_HUMAN, HCD2_HUMAN, KLOTB_HUMAN, ATG9A_HUMAN, THOC4_HUMAN, 2AAA_HUMAN, PPAC_HUMAN, ANM2_HUMAN, FACR1_HUMAN, RM40_HUMAN, SIR6_HUMAN, PR20D_HUMAN.PR20E_HUMAN, ML12B_HUMAN, KLH10_HUMAN, NR1D1_HUMAN, GARS_HUMAN, ARRD3_HUMAN, OBSCN_HUMAN, PABP4_HUMAN, PGFRB_HUMAN, H12_HUMAN, APR_HUMAN, RAB3I_HUMAN, PIGS_HUMAN, CDC6_HUMAN, GSTM3_HUMAN, BAHD1_HUMAN, VHL_HUMAN, SYTC_HUMAN, RS15_HUMAN, PAK2_HUMAN, COG6_HUMAN, MICA_HUMAN, S40A1_HUMAN, K1C40_HUMAN, SYRC_HUMAN, TRAM1_HUMAN, DPF3_HUMAN, OTUB1_HUMAN, TNF12_HUMAN, GYS1_HUMAN, H15_HUMAN, RPGF4_HUMAN, HNRPD_HUMAN, YETS4_HUMAN, TCEA2_HUMAN, ATG5_HUMAN, GMCL1_HUMAN, RO52_HUMAN, VINC_HUMAN, BBC3_HUMAN, HSF2B_HUMAN, CTCFL_HUMAN, TNR6A_HUMAN, DICER_HUMAN, CNOT7_HUMAN, PIGG_HUMAN, LUZP4_HUMAN, AHNK2_HUMAN, ACINU_HUMAN, DP13B_HUMAN, DVL3_HUMAN, UBP8_HUMAN, TM14B_HUMAN, PRC2A_HUMAN, CENPH_HUMAN, ETFB_HUMAN, PLPP4_HUMAN, VAMP4_HUMAN, ZSC30_HUMAN, TELT_HUMAN, NDRG2_HUMAN, TIDC1_HUMAN, NEDD4_HUMAN, SIVA_HUMAN, CD177_HUMAN, PNPT1_HUMAN, BRID5_HUMAN, MYPC2_HUMAN, CH10_HUMAN, K1C18_HUMAN, HYOU1_HUMAN, SELM_HUMAN, APBB2_HUMAN, RRAGA_HUMAN, VATB2_HUMAN, LTOR1_HUMAN, S38A9_HUMAN, NKX31_HUMAN, DEST_HUMAN, DOK3_HUMAN, U2AF1_HUMAN, SH3G3_HUMAN, TCPG_HUMAN, CAVN1_HUMAN, STB5L_HUMAN, NR1H4_HUMAN, NECD_HUMAN, MACD1_HUMAN, LIMK1_HUMAN, RNF8_HUMAN, RBM39_HUMAN, PEBP4_HUMAN, CIC_HUMAN, CE170_HUMAN, DCAF7_HUMAN, INP5E_HUMAN, PFKAM_HUMAN, RIC8A_HUMAN, EPS15_HUMAN, RASF5_HUMAN, HACD2_HUMAN, FHOD3_HUMAN, HG2A_HUMAN, PEPA4_HUMAN.PEPA5_HUMAN, P73_HUMAN, RD23B_HUMAN, SYT17_HUMAN, SPTA1_HUMAN, MAN1_HUMAN, S35A4_HUMAN, TM52B_HUMAN, KRA44_HUMAN, OTUD5_HUMAN, A0A024R0E9_HUMAN.A0A024R0H3_HUMAN.MAGI3_HUMAN, GLRX1_HUMAN, NAA20_HUMAN, GLRX5_HUMAN, HSC20_HUMAN, AAKB2_HUMAN, MARK2_HUMAN, BORG2_HUMAN, TCPZ_HUMAN, RM45_HUMAN, NDUV3_HUMAN, EFTS_HUMAN, GEMI4_HUMAN, TECT2_HUMAN, EGLN3_HUMAN, RL26_HUMAN, RL7_HUMAN, KR108_HUMAN, TRAK1_HUMAN, ECHM_HUMAN, RAD51_HUMAN, RFC5_HUMAN, GID8_HUMAN, PP2AB_HUMAN, COF2_HUMAN, H2B1H_HUMAN, UB2L3_HUMAN, ERN1_HUMAN, ERF3B_HUMAN, BCAR1_HUMAN, TRI55_HUMAN, A4PIW0_HUMAN, TLE1_HUMAN, MTMR3_HUMAN, RND3_HUMAN, SELK_HUMAN, M4A13_HUMAN, THIL_HUMAN, KIF1C_HUMAN, REQU_HUMAN, FXL15_HUMAN, DDX6_HUMAN, ATX2L_HUMAN, ATX2_HUMAN, SAR1A_HUMAN, ABCA1_HUMAN, UBP30_HUMAN, RPAP3_HUMAN, ECD_HUMAN, PSB2_HUMAN, TBB2B_HUMAN, PSB3_HUMAN, PROF1_HUMAN, CELF4_HUMAN, NAA10_HUMAN, AAKB1_HUMAN, RAC1_HUMAN, SCHI1_HUMAN, MKLN1_HUMAN, Q59F66_HUMAN, NOL8_HUMAN, DAAF4_HUMAN, LCAP_HUMAN, VMA21_HUMAN, NH2L1_HUMAN, LFG4_HUMAN, LRRK1_HUMAN, LERL1_HUMAN, SMRP1_HUMAN, P55G_HUMAN, SMCA2_HUMAN, DACT1_HUMAN, MSRB2_HUMAN, ACPH_HUMAN, PAQRB_HUMAN, LDHA_HUMAN, RHXF2_HUMAN, CC115_HUMAN, CAV2_HUMAN, NR1H2_HUMAN, WASF1_HUMAN, GOGA2_HUMAN, RABX5_HUMAN, PSA2_HUMAN, AP2C_HUMAN, COX17_HUMAN, MD2L2_HUMAN, TOP3A_HUMAN, FA35A_HUMAN, BLM_HUMAN, SC24C_HUMAN, PBIP1_HUMAN, FGF8_HUMAN, CDN2A_HUMAN.G3XAG3_HUMAN, 41_HUMAN, ABCD3_HUMAN, BRF2_HUMAN, YIPF6_HUMAN, ENOA_HUMAN, GPR25_HUMAN, SUN2_HUMAN, CBX5_HUMAN, LBR_HUMAN, INCE_HUMAN, MNS1_HUMAN, TS101_HUMAN, BAG5_HUMAN, GCR_HUMAN, STX3_HUMAN, POLH_HUMAN, RS23_HUMAN, INS_HUMAN, TPPC4_HUMAN, MAGD1_HUMAN, FURIN_HUMAN, A1CF_HUMAN, RTN4_HUMAN, FND3B_HUMAN, COF1_HUMAN, DAXX_HUMAN, IL1AP_HUMAN, IL1B_HUMAN, FAS_HUMAN, KANK2_HUMAN, MSH6_HUMAN, CTSR1_HUMAN, DNJC2_HUMAN, FBX7_HUMAN, ARF6_HUMAN, FA84B_HUMAN, CLUS_HUMAN, SGO2_HUMAN, ETV7_HUMAN, MGN_HUMAN, GCN1_HUMAN, SYNE2_HUMAN, INCA1_HUMAN, TCL1A_HUMAN, PSME3_HUMAN, ASPP1_HUMAN, VP37B_HUMAN, WWP1_HUMAN, TLK1_HUMAN, NMUR2_HUMAN, SND1_HUMAN, NDUF4_HUMAN, NDUF3_HUMAN, VAV2_HUMAN, TEBP_HUMAN, SRPK2_HUMAN, ODO2_HUMAN, TMM98_HUMAN, EMSY_HUMAN, KHDR3_HUMAN, PTPRB_HUMAN, HMDH_HUMAN, HSPB2_HUMAN, SYT6_HUMAN, TAF9_HUMAN, RIR1_HUMAN, POLK_HUMAN, SBP1_HUMAN, TNNI1_HUMAN, COX5B_HUMAN, LOX15_HUMAN, SERC3_HUMAN, ATPF2_HUMAN, H32_HUMAN, NUFP2_HUMAN, SC61B_HUMAN, UB2D3_HUMAN, NEK9_HUMAN, PLS4_HUMAN, UBC9_HUMAN, ACOX2_HUMAN, CIDEB_HUMAN, POMP_HUMAN, PSB1_HUMAN, HIF1N_HUMAN, OTU7B_HUMAN, SYCE1_HUMAN, H31T_HUMAN, DYH10_HUMAN, NR4A1_HUMAN, KR107_HUMAN, NB5R2_HUMAN, ZN330_HUMAN, GNAS1_HUMAN, ARP3_HUMAN, PP2AA_HUMAN, APBA1_HUMAN, NADL2_HUMAN, VAMP1_HUMAN, EFC4B_HUMAN, CLIC1_HUMAN, TMED9_HUMAN, Q96AL5_HUMAN, EFNA4_HUMAN, EPHA7_HUMAN, T22D4_HUMAN, ZN703_HUMAN, PGAM5_HUMAN, RALY_HUMAN, DMD_HUMAN, RN146_HUMAN, KLC3_HUMAN, IMA7_HUMAN, RAB5B_HUMAN, CLD19_HUMAN, ARAF_HUMAN, LDHB_HUMAN, TM50B_HUMAN, CNPY2_HUMAN, PIPNB_HUMAN, B2L13_HUMAN, RXRG_HUMAN, HIF1A_HUMAN, K22O_HUMAN, DDIT3_HUMAN, SYAC_HUMAN, MLH1_HUMAN, IPSP_HUMAN, FBX25_HUMAN, GLYC_HUMAN, SMG1_HUMAN, TTI1_HUMAN, SNAPN_HUMAN, DPF1_HUMAN, DUS19_HUMAN, TIRR_HUMAN, FANCC_HUMAN, RNF5_HUMAN, KCD12_HUMAN, A0A087X1U6_HUMAN.EPIPL_HUMAN, TM115_HUMAN, NCK2_HUMAN, TM187_HUMAN, SENP3_HUMAN, RBP10_HUMAN, RSAD2_HUMAN, STAM2_HUMAN, MSRB3_HUMAN, TFG_HUMAN, FZD7_HUMAN, PNMA1_HUMAN, COIL_HUMAN, E41L3_HUMAN, SEPT2_HUMAN, RL10A_HUMAN, SERB_HUMAN, RRP1B_HUMAN, NTCP_HUMAN, MD1L1_HUMAN, S15A4_HUMAN, S15A3_HUMAN, FIS1_HUMAN, DNJB6_HUMAN, NPSR1_HUMAN, RRP5_HUMAN, TF3C2_HUMAN, MTNB_HUMAN, PR40A_HUMAN, RPB7_HUMAN, LCOR_HUMAN, RGS2_HUMAN, SMAD6_HUMAN, STR3N_HUMAN, ATG10_HUMAN, KHK_HUMAN, WWOX_HUMAN, MAST1_HUMAN, SRBS2_HUMAN, BIRC5_HUMAN, MCM6_HUMAN, RS3A_HUMAN, RM03_HUMAN, RT29_HUMAN, FST_HUMAN, YYAP1_HUMAN, NTF2_HUMAN, ADPPT_HUMAN, YIPF4_HUMAN, ID1_HUMAN, CQ062_HUMAN, IFG15_HUMAN, DDX56_HUMAN, CKS1_HUMAN, RBTN1_HUMAN, TAGL2_HUMAN, GRIK3_HUMAN, TCF23_HUMAN, GSTA2_HUMAN, URAD_HUMAN, T22D1_HUMAN, LRIF1_HUMAN, A0A075B738_HUMAN.PECA1_HUMAN, H33_HUMAN, SP100_HUMAN, UBA6_HUMAN, SURF4_HUMAN, ETV1_HUMAN, A0AVN2_HUMAN, B2Y833_HUMAN, ERG_HUMAN, AIMP2_HUMAN, AASD1_HUMAN, SYVN1_HUMAN, HLAH_HUMAN, R144B_HUMAN, MDM4_HUMAN, DCPS_HUMAN, SRBS1_HUMAN, KR122_HUMAN, FDFT_HUMAN, CLK3_HUMAN, KC1G2_HUMAN, ERG28_HUMAN, PIAS4_HUMAN, UBS3B_HUMAN, NACA_HUMAN, KASH5_HUMAN, CREB3_HUMAN, KLH20_HUMAN, HUWE1_HUMAN, SNRPA_HUMAN, AN32B_HUMAN, FOXH1_HUMAN, PRAF2_HUMAN, DTX1_HUMAN, TPC1_HUMAN, NICA_HUMAN, ZFYV9_HUMAN, SPDYA_HUMAN, RGS20_HUMAN, RL29_HUMAN, JUPI2_HUMAN, RAP1A_HUMAN, CD5R1_HUMAN, STRN_HUMAN, SGO1_HUMAN, SRRM2_HUMAN, PB1_HUMAN, PARN_HUMAN, DNJB5_HUMAN, ISCU_HUMAN, UCRI_HUMAN, TFE3_HUMAN, PRPK_HUMAN, ORML2_HUMAN, TY3H_HUMAN, TIM16_HUMAN, STK3_HUMAN, SEPT7_HUMAN, LITAF_HUMAN, CCHCR_HUMAN, LURA1_HUMAN, RL3R1_HUMAN, CDN2B_HUMAN, ZBT25_HUMAN, A6NNN6_HUMAN.E7ETA6_HUMAN.PCM1_HUMAN.RET_HUMAN, ATG3_HUMAN, CISY_HUMAN, SHLB2_HUMAN, HD_HUMAN, PD1L1_HUMAN, MLC1_HUMAN, STIM1_HUMAN, TRPC1_HUMAN, CSTF2_HUMAN, SKT_HUMAN, HMCS1_HUMAN, C1TC_HUMAN, GRP4_HUMAN, CLD7_HUMAN, NIPA4_HUMAN, S100B_HUMAN, KIF15_HUMAN, PEX14_HUMAN, CENPL_HUMAN, FAM9B_HUMAN, RAB12_HUMAN, JHD2C_HUMAN, PTMA_HUMAN, APLP1_HUMAN, APLF_HUMAN, PSMD8_HUMAN, DESM_HUMAN, TM201_HUMAN, RNF43_HUMAN, RL11_HUMAN, CXA8_HUMAN, APOA1_HUMAN, EFNA2_HUMAN, BBS4_HUMAN, VENTX_HUMAN, HTRA2_HUMAN, NOA1_HUMAN, RRP44_HUMAN, YES_HUMAN, DRD2_HUMAN, TSSK6_HUMAN, PSMD2_HUMAN, SKI_HUMAN, SPAG5_HUMAN, HTF4_HUMAN, AATC_HUMAN, GLRX3_HUMAN, SIM2_HUMAN, AT132_HUMAN, MPIP1_HUMAN, BAP1_HUMAN, PMS2_HUMAN, RAB7L_HUMAN, OXYR_HUMAN, ITPK1_HUMAN, TNKS1_HUMAN, APOA4_HUMAN, RS28_HUMAN, GP1BA_HUMAN, PKCB1_HUMAN, KHDR2_HUMAN, MEOX2_HUMAN, SNAB_HUMAN, B4GT2_HUMAN, NRAP_HUMAN, KI67_HUMAN, CBR3_HUMAN, LDLR_HUMAN, OPRM_HUMAN, BBS1_HUMAN, PSPC1_HUMAN, EBP_HUMAN, UHRF2_HUMAN, RAB32_HUMAN, MRT4_HUMAN, STABP_HUMAN, SOAT_HUMAN, H2B1D_HUMAN, NDUB9_HUMAN, SEC13_HUMAN, DUSTY_HUMAN, MPP5_HUMAN, TBCD1_HUMAN, MORC3_HUMAN, ROR1_HUMAN, ARIP4_HUMAN, A0A087WYH8_HUMAN.TR64C_HUMAN, VPS52_HUMAN, ARPC2_HUMAN, APOA2_HUMAN, USF1_HUMAN, PPIB_HUMAN, MDFI_HUMAN, ASAP2_HUMAN, ATRX_HUMAN, CHD1L_HUMAN, CQ053_HUMAN, CXG2_HUMAN, RL23A_HUMAN, RS6_HUMAN, U2AFL_HUMAN, DLG1_HUMAN, S10AA_HUMAN, CHM2B_HUMAN, H31_HUMAN, FACD2_HUMAN, WAP53_HUMAN, HDAC9_HUMAN, SNIP1_HUMAN, TRXR1_HUMAN, FANCI_HUMAN, CHSS2_HUMAN, 5HT1A_HUMAN, RAC3_HUMAN, PCGF2_HUMAN, KIF23_HUMAN, SCN3B_HUMAN, FYCO1_HUMAN, TM86B_HUMAN, MPH6_HUMAN, ABCD4_HUMAN, KHDR1_HUMAN, HCFC1_HUMAN, RPR1A_HUMAN, NCOA2_HUMAN, CE104_HUMAN, TFAM_HUMAN, REN3B_HUMAN, SMG5_HUMAN, ERMP1_HUMAN, PNPH_HUMAN, HMBX1_HUMAN, NHP2_HUMAN, PDIA5_HUMAN, EXOSX_HUMAN, SUMO3_HUMAN, CDK9_HUMAN, LIMS2_HUMAN, A0A0A0MRM0_HUMAN.MYOME_HUMAN, IKBE_HUMAN, CBX8_HUMAN, V9HW56_HUMAN, MKRN3_HUMAN, KANK1_HUMAN, NKG7_HUMAN, GBG4_HUMAN, DGLA_HUMAN, HS71B_HUMAN.HSP77_HUMAN, HAUS1_HUMAN, BNI3L_HUMAN, PTPRR_HUMAN, LIMS1_HUMAN, DUX1_HUMAN, PROF2_HUMAN, MALL_HUMAN, HACE1_HUMAN, EDRF1_HUMAN, BRAP_HUMAN, HENMT_HUMAN, SE6L1_HUMAN, K0319_HUMAN, AL9A1_HUMAN, ZN363_HUMAN, TSN33_HUMAN, POLI_HUMAN, GRAN_HUMAN, S10A6_HUMAN, ZN792_HUMAN, M3K8_HUMAN, STF1_HUMAN, HDAC7_HUMAN, MARE2_HUMAN, EHBP1_HUMAN, ZBT24_HUMAN, RETR1_HUMAN, FOXN1_HUMAN, AQP3_HUMAN, PDS5A_HUMAN, S38A4_HUMAN, MYPT1_HUMAN, DLGP5_HUMAN, A0A0C4DFN1_HUMAN.MFN1_HUMAN, SARNP_HUMAN, RPAB3_HUMAN, UXT_HUMAN, HEXB_HUMAN, SPAG4_HUMAN, SEP12_HUMAN, MOFA1_HUMAN, DP13A_HUMAN, AP1M2_HUMAN, RASF1_HUMAN, EDA_HUMAN, KR412_HUMAN, DCTN2_HUMAN, PRDX1_HUMAN, MCRS1_HUMAN, K1C16_HUMAN, Q6PKD3_HUMAN, NDRG4_HUMAN, SODC_HUMAN, CCR5_HUMAN, UVRAG_HUMAN, CAPZB_HUMAN, NAF1_HUMAN, GAS8_HUMAN, ACOD_HUMAN, PKHA7_HUMAN, AGO2_HUMAN, STK38_HUMAN, ITF2_HUMAN, SPOPL_HUMAN, CDCA4_HUMAN, THIOM_HUMAN, HEXDC_HUMAN, AR6P1_HUMAN, T229B_HUMAN, MBD3_HUMAN, PDE9A_HUMAN, HHLA2_HUMAN, TE2IP_HUMAN, RS13_HUMAN, ZN398_HUMAN, KAD2_HUMAN, MPU1_HUMAN, SLTM_HUMAN, DVL1_HUMAN, EMRE_HUMAN, ETV5_HUMAN, SODM_HUMAN, RMD2_HUMAN, RDH10_HUMAN, TPP2_HUMAN, LMBL2_HUMAN, SC5A4_HUMAN, TF2B_HUMAN, REST_HUMAN, KLC1_HUMAN, UT2_HUMAN, LZTS1_HUMAN, FABP4_HUMAN, CD44_HUMAN, LIRB2_HUMAN, POC1A_HUMAN, SMO_HUMAN, IPO7_HUMAN, MID49_HUMAN, RL7A_HUMAN, XPO2_HUMAN, NFAC2_HUMAN, TNPO1_HUMAN, HBA_HUMAN, TSKS_HUMAN, UD17_HUMAN, SRP72_HUMAN, IF2G_HUMAN, ROA0_HUMAN, F107A_HUMAN, ZNF44_HUMAN, MBD4_HUMAN, FUS_HUMAN, KRA59_HUMAN, LAX1_HUMAN, DACH1_HUMAN, CING_HUMAN, KLF5_HUMAN, GNDS_HUMAN, UBXN7_HUMAN, SENP5_HUMAN, PR15A_HUMAN, STT3A_HUMAN, PF4V_HUMAN, BEX2_HUMAN, MD2L1_HUMAN, KLF13_HUMAN, EAF1_HUMAN, SC24A_HUMAN, GCDH_HUMAN, ERP29_HUMAN, NDUA3_HUMAN, MCM2_HUMAN, ATG12_HUMAN, YBOX1_HUMAN, YBOX3_HUMAN, PABP2_HUMAN, ATR_HUMAN, F133B_HUMAN, PXK_HUMAN, RT06_HUMAN, RHES_HUMAN, CAZA1_HUMAN, RUS1_HUMAN, TBCE_HUMAN, SEC63_HUMAN, IF4A3_HUMAN, TNKS2_HUMAN, PRP16_HUMAN, RPA34_HUMAN, F173A_HUMAN, TBB1_HUMAN, RM15_HUMAN, NEBU_HUMAN, MYF5_HUMAN, SDHB_HUMAN, H11_HUMAN, TM208_HUMAN, ZMYM2_HUMAN, CDK13_HUMAN, CHIP_HUMAN, NEBL_HUMAN, NUP50_HUMAN, IMDH2_HUMAN, INT13_HUMAN, PEPL_HUMAN, PELO_HUMAN, CSR2B_HUMAN, DRG1_HUMAN, PDIA3_HUMAN, RED_HUMAN, MARE1_HUMAN, DLRB1_HUMAN, SSMM1_HUMAN, CO8A_HUMAN, GLP1R_HUMAN, TGFB2_HUMAN, F161A_HUMAN, IF2B2_HUMAN, MYOD1_HUMAN, SRSF9_HUMAN, CHP3_HUMAN, SGTA_HUMAN, VAPB_HUMAN, CCD40_HUMAN, T2H2L_HUMAN, ASXL2_HUMAN.KAT6A_HUMAN, SESN2_HUMAN, RHOA_HUMAN, TAOK3_HUMAN, K2C75_HUMAN, RS14_HUMAN, CIP1_HUMAN, SNG1_HUMAN, CENPU_HUMAN, GSAP_HUMAN, STAM1_HUMAN, CSF3R_HUMAN, CHSP1_HUMAN, HIKES_HUMAN, VNN2_HUMAN, RN19B_HUMAN, SPF30_HUMAN, HAT1_HUMAN, KAT2B_HUMAN, KAT2A_HUMAN, ERP27_HUMAN, PINX1_HUMAN, ITCH_HUMAN, MYO6_HUMAN, OBSL1_HUMAN, KDM1A_HUMAN, RCOR2_HUMAN, BAG6_HUMAN, TBB4A_HUMAN, STK24_HUMAN, SCAP_HUMAN, PRP4_HUMAN, LPP_HUMAN, CPNS1_HUMAN, NECT2_HUMAN, NELFB_HUMAN, PFKAP_HUMAN, MYO1B_HUMAN, LHX6_HUMAN, Q6FGM0_HUMAN, SYQ_HUMAN, T53I1_HUMAN, ERF3A_HUMAN, APOC1_HUMAN, MEP50_HUMAN, ANM5_HUMAN, CDK4_HUMAN, SH3G1_HUMAN, PSIP1_HUMAN, SLU7_HUMAN, XBP1_HUMAN, RS15A_HUMAN, SHIP2_HUMAN, CNST_HUMAN, CLAP2_HUMAN, SNX15_HUMAN, SRSF2_HUMAN, SNX11_HUMAN, SL9A1_HUMAN, RECQ5_HUMAN, PLD3_HUMAN, SC11C_HUMAN, KR109_HUMAN, F264_HUMAN, LRFN4_HUMAN, PAQR3_HUMAN, PRP4B_HUMAN, VASP_HUMAN, UB2E1_HUMAN, KRA32_HUMAN, VKGC_HUMAN, MED18_HUMAN, Q6FHM2_HUMAN, GPR35_HUMAN, PGK1_HUMAN, FKBP4_HUMAN, KPYM_HUMAN, KDEL1_HUMAN, GPAA1_HUMAN, UBP25_HUMAN, BHE40_HUMAN, ZN121_HUMAN, MCM5_HUMAN, ILF3_HUMAN, UBA1_HUMAN, FM25C_HUMAN.FM25G_HUMAN, PININ_HUMAN, NINJ2_HUMAN, POTE1_HUMAN, UHMK1_HUMAN, CSDE1_HUMAN, 1A66_HUMAN, CYBP_HUMAN, CLIP2_HUMAN, BCLF1_HUMAN, HAP1_HUMAN, STRN3_HUMAN, FBF1_HUMAN, DNHD1_HUMAN, FBXL5_HUMAN, PROP1_HUMAN, ATF7_HUMAN, GIT2_HUMAN, TGFA1_HUMAN, RAB1B_HUMAN, DMPK_HUMAN, RHBT3_HUMAN, TOM1_HUMAN, CNBP1_HUMAN, MYOF_HUMAN, TM237_HUMAN, SYNE4_HUMAN, SDCB1_HUMAN, EMC6_HUMAN, AMGO1_HUMAN, EP400_HUMAN, S38A7_HUMAN, ZN675_HUMAN, PKHB2_HUMAN, PYR1_HUMAN, RNF4_HUMAN, CHM4C_HUMAN, CALM1_HUMAN.CALM2_HUMAN.CALM3_HUMAN, SEC20_HUMAN, TRIPC_HUMAN, LDOC1_HUMAN, HDAC2_HUMAN, NR2E1_HUMAN, GET4_HUMAN, SRP14_HUMAN, IN80E_HUMAN, S39A4_HUMAN, DDX24_HUMAN, PARD3_HUMAN.PKHD1_HUMAN, ZFP57_HUMAN, CCNH_HUMAN, CCND2_HUMAN, FAP24_HUMAN, KR261_HUMAN, SYMC_HUMAN, PFD5_HUMAN, GLT18_HUMAN, ZDH17_HUMAN, Z280C_HUMAN, RB11A_HUMAN, UBAC1_HUMAN, KC1G3_HUMAN, E2AK2_HUMAN, CCG1_HUMAN, DERL1_HUMAN, MBNL2_HUMAN, GSK3A_HUMAN, PDK4_HUMAN, SPERT_HUMAN, TPR_HUMAN, RUXG_HUMAN, SYFM_HUMAN, GRPL2_HUMAN, KLDC1_HUMAN, KAP1_HUMAN, MLRA_HUMAN, LAMP2_HUMAN, STRBP_HUMAN, MCR_HUMAN, WNK1_HUMAN, S100P_HUMAN, CACL1_HUMAN, GASR_HUMAN, MED10_HUMAN, GA45G_HUMAN, RBP56_HUMAN, TCPA_HUMAN, ALKB8_HUMAN, TCPB_HUMAN, TR112_HUMAN, CGNL1_HUMAN, A4PIV7_HUMAN, AHSA1_HUMAN, SCAM5_HUMAN, BUB3_HUMAN, UBP19_HUMAN, TXTP_HUMAN, LAP2B_HUMAN, SHSA4_HUMAN, CCHL_HUMAN, DDX20_HUMAN, BKRB1_HUMAN, CAMLG_HUMAN, PITX2_HUMAN, RFWD2_HUMAN, ZFY21_HUMAN, DUS21_HUMAN, TPM4_HUMAN, UB2G2_HUMAN, MYO10_HUMAN, TCHP_HUMAN, NDUF7_HUMAN, CHC10_HUMAN, TRI41_HUMAN, MFSD6_HUMAN, SNAT_HUMAN, MGAP_HUMAN, H4_HUMAN, H2B1J_HUMAN, ILK_HUMAN, NLTP_HUMAN, TCPD_HUMAN, DNJA1_HUMAN, DDB1_HUMAN, Q5T081_HUMAN, ABCG2_HUMAN, FUMH_HUMAN, CYB5B_HUMAN, MED29_HUMAN, CAP2_HUMAN, RFIP2_HUMAN, ZN219_HUMAN, TEX37_HUMAN, ZFP62_HUMAN, THAP1_HUMAN, IN80B_HUMAN, CAPR1_HUMAN, DUS7_HUMAN, ANM6_HUMAN, DCTN1_HUMAN, GBRAP_HUMAN, REPS2_HUMAN, PDC6I_HUMAN, NTAQ1_HUMAN, EFNB2_HUMAN, 3MG_HUMAN, RL34_HUMAN, DC1L2_HUMAN, TAL1_HUMAN, TRI33_HUMAN, UTP20_HUMAN, RPA1_HUMAN, ARGL1_HUMAN, STK16_HUMAN, CNBP_HUMAN, H2A3_HUMAN, GCH1_HUMAN, TNNT1_HUMAN, NRBP_HUMAN, ELOA2_HUMAN, NKG2F_HUMAN, BACD1_HUMAN, PTN6_HUMAN, SC22A_HUMAN, JAGN1_HUMAN, ZN165_HUMAN, STX5_HUMAN, A0A087X1W2_HUMAN.ANM1_HUMAN.H7C2I1_HUMAN, H2BFS_HUMAN, Z385A_HUMAN, CLC9A_HUMAN, ASNA_HUMAN, HS74L_HUMAN, CDX1_HUMAN, F168A_HUMAN, PAK4_HUMAN, FIBB_HUMAN, HACD3_HUMAN, PUR9_HUMAN, FBXW2_HUMAN, INP5K_HUMAN, SACS_HUMAN, LARP7_HUMAN, SPA24_HUMAN, SPT6H_HUMAN, GLO2_HUMAN, PP1B_HUMAN, UBP11_HUMAN, PP16B_HUMAN, RIC3_HUMAN, ERO1B_HUMAN, SNX10_HUMAN, RING1_HUMAN, SDCG3_HUMAN, SAT1_HUMAN, TPD53_HUMAN, NXF1_HUMAN, ZN611_HUMAN, EZRI_HUMAN, ADNP_HUMAN, GRAP2_HUMAN, Q549N0_HUMAN, IFM3_HUMAN, ELF3_HUMAN, TM1L1_HUMAN, MVP_HUMAN, ZN232_HUMAN, PPP5_HUMAN, MCM3_HUMAN, MAGAB_HUMAN, HNRPM_HUMAN, NUP43_HUMAN, UBIA1_HUMAN, PUR4_HUMAN, IDHP_HUMAN, TBB3_HUMAN, PTPRO_HUMAN, NCOA1_HUMAN, PRS6B_HUMAN, SC11A_HUMAN, LT4R2_HUMAN, CENPB_HUMAN, RINI_HUMAN, K1C20_HUMAN, IF122_HUMAN, CANB1_HUMAN, AQP10_HUMAN, SC23A_HUMAN, F214B_HUMAN, ELOA1_HUMAN, BRE1A_HUMAN, A0A024QZG0_HUMAN.BRE1B_HUMAN, UBE2A_HUMAN, A0A087WYI6_HUMAN.B6EC88_HUMAN.CD24_HUMAN.R4I4T5_HUMAN, TMUB1_HUMAN, MBTD1_HUMAN, PLXA3_HUMAN, SE1L1_HUMAN, RBM4_HUMAN, AGRE2_HUMAN, CAH12_HUMAN, AHNK_HUMAN, NU205_HUMAN, H14_HUMAN, LRC45_HUMAN, H2B2E_HUMAN, RCC1_HUMAN, GBP2_HUMAN, MO4L2_HUMAN, GOLM1_HUMAN, PLPR2_HUMAN, SP110_HUMAN, MIF_HUMAN, BANP_HUMAN, GPBL1_HUMAN, 1C04_HUMAN, TRFR_HUMAN, RGPA1_HUMAN, TTHY_HUMAN, PRDX4_HUMAN, TA2R_HUMAN, COE3_HUMAN, A0A0J9YVZ6_HUMAN.MY15B_HUMAN, RHOC_HUMAN, T2FB_HUMAN, DYR1A_HUMAN, ZBT16_HUMAN, UQCC2_HUMAN, EXOS4_HUMAN, MYDGF_HUMAN, BCCIP_HUMAN, PAK5_HUMAN, METK2_HUMAN, ARL8B_HUMAN, FOXK1_HUMAN, TADA3_HUMAN, CAVN2_HUMAN, CDCA5_HUMAN, SYNE1_HUMAN.SYNE2_HUMAN, PPR3D_HUMAN, NIPS1_HUMAN, ZC3HF_HUMAN, MYBPH_HUMAN, CHK1_HUMAN, MBP_HUMAN, ERGI3_HUMAN, RL5_HUMAN, PRAF3_HUMAN, SOS1_HUMAN, TM109_HUMAN, S35F6_HUMAN, GSC2_HUMAN, ARF_HUMAN, PDCD6_HUMAN, RAD52_HUMAN, TIE2_HUMAN, PHF3_HUMAN, DHYS_HUMAN, PP2BC_HUMAN, SYYC_HUMAN, F16A2_HUMAN, RS2_HUMAN, CENPA_HUMAN, FAN_HUMAN, PNKP_HUMAN, PRR13_HUMAN, SPB1_HUMAN, CYREN_HUMAN, DEN5A_HUMAN, STRN4_HUMAN, FAK1_HUMAN, CTGF_HUMAN, KCNJ8_HUMAN, MMAD_HUMAN, RL19_HUMAN, ITBP2_HUMAN, SC16A_HUMAN, CDYL2_HUMAN, EIF3K_HUMAN, XRN2_HUMAN, NAA25_HUMAN, ETAA1_HUMAN, SYTC2_HUMAN, K7ENV2_HUMAN, MAPK5_HUMAN, FRIH_HUMAN, CHCH2_HUMAN, OTOP3_HUMAN, GNPTA_HUMAN, RAB21_HUMAN, GZF1_HUMAN, GRM1_HUMAN, NTCP4_HUMAN, TM203_HUMAN, HAX1_HUMAN, S30BP_HUMAN, TNR6C_HUMAN, F192A_HUMAN, PLEC_HUMAN, KR10B_HUMAN, FPPS_HUMAN, IF3M_HUMAN, ARI1_HUMAN, MLEC_HUMAN, SUV91_HUMAN, SNP29_HUMAN, CDK14_HUMAN, KCC1A_HUMAN, RBM14_HUMAN, CRUM3_HUMAN, MKNK1_HUMAN, EYA4_HUMAN, VIP2_HUMAN, MRCKB_HUMAN, RL24_HUMAN, CALU_HUMAN, RARG_HUMAN, TIM23_HUMAN, RHPN2_HUMAN, F10A1_HUMAN, NDRG1_HUMAN, H2A1H_HUMAN, DUS3_HUMAN, BRI3B_HUMAN, FL2D_HUMAN, QOR_HUMAN, FKBP2_HUMAN, RBMS2_HUMAN, KR212_HUMAN, FUCT1_HUMAN, LACTB_HUMAN, TCAL7_HUMAN, MYBA_HUMAN, PALB2_HUMAN, HDGR2_HUMAN, EAA1_HUMAN, PA1B3_HUMAN, GT253_HUMAN, ID2_HUMAN, STX1B_HUMAN, SPF27_HUMAN, A0A024R4Q5_HUMAN, ASF1B_HUMAN, ASXL1_HUMAN, BACE1_HUMAN, PCDA4_HUMAN, SH3R1_HUMAN, AP1S1_HUMAN, ZO2_HUMAN, GRM2_HUMAN, SAM50_HUMAN, HRK_HUMAN, DESI1_HUMAN, MFSD5_HUMAN, Q08AG9_HUMAN, ORML1_HUMAN, ERBB4_HUMAN, DUS9_HUMAN, ATPF1_HUMAN, UBFL6_HUMAN, APLP2_HUMAN, PE2R2_HUMAN, PEF1_HUMAN, SPRC_HUMAN, MARH5_HUMAN, SYNE1_HUMAN, THB_HUMAN, PRG2_HUMAN, MOG_HUMAN, CSN6_HUMAN, COMD1_HUMAN, IFT80_HUMAN, GP152_HUMAN, GATA6_HUMAN, WDR26_HUMAN, CHMP6_HUMAN, QKI_HUMAN, RCAS1_HUMAN, BTG1_HUMAN, KRA56_HUMAN, PPIP1_HUMAN, PQBP1_HUMAN, RIN1_HUMAN, CAVN4_HUMAN, SPAS2_HUMAN, MYOM1_HUMAN, CR025_HUMAN.Q5BIX2_HUMAN, RHBD2_HUMAN, IF2A_HUMAN, GRIA4_HUMAN, INT10_HUMAN, KIF9_HUMAN, OPA1_HUMAN, TXLNA_HUMAN, FLNC_HUMAN, DX39B_HUMAN, MYCT_HUMAN, PAQRA_HUMAN, BAFL_HUMAN, TCPH_HUMAN, RXRB_HUMAN, NFE2_HUMAN, UBP2_HUMAN, PROM1_HUMAN, CCR4_HUMAN, GLYR1_HUMAN, FBX17_HUMAN, DAZP1_HUMAN, SART3_HUMAN, EHD4_HUMAN, ACO13_HUMAN, CETN3_HUMAN, HCN2_HUMAN, 2A5E_HUMAN, MED1_HUMAN, MED24_HUMAN, MYRIP_HUMAN, UBP18_HUMAN, COX6C_HUMAN, UBE2K_HUMAN, NKD2_HUMAN, AA2AR_HUMAN, MIC25_HUMAN, PSA6_HUMAN, 6PGD_HUMAN, TRA2B_HUMAN, JIP4_HUMAN, BNIP2_HUMAN, PAIP1_HUMAN, TMM62_HUMAN, WBP4_HUMAN, Q6FGD7_HUMAN, COQ8A_HUMAN, H2B2F_HUMAN, TF3C5_HUMAN, RM16_HUMAN, RL10_HUMAN, GOGB1_HUMAN, IPO11_HUMAN, PLCD4_HUMAN, FBX9_HUMAN, KBP_HUMAN, SIR5_HUMAN, PAXX_HUMAN, CCR1_HUMAN, T4S18_HUMAN, NR2F6_HUMAN, ZN774_HUMAN, SP1_HUMAN, ASAP1_HUMAN, AURKB_HUMAN, OXA1L_HUMAN, FRMD3_HUMAN, RN168_HUMAN, F209A_HUMAN, TNR19_HUMAN, SHPRH_HUMAN, GLCE_HUMAN, KR105_HUMAN, ZBT7A_HUMAN, DYH3_HUMAN, AGRG7_HUMAN, CFTR_HUMAN, S35E4_HUMAN, ACL6A_HUMAN, INO80_HUMAN, CLP1_HUMAN, A0A075B7F8_HUMAN.A0A087WY75_HUMAN.P121C_HUMAN, CC125_HUMAN, PDCD2_HUMAN, STX1A_HUMAN, EIF1A_HUMAN, SETB1_HUMAN, B4DYC6_HUMAN, CPSM_HUMAN, DBF4A_HUMAN, L2GL1_HUMAN, TIF1A_HUMAN, MAGE1_HUMAN, CYHR1_HUMAN, ITB5_HUMAN, DCAF6_HUMAN, GNAO_HUMAN, AFAD_HUMAN, SYPH_HUMAN, STX4_HUMAN, MYCB2_HUMAN, PHLA3_HUMAN, TFDP2_HUMAN, UBR1_HUMAN, CUL2_HUMAN, FAF2_HUMAN, ERRFI_HUMAN, KMT2D_HUMAN, ARAP1_HUMAN, RS27_HUMAN, CPSF5_HUMAN, HMGN2_HUMAN, PRD13_HUMAN, GOLP3_HUMAN, S10A8_HUMAN, WASC3_HUMAN, PROC_HUMAN, RB_HUMAN, LMBL1_HUMAN, HSPB9_HUMAN, TERF1_HUMAN, KR123_HUMAN, MMP14_HUMAN, PAR2_HUMAN, CNIH1_HUMAN, AAPK2_HUMAN, RDH11_HUMAN, RAB5A_HUMAN, GUAA_HUMAN, SMKR1_HUMAN, SIK2_HUMAN, Q68CM6_HUMAN.STXB1_HUMAN, BI1_HUMAN, DC1I2_HUMAN, CTXN3_HUMAN, KS6B2_HUMAN, GA45A_HUMAN, BIRC7_HUMAN, STA13_HUMAN, TCOF_HUMAN, RPA2_HUMAN, GGA3_HUMAN, NP1L2_HUMAN, USO1_HUMAN, ACER1_HUMAN, HPT_HUMAN, ANXA7_HUMAN, IF_HUMAN, CD27_HUMAN, MAK_HUMAN, RER1_HUMAN, PEX19_HUMAN, NDUA7_HUMAN, IASPP_HUMAN, SCN3A_HUMAN, DBF4B_HUMAN, GIMA1_HUMAN, RTCA_HUMAN, TOM7_HUMAN, ZFY26_HUMAN, TMM60_HUMAN, SRRM4_HUMAN, PITX1_HUMAN, KCNK3_HUMAN, CDK7_HUMAN, IDLC_HUMAN, ROAA_HUMAN, ETBR2_HUMAN, ZN410_HUMAN, PGRC2_HUMAN, NTM1A_HUMAN, UB2D1_HUMAN, COPG1_HUMAN, ARK72_HUMAN, ERI1_HUMAN, ANR27_HUMAN, AP2D_HUMAN, A4D2J0_HUMAN, CDK5_HUMAN, RNF10_HUMAN, LIME1_HUMAN, VKORL_HUMAN, SMAGP_HUMAN, CENPQ_HUMAN, CP250_HUMAN, RAB6B_HUMAN, WRP73_HUMAN, NCBP2_HUMAN, DYL2_HUMAN, HXA1_HUMAN, TICN2_HUMAN, MOAP1_HUMAN, LANC1_HUMAN, PTH2_HUMAN, TPD54_HUMAN, CIAO1_HUMAN, PAN3_HUMAN, DPPA2_HUMAN, C1GLT_HUMAN, SNX8_HUMAN, BRD7_HUMAN, MUC1_HUMAN, RANB9_HUMAN, AP2A1_HUMAN, RU17_HUMAN, SPT5H_HUMAN, AICDA_HUMAN, ROA1_HUMAN, NMNA2_HUMAN, ZN341_HUMAN, Z512B_HUMAN, HFE_HUMAN, SRCAP_HUMAN, SERP2_HUMAN, H2A2B_HUMAN, CATD_HUMAN, KRA93_HUMAN, KCY_HUMAN, PPIG_HUMAN, NXP20_HUMAN, BLMH_HUMAN, HOGA1_HUMAN, FBX24_HUMAN, TRI69_HUMAN, TZAP_HUMAN, SUIS_HUMAN, CHSS1_HUMAN, KBTB7_HUMAN, CHSS3_HUMAN, FOXN3_HUMAN, PDK2_HUMAN, VTA1_HUMAN, TI17A_HUMAN, JIP2_HUMAN, RPOM_HUMAN, CNDG2_HUMAN, RMI1_HUMAN, RMI2_HUMAN, STX6_HUMAN, VTI1A_HUMAN, SRRM1_HUMAN, E2AK3_HUMAN, IMA3_HUMAN, S35B1_HUMAN, NCOA5_HUMAN, S10A1_HUMAN, ZN660_HUMAN, SHL2A_HUMAN, GAB2_HUMAN, SRSF6_HUMAN, TSN4_HUMAN, PAIP2_HUMAN, UPK1B_HUMAN, TOB2_HUMAN, LHX8_HUMAN, UFL1_HUMAN, CBX4_HUMAN, CLCN3_HUMAN, UBE2B_HUMAN, SSH1_HUMAN, SAE2_HUMAN, RAB6A_HUMAN, KIBRA_HUMAN, HACD1_HUMAN, SC24D_HUMAN, ZN257_HUMAN, TFB2M_HUMAN, MAGA2_HUMAN, MAEL_HUMAN, RS17_HUMAN, DNJA2_HUMAN, FXYD3_HUMAN, CCNC_HUMAN, REN3A_HUMAN, WRB_HUMAN, CAF1A_HUMAN, PA2G4_HUMAN, ZBT42_HUMAN, CD2B2_HUMAN, TTK_HUMAN, A0A024QZR6_HUMAN.DS13B_HUMAN, LSM1_HUMAN, STAB1_HUMAN, K1C17_HUMAN, GAS7_HUMAN, RUBIC_HUMAN, AUTS2_HUMAN, RYBP_HUMAN, 4ET_HUMAN, ALPK3_HUMAN, DVL2_HUMAN, FAKD2_HUMAN, RAB14_HUMAN, C1T9A_HUMAN.C1T9B_HUMAN, TMEDA_HUMAN, UBP33_HUMAN, MCM7_HUMAN, TM140_HUMAN, BPNT1_HUMAN, K1C19_HUMAN, CKLF5_HUMAN, MLF1_HUMAN, DUS1_HUMAN, S27A4_HUMAN, DEN1C_HUMAN, CCD91_HUMAN, VAV3_HUMAN, FRIL_HUMAN, CPSF7_HUMAN, IF2B1_HUMAN, MSI2H_HUMAN, STX2_HUMAN, FGFR2_HUMAN, COPZ1_HUMAN, KRA57_HUMAN, SEPT1_HUMAN, ELOV4_HUMAN, KI21B_HUMAN, A1BG_HUMAN, TGIF1_HUMAN, MP2K5_HUMAN, FWCH1_HUMAN, X3CL1_HUMAN, KRA53_HUMAN, RBCC1_HUMAN, DYRK2_HUMAN, DYRK4_HUMAN, S45A4_HUMAN, ESTD_HUMAN, CRYAB_HUMAN, CD3Z_HUMAN, EMP1_HUMAN, ZN394_HUMAN, FNIP1_HUMAN, MID51_HUMAN, KRA98_HUMAN, UB2R2_HUMAN, JAK3_HUMAN, TIA1_HUMAN, CALM2_HUMAN, CCNL1_HUMAN, CHMP5_HUMAN, TM254_HUMAN, CCAR1_HUMAN, DDX52_HUMAN, TMM11_HUMAN, AEBP2_HUMAN, I10R1_HUMAN, ATP5J_HUMAN, AT5EL_HUMAN, S38A2_HUMAN, MCM4_HUMAN, GG12F_HUMAN.GG12G_HUMAN.GG12I_HUMAN, VPS4A_HUMAN, G3V5R9_HUMAN, AP3D1_HUMAN, PPHLN_HUMAN, PSB9_HUMAN, KR411_HUMAN, NEK6_HUMAN, IF4G3_HUMAN, ICE1_HUMAN, ANM7_HUMAN, C9JA28_HUMAN, LC7L3_HUMAN, PACN1_HUMAN, STX8_HUMAN, LPXN_HUMAN, ML12A_HUMAN, RAGP1_HUMAN, MAT2B_HUMAN, APOB_HUMAN, VP37C_HUMAN, ZN648_HUMAN, CDK6_HUMAN, NTNG2_HUMAN, CLCN7_HUMAN, KR124_HUMAN, SDHF1_HUMAN, CENPI_HUMAN, RTP2_HUMAN, PIWL1_HUMAN, SHRM3_HUMAN, GRSF1_HUMAN, FAT1_HUMAN, GSTO1_HUMAN, PA1B2_HUMAN, NAPSA_HUMAN, ZN549_HUMAN, PACS1_HUMAN, SCAM1_HUMAN, KCTD5_HUMAN, COEA1_HUMAN, RTL9_HUMAN, CEBPG_HUMAN, ZCH18_HUMAN, SEP11_HUMAN, DHE3_HUMAN, SUOX_HUMAN, HHATL_HUMAN, MET17_HUMAN, RN185_HUMAN, MTURN_HUMAN, I6L9I8_HUMAN, TM147_HUMAN, PYRG2_HUMAN, RNF32_HUMAN, CLN6_HUMAN, KCNA5_HUMAN, GT2D1_HUMAN, BUB1B_HUMAN, PPOX_HUMAN, S41A1_HUMAN, NAT14_HUMAN, RYR1_HUMAN, PTK6_HUMAN, PAN2_HUMAN, CAVN3_HUMAN, PIMT_HUMAN, LHX2_HUMAN, CYBR1_HUMAN, SNR25_HUMAN, HIPK2_HUMAN, EEA1_HUMAN, VDR_HUMAN, HNRPL_HUMAN, SRSF4_HUMAN, MYL9_HUMAN, COX7B_HUMAN, KRT83_HUMAN, MARK1_HUMAN, GPR37_HUMAN, THAP7_HUMAN, MYO1G_HUMAN, FA20C_HUMAN, AEN_HUMAN, ABT1_HUMAN, DJC10_HUMAN, FANCM_HUMAN, RM20_HUMAN, RAB1A_HUMAN, PIWL4_HUMAN, SMAD5_HUMAN, KELL_HUMAN, CAV3_HUMAN, ACM5_HUMAN, CF136_HUMAN, NMDE2_HUMAN, DNJC1_HUMAN, FOSL2_HUMAN, S12A4_HUMAN, MTR1B_HUMAN, MAP1B_HUMAN, CP092_HUMAN, A1A4E9_HUMAN, PHF10_HUMAN, PIPNA_HUMAN, LMBL4_HUMAN, DEN2D_HUMAN, CTBP2_HUMAN, EI24_HUMAN, RASN_HUMAN, TBL1Y_HUMAN, VAC14_HUMAN, IF4G2_HUMAN, RU2A_HUMAN, TYB4_HUMAN, MFF_HUMAN, S10AB_HUMAN, C2D1A_HUMAN, BRCC3_HUMAN, ASSY_HUMAN, PYM1_HUMAN, RLA2_HUMAN, ELOF1_HUMAN, CLK2_HUMAN, BRD1_HUMAN, MED15_HUMAN, DOCK7_HUMAN, PDLI1_HUMAN, LUZP1_HUMAN, YIPF5_HUMAN, DPP3_HUMAN, SC23B_HUMAN, OVOL1_HUMAN, NFAC4_HUMAN, ZN724_HUMAN, ANK1_HUMAN, A0A0C4DG91_HUMAN, TRRAP_HUMAN, MAFG_HUMAN, S39A2_HUMAN, EIF3I_HUMAN, ELP1_HUMAN, LKHA4_HUMAN, ORC1_HUMAN, ORC2_HUMAN, PTBP2_HUMAN, KCTD3_HUMAN, PURA2_HUMAN, DNJC5_HUMAN, SRS11_HUMAN, FABP5_HUMAN, HRG_HUMAN, SYK_HUMAN, SRGP2_HUMAN, PUR6_HUMAN, MSL2_HUMAN, IQCB1_HUMAN, KR192_HUMAN, CATB_HUMAN, CE290_HUMAN, CX3C1_HUMAN, SKIL_HUMAN, TR10C_HUMAN, RORB_HUMAN, HSDL2_HUMAN, ACOC_HUMAN, ACD_HUMAN, ADA10_HUMAN, PRKRA_HUMAN, NU153_HUMAN, TSN7_HUMAN, DCAKD_HUMAN, AKTIP_HUMAN, MF14B_HUMAN, NCF2_HUMAN, PTN_HUMAN, PK3C3_HUMAN, 2AAB_HUMAN, RCC2_HUMAN, NDKB_HUMAN, GIMA8_HUMAN, 2A5G_HUMAN, GBP5_HUMAN, BRMS1_HUMAN, PMP22_HUMAN, MA2A2_HUMAN, BOP1_HUMAN, CKLF7_HUMAN, LPIN1_HUMAN, GNAQ_HUMAN, RARA_HUMAN, TIFA_HUMAN, MYCBP_HUMAN, RL35A_HUMAN, RIR2_HUMAN, HPRT_HUMAN, TM86A_HUMAN, KRA23_HUMAN, NPC1_HUMAN, PFD1_HUMAN, UBA3_HUMAN, UB2V2_HUMAN, TROAP_HUMAN, PRP18_HUMAN, TBC15_HUMAN, DCA11_HUMAN, SPRE_HUMAN, SYNC_HUMAN, ERF1_HUMAN, SPEE_HUMAN, SSX9_HUMAN, RASM_HUMAN, TRPM6_HUMAN, ASH2L_HUMAN, DLG4_HUMAN, PGBM_HUMAN, KR196_HUMAN, MS18B_HUMAN, AIG1_HUMAN, RBP1_HUMAN, NAA15_HUMAN, SGCG_HUMAN, CKLF4_HUMAN, WIPI2_HUMAN, SMYD2_HUMAN, SYN1_HUMAN, KANL1_HUMAN, DOPD_HUMAN, CLRN2_HUMAN, ATIF1_HUMAN, GDIA_HUMAN, TNR6_HUMAN, RGAP1_HUMAN, SPB9_HUMAN, RBX1_HUMAN, SIR3_HUMAN, SYNEM_HUMAN, MYOM2_HUMAN, ECH1_HUMAN, RB33A_HUMAN, MAL_HUMAN, ERG7_HUMAN, VIR_HUMAN, TSR1_HUMAN, TBG1_HUMAN, MARK4_HUMAN, NUP58_HUMAN, KLK6_HUMAN, HERP2_HUMAN, AK1C1_HUMAN, IKBD_HUMAN, TAF1D_HUMAN, LYPA1_HUMAN, HMOX2_HUMAN, MUL1_HUMAN, PSB4_HUMAN, FNDC9_HUMAN, UGGG1_HUMAN, NSD1_HUMAN, MP2K7_HUMAN, CHM4A_HUMAN, SBDS_HUMAN, H2AW_HUMAN, ZNF41_HUMAN, SYHC_HUMAN, SPAG1_HUMAN, GRPE1_HUMAN, NDE1_HUMAN, MED12_HUMAN, SNX17_HUMAN, 5HT2B_HUMAN, CE350_HUMAN, SMC6_HUMAN, VRK3_HUMAN, AAPK1_HUMAN, SELPL_HUMAN, TSPO2_HUMAN, NEK4_HUMAN, ARHGG_HUMAN, IEX1_HUMAN, NDUAD_HUMAN, SAMD1_HUMAN, A0A024R9F6_HUMAN, LMBL3_HUMAN, UIMC1_HUMAN, UT14A_HUMAN, AQP8_HUMAN, M3K2_HUMAN, GNAS2_HUMAN, VPS36_HUMAN, TTL10_HUMAN, MAD1_HUMAN, CN37_HUMAN, NDUAA_HUMAN, CDCA7_HUMAN, PRP8_HUMAN, HS71L_HUMAN, ABL2_HUMAN, E2F4_HUMAN, PCBP3_HUMAN, PDC10_HUMAN, TNR6B_HUMAN, MK15_HUMAN, APJ_HUMAN, CFA52_HUMAN, FANCL_HUMAN, DMBT1_HUMAN, BACH1_HUMAN, BDP1_HUMAN, NLGN3_HUMAN, MYO7B_HUMAN, NPS3A_HUMAN, GLOD4_HUMAN, ARPC3_HUMAN, NCOA3_HUMAN, BET1_HUMAN, PRP6_HUMAN, HABP4_HUMAN, KR121_HUMAN, MUC12_HUMAN, U3IP2_HUMAN, COX10_HUMAN, ETHE1_HUMAN, HXB5_HUMAN, CASC3_HUMAN, ZFP91_HUMAN, SMIM1_HUMAN, DDX27_HUMAN, AAAS_HUMAN, GSTM4_HUMAN, DTX3_HUMAN, CSN2_HUMAN, CYH1_HUMAN, GNB5_HUMAN, DYH6_HUMAN, DDX42_HUMAN, SKP2_HUMAN, DUS2_HUMAN, GLT15_HUMAN, GATA_HUMAN, WASH1_HUMAN, STXB2_HUMAN, MSL1_HUMAN, DUS5_HUMAN, DNJA3_HUMAN, MFSD3_HUMAN, PNRC2_HUMAN, TGFI1_HUMAN, RILP_HUMAN, RBM5_HUMAN, ZN329_HUMAN, SMC5_HUMAN, AKA11_HUMAN, ZF69B_HUMAN, RPC6_HUMAN, EPN3_HUMAN, CHM1B_HUMAN, TET2_HUMAN, SDCB2_HUMAN, RL21_HUMAN, ARHG6_HUMAN, STX7_HUMAN, NDUB1_HUMAN, ERC2_HUMAN, OGA_HUMAN, K1C14_HUMAN, WDR33_HUMAN, TF2LX_HUMAN, SPI1_HUMAN, ATN1_HUMAN, ACTN1_HUMAN, LBX1_HUMAN, GDIR1_HUMAN, PTSS1_HUMAN, RN123_HUMAN, SETX_HUMAN, ELP2_HUMAN, NSG2_HUMAN, WDR62_HUMAN, Q5SQT9_HUMAN, TEKT3_HUMAN, PPR26_HUMAN, RPP14_HUMAN, K1C24_HUMAN, BT2A2_HUMAN, YTDC1_HUMAN, DCC_HUMAN, PTN3_HUMAN, IPIL1_HUMAN, ACK1_HUMAN, YIF1A_HUMAN, PP16A_HUMAN, BIG1_HUMAN, DJC14_HUMAN, ETS1_HUMAN, GGT7_HUMAN, GA2L2_HUMAN, RNF37_HUMAN, ZN827_HUMAN, ING1_HUMAN.KLK5_HUMAN, ZFPL1_HUMAN, OSBL1_HUMAN, IF2P_HUMAN, RBBP5_HUMAN, WDR5B_HUMAN, GIMA5_HUMAN, ESRP2_HUMAN, ZBT21_HUMAN, PRUN2_HUMAN, SYPL1_HUMAN, PTPRK_HUMAN, BATF3_HUMAN, A0A024R6X1_HUMAN.EST2_HUMAN, DNJB9_HUMAN, FXYD6_HUMAN, OSBP1_HUMAN, RA51B_HUMAN, CD3D_HUMAN, MOB1B_HUMAN, TRY1_HUMAN, MOB1A_HUMAN, PTPRG_HUMAN, B7ZVY7_HUMAN.CD11B_HUMAN.J3QR29_HUMAN.J3QR44_HUMAN, HNRH3_HUMAN, DMRT3_HUMAN, KRT38_HUMAN, F4ZW62_HUMAN, MAF1_HUMAN, CLPP_HUMAN, EIF3F_HUMAN, SCRIB_HUMAN, NKAP_HUMAN, ARP5_HUMAN, DTX2_HUMAN, PRPF3_HUMAN, ACTZ_HUMAN, MYO5C_HUMAN, ALDH2_HUMAN, RPC9_HUMAN, FKBP3_HUMAN, NIF3L_HUMAN, KISHB_HUMAN, MBIP1_HUMAN, A1AT_HUMAN, GCC2_HUMAN, PO6F2_HUMAN, TXD11_HUMAN, MYL6_HUMAN, NLS1_HUMAN, AMER1_HUMAN, SUN1_HUMAN, OFD1_HUMAN, IR3IP_HUMAN, NPT2B_HUMAN, IMA8_HUMAN, ESYT1_HUMAN, FBX11_HUMAN, ATTY_HUMAN, SUV92_HUMAN, P121A_HUMAN, PKHF2_HUMAN, S38A1_HUMAN, CLAP1_HUMAN, SPTN2_HUMAN, UBC12_HUMAN, MTDC_HUMAN, PFKAL_HUMAN, A2AP_HUMAN, RL22_HUMAN, A4PIV8_HUMAN, CIB1_HUMAN, KLF1_HUMAN, G3V1Q7_HUMAN.PMFBP_HUMAN, NOS2_HUMAN, TRPV5_HUMAN, DNLI3_HUMAN, SNX2_HUMAN, TBPL1_HUMAN, IPO5_HUMAN, AL1B1_HUMAN, SUH_HUMAN, RBPMS_HUMAN, TIPRL_HUMAN, O10J1_HUMAN, TMED8_HUMAN, GLSK_HUMAN, ZN764_HUMAN, PYGO1_HUMAN, ANGP2_HUMAN, RIT1_HUMAN, RL32_HUMAN, HS71A_HUMAN.HS71B_HUMAN, TPD52_HUMAN, SNAA_HUMAN, RABE1_HUMAN, HSFY1_HUMAN, E2F7_HUMAN, TLX3_HUMAN, ST1E1_HUMAN, RL3_HUMAN, DDX23_HUMAN, MPRIP_HUMAN, KMT2C_HUMAN, FAF1_HUMAN, COR1C_HUMAN, PRS10_HUMAN, RSMN_HUMAN, Q6PK50_HUMAN, TCRG1_HUMAN, FANCA_HUMAN, COA3_HUMAN, UTRO_HUMAN, KIF11_HUMAN, SOLH1_HUMAN, PTN22_HUMAN, CSTN3_HUMAN, MAGC2_HUMAN, TLK2_HUMAN, STX11_HUMAN, PDK3_HUMAN, SPON1_HUMAN, H7C5Q0_HUMAN, NFXL1_HUMAN, TSNAX_HUMAN, ATF1_HUMAN.FUS_HUMAN, B7Z2Q3_HUMAN.CCD14_HUMAN, SCN2A_HUMAN, EPHA2_HUMAN, THOC6_HUMAN, SNX9_HUMAN, AGRL3_HUMAN, A0A0A0MRV0_HUMAN.RRBP1_HUMAN, SWET1_HUMAN, SIR4_HUMAN, ANXA1_HUMAN.B5BU38_HUMAN, PACE1_HUMAN, XPO5_HUMAN, GRN_HUMAN, PDXK_HUMAN, EST1A_HUMAN, SNX3_HUMAN, TPC2_HUMAN, RA1L2_HUMAN, PAR6B_HUMAN, F262_HUMAN, VRK1_HUMAN, MYO1F_HUMAN, AMPD3_HUMAN, NOL12_HUMAN, KR511_HUMAN, CEMIP_HUMAN, CPSF2_HUMAN, GAPD1_HUMAN, S7A14_HUMAN, RFX3_HUMAN, KCNF1_HUMAN, PICK1_HUMAN, RFT1_HUMAN, TPM2_HUMAN, MYO3A_HUMAN, P121A_HUMAN.P121C_HUMAN, OLIG1_HUMAN, CNTRL_HUMAN, RAB10_HUMAN, MCES_HUMAN, TPH2_HUMAN, FBXW7_HUMAN, PASK_HUMAN, NEMP1_HUMAN, PPM1G_HUMAN, PSB6_HUMAN, CHMP7_HUMAN, UGPA_HUMAN, EXOS8_HUMAN, DHX15_HUMAN, KCNK1_HUMAN, ACLY_HUMAN, RIR2B_HUMAN, MBOA7_HUMAN, TINF2_HUMAN, RL17_HUMAN, ERR2_HUMAN, EMAL1_HUMAN, ZBTB3_HUMAN, P3C2B_HUMAN, LIPA1_HUMAN, ELOC_HUMAN, DC2L1_HUMAN, NXT1_HUMAN, URGCP_HUMAN, TNNC1_HUMAN, SNG3_HUMAN, NDUS8_HUMAN, ASCC1_HUMAN, CLD10_HUMAN, ACKR2_HUMAN, ZDH21_HUMAN, APOL2_HUMAN, ARI3B_HUMAN, TTP_HUMAN, MTR1A_HUMAN, NADK_HUMAN, AKP8L_HUMAN, TCPR1_HUMAN, PSMD9_HUMAN, RPB3_HUMAN, EFNB3_HUMAN, NECP2_HUMAN, CBS_HUMAN, MITF_HUMAN, CRY2_HUMAN, RT09_HUMAN, UBL4A_HUMAN, MAST3_HUMAN, RTL8C_HUMAN, ZN395_HUMAN, ERBB3_HUMAN, CLIC4_HUMAN, KIRR3_HUMAN, QCR8_HUMAN, QCR9_HUMAN, C1D_HUMAN, OTU1_HUMAN, CEP72_HUMAN, SRSF3_HUMAN, DCE2_HUMAN, SF3B3_HUMAN, TMM42_HUMAN, PCGF3_HUMAN, RPRM_HUMAN, GEM_HUMAN, POGZ_HUMAN, ZC3HE_HUMAN, PLK4_HUMAN, PLCD1_HUMAN, 5HT2C_HUMAN, MGN2_HUMAN, RPC5_HUMAN, RPB1_HUMAN, RGR_HUMAN, DNJB4_HUMAN, STA5B_HUMAN, MK06_HUMAN, T161A_HUMAN, AFF1_HUMAN, OXLA_HUMAN, TPK1_HUMAN, D3DR86_HUMAN, NU160_HUMAN, LIPA4_HUMAN, RT12_HUMAN, CNTN4_HUMAN, HDHD3_HUMAN, KRT34_HUMAN, UBQL4_HUMAN, MTEF2_HUMAN, SAC1_HUMAN, ARHG5_HUMAN, Z280D_HUMAN, THOC7_HUMAN, HS2ST_HUMAN, BOP_HUMAN, FOXI1_HUMAN, TLE2_HUMAN, PSD1_HUMAN, PHTF1_HUMAN, RFXAP_HUMAN, TMX3_HUMAN, TMX2_HUMAN, TACC3_HUMAN, CKAP5_HUMAN, CLH2_HUMAN, ZNF16_HUMAN, RBFA_HUMAN, EXOC6_HUMAN, SPAT2_HUMAN, DHX36_HUMAN, IFNA4_HUMAN, ALDOA_HUMAN, RECQ1_HUMAN, H2B1L_HUMAN, H2A1A_HUMAN, MED4_HUMAN, MED23_HUMAN, NUP62_HUMAN, RCOR3_HUMAN, FBXL7_HUMAN, DHC24_HUMAN, PI3R4_HUMAN, LETM1_HUMAN, RIDA_HUMAN, GDIB_HUMAN, ACSF2_HUMAN, SAE1_HUMAN, HBG1_HUMAN.HBG2_HUMAN, CACP_HUMAN, PDE1A_HUMAN, PKHA4_HUMAN, KDM4B_HUMAN, TBL3_HUMAN, MYH8_HUMAN, TALDO_HUMAN, RBMS1_HUMAN, NCLN_HUMAN, BHE41_HUMAN, CERS4_HUMAN, ANR28_HUMAN, PTN23_HUMAN, CRYM_HUMAN, PBX4_HUMAN, SERF2_HUMAN, MYCPP_HUMAN, TM199_HUMAN, PEMT_HUMAN, PFD2_HUMAN, IF4H_HUMAN, NIPS2_HUMAN, NS1BP_HUMAN, LIRB3_HUMAN, HNRH2_HUMAN, KCRS_HUMAN, FLRT1_HUMAN, GFI1B_HUMAN, A0A087WZG2_HUMAN.RON_HUMAN, GPC5B_HUMAN, LRSM1_HUMAN, EXOC1_HUMAN, CCDB1_HUMAN, I15RA_HUMAN, WDR61_HUMAN, MMS19_HUMAN, CSTF3_HUMAN, TRIPB_HUMAN, REXO1_HUMAN, PHP14_HUMAN, PSD10_HUMAN, MYH15_HUMAN, ZN835_HUMAN, LAT_HUMAN, TLE6_HUMAN, PP2BA_HUMAN, EIF3M_HUMAN, ROCK2_HUMAN, Q6FHQ0_HUMAN, F263_HUMAN, TM154_HUMAN, MSX2_HUMAN, SSBP2_HUMAN, NSMA2_HUMAN, AIM2_HUMAN, TMX4_HUMAN, MYNN_HUMAN, SCND1_HUMAN, GTPB3_HUMAN, SYMPK_HUMAN, A2MG_HUMAN, RN139_HUMAN, TMCO1_HUMAN, KIF14_HUMAN, NPA1P_HUMAN, PTPRF_HUMAN, ENKD1_HUMAN, ZHX2_HUMAN, CDC5L_HUMAN, CPTP_HUMAN, BECN2_HUMAN, CE030_HUMAN, CD53_HUMAN, DDX41_HUMAN, CC181_HUMAN, CHD8_HUMAN, PAK6_HUMAN, DYST_HUMAN, CEP63_HUMAN, Q6FHT8_HUMAN, RGS1_HUMAN, ZN451_HUMAN, NGEF_HUMAN, AT1A4_HUMAN, GDPD2_HUMAN, PSA5_HUMAN, CCAR2_HUMAN, RRP15_HUMAN, UBP14_HUMAN, IL33_HUMAN, IF2B3_HUMAN, HELZ_HUMAN, WDR1_HUMAN, ACL6B_HUMAN, KRA54_HUMAN, PHOCN_HUMAN, LAMP3_HUMAN, CDYL_HUMAN, PPR18_HUMAN, HEMH_HUMAN, CNTP2_HUMAN, RBM45_HUMAN, KI16B_HUMAN, SDHF2_HUMAN, SVIL_HUMAN, Q17RL8_HUMAN, HSP77_HUMAN, RT27_HUMAN, KDM3B_HUMAN, DEP1A_HUMAN, ZN526_HUMAN, MAGIX_HUMAN, DTX4_HUMAN, NSG1_HUMAN, PACN3_HUMAN, MDR1_HUMAN, VPS28_HUMAN, ACTA_HUMAN, CYLC2_HUMAN, RS18_HUMAN, NASP_HUMAN, TM35A_HUMAN, SMTL1_HUMAN, PP4C_HUMAN, DPYL3_HUMAN, CY561_HUMAN, KR133_HUMAN, ZIC1_HUMAN, CNIH3_HUMAN, RPAP2_HUMAN, RPGP1_HUMAN, GRL1A_HUMAN, FIBA_HUMAN, STMN1_HUMAN, WDR35_HUMAN, NOC4L_HUMAN, RPA49_HUMAN, ACMSD_HUMAN, ZYX_HUMAN, PP1R7_HUMAN, CHM2A_HUMAN, PDP1_HUMAN, CSN4_HUMAN, DNM3B_HUMAN, RCOR1_HUMAN, CDIP1_HUMAN, CLD5_HUMAN, KI20B_HUMAN, PLCB1_HUMAN, SERC1_HUMAN, GEMI7_HUMAN, PHLB2_HUMAN, ZN438_HUMAN, SNP47_HUMAN, GSG1_HUMAN, JPH1_HUMAN, EIF3D_HUMAN, MGLL_HUMAN, UBE2C_HUMAN, STXB5_HUMAN, WDR83_HUMAN, TERF2_HUMAN, INSI1_HUMAN, RL36A_HUMAN, SF3B4_HUMAN, PHF19_HUMAN, SRS10_HUMAN, VINEX_HUMAN, TRPV4_HUMAN, KS6A6_HUMAN, WAPL_HUMAN, UST_HUMAN, SMAD7_HUMAN, FGD2_HUMAN, SNX18_HUMAN, TM243_HUMAN, FXDC2_HUMAN, SDS3_HUMAN, SCMH1_HUMAN, NFIL3_HUMAN, EP15R_HUMAN, ASPM_HUMAN, ORN_HUMAN, IL18R_HUMAN, EXOS9_HUMAN, TM9S3_HUMAN, VASH2_HUMAN, A0A087WTE7_HUMAN.LENG8_HUMAN, ABI2_HUMAN, GBB2_HUMAN, MAT1_HUMAN, SPART_HUMAN, RORA_HUMAN, PP1R8_HUMAN, PSPC_HUMAN, TRA2A_HUMAN, RL13_HUMAN, PQLC1_HUMAN, SAV1_HUMAN, RINT1_HUMAN, ZN189_HUMAN, CNOT8_HUMAN, NOTO_HUMAN, RFC4_HUMAN, VIGLN_HUMAN, DPOD1_HUMAN, COX1_HUMAN, PKD2_HUMAN, MGST2_HUMAN, HSP72_HUMAN, HBP1_HUMAN, WWP2_HUMAN, ABLM2_HUMAN, VLDLR_HUMAN, SYT2_HUMAN, WIPF1_HUMAN, PRP31_HUMAN, AK1C3_HUMAN, LDB1_HUMAN, PDCD5_HUMAN, VPS72_HUMAN, MRGBP_HUMAN, NUDT3_HUMAN, Q31604_HUMAN, KCNA3_HUMAN, T106C_HUMAN, LHX1_HUMAN, RBM42_HUMAN, FEZ1_HUMAN, UMPS_HUMAN, CAB45_HUMAN, RNF11_HUMAN, CTIP_HUMAN, NUMB_HUMAN, BAZ2A_HUMAN, NOL11_HUMAN, SRTD3_HUMAN, KIF22_HUMAN, SPAG8_HUMAN, BL1S6_HUMAN, PACS2_HUMAN, TPIS_HUMAN, RU1C_HUMAN, CDHR1_HUMAN, RM22_HUMAN, NAA50_HUMAN, PSMG2_HUMAN, KMT5C_HUMAN, STK4_HUMAN, ANKR1_HUMAN, Q6IAM1_HUMAN, CARF_HUMAN, CBPC1_HUMAN, 1C12_HUMAN, RPGR1_HUMAN, IMP3_HUMAN, RTN1_HUMAN, CBPE_HUMAN, VGLU3_HUMAN, NOTC3_HUMAN, DUPD1_HUMAN, PSB8_HUMAN, PSB7_HUMAN, SPDEF_HUMAN, TCF25_HUMAN, GCNT1_HUMAN, A0A0B4J1S4_HUMAN.SEP15_HUMAN, NRAM2_HUMAN, GNPI1_HUMAN, CIR1_HUMAN, FXR1_HUMAN, MOT13_HUMAN, STK25_HUMAN, IFI44_HUMAN, SYF1_HUMAN, MZT2B_HUMAN, TNFB_HUMAN, CHST1_HUMAN, RFWD3_HUMAN, TRPM7_HUMAN, EID1_HUMAN, FOXG1_HUMAN, BAG4_HUMAN, TRDMT_HUMAN, INT11_HUMAN, IF2M_HUMAN, TBR1_HUMAN, CSRP1_HUMAN, TNI3K_HUMAN, KRA45_HUMAN, RENT2_HUMAN, PP4R2_HUMAN, RASL3_HUMAN, LRWD1_HUMAN, KCNE5_HUMAN, TOE1_HUMAN, MIPT3_HUMAN, LTOR2_HUMAN, RL37A_HUMAN, VGFR2_HUMAN, CKLF2_HUMAN, SF3B2_HUMAN, COPB_HUMAN, PARP2_HUMAN, LHPL5_HUMAN, RETR3_HUMAN, NLE1_HUMAN, AF9_HUMAN, CCL21_HUMAN.Q6ICR7_HUMAN, VATB1_HUMAN, ZFP1_HUMAN, SNX24_HUMAN, 2ABB_HUMAN, MON2_HUMAN, PAR1_HUMAN, TNR21_HUMAN, BCL7C_HUMAN, H7C1F9_HUMAN, RAB35_HUMAN, ADDA_HUMAN, FA2H_HUMAN, KGP1_HUMAN, PDE5A_HUMAN, PMS1_HUMAN, TTI2_HUMAN, TRI54_HUMAN, DNS2A_HUMAN, XPO4_HUMAN, TM102_HUMAN, GSTO2_HUMAN, BNIP3_HUMAN, IN35_HUMAN, CE164_HUMAN, KRA81_HUMAN, FPR1_HUMAN, SLIRP_HUMAN, TRIB3_HUMAN, CYTB_HUMAN, NPAS2_HUMAN, EFGM_HUMAN, TGS1_HUMAN, TEAD2_HUMAN, TGM1_HUMAN, SAHH2_HUMAN, A0A0A0MS80_HUMAN.TMM80_HUMAN, PEX7_HUMAN, NCK1_HUMAN, COR2B_HUMAN, NUFP1_HUMAN, ANS4B_HUMAN, CD59_HUMAN, TMED2_HUMAN, F16P1_HUMAN, S2548_HUMAN, U520_HUMAN, RL38_HUMAN, LRP2_HUMAN, IPO4_HUMAN, PDE3A_HUMAN, CDS1_HUMAN, KCNN3_HUMAN, HNRL1_HUMAN, PAEP_HUMAN, CSK_HUMAN, PKN2_HUMAN, PF2R_HUMAN, CCR2_HUMAN, TTMP_HUMAN, RB27B_HUMAN, GRB14_HUMAN, SCN8A_HUMAN, TMM70_HUMAN, ANK3_HUMAN, SESN1_HUMAN, CITE2_HUMAN, COBL_HUMAN, SFT2B_HUMAN, M3K6_HUMAN, NACC1_HUMAN, Q86WV8_HUMAN, PVR_HUMAN, ANR46_HUMAN, HACD4_HUMAN, MOXD1_HUMAN, CP2C8_HUMAN, PNO1_HUMAN, TEC_HUMAN, FBW1B_HUMAN, SKP1_HUMAN, CABP2_HUMAN, KRA31_HUMAN, KI13B_HUMAN, STT3B_HUMAN, MYOG_HUMAN, SWP70_HUMAN, JAM1_HUMAN, RL14_HUMAN, CR3L4_HUMAN, HEXI2_HUMAN, CDC73_HUMAN, E9PJ24_HUMAN, CRBG1_HUMAN, SRSF7_HUMAN, CHD9_HUMAN, PRCC_HUMAN, SYVC_HUMAN, EPCR_HUMAN, HSPB7_HUMAN, A0A0C4DFT9_HUMAN.WHRN_HUMAN, M4K2_HUMAN, KAT7_HUMAN, KANL3_HUMAN, ARMX3_HUMAN, TRDN_HUMAN, ZNF71_HUMAN, PCNT_HUMAN, CHMP3_HUMAN, BIEA_HUMAN, COG8_HUMAN, ZNHI1_HUMAN, PPCE_HUMAN, FGF19_HUMAN, ABLM1_HUMAN, SRP68_HUMAN, RM14_HUMAN, SCMC2_HUMAN, UTP11_HUMAN, PDLI2_HUMAN, CK5P2_HUMAN, NRIP1_HUMAN, F16P2_HUMAN, PER3_HUMAN, PDIA1_HUMAN, LAPM5_HUMAN, Q5VU21_HUMAN, CREL1_HUMAN, OS9_HUMAN, MED31_HUMAN, NU6M_HUMAN, RGSL_HUMAN, BKRB2_HUMAN, TEX10_HUMAN, PELP1_HUMAN, WDR18_HUMAN, OSBP2_HUMAN, MTMR9_HUMAN, TKFC_HUMAN, DEFI6_HUMAN, GOT1A_HUMAN, CASP7_HUMAN, MUSC_HUMAN, DDX11_HUMAN, CXCR1_HUMAN, NFAC3_HUMAN, ANFY1_HUMAN, FNBP1_HUMAN, CL065_HUMAN, DC1L1_HUMAN, U5S1_HUMAN, NOS1_HUMAN, ALDR_HUMAN, S13A3_HUMAN, CDN2C_HUMAN, MD2BP_HUMAN, DESP_HUMAN, CH033_HUMAN, PHC1_HUMAN, ERCC8_HUMAN, CC90B_HUMAN, NRP1_HUMAN, EDC3_HUMAN, PPIE_HUMAN, ARL3_HUMAN, TSN_HUMAN, ZN607_HUMAN, STAC_HUMAN, NUP85_HUMAN, UBE4B_HUMAN, GA45B_HUMAN, CISH_HUMAN, ENOG_HUMAN, U17L2_HUMAN, U17L7_HUMAN, U17LO_HUMAN, INSI2_HUMAN, DDHD1_HUMAN, USF3_HUMAN, PI42B_HUMAN, M3K4_HUMAN, LEG2_HUMAN, CLC2D_HUMAN, TF2H1_HUMAN, WDR60_HUMAN, A8K1F4_HUMAN, PURA1_HUMAN, GEMI5_HUMAN, Z3H7B_HUMAN, PYGM_HUMAN, CLC4K_HUMAN, A0A0A0MT22_HUMAN.PTPRC_HUMAN.X6R433_HUMAN, ASF1A_HUMAN, TF2H3_HUMAN, HEMGN_HUMAN, KRA61_HUMAN, DISP3_HUMAN, UT14C_HUMAN, SP3_HUMAN, STEA4_HUMAN, NU133_HUMAN, DLDH_HUMAN, SFI1_HUMAN, CIP2A_HUMAN, 5HT4R_HUMAN, F120A_HUMAN, DUX3_HUMAN, HIP1_HUMAN, CP2C9_HUMAN, BCR_HUMAN, NR2C1_HUMAN, XPO6_HUMAN, RANG_HUMAN, MCAF2_HUMAN, PDPR_HUMAN, EXOC3_HUMAN, F261_HUMAN, TRPC4_HUMAN, MVD1_HUMAN, TEAD3_HUMAN, KCMB1_HUMAN, LRP1_HUMAN, ABCA7_HUMAN, ARP2_HUMAN, PRC1_HUMAN, MY18A_HUMAN, 5HT1B_HUMAN, AL2CL_HUMAN, LRP10_HUMAN, EVI5_HUMAN, ABHD5_HUMAN, SKA1_HUMAN, NAT10_HUMAN, TPPP_HUMAN, IP6K2_HUMAN, ING2_HUMAN, EM55_HUMAN, AACT_HUMAN, ANTR2_HUMAN, KIF5A_HUMAN, Q6IAW1_HUMAN, HM13_HUMAN, KRA42_HUMAN, IRS2_HUMAN, H13_HUMAN, GEMI2_HUMAN, ICAM1_HUMAN, FOSB_HUMAN, FBX5_HUMAN, JAG1_HUMAN, PLAL2_HUMAN, CTC1_HUMAN, TOPB1_HUMAN, KAP2_HUMAN, MAPK3_HUMAN, NDUA6_HUMAN, CWC15_HUMAN, RUFY1_HUMAN, KR197_HUMAN, FUND2_HUMAN, NRAC_HUMAN, COPD_HUMAN, 1B27_HUMAN, DCUP_HUMAN, CP3A4_HUMAN, CKAP4_HUMAN, STBD1_HUMAN, CNOT1_HUMAN, LOXL4_HUMAN, Q6FGG2_HUMAN, M4K4_HUMAN, ES8L2_HUMAN, RGCC_HUMAN, CDC27_HUMAN, PHS_HUMAN, MADD_HUMAN, GCP3_HUMAN, OGT1_HUMAN, PFD3_HUMAN, HEAT1_HUMAN, WDTC1_HUMAN, DERL2_HUMAN, FZD1_HUMAN, RBM26_HUMAN, ASM_HUMAN, ZFHX3_HUMAN, LUC7L_HUMAN, A0A087WZY3_HUMAN.ALMS1_HUMAN, SCAM2_HUMAN, NOC2L_HUMAN, TRI31_HUMAN, SCC4_HUMAN, NIPBL_HUMAN, NSD3_HUMAN, G45IP_HUMAN, GP143_HUMAN, TCP4_HUMAN, NISCH_HUMAN, PHTF2_HUMAN, SPTB1_HUMAN, ZN345_HUMAN, FUBP3_HUMAN, C560_HUMAN, FKBPL_HUMAN, POC1B_HUMAN, DCAF4_HUMAN, NSL1_HUMAN, ERR3_HUMAN, DLGP4_HUMAN, ZNF24_HUMAN, 2ABD_HUMAN, BPL1_HUMAN, PTN5_HUMAN, ERCC6_HUMAN, A0A140T8X2_HUMAN.CFA47_HUMAN, EMX2_HUMAN, SRGP1_HUMAN, MCF2L_HUMAN, KAT8_HUMAN, S52A2_HUMAN, CDKA1_HUMAN, HERC1_HUMAN, DCA10_HUMAN, ARI3A_HUMAN, FFAR2_HUMAN, MED21_HUMAN, MED19_HUMAN, ZZZ3_HUMAN, PLSI_HUMAN, ERO1A_HUMAN, SHAN1_HUMAN, CUTA_HUMAN, SIK3_HUMAN, NO40_HUMAN, ZDHC3_HUMAN, NSUN4_HUMAN, LATS2_HUMAN, MYOME_HUMAN, SPN1_HUMAN, PLCE1_HUMAN, SRBP1_HUMAN, NOP10_HUMAN, PGES2_HUMAN, CNKR2_HUMAN, HEXI1_HUMAN, UBL5_HUMAN, KDM4D_HUMAN, CMC4_HUMAN, XRN1_HUMAN, CLCA4_HUMAN, CRBL2_HUMAN, KPCB_HUMAN, RGRF2_HUMAN, DERL3_HUMAN, ADHX_HUMAN, FA13B_HUMAN, CEP95_HUMAN, HMGN1_HUMAN, LTOR4_HUMAN, V9HWA4_HUMAN, ACES_HUMAN, NEMF_HUMAN, S27A2_HUMAN, Q86WA0_HUMAN, MTG8_HUMAN.RUNX1_HUMAN, BI2L1_HUMAN, DCP1A_HUMAN, UBE2O_HUMAN, HSPB3_HUMAN, RHOH_HUMAN, THAS_HUMAN, SCNM1_HUMAN, NDUB3_HUMAN, EDF1_HUMAN, BBS7_HUMAN, G6PI_HUMAN, EYA2_HUMAN, DYH7_HUMAN, NTNG1_HUMAN, PLPP6_HUMAN, ERGI1_HUMAN, DAAF1_HUMAN, DCAF8_HUMAN, H2B1N_HUMAN, ABCA3_HUMAN, TIMP2_HUMAN, SGMR1_HUMAN, TMC6_HUMAN, ST14_HUMAN, MAAI_HUMAN, XPA_HUMAN, CCD58_HUMAN, M1AP_HUMAN, S19A3_HUMAN, ANR23_HUMAN, PAG15_HUMAN, ZNF57_HUMAN, SMD2_HUMAN, CAB39_HUMAN, CRPAK_HUMAN, ATGA1_HUMAN, BCAS3_HUMAN.BCAS4_HUMAN, FGFR3_HUMAN, RS7_HUMAN, PITC1_HUMAN, Q86YI5_HUMAN, AMPO_HUMAN, DAAM1_HUMAN, ODF2L_HUMAN, TONSL_HUMAN, BBC3B_HUMAN, SEN54_HUMAN, CDK16_HUMAN, 2ABA_HUMAN, CC113_HUMAN, HLTF_HUMAN, EXOS5_HUMAN, KRT85_HUMAN, TM14A_HUMAN, RM13_HUMAN, PANK1_HUMAN, CC167_HUMAN, RL39_HUMAN, TIM13_HUMAN, PREB_HUMAN, E2F3_HUMAN, MARCS_HUMAN, CGL_HUMAN, FGF23_HUMAN, PCNP_HUMAN, EIF3H_HUMAN, MYBB_HUMAN, HDGF_HUMAN, RUXF_HUMAN, DGAT1_HUMAN, PSCA_HUMAN, P4K2A_HUMAN, RPGP2_HUMAN, AURKC_HUMAN, DAPK2_HUMAN, PIGU_HUMAN, LORF1_HUMAN, Q8TE30_HUMAN, MYPC1_HUMAN, NPHP4_HUMAN, PAB4L_HUMAN, PKHA3_HUMAN, HTR5A_HUMAN, CHD2_HUMAN, ILRL1_HUMAN, CLP1L_HUMAN, RAG1_HUMAN, IF5A1_HUMAN, GLNA_HUMAN, RHG09_HUMAN, HUS1_HUMAN, SPT4H_HUMAN, PDLI7_HUMAN, ERF_HUMAN, MAGA1_HUMAN, SC24B_HUMAN, SFR19_HUMAN, RN165_HUMAN, SARAF_HUMAN, KAD5_HUMAN, SMC2_HUMAN, SYSC_HUMAN, A0A0A0MS56_HUMAN.ADH6_HUMAN, TP53B_HUMAN, CDK8_HUMAN, CAF1B_HUMAN, SYNCI_HUMAN, RT14_HUMAN, SHRM2_HUMAN, MBRL_HUMAN, CBX2_HUMAN, GLPA_HUMAN, TAF4_HUMAN, CC50A_HUMAN, EIF2D_HUMAN, KC1G1_HUMAN, CASP2_HUMAN, OR1D4_HUMAN, ITSN1_HUMAN, OCAD1_HUMAN, SLK_HUMAN, TOM34_HUMAN, PR38A_HUMAN, CCYL1_HUMAN, SCRB1_HUMAN, MECP2_HUMAN, CC14B_HUMAN, PSME2_HUMAN, NCDN_HUMAN, NHLC1_HUMAN, SC6A4_HUMAN, DYH5_HUMAN, DHX16_HUMAN, MKL1_HUMAN.RBM15_HUMAN, HOOK2_HUMAN, ASXL3_HUMAN, ESRP1_HUMAN, SDCG8_HUMAN, LAS1L_HUMAN, A0A0A6YY96_HUMAN.IREB2_HUMAN, NCKP1_HUMAN, STAT4_HUMAN, KRR1_HUMAN, ARP6_HUMAN, TBKB1_HUMAN, RABL6_HUMAN, CAND1_HUMAN, TBCD_HUMAN, UCHL3_HUMAN, ADCY6_HUMAN, ERAP2_HUMAN, PCCB_HUMAN, SHOX2_HUMAN, TDRD6_HUMAN, MYPC3_HUMAN, VN1R1_HUMAN, PTSS2_HUMAN, CREL2_HUMAN, PIGT_HUMAN, RSF1_HUMAN, AK17A_HUMAN, TBB6_HUMAN, ACM3_HUMAN, PRDX5_HUMAN, RHG08_HUMAN, RFC1_HUMAN, SGIP1_HUMAN, GRP1_HUMAN, ASNS_HUMAN, PHF8_HUMAN, DUS23_HUMAN, KMT5B_HUMAN, ATLA2_HUMAN, UCRIL_HUMAN, LMBD1_HUMAN, TTC4_HUMAN, CDT1_HUMAN, NUD14_HUMAN, SPB8_HUMAN, ATX7_HUMAN, HCFC2_HUMAN, APOC2_HUMAN, ANR26_HUMAN, OXSR1_HUMAN, CRTC2_HUMAN, S22AE_HUMAN, RB6I2_HUMAN, ABC3G_HUMAN, SALL2_HUMAN, PMS2L_HUMAN, MCTS1_HUMAN, GDF5O_HUMAN, REBL1_HUMAN, DJC11_HUMAN, UBE2Z_HUMAN, STK33_HUMAN, PDE6D_HUMAN, KI18B_HUMAN, PO3F3_HUMAN, TISD_HUMAN, SNX27_HUMAN, NU107_HUMAN, SARM1_HUMAN, XLRS1_HUMAN, S61A2_HUMAN, IMA6_HUMAN, T2FA_HUMAN, TNNI3_HUMAN, B2MG_HUMAN, GNAI2_HUMAN, INO1_HUMAN, S10AD_HUMAN, RBGP1_HUMAN, RAB4A_HUMAN, CYB5_HUMAN, DNLI1_HUMAN, MARK3_HUMAN, RT10_HUMAN, BRD4_HUMAN, URM1_HUMAN, PGH2_HUMAN, PIAS1_HUMAN, COT1_HUMAN, RT18B_HUMAN, AXIN2_HUMAN, VPS51_HUMAN, CHD7_HUMAN, RM37_HUMAN, PCM1_HUMAN, ZBT17_HUMAN, FGF5_HUMAN, TCEA1_HUMAN, FBXW5_HUMAN, MKKS_HUMAN, PIAS3_HUMAN, CALM3_HUMAN, Q7Z3E4_HUMAN, SRCN1_HUMAN, CEAM5_HUMAN, ING1_HUMAN, Q6PJ73_HUMAN, MTCP1_HUMAN, MAGI3_HUMAN, PPAP_HUMAN, ANXA1_HUMAN, SCRB2_HUMAN, MYO1A_HUMAN, MTA3_HUMAN, Q5T8J1_HUMAN, Q5JPB8_HUMAN, SHB_HUMAN, U2AF1_HUMAN.U2AF5_HUMAN, CNKR1_HUMAN, Q86SZ9_HUMAN, Q5QPM7_HUMAN, PECA1_HUMAN, SRC8_HUMAN, Q53FG3_HUMAN, ELYS_HUMAN, DMRTB_HUMAN, DHX30_HUMAN, ZO1_HUMAN, Q7Z763_HUMAN, Q53FP9_HUMAN, CRML_HUMAN, SNURF_HUMAN, SEP15_HUMAN, Q6N083_HUMAN, PCM1_HUMAN.RET_HUMAN, UBF1_HUMAN, TP4A2_HUMAN, VTDB_HUMAN, TCF20_HUMAN, DPOG1_HUMAN, CAC1B_HUMAN, SNP25_HUMAN, CLAT_HUMAN, BSPRY_HUMAN, FGF6_HUMAN, ITK_HUMAN, OTC_HUMAN, AIP_HUMAN, GAR1_HUMAN, GOSR1_HUMAN, SARCO_HUMAN, SOX9_HUMAN, UBR5_HUMAN, BUB1_HUMAN, LAMA1_HUMAN, 2A5A_HUMAN, BMR1B_HUMAN, RIMS2_HUMAN, RAB4B_HUMAN, RB22A_HUMAN, GRK5_HUMAN, CO1A2_HUMAN, RUNX2_HUMAN, SYUB_HUMAN, IKZF3_HUMAN, BBC3B_HUMAN.BBC3_HUMAN, MYPR_HUMAN, FA8_HUMAN, PAPOA_HUMAN, ARG28_HUMAN, UN13B_HUMAN, EXOC4_HUMAN, EXOC7_HUMAN, RGDSR_HUMAN, RAD9A_HUMAN, ADX_HUMAN, ANTR1_HUMAN, B2L14_HUMAN, FA57A_HUMAN, UBP2L_HUMAN, BACE2_HUMAN, PRD12_HUMAN, FXYD7_HUMAN, UBP28_HUMAN, RNF14_HUMAN, RMP_HUMAN, STAP1_HUMAN, MTP_HUMAN, SPERI_HUMAN, AP180_HUMAN, PAX6_HUMAN, VAMP2_HUMAN, S22A4_HUMAN, FGR_HUMAN, MYOC_HUMAN, NTRK2_HUMAN, TAF10_HUMAN, AP1B1_HUMAN, KPCL_HUMAN, NEST_HUMAN, UBP16_HUMAN, SYCP3_HUMAN, APC5_HUMAN, 5NTD_HUMAN, SPN90_HUMAN, GDN_HUMAN, CNN1_HUMAN, TMOD2_HUMAN, CEP55_HUMAN, NTRK3_HUMAN, EFNB1_HUMAN, REPS1_HUMAN, RAE1_HUMAN, PGTB2_HUMAN, NPTX2_HUMAN, NPTX1_HUMAN, NPTXR_HUMAN, 5HT3A_HUMAN, ASGR1_HUMAN, JIP3_HUMAN, EPHA5_HUMAN, BCL3_HUMAN, THYG_HUMAN, UCP2_HUMAN, UCP3_HUMAN, CXB2_HUMAN, PPARA_HUMAN, PO2F2_HUMAN, 1A01_HUMAN.1A02_HUMAN.1A03_HUMAN.1A11_HUMAN.1A23_HUMAN.1A24_HUMAN.1A25_HUMAN.1A26_HUMAN.1A29_HUMAN.1A30_HUMAN.1A31_HUMAN.1A32_HUMAN.1A33_HUMAN.1A34_HUMAN.1A36_HUMAN.1A43_HUMAN.1A66_HUMAN.1A68_HUMAN.1A69_HUMAN.1A74_HUMAN.1A80_HUMAN, GGA2_HUMAN, CHD1_HUMAN, DRA_HUMAN, SIX1_HUMAN, RPB4_HUMAN, DUT_HUMAN, KIF1A_HUMAN, ANF_HUMAN, IGHD_HUMAN, CP110_HUMAN, ACBP_HUMAN, PGFRA_HUMAN, MERL_HUMAN, E41L1_HUMAN, FLII_HUMAN, AMRP_HUMAN, TRPC3_HUMAN, CABP1_HUMAN, HOME1_HUMAN, WT1_HUMAN, TNF11_HUMAN, CMTA2_HUMAN, ANR11_HUMAN, PTHR_HUMAN, ACHB4_HUMAN, PGS1_HUMAN, AP1G1_HUMAN, E2F6_HUMAN, SDC2_HUMAN, RSU1_HUMAN, RAP2A_HUMAN, ODPX_HUMAN, PDLI5_HUMAN, SCNAA_HUMAN, MMP2_HUMAN, S1PR1_HUMAN, CD5_HUMAN, MYLK_HUMAN, M4K5_HUMAN, TRAIP_HUMAN, SEPT4_HUMAN, SYT11_HUMAN, PTPRH_HUMAN, CD28_HUMAN, DQB1_HUMAN, FGF3_HUMAN, CXA1_HUMAN, FGF7_HUMAN, RRBP1_HUMAN, ARH_HUMAN, GCM1_HUMAN, NECA3_HUMAN, PGS2_HUMAN, NMT1_HUMAN, TAZ_HUMAN, LPH_HUMAN, ARNT_HUMAN, ELNE_HUMAN, KPCG_HUMAN, QCR6_HUMAN, TLN2_HUMAN, GNAI1_HUMAN, APRIO_HUMAN.PRIO_HUMAN, SSH2_HUMAN, MTG8_HUMAN, FANCG_HUMAN, CNTF_HUMAN, ID3_HUMAN, PO4F1_HUMAN, RORG_HUMAN, MINK1_HUMAN, HABP2_HUMAN, CKLF3_HUMAN, BLNK_HUMAN, SYNJ1_HUMAN, PAK3_HUMAN, FUT1_HUMAN, SIAT1_HUMAN, B4DSX9_HUMAN.CEL_HUMAN, GNB1L_HUMAN, MIS12_HUMAN, DSN1_HUMAN, CENPJ_HUMAN, AT2A1_HUMAN, CRYAA_HUMAN, NEP_HUMAN, GRM5_HUMAN, S4A7_HUMAN, CO1A1_HUMAN, TF2H4_HUMAN, GORS1_HUMAN, BTBD2_HUMAN, NFH_HUMAN, NMDZ1_HUMAN, BOK_HUMAN, MARH4_HUMAN, TBX5_HUMAN, ALBU_HUMAN, FA12_HUMAN, MCH_HUMAN, TSYL2_HUMAN, HXK2_HUMAN, CDC45_HUMAN, RN115_HUMAN, MAP6_HUMAN, TPIP1_HUMAN, LOX5_HUMAN, CDX2_HUMAN, TMOD1_HUMAN, FLI1_HUMAN, PLK3_HUMAN, SAA1_HUMAN, IL13_HUMAN, ETS2_HUMAN, CTCF_HUMAN, HCK_HUMAN, EPB42_HUMAN, NB5R1_HUMAN, MRP2_HUMAN, FSHR_HUMAN, FZR1_HUMAN, CD47_HUMAN, GUC1A_HUMAN, GUC2D_HUMAN, HXC4_HUMAN, GRIA1_HUMAN, CD11A_HUMAN, ICAM4_HUMAN, MEF2D_HUMAN, CD5R2_HUMAN, IBP3_HUMAN, PEX5R_HUMAN, SYCC_HUMAN, TMF1_HUMAN, MATN2_HUMAN, TOPRS_HUMAN, CRX_HUMAN, ATP23_HUMAN, PTTG1_HUMAN, CD1D_HUMAN, HXB6_HUMAN, FAK2_HUMAN, ACVR1_HUMAN, DPA1_HUMAN, TFE2_HUMAN, LMOD1_HUMAN, TAF7_HUMAN, I17RB_HUMAN, GNA15_HUMAN, GNA11_HUMAN, DPOE1_HUMAN, HELB_HUMAN, IKZF4_HUMAN, PARD3_HUMAN, ZNT9_HUMAN, PKHA8_HUMAN, AP3B1_HUMAN, CCL22_HUMAN, EPHA8_HUMAN, NFYA_HUMAN, CLIC5_HUMAN, ECT2_HUMAN, DCP2_HUMAN, DCP1B_HUMAN, TOIP1_HUMAN, URB2_HUMAN, BTBD1_HUMAN, CDC7_HUMAN, CATG_HUMAN, PCY1A_HUMAN, MEX3D_HUMAN, EDC4_HUMAN, HIRA_HUMAN, DOC2B_HUMAN, MS4A3_HUMAN, EDNRB_HUMAN, NEUR3_HUMAN, AKAP1_HUMAN, STML3_HUMAN, ANKR2_HUMAN, PTPRC_HUMAN, TAF1_HUMAN, EHMT1_HUMAN, TFDP1_HUMAN, CCNT1_HUMAN, RBNS5_HUMAN, SRP54_HUMAN, EXC6B_HUMAN, RRAS_HUMAN, PFD4_HUMAN, NCALD_HUMAN, KDM5A_HUMAN, RO60_HUMAN, COX42_HUMAN, FBLN1_HUMAN, RAC2_HUMAN, SYBU_HUMAN, CD11B_HUMAN, RGRF1_HUMAN, PSMF1_HUMAN, CAP1_HUMAN, TBL1X_HUMAN, UHRF1_HUMAN, MED8_HUMAN, DPOE2_HUMAN, DC1I1_HUMAN, PCSK7_HUMAN, THA_HUMAN, AMPH_HUMAN, HMGA2_HUMAN, MEF2A_HUMAN, ABCA4_HUMAN, SH2B1_HUMAN, LIPS_HUMAN, TRI26_HUMAN, ASIC2_HUMAN, DNM3A_HUMAN, GNA12_HUMAN, VISL1_HUMAN, DSRAD_HUMAN, KIT_HUMAN, AP3B2_HUMAN, IRF5_HUMAN, HNF4A_HUMAN, SSH3_HUMAN, CNN2_HUMAN, CD38_HUMAN, IFNB_HUMAN, UBA7_HUMAN, PK3CG_HUMAN, MYH4_HUMAN, RCN3_HUMAN, UCP1_HUMAN, PLM_HUMAN, ATNG_HUMAN, ADCY2_HUMAN, APBA2_HUMAN, LASP1_HUMAN, TIAM1_HUMAN, DNJB2_HUMAN, TRFE_HUMAN, SNTA1_HUMAN, INADL_HUMAN, AHR_HUMAN, WASF2_HUMAN, SATB1_HUMAN, EPOR_HUMAN, FHIT_HUMAN, ADRO_HUMAN, CD82_HUMAN, CREB5_HUMAN, DPP4_HUMAN, CD2_HUMAN, GNA13_HUMAN, PK3CB_HUMAN, NMDE4_HUMAN, MYL1_HUMAN, TOB1_HUMAN, PI51A_HUMAN, CREM_HUMAN, GRK6_HUMAN, NAC2_HUMAN, NAC1_HUMAN, NAC3_HUMAN, WIPI1_HUMAN, PTPRE_HUMAN, EDAR_HUMAN, TNFL4_HUMAN, CASP_HUMAN.CUX1_HUMAN, NEB2_HUMAN, TNR25_HUMAN, TNS2_HUMAN, AKA12_HUMAN, PLCG2_HUMAN, OCLN_HUMAN, ASIC1_HUMAN, VAMP3_HUMAN, NHRF3_HUMAN, TAP1_HUMAN, NFM_HUMAN, CTDP1_HUMAN, COR1A_HUMAN, MNDA_HUMAN, TBCB_HUMAN, MAP1A_HUMAN, RHG01_HUMAN, CDK20_HUMAN, DNLI4_HUMAN, KCNJ9_HUMAN, CD8A_HUMAN, FGFR4_HUMAN, TYK2_HUMAN, COX2_HUMAN, COX3_HUMAN, TXK_HUMAN, PHOS_HUMAN, RFX4_HUMAN, SCAFB_HUMAN, U2AFM_HUMAN, GTF2I_HUMAN, TNNI2_HUMAN, RAB9A_HUMAN, PLMN_HUMAN, HPF1_HUMAN, RT31_HUMAN, SEPT3_HUMAN, WFS1_HUMAN, B4GT1_HUMAN, SAA4_HUMAN, CAC1C_HUMAN, TRAF7_HUMAN, KCAB2_HUMAN, WASF3_HUMAN, MYO5A_HUMAN, CAH2_HUMAN, FOG2_HUMAN, CSF1_HUMAN, 5HT1F_HUMAN, TM189_HUMAN.UB2V1_HUMAN, TDG_HUMAN, ADRB3_HUMAN, CUL4B_HUMAN, BST1_HUMAN, G3ST4_HUMAN, FCG2B_HUMAN.FCG2C_HUMAN, NCOA7_HUMAN, AFAP1_HUMAN, DCE1_HUMAN, TOM6_HUMAN, TOM5_HUMAN, SYVM_HUMAN, PLIN2_HUMAN, PPARD_HUMAN, HAIR_HUMAN, RNF12_HUMAN, LIFR_HUMAN, TRIP4_HUMAN, MY18B_HUMAN, TRM7_HUMAN, VAMP8_HUMAN, CALD1_HUMAN, GRM3_HUMAN, ASIC3_HUMAN, ABRA_HUMAN, MAFA_HUMAN, GBRR1_HUMAN, GP2_HUMAN, STK26_HUMAN, PTN13_HUMAN, SCNNG_HUMAN, ONCM_HUMAN, TNNT2_HUMAN, VTCN1_HUMAN, COPA1_HUMAN, MED17_HUMAN, SH2D3_HUMAN, NP1L4_HUMAN, EDEM1_HUMAN, CPT1A_HUMAN, CAH8_HUMAN, CAN1_HUMAN, RYK_HUMAN, RAB3A_HUMAN, GABR1_HUMAN, ERR1_HUMAN, NR0B1_HUMAN, KPCD3_HUMAN, BRCA2_HUMAN, NCF4_HUMAN, IPRI_HUMAN, JARD2_HUMAN, ENAH_HUMAN, LTK_HUMAN, INGR1_HUMAN, CXA3_HUMAN, UD2B7_HUMAN, CD99_HUMAN, NACAM_HUMAN.NACA_HUMAN, HIP1R_HUMAN, SUFU_HUMAN, RK_HUMAN, PIN4_HUMAN, COPG2_HUMAN, ARRC_HUMAN, CLCB_HUMAN, UTF1_HUMAN, CCDC6_HUMAN, STMN2_HUMAN, CNRG_HUMAN, DUS10_HUMAN, OBF1_HUMAN, NPAT_HUMAN, TAOK2_HUMAN, KCNA2_HUMAN, NDOR1_HUMAN, NUMBL_HUMAN, NKX21_HUMAN, KLOT_HUMAN, REXO4_HUMAN, KS6C1_HUMAN, CCNF_HUMAN, ITA5_HUMAN, DDX54_HUMAN, SNP23_HUMAN, COT2_HUMAN, SH2B2_HUMAN, RBX2_HUMAN, SNTG1_HUMAN, PHLD_HUMAN, DLG2_HUMAN, FBLN2_HUMAN, EFNA3_HUMAN, P2RX7_HUMAN, NUP98_HUMAN, MBTP1_HUMAN, DPOD2_HUMAN, BAZ1B_HUMAN, CSKP_HUMAN, CD9_HUMAN, RET4_HUMAN, STAT2_HUMAN, MUTYH_HUMAN, PIM1_HUMAN, NOV_HUMAN, RPGR_HUMAN, ADAM2_HUMAN, BET1L_HUMAN, TYDP1_HUMAN, PAI2B_HUMAN, DLG3_HUMAN, ADA2C_HUMAN, NR2C2_HUMAN, EMIL1_HUMAN, NOL3_HUMAN, ARFP1_HUMAN, TANC1_HUMAN, AR2BP_HUMAN, ARL2_HUMAN, DEFB1_HUMAN, FIBP_HUMAN, ANK2_HUMAN, KNG1_HUMAN, DQA2_HUMAN, PI4KA_HUMAN, LYAM1_HUMAN, GNA14_HUMAN, NOSIP_HUMAN, LSHR_HUMAN, V2R_HUMAN, RBM23_HUMAN, ERD21_HUMAN, RYR2_HUMAN, CD63_HUMAN, CCG2_HUMAN, EXOC8_HUMAN, EXOC5_HUMAN, ULA1_HUMAN, ZEP3_HUMAN, BFAR_HUMAN, BNIPL_HUMAN, PICAL_HUMAN, PITM1_HUMAN, FGF17_HUMAN, FGF9_HUMAN, FGF18_HUMAN, ADA2A_HUMAN, GPI8_HUMAN, DNAS1_HUMAN, PLTP_HUMAN, MAGA4_HUMAN, IL2RA_HUMAN, MMP9_HUMAN, GEPH_HUMAN, BLK_HUMAN, SYCY1_HUMAN, SATT_HUMAN, HAND2_HUMAN, GABT_HUMAN, A2IXV5_HUMAN.LIRB2_HUMAN, LIRB1_HUMAN, KLRD1_HUMAN, KI3S1_HUMAN, KI3L1_HUMAN, GRIA2_HUMAN, NHRF4_HUMAN, MPRD_HUMAN, FCG3A_HUMAN, TDIF2_HUMAN, BGH3_HUMAN, HSPB8_HUMAN, HS71A_HUMAN, KCJ10_HUMAN, AQP4_HUMAN, HECAM_HUMAN, S1PR5_HUMAN, S1PR2_HUMAN, DTBP1_HUMAN, CHDH_HUMAN, GIT1_HUMAN, S1PR3_HUMAN, PKD1_HUMAN, PEN2_HUMAN, APH1A_HUMAN, TWST1_HUMAN, LARP1_HUMAN, RYDEN_HUMAN, FGF21_HUMAN, RN170_HUMAN, MYCD_HUMAN, DEAF1_HUMAN, DNJC7_HUMAN, DNJC3_HUMAN, SGCE_HUMAN, DAG1_HUMAN, PLXA4_HUMAN, ESPL1_HUMAN, Q59EJ3_HUMAN, TIM44_HUMAN, GRPE2_HUMAN, MRP_HUMAN, HMMR_HUMAN, DTNA_HUMAN, KCMA1_HUMAN, 3BHS2_HUMAN, MOV10_HUMAN, CABIN_HUMAN, UBN1_HUMAN, NDUA2_HUMAN, NU1M_HUMAN, NDUS7_HUMAN, ACH10_HUMAN, ACHA9_HUMAN, PKHM2_HUMAN, S35A3_HUMAN, S35A2_HUMAN, MIC10_HUMAN, NDUA1_HUMAN, EHMT2_HUMAN, MIP18_HUMAN, PLRG1_HUMAN, ORC6_HUMAN, ORC4_HUMAN, ORC3_HUMAN, MB3L1_HUMAN, MTREX_HUMAN, RBM25_HUMAN, NELFD_HUMAN, DNPEP_HUMAN, TCAL1_HUMAN, STRP1_HUMAN, CATIN_HUMAN, EIF1B_HUMAN, HBG1_HUMAN, CENPC_HUMAN, HDA10_HUMAN, HDAC8_HUMAN, MED9_HUMAN, MED28_HUMAN, MED26_HUMAN, SNX5_HUMAN, CSTN1_HUMAN, PI5L1_HUMAN, MYPN_HUMAN, TRPC5_HUMAN, TRPC6_HUMAN, CLK1_HUMAN, RASE_HUMAN, LIPL_HUMAN, GCYB1_HUMAN, ACTH_HUMAN, KPB2_HUMAN, NOP2_HUMAN, MBD2_HUMAN, IKZF2_HUMAN, MGMT_HUMAN, AP3S2_HUMAN, EHD1_HUMAN, HXD4_HUMAN, DLX2_HUMAN, MYPT2_HUMAN, KCNA1_HUMAN, CUL4A_HUMAN, EIF3C_HUMAN, EIF3J_HUMAN, RRN3_HUMAN, VWF_HUMAN, CTTB2_HUMAN, AP2A2_HUMAN, UB2J1_HUMAN, SYN2_HUMAN, AVEN_HUMAN, MOT5_HUMAN, EPHA3_HUMAN, RPC4_HUMAN, LYST_HUMAN, MED14_HUMAN, MED16_HUMAN, MED6_HUMAN, MED7_HUMAN, MED13_HUMAN, UBP3_HUMAN, YAF2_HUMAN, PCGF6_HUMAN, ARF_HUMAN.CDN2A_HUMAN, MED30_HUMAN, SVIP_HUMAN, TIM14_HUMAN, UBP36_HUMAN, WDR48_HUMAN, UBP1_HUMAN, UBP49_HUMAN, BABA1_HUMAN, BABA2_HUMAN, RAE1L_HUMAN, TF2AA_HUMAN, NTPCR_HUMAN, GPN1_HUMAN, RPAP1_HUMAN, RPB11_HUMAN, RPC8_HUMAN, SORCN_HUMAN, BSCL2_HUMAN, PACN2_HUMAN, ALK_HUMAN, CLN3_HUMAN, TM160_HUMAN, AAKG2_HUMAN, PEO1_HUMAN, ABHDA_HUMAN, CEP78_HUMAN, DIP2B_HUMAN, AINX_HUMAN, ASPH_HUMAN, GSLG1_HUMAN, RM38_HUMAN, TF3C3_HUMAN, GOGA3_HUMAN, UBA5_HUMAN, BORG1_HUMAN, C42S1_HUMAN, RHG15_HUMAN, CREST_HUMAN, ARHG4_HUMAN, LRMP_HUMAN, TENS1_HUMAN, RIPR2_HUMAN, MPP9_HUMAN, SYNPO_HUMAN, FHOD1_HUMAN, SYNP2_HUMAN, ST65G_HUMAN, DDB2_HUMAN, DPY30_HUMAN, APTX_HUMAN, SMD3_HUMAN, LBN_HUMAN, XPC_HUMAN, NR4A2_HUMAN, MCPH1_HUMAN, RPC1_HUMAN, E2F8_HUMAN, ZN383_HUMAN, ALX4_HUMAN, HXC11_HUMAN, MAFF_HUMAN, ZN490_HUMAN, CHD6_HUMAN, CDCA2_HUMAN, SETMR_HUMAN, MSH3_HUMAN, PAF1_HUMAN, MEN1_HUMAN, H2A2C_HUMAN, ZN461_HUMAN, MYSM1_HUMAN, NAB2_HUMAN, NAB1_HUMAN, AHRR_HUMAN, SMRD2_HUMAN, NU214_HUMAN, PDX1_HUMAN, ANM3_HUMAN, TAF1A_HUMAN, TAF1B_HUMAN, TAF6_HUMAN, NUCG_HUMAN, BC11A_HUMAN, ZMIZ2_HUMAN, GEMI_HUMAN, NGN2_HUMAN, NDF1_HUMAN, PHF1_HUMAN, TBX3_HUMAN, S2A4R_HUMAN, SRY_HUMAN, ERCC6_HUMAN.ERPG3_HUMAN, MKL1_HUMAN, CENPE_HUMAN, CTBL1_HUMAN, FAN1_HUMAN, BLID_HUMAN, APC1_HUMAN, CDC16_HUMAN, BCORL_HUMAN, KAT6A_HUMAN, KLF6_HUMAN, SP130_HUMAN, LSM8_HUMAN, LSM2_HUMAN, ZRAB2_HUMAN, SAMN1_HUMAN, KMT2E_HUMAN, DOT1L_HUMAN, ZEB1_HUMAN, EXO1_HUMAN, ZN382_HUMAN, RL18_HUMAN, RS4X_HUMAN, RBBP6_HUMAN, ZNF10_HUMAN, ZN496_HUMAN, HIC1_HUMAN, WDR82_HUMAN, TAD2A_HUMAN, SELS_HUMAN, ANS1B_HUMAN, ANS1A_HUMAN, UBTD2_HUMAN, H2AZ_HUMAN, GCP5_HUMAN, MYH1_HUMAN, RFC3_HUMAN, RFC2_HUMAN, PURA_HUMAN, METH_HUMAN, DHCR7_HUMAN, CBSL_HUMAN.CBS_HUMAN, ALDOC_HUMAN, PYGL_HUMAN, SERC_HUMAN, MAEA_HUMAN, RIMKB_HUMAN, PPAL_HUMAN, PUR8_HUMAN, PPIH_HUMAN, EXOS2_HUMAN, HNRPR_HUMAN, RBM3_HUMAN, DDX18_HUMAN, G3BP2_HUMAN, TXNL1_HUMAN, ZEP1_HUMAN, RT07_HUMAN, RL9_HUMAN, RT22_HUMAN, RT35_HUMAN, RM27_HUMAN, NUP37_HUMAN, SYFA_HUMAN, APC7_HUMAN, UBR2_HUMAN, RN213_HUMAN, GRWD1_HUMAN, ABRX1_HUMAN, PDE12_HUMAN, CJ090_HUMAN, MIB1_HUMAN, MARC1_HUMAN, DCAF5_HUMAN, PP6R1_HUMAN, TROP_HUMAN, RPAC1_HUMAN, RBM12_HUMAN, MLF2_HUMAN, BACD3_HUMAN, UBR4_HUMAN, RNF25_HUMAN, UBE2T_HUMAN, AGO3_HUMAN, ZNRF4_HUMAN, IN80C_HUMAN, NFRKB_HUMAN, ARP8_HUMAN, IN80D_HUMAN, BAZ1A_HUMAN, CHRC1_HUMAN, DPOE3_HUMAN, ARI4A_HUMAN, ACADV_HUMAN, ACOT9_HUMAN, AFG32_HUMAN, AL1L2_HUMAN, AASS_HUMAN, ABCB7_HUMAN, CPT2_HUMAN, HDHD5_HUMAN, GTPBA_HUMAN, CLPX_HUMAN, MMAB_HUMAN, MCU_HUMAN, CHCH1_HUMAN, DDX28_HUMAN, PDIP2_HUMAN, ECI1_HUMAN, ERAL1_HUMAN, FAD1_HUMAN, MTG1_HUMAN, SYHM_HUMAN, MASU1_HUMAN, CF203_HUMAN, MAOM_HUMAN, MCCB_HUMAN, MUTA_HUMAN, LONM_HUMAN, FABD_HUMAN, MPPB_HUMAN, RM17_HUMAN, RM18_HUMAN, RM02_HUMAN, RM23_HUMAN, RM24_HUMAN, RM32_HUMAN, RM39_HUMAN, RM04_HUMAN, RM41_HUMAN, A0A087WU62_HUMAN.RM45_HUMAN, RM48_HUMAN, RM50_HUMAN, RM51_HUMAN, RM54_HUMAN, RM55_HUMAN, RM09_HUMAN, RT11_HUMAN, RT15_HUMAN, RT16_HUMAN, RT17_HUMAN, RT02_HUMAN, RT21_HUMAN, RT23_HUMAN, RT25_HUMAN, RT26_HUMAN, RT28_HUMAN, RT30_HUMAN, RT34_HUMAN, RT05_HUMAN, RRFM_HUMAN, MRM1_HUMAN, MTEF1_HUMAN, MTEF4_HUMAN, AGK_HUMAN, NDKM_HUMAN, PTCD3_HUMAN, MPPA_HUMAN, SYPM_HUMAN, TRUA_HUMAN, P5CS_HUMAN, SYSM_HUMAN, GHC2_HUMAN, CMC1_HUMAN, SUCB1_HUMAN, SUV3_HUMAN, SYTM_HUMAN, SYYM_HUMAN, ISCA1_HUMAN, YMEL1_HUMAN, AGO4_HUMAN, ANXA6_HUMAN, RSSA_HUMAN, DGCR8_HUMAN, TLR9_HUMAN, KPCD2_HUMAN, H2B1K_HUMAN, PRP39_HUMAN, NEUR1_HUMAN, XPOT_HUMAN, EIF3L_HUMAN, NDKA_HUMAN, DJB11_HUMAN, NFS1_HUMAN, HNRLL_HUMAN, DDX47_HUMAN, RBMX_HUMAN, ABRX2_HUMAN, IL17_HUMAN, HERC2_HUMAN, MMS22_HUMAN, MBB1A_HUMAN, PWP1_HUMAN, BRX1_HUMAN, RL8_HUMAN, RL15_HUMAN, RL27A_HUMAN, RNF13_HUMAN, PNMA2_HUMAN, CYFP1_HUMAN, CYFP2_HUMAN, PAR6G_HUMAN, ZWINT_HUMAN, LST2_HUMAN, ATX3L_HUMAN, SHQ1_HUMAN, 2B11_HUMAN.2B13_HUMAN.2B14_HUMAN.2B17_HUMAN.2B18_HUMAN.2B19_HUMAN.2B1A_HUMAN.2B1B_HUMAN.2B1C_HUMAN.2B1D_HUMAN.2B1E_HUMAN.2B1F_HUMAN.2B1G_HUMAN, DRB3_HUMAN, DRB4_HUMAN, DRB5_HUMAN, 3BP5_HUMAN, MED25_HUMAN, UN93B_HUMAN, TRI13_HUMAN, DNLZ_HUMAN, SOS2_HUMAN, GLCM_HUMAN, PIDD1_HUMAN, TAF11_HUMAN, REV1_HUMAN, CHD5_HUMAN, P66A_HUMAN, P66B_HUMAN, SMRCD_HUMAN, EZH1_HUMAN, LEO1_HUMAN, CND1_HUMAN, CND3_HUMAN, CND2_HUMAN, KDM5B_HUMAN, H2AB1_HUMAN, ZNF8_HUMAN, TRAT1_HUMAN, UFD1_HUMAN, EPIPL_HUMAN, TBA1C_HUMAN, FLNB_HUMAN, MDN1_HUMAN, RRP12_HUMAN, BMS1_HUMAN, SON_HUMAN, NVL_HUMAN, MYH14_HUMAN, CEBPZ_HUMAN, ZFR_HUMAN, SMHD1_HUMAN, TF3C1_HUMAN, YLPM1_HUMAN, ACACA_HUMAN, SUGP2_HUMAN, WDR3_HUMAN, NOL6_HUMAN, PWP2_HUMAN, ZN638_HUMAN, ANKH1_HUMAN, PUM3_HUMAN, MINT_HUMAN, MK67I_HUMAN, ZCCHV_HUMAN, WDR75_HUMAN, SR140_HUMAN, NKRF_HUMAN, NOP14_HUMAN, CPSF1_HUMAN, HELZ2_HUMAN, NOC3L_HUMAN, ANR17_HUMAN, KMT2A_HUMAN, WDR43_HUMAN, RAI1_HUMAN, ZN512_HUMAN, CUL9_HUMAN, THOC2_HUMAN, MTMR5_HUMAN, MPP10_HUMAN, NSUN2_HUMAN, PLSL_HUMAN, NOG2_HUMAN, ZN318_HUMAN, RBM15_HUMAN, DDX31_HUMAN, UTP6_HUMAN, ECM29_HUMAN, PP6R3_HUMAN, UTP18_HUMAN, WDR12_HUMAN, SMU1_HUMAN, NUP88_HUMAN, OASL_HUMAN, UTP4_HUMAN, UTP15_HUMAN, POP1_HUMAN, C1TM_HUMAN, DHX8_HUMAN, SRSF5_HUMAN, NU188_HUMAN, TB182_HUMAN, RBM34_HUMAN, RRS1_HUMAN, UBP47_HUMAN, ACSL3_HUMAN, NOL10_HUMAN, AATF_HUMAN, PLOD1_HUMAN, GANP_HUMAN, RRP1_HUMAN, ESF1_HUMAN, CCD86_HUMAN, RS26_HUMAN, STAG2_HUMAN, RCL1_HUMAN, CENPF_HUMAN, DCA13_HUMAN, NSA2_HUMAN, NOP53_HUMAN, AQR_HUMAN, ARF3_HUMAN, CUL7_HUMAN, DIDO1_HUMAN, NOL9_HUMAN, PHRF1_HUMAN, INT1_HUMAN, RS24_HUMAN, CRNL1_HUMAN, DDX46_HUMAN, RPF2_HUMAN, DIEXF_HUMAN, MYO1D_HUMAN, CPSF3_HUMAN, SKIV2_HUMAN, MAK16_HUMAN, RRP8_HUMAN, ABCE1_HUMAN, RBM6_HUMAN, PDIP3_HUMAN, SYIM_HUMAN, ZBT11_HUMAN, ZCHC8_HUMAN, WDR6_HUMAN, DDX51_HUMAN, NNTM_HUMAN, PDS5B_HUMAN, TTF1_HUMAN, KIF4A_HUMAN, ANX11_HUMAN, XPO7_HUMAN, TAF2_HUMAN, CCND3_HUMAN, SETD7_HUMAN, CHFR_HUMAN, UBE3C_HUMAN, AUP1_HUMAN, DCR1A_HUMAN, KDM6A_HUMAN, RPGF3_HUMAN, SLD5_HUMAN, UBP10_HUMAN, PTCRA_HUMAN, KI26B_HUMAN, UBXN4_HUMAN, UB2Q2_HUMAN, SCNNB_HUMAN, DCAF1_HUMAN, ELOB_HUMAN, TDRD3_HUMAN, HAKAI_HUMAN, ERLEC_HUMAN, DPH1_HUMAN, RN182_HUMAN, CSN7A_HUMAN, NFX1_HUMAN, ZNRF2_HUMAN, ZNRF1_HUMAN, KLHL7_HUMAN, SNAG_HUMAN, CCNG1_HUMAN, TRI50_HUMAN, TFAP4_HUMAN, CUL5_HUMAN, KPRP_HUMAN, DPYL2_HUMAN, PODXL_HUMAN, ARF4_HUMAN, CYTA_HUMAN, HBB_HUMAN, RABP1_HUMAN, LEG7_HUMAN, ANXA5_HUMAN, CP2S1_HUMAN, RL10L_HUMAN, IDHC_HUMAN, RABP2_HUMAN, DHRS1_HUMAN, COQ6_HUMAN, RB11B_HUMAN, BACH_HUMAN, NACA2_HUMAN, AKIP_HUMAN, VPS39_HUMAN, RUXE_HUMAN, IF5A2_HUMAN, AT2A3_HUMAN, DCNL1_HUMAN, SLX4_HUMAN, VCIP1_HUMAN, UB2J2_HUMAN, PSMD5_HUMAN, TRI36_HUMAN, ARI2_HUMAN, PTN14_HUMAN, HERC5_HUMAN, NLRC3_HUMAN, CNOT6_HUMAN, UB2E3_HUMAN, HERC4_HUMAN, KCND3_HUMAN, TR19L_HUMAN, BACD2_HUMAN, RFPLA_HUMAN, IBTK_HUMAN, ICK_HUMAN, KCNRG_HUMAN, TR13C_HUMAN, EGF_HUMAN, MEX3A_HUMAN, ATX1L_HUMAN, BIG3_HUMAN, UIF_HUMAN, LMAN1_HUMAN, TRIM5_HUMAN, SCFD1_HUMAN, AKAP8_HUMAN, ARPC4_HUMAN, ARPC5_HUMAN, CAZA2_HUMAN, DREB_HUMAN, MPC2_HUMAN, EFHD2_HUMAN, HINFP_HUMAN, PAR10_HUMAN, NHS_HUMAN, ACHA5_HUMAN, NF2IP_HUMAN, ZN131_HUMAN, SNAI2_HUMAN, SC6A2_HUMAN, CY24B_HUMAN, FBX6_HUMAN, ELK3_HUMAN, LSM4_HUMAN, TRI32_HUMAN, TBD_HUMAN, ENSA_HUMAN, BDH2_HUMAN, ARP19_HUMAN, PLK2_HUMAN, NSE1_HUMAN, RN151_HUMAN, MIRO2_HUMAN, MZT2A_HUMAN, SOX5_HUMAN, RITA1_HUMAN, OAS2_HUMAN, DCLK1_HUMAN, DDRGK_HUMAN, PCIF1_HUMAN, SPXN_HUMAN, CHKA_HUMAN, AAMDC_HUMAN, BEND5_HUMAN, ITBP1_HUMAN, TSSK2_HUMAN, NC2A_HUMAN, SKA3_HUMAN, GAS2_HUMAN, HEM3_HUMAN, CN093_HUMAN, LETM2_HUMAN, LMX1B_HUMAN, SRSF8_HUMAN, ABR_HUMAN, SETD3_HUMAN, HBAZ_HUMAN, SRR_HUMAN, MYOZ1_HUMAN, KANL2_HUMAN, HMCS2_HUMAN, SP14L_HUMAN, RLBP1_HUMAN, SYWC_HUMAN, EXOS3_HUMAN, HELLS_HUMAN, DNJC4_HUMAN, TICRR_HUMAN, CINP_HUMAN, GNAZ_HUMAN, SULF1_HUMAN, GPAT1_HUMAN, CCZ1B_HUMAN.CCZ1_HUMAN, TFPI1_HUMAN, AGFG1_HUMAN, DECR2_HUMAN, CPEB1_HUMAN, WASL_HUMAN, KIFC1_HUMAN, DAPLE_HUMAN, SSR2_HUMAN, RL37_HUMAN, LTMD1_HUMAN, EFS_HUMAN, EI2BB_HUMAN, CV046_HUMAN, LIN7A_HUMAN, VPS41_HUMAN, SO2B1_HUMAN, SYMM_HUMAN, PLBL1_HUMAN, PCKGM_HUMAN, COLI_HUMAN, IL26_HUMAN, IGS10_HUMAN, HXC6_HUMAN, PPR17_HUMAN, GRP2_HUMAN, VMA5A_HUMAN, GNAT2_HUMAN, T53G1_HUMAN, FA50A_HUMAN, RASA3_HUMAN, BHMT2_HUMAN, RIT2_HUMAN, IFT81_HUMAN, TXND5_HUMAN, FRMD8_HUMAN, NPL_HUMAN, RM53_HUMAN, F19A4_HUMAN, MTMRE_HUMAN, BORG4_HUMAN, RUFY3_HUMAN, CK045_HUMAN, PAI2_HUMAN, MOBP_HUMAN, NOVA1_HUMAN, IRF2_HUMAN, RHG17_HUMAN, VPS29_HUMAN, S10AG_HUMAN, LIPT_HUMAN, ASB6_HUMAN, MB12A_HUMAN, EOGT_HUMAN, IGHM_HUMAN, MICU1_HUMAN, RL3L_HUMAN, PRIC2_HUMAN, CXL16_HUMAN, PTBP3_HUMAN, CLUA1_HUMAN, PHLA1_HUMAN, HM20B_HUMAN, MCFD2_HUMAN, SCAM3_HUMAN, STRP2_HUMAN, NOE3_HUMAN, CD36_HUMAN, PIBF1_HUMAN, CENPT_HUMAN, RAB43_HUMAN, LFA3_HUMAN, AAK1_HUMAN, FMNL2_HUMAN, GALE_HUMAN, PARVG_HUMAN, URP2_HUMAN, SYWM_HUMAN, ES1_HUMAN, LFNG_HUMAN, KCMB2_HUMAN, TEAN2_HUMAN, I23O1_HUMAN, LY86_HUMAN, WIPI3_HUMAN, PD2R_HUMAN, TI17B_HUMAN, DGUOK_HUMAN, TPPC3_HUMAN, FMT_HUMAN, G3ST1_HUMAN, TBX22_HUMAN, EXOS1_HUMAN, RETST_HUMAN, MP17L_HUMAN, RPAB2_HUMAN, SKAP2_HUMAN, GDIR2_HUMAN, GAGE1_HUMAN.GAGE4_HUMAN, PMGT2_HUMAN, DEF6_HUMAN, CERK1_HUMAN, WASH3_HUMAN, PARP3_HUMAN, CEGT_HUMAN, CLASR_HUMAN, RAB7B_HUMAN, SNX21_HUMAN, SRAC1_HUMAN, WIPI4_HUMAN, GRAM4_HUMAN, COL12_HUMAN, PLPP3_HUMAN, FYV1_HUMAN, OPA3_HUMAN, PA24C_HUMAN, NXF2_HUMAN, SPIT2_HUMAN, RNF34_HUMAN, REG1A_HUMAN, PI3R5_HUMAN, CAPSL_HUMAN, MYOTI_HUMAN, CRFR2_HUMAN, SPAG6_HUMAN, FMNL3_HUMAN, VIPR2_HUMAN, KLK7_HUMAN, MTG8R_HUMAN, COE4_HUMAN, SPIC_HUMAN, GSDMB_HUMAN, FERM2_HUMAN, VP37A_HUMAN, P2RX6_HUMAN, G3PT_HUMAN, STN1_HUMAN, SPC24_HUMAN, HRG1_HUMAN, SGMR2_HUMAN, LANC2_HUMAN, PGM1_HUMAN, TBC20_HUMAN, UGGG2_HUMAN, FUCO_HUMAN, CS012_HUMAN, CALI_HUMAN, CP070_HUMAN, NALP2_HUMAN, FP100_HUMAN, IFI6_HUMAN, CRSPL_HUMAN, NGLY1_HUMAN, CAMKV_HUMAN, MEST_HUMAN, PARVA_HUMAN, PTMS_HUMAN, BDH_HUMAN, CXX1_HUMAN.RTL8C_HUMAN, I5P2_HUMAN, DYH14_HUMAN, TSN13_HUMAN, PEX2_HUMAN, DRS7B_HUMAN, RBPJL_HUMAN, CK054_HUMAN, H2B1B_HUMAN, CXXC4_HUMAN.J9JIF5_HUMAN, MARH3_HUMAN, RAB28_HUMAN, ACBG1_HUMAN, RGS18_HUMAN, NNAT_HUMAN, SIA10_HUMAN, FITM1_HUMAN, IIGP5_HUMAN, K0513_HUMAN, COA5_HUMAN, KLK9_HUMAN, WAC_HUMAN, MB212_HUMAN, KTU_HUMAN, KISS1_HUMAN, GLB1L_HUMAN, TLL1_HUMAN, CCD14_HUMAN, RSMN_HUMAN.SNURF_HUMAN, SIX2_HUMAN, CHID1_HUMAN, GGCT_HUMAN, EXOS7_HUMAN, RM52_HUMAN, NDK6_HUMAN, DCXR_HUMAN, RNS11_HUMAN, MYL10_HUMAN, PABP3_HUMAN, TTLL6_HUMAN, LYPA2_HUMAN, ORML3_HUMAN, GLT12_HUMAN, FHR2_HUMAN, KPTN_HUMAN, S17A5_HUMAN, PAR15_HUMAN, WNT4_HUMAN, TAP2_HUMAN, ZEB2_HUMAN, TCAL8_HUMAN, UD110_HUMAN, CXL14_HUMAN, DTD2_HUMAN, PTGIS_HUMAN, GTPB8_HUMAN, ISK6_HUMAN, SCO2_HUMAN, FCERB_HUMAN, RA51C_HUMAN, CCG3_HUMAN, NXPE3_HUMAN, CENPS_HUMAN, OSBL5_HUMAN, RASF3_HUMAN, GTR2_HUMAN, GLUCM_HUMAN, MAG_HUMAN, MOGT3_HUMAN, IOD3_HUMAN, PNPO_HUMAN, RB27A_HUMAN, ZFY16_HUMAN, DRAM1_HUMAN, CMKMT_HUMAN, ACL7A_HUMAN, ARFG3_HUMAN, RAB2B_HUMAN, P2RY2_HUMAN, OCAD2_HUMAN, CNDP1_HUMAN, DIXC1_HUMAN, OLFM4_HUMAN, NEUL_HUMAN, VTNC_HUMAN, ICAM3_HUMAN, SPEG_HUMAN, S22A6_HUMAN, HAUS8_HUMAN, ODFP4_HUMAN, MTND_HUMAN, RAB3D_HUMAN, CEAM6_HUMAN, ETV4_HUMAN, KCIP4_HUMAN, N62CL_HUMAN, PASD1_HUMAN, RS25_HUMAN, BSND_HUMAN, PIGO_HUMAN, LPAR3_HUMAN, CYTT_HUMAN, JTB_HUMAN, MAIP1_HUMAN, EPHB4_HUMAN, PDYN_HUMAN, PLA1A_HUMAN, GALD1_HUMAN, ANGL7_HUMAN, CP2CI_HUMAN, FXL12_HUMAN, PAXI1_HUMAN, ANKH_HUMAN, HTRA1_HUMAN, M1IP1_HUMAN, TYRO3_HUMAN, SMD1_HUMAN, SF3B5_HUMAN, PHF5A_HUMAN, RS21_HUMAN, RS29_HUMAN, NDUAC_HUMAN, NDUS6_HUMAN, NDUBA_HUMAN, NDUB5_HUMAN, NDUB8_HUMAN, PSA7L_HUMAN, NDUBB_HUMAN, SNUT2_HUMAN, CIRBP_HUMAN, RM42_HUMAN, RPB2_HUMAN, RS27L_HUMAN, ODO1_HUMAN, SURF1_HUMAN, SYFB_HUMAN, ZN326_HUMAN, IPO9_HUMAN, VATF_HUMAN, CTR9_HUMAN, RCN1_HUMAN, RLA0L_HUMAN, S23IP_HUMAN, THIK_HUMAN, T126A_HUMAN, SPCS2_HUMAN, NFIA_HUMAN, VPP2_HUMAN, TIM9_HUMAN, NPTN_HUMAN, SOSB1_HUMAN, RM21_HUMAN, UFM1_HUMAN, SRXN1_HUMAN, RHOB_HUMAN, VATH_HUMAN, KYNU_HUMAN, SSU72_HUMAN, MGST3_HUMAN, PREP_HUMAN, TMEM9_HUMAN, NOP16_HUMAN, TBD2A_HUMAN, SUCB2_HUMAN, SAP_HUMAN, TRI56_HUMAN, MTX1_HUMAN, PYRD_HUMAN, PPGB_HUMAN, MPLKI_HUMAN, HNRL2_HUMAN, MPV17_HUMAN, PLOD3_HUMAN, NOTC2_HUMAN, SUCA_HUMAN, TM177_HUMAN, TMED4_HUMAN, TIM10_HUMAN, THY1_HUMAN, ZN593_HUMAN, MTX2_HUMAN, MOGS_HUMAN, LS14A_HUMAN, ST1A1_HUMAN, SMCA1_HUMAN, MI4GD_HUMAN, ABCB6_HUMAN, K2C7_HUMAN, NDUB7_HUMAN, MDHC_HUMAN, RAI3_HUMAN, PPT2_HUMAN, ECE1_HUMAN, SRP09_HUMAN, ZBT8B_HUMAN, GALT2_HUMAN, COX7R_HUMAN, GRHPR_HUMAN, EVPL_HUMAN, K2C3_HUMAN, RS10L_HUMAN, PA24A_HUMAN, DJB12_HUMAN, NUBP2_HUMAN, THTM_HUMAN, MCCA_HUMAN, PATL1_HUMAN, TM9S2_HUMAN, VPP3_HUMAN, QSOX2_HUMAN, ABCB8_HUMAN, HYPK_HUMAN, ZSC18_HUMAN, MIA40_HUMAN, TM9S4_HUMAN, GBG12_HUMAN, B4DDK6_HUMAN.TI23B_HUMAN, XPP1_HUMAN, TMM65_HUMAN, MSLN_HUMAN, VATC1_HUMAN, DAF_HUMAN, THOC1_HUMAN, K1C10_HUMAN, TAGL_HUMAN, ACOX1_HUMAN, TOX4_HUMAN, DD19A_HUMAN, THTR_HUMAN, ANXA3_HUMAN, PTGR1_HUMAN, S26A2_HUMAN, CD123_HUMAN, RUSD4_HUMAN, ABCD1_HUMAN, HEM6_HUMAN, SFXN2_HUMAN, WDR44_HUMAN, FAM3C_HUMAN, UGDH_HUMAN, H2A1D_HUMAN, ODB2_HUMAN, HS902_HUMAN, DHSO_HUMAN, MIC13_HUMAN, FUT8_HUMAN, TXD17_HUMAN, LAMP1_HUMAN, NDUF2_HUMAN, TM256_HUMAN, HS905_HUMAN, K2013_HUMAN, ABCBA_HUMAN, XRCC1_HUMAN, MPI_HUMAN, MSMO1_HUMAN, BASP1_HUMAN, DCTN3_HUMAN, SQOR_HUMAN, SC31A_HUMAN, PCYOX_HUMAN, CA2D1_HUMAN, PM34_HUMAN, PALLD_HUMAN, RM30_HUMAN, TX1B3_HUMAN, ACTBM_HUMAN, IWS1_HUMAN, SPEB_HUMAN, MBNL1_HUMAN, ULK4_HUMAN, REM1_HUMAN, CENPM_HUMAN, CENPN_HUMAN, MYLK2_HUMAN, ARGI1_HUMAN, DSG1_HUMAN, BUD13_HUMAN, EMSA1_HUMAN, RL36L_HUMAN, ALKB7_HUMAN, ARFG2_HUMAN, ARSB_HUMAN, ATP9A_HUMAN, DDX50_HUMAN, DECR_HUMAN, DYH2_HUMAN, GBB4_HUMAN, LYRIC_HUMAN, SAS10_HUMAN, MYL6B_HUMAN, RADI_HUMAN, S10A7_HUMAN, SRA1_HUMAN, VAMP5_HUMAN, ZN251_HUMAN, CSRP2_HUMAN, P5CR1_HUMAN, RSMB_HUMAN, CDC23_HUMAN, PCH2_HUMAN, SNR40_HUMAN, APC10_HUMAN, CPSF4_HUMAN, ANC2_HUMAN, APC4_HUMAN, PDZ11_HUMAN, ZN768_HUMAN, GHC1_HUMAN, APC16_HUMAN, CHAP1_HUMAN, MAML1_HUMAN, R3HD4_HUMAN, ZN716_HUMAN, Z705G_HUMAN, GCP2_HUMAN, THG1_HUMAN, TRHY_HUMAN, SNTB2_HUMAN, SLIT2_HUMAN, RL7L_HUMAN, PTOV1_HUMAN, OR7G3_HUMAN, 5NT1B_HUMAN, MUC16_HUMAN, TRFL_HUMAN, ISX_HUMAN, GFPT2_HUMAN, ECE2_HUMAN, DNS2B_HUMAN, DMBX1_HUMAN, RABE2_HUMAN, CE192_HUMAN, BTD_HUMAN, FBX44_HUMAN, ZN148_HUMAN, DOCK6_HUMAN, PTH1R_HUMAN, MUC5B_HUMAN, BARX1_HUMAN, ADH7_HUMAN, AN30A_HUMAN, CMGA_HUMAN, PPM1D_HUMAN, NDC1_HUMAN, FCL_HUMAN, MTMRD_HUMAN, A0A087WUF1_HUMAN.NBPFC_HUMAN, A0A087WZJ2_HUMAN.NBPFE_HUMAN, A0A075B762_HUMAN.NBPFA_HUMAN, NBPF8_HUMAN, NBPF9_HUMAN.NBPFK_HUMAN, NBPF1_HUMAN, POP5_HUMAN, ELL_HUMAN, TF3B_HUMAN, ZN213_HUMAN, P4HTM_HUMAN, TALD3_HUMAN, CYTSA_HUMAN, CAH9_HUMAN, MARH2_HUMAN, CLN8_HUMAN, USP9Y_HUMAN, UBP48_HUMAN, VKOR1_HUMAN, 2A5B_HUMAN, KCNQ4_HUMAN, SGT1_HUMAN, TYSY_HUMAN, AP2S1_HUMAN, PPIL1_HUMAN, STON2_HUMAN, K22E_HUMAN, DIAP1_HUMAN, RAP2B_HUMAN, MYL4_HUMAN, CD2AP_HUMAN, ZCH10_HUMAN, SSX2_HUMAN, LSR_HUMAN, KIF1B_HUMAN, RFIP1_HUMAN, REEP1_HUMAN, DHE4_HUMAN, GT251_HUMAN, TAF8_HUMAN, TAF3_HUMAN, MCAT_HUMAN, GAGE7_HUMAN.GG12F_HUMAN.GG12G_HUMAN.GG12I_HUMAN, ZBT7B_HUMAN, MET18_HUMAN, ETKMT_HUMAN, K2C6A_HUMAN, FCG2C_HUMAN, FCG2A_HUMAN, ARF5_HUMAN, CBX6_HUMAN, CBX7_HUMAN, RAD_HUMAN, ACSL1_HUMAN, PAAF1_HUMAN, NFYB_HUMAN, NFYC_HUMAN, RAPH1_HUMAN, RHG07_HUMAN, S12A3_HUMAN, OST4_HUMAN, YIPF3_HUMAN, PAF15_HUMAN, CLN5_HUMAN, ACE_HUMAN, BMR1A_HUMAN, HDA11_HUMAN, ENC1_HUMAN, FBXW4_HUMAN, LCAT_HUMAN, CLGN_HUMAN, SV2A_HUMAN, JKAMP_HUMAN, DBNL_HUMAN, G6PD_HUMAN, GALK1_HUMAN, SIAS_HUMAN, NQO1_HUMAN, PGM2_HUMAN, S10AE_HUMAN, SRP19_HUMAN, TPRKB_HUMAN, PLCA_HUMAN, AK1C4_HUMAN, ARK73_HUMAN, AL3B1_HUMAN, ALG1_HUMAN, ANX10_HUMAN, APOP1_HUMAN, ARLY_HUMAN, CU059_HUMAN, AIF1L_HUMAN, CAH3_HUMAN, CLCN5_HUMAN, CMBL_HUMAN, DPH2_HUMAN, DPP10_HUMAN, ELMO1_HUMAN, EVL_HUMAN, FLCN_HUMAN, GFRA1_HUMAN, GPC4_HUMAN, LPAR4_HUMAN, GSKIP_HUMAN, GSTA3_HUMAN, OLA1_HUMAN, 3HAO_HUMAN, IGKC_HUMAN.KVD16_HUMAN, JERKY_HUMAN.Q86XJ5_HUMAN, LSM5_HUMAN, LSP1_HUMAN, TPOR_HUMAN, 5NT3A_HUMAN, PIGV_HUMAN, AAKG3_HUMAN, NECT3_HUMAN, RAPSN_HUMAN, S100G_HUMAN, ADSV_HUMAN, SEM1_HUMAN.SEML_HUMAN, CTR1_HUMAN, SNN_HUMAN, SOAT2_HUMAN, SPY1_HUMAN, SIA7D_HUMAN, STAR7_HUMAN, TRIA1_HUMAN, XPP3_HUMAN, YKT6_HUMAN, BATF_HUMAN, FOSL1_HUMAN, DBP_HUMAN, CEBPE_HUMAN, MYCN_HUMAN, GAPR1_HUMAN, SAMH1_HUMAN, ATP4A_HUMAN, ELOV1_HUMAN, CERS2_HUMAN, ADA1D_HUMAN, TIM8B_HUMAN, ABCF2_HUMAN, SP20H_HUMAN, PHC2_HUMAN, GAMT_HUMAN, SHAN3_HUMAN, DMA_HUMAN.Q31604_HUMAN, A0A0G2JPK4_HUMAN.A1ATR_HUMAN, CDK12_HUMAN, ZA2G_HUMAN, GLPK_HUMAN, OAS1_HUMAN, RPAC2_HUMAN.RPC22_HUMAN, FEM1C_HUMAN, ADIP_HUMAN, HMHA1_HUMAN, PGH1_HUMAN, CELF2_HUMAN, HIPK4_HUMAN, NLK_HUMAN, NAV1_HUMAN, CDN1C_HUMAN, PE2R1_HUMAN, PI2R_HUMAN, DIM1_HUMAN, MSI1H_HUMAN, PKP1_HUMAN, CELF1_HUMAN, PURB_HUMAN, ZN346_HUMAN, SCMC3_HUMAN, SDA1_HUMAN, PP6R2_HUMAN, RASF2_HUMAN, SLMAP_HUMAN, GSDMA_HUMAN, VGF_HUMAN, GPDM_HUMAN, GNT2A_HUMAN, RL26L_HUMAN, PCCA_HUMAN, HNRC1_HUMAN, EF1A3_HUMAN, SCMC1_HUMAN, HEXA_HUMAN, HMGB3_HUMAN, AP3M1_HUMAN, GBP1_HUMAN, ATX10_HUMAN, EI2BG_HUMAN, TLS1_HUMAN, CD37L_HUMAN, CNDP2_HUMAN, FTO_HUMAN, CMYA5_HUMAN, CUTC_HUMAN, DCK_HUMAN, DNMBP_HUMAN, GSHR_HUMAN, TYPH_HUMAN, TFIP8_HUMAN, VPS25_HUMAN, TRI47_HUMAN, PSF3_HUMAN, TF3C4_HUMAN, FKBP9_HUMAN, PLPHP_HUMAN, SHOT1_HUMAN, PHAX_HUMAN, HSP76_HUMAN, PNCB_HUMAN, THOP1_HUMAN, IMDH1_HUMAN, I2BP2_HUMAN, ISOC1_HUMAN, ARP10_HUMAN, MTMR2_HUMAN, COG3_HUMAN, RANB3_HUMAN, COR1B_HUMAN, NIBL1_HUMAN, VP26A_HUMAN, SCOT1_HUMAN, PAPS1_HUMAN, GSHB_HUMAN, PCP_HUMAN, TWF2_HUMAN, AAMP_HUMAN, PLOD2_HUMAN, RPP38_HUMAN, PSME4_HUMAN, SCLY_HUMAN, PUR2_HUMAN, GFPT1_HUMAN, P4R3A_HUMAN, P4R3B_HUMAN, TATD1_HUMAN, TRNT1_HUMAN, TBA4B_HUMAN, GPX1_HUMAN, VAT1_HUMAN, WDR4_HUMAN, RISC_HUMAN, NARR_HUMAN.RAB34_HUMAN, MGRN1_HUMAN, LN28B_HUMAN, ASB8_HUMAN, ZBTB1_HUMAN, ZC12A_HUMAN, NPHN_HUMAN, LGR4_HUMAN, LGMN_HUMAN, KAPCB_HUMAN, CCNJ_HUMAN, RNC_HUMAN, NMD3_HUMAN, LN28A_HUMAN, CORO7_HUMAN, RHOD_HUMAN, CEAM1_HUMAN, GMPR2_HUMAN, RGS8_HUMAN, RGS17_HUMAN, AGRG1_HUMAN, RAP2C_HUMAN, RGS11_HUMAN, RGS9_HUMAN, IL6RA_HUMAN, ADCY3_HUMAN, CD68_HUMAN, KCNE1_HUMAN, VEGFB_HUMAN, GRIA3_HUMAN, RHG05_HUMAN, MUC18_HUMAN, TBX21_HUMAN, LSM6_HUMAN, CBLC_HUMAN, MARH6_HUMAN, GOLI_HUMAN, FOXN2_HUMAN, KI2L4_HUMAN, RBGPR_HUMAN, NACC2_HUMAN, GBRB1_HUMAN, IRS4_HUMAN, OTU7A_HUMAN, ARNT2_HUMAN, CEP76_HUMAN, FOXP2_HUMAN, DPOD4_HUMAN, HAUS2_HUMAN, NEDD1_HUMAN, GCP4_HUMAN, PLPL6_HUMAN, GBB3_HUMAN, TRI68_HUMAN, CD209_HUMAN, DCBD2_HUMAN, PRDM6_HUMAN, EHF_HUMAN, STAR_HUMAN, DTL_HUMAN, PP4R1_HUMAN, RPB9_HUMAN, RPAB5_HUMAN, APC11_HUMAN, TMC8_HUMAN, PCSK9_HUMAN, RPGF2_HUMAN, TTC5_HUMAN, ECHP_HUMAN, FKB1B_HUMAN, MTRR_HUMAN, PAX4_HUMAN, PBX3_HUMAN, KR103_HUMAN, FXL18_HUMAN.Q96D16_HUMAN, ZBT14_HUMAN, ZN473_HUMAN, ZFN2B_HUMAN, FSBP_HUMAN.RA54B_HUMAN, GAG2E_HUMAN.GGE2D_HUMAN, ZN250_HUMAN, MPPE1_HUMAN, SNX20_HUMAN, GAGE7_HUMAN.GG12C_HUMAN, KRA23_HUMAN.KRA24_HUMAN, NIPA_HUMAN, CXB5_HUMAN, INT3_HUMAN, INT7_HUMAN, PHF6_HUMAN, ZFHX4_HUMAN, BAP18_HUMAN, PRAME_HUMAN, CCDC8_HUMAN, ATG4D_HUMAN, TRI18_HUMAN, EMC7_HUMAN, EMC8_HUMAN, EMC1_HUMAN, EMC2_HUMAN, EMC10_HUMAN, CLPT1_HUMAN, EMC4_HUMAN, MCF2_HUMAN, LMTK1_HUMAN, LIN37_HUMAN, MT1E_HUMAN, LIMK2_HUMAN, TNK1_HUMAN, PPT1_HUMAN, NUB1_HUMAN, SEPT8_HUMAN, FBH1_HUMAN, MED27_HUMAN, BCAS3_HUMAN, LAP4B_HUMAN, BMAL1_HUMAN, CRY1_HUMAN, PER1_HUMAN, PER2_HUMAN, CLOCK_HUMAN, Q58EY0_HUMAN.RORB_HUMAN, ADA_HUMAN, F187B_HUMAN, LGAT1_HUMAN, TPST1_HUMAN, 5HT1E_HUMAN, NXF5_HUMAN, POPD2_HUMAN, ACKR3_HUMAN, TSSK1_HUMAN, AA3R_HUMAN, OVCA2_HUMAN, VTI1B_HUMAN, DQA1_HUMAN, KLK11_HUMAN, NXPH3_HUMAN, RBMS3_HUMAN, S2541_HUMAN, CERS6_HUMAN, S19A2_HUMAN, DHRS4_HUMAN, SPI2B_HUMAN, SYNG1_HUMAN, GA2L1_HUMAN, SOCS6_HUMAN, CGBP1_HUMAN, ZGPAT_HUMAN, PAX3_HUMAN, F234B_HUMAN, EI2BD_HUMAN, STX18_HUMAN, STX10_HUMAN, F234A_HUMAN, MSPD2_HUMAN, ANM9_HUMAN, VAMP7_HUMAN, TRAK2_HUMAN, TCPW_HUMAN, INT5_HUMAN, CP062_HUMAN, TARB1_HUMAN, GPD1L_HUMAN, SYLM_HUMAN, FAKD4_HUMAN, PLCE_HUMAN, CC033_HUMAN, DDC_HUMAN, COG2_HUMAN, GNPAT_HUMAN, STEA3_HUMAN, FAKD1_HUMAN, SYEM_HUMAN, FAKD3_HUMAN, KNTC1_HUMAN, COG1_HUMAN, COG4_HUMAN, GCFC2_HUMAN, PARL_HUMAN, KMCP1_HUMAN, RSAD1_HUMAN, GNL3L_HUMAN, VPS53_HUMAN, BTAF1_HUMAN, SNX16_HUMAN, NDUF5_HUMAN, SGCZ_HUMAN, TSN5_HUMAN, T131L_HUMAN, AT12A_HUMAN, ALG9_HUMAN, MANEL_HUMAN, REEP5_HUMAN, LNP_HUMAN, PCD20_HUMAN, F241A_HUMAN, TBB8_HUMAN, FADS2_HUMAN, TMPPE_HUMAN, SEM4C_HUMAN, POMT1_HUMAN, IMPA3_HUMAN, GALT7_HUMAN, SEM4F_HUMAN, RTN2_HUMAN, NRP2_HUMAN, TGBR3_HUMAN, F241B_HUMAN, SEGN_HUMAN, GPN3_HUMAN, ASGR2_HUMAN, CROCC_HUMAN, KLH21_HUMAN, CNTLN_HUMAN, SCLT1_HUMAN, TSAP1_HUMAN, ZMAT3_HUMAN, KLK5_HUMAN, PDRG1_HUMAN, GL1AD_HUMAN.GRL1A_HUMAN.MYZAP_HUMAN, RPC10_HUMAN, ST1A2_HUMAN, SGF29_HUMAN, DR9C7_HUMAN, NGRN_HUMAN, NRG1_HUMAN, LEG8_HUMAN, GPR55_HUMAN, MCLN3_HUMAN, EGFLA_HUMAN, PMF1_HUMAN, DJC30_HUMAN, TF_HUMAN, FOXR2_HUMAN, ATF6B_HUMAN, KNOP1_HUMAN, ZNF93_HUMAN, ZN430_HUMAN, ZN629_HUMAN, Z324A_HUMAN, RNBP6_HUMAN, SRFB1_HUMAN, NOM1_HUMAN, NP1L3_HUMAN, E9PAV9_HUMAN.GPTC4_HUMAN, HASP_HUMAN, ZN644_HUMAN, ZN281_HUMAN, RECQ4_HUMAN, ZN316_HUMAN, CRHBP_HUMAN, ETFR1_HUMAN, ACPM_HUMAN, GIMA2_HUMAN, UPAR_HUMAN, ANM8_HUMAN, SUCR1_HUMAN, BT2A1_HUMAN, CHSTA_HUMAN, PP2BB_HUMAN, RBM4B_HUMAN, TXD15_HUMAN, ARHGA_HUMAN, HLAE_HUMAN, IPO13_HUMAN, BIG2_HUMAN, HEAT6_HUMAN, WDR11_HUMAN, LTN1_HUMAN, S39A3_HUMAN, CNDH2_HUMAN, INT4_HUMAN, ERAP1_HUMAN, CA112_HUMAN, FCGRN_HUMAN, TTC28_HUMAN, UXS1_HUMAN, SGSM3_HUMAN, F91A1_HUMAN, MMRN1_HUMAN, PCFT_HUMAN, GOLI4_HUMAN, ALG8_HUMAN, TM192_HUMAN, FACR2_HUMAN, MGAT1_HUMAN, CA043_HUMAN, B3A2_HUMAN, TPST2_HUMAN, S35B2_HUMAN, GOGA5_HUMAN, ERD23_HUMAN, PLCD_HUMAN, SELN_HUMAN, SLIK5_HUMAN, TM246_HUMAN, TM186_HUMAN, LEMD2_HUMAN, TM143_HUMAN, PMGT1_HUMAN, RMND1_HUMAN, LRC8A_HUMAN, FZD2_HUMAN, SIDT2_HUMAN, GPHRA_HUMAN.GPHRB_HUMAN, GPAT3_HUMAN, AG10A_HUMAN, OMA1_HUMAN, PIGW_HUMAN, CSCL2_HUMAN, MGT5A_HUMAN, MRS2_HUMAN, ABD12_HUMAN, MPZL1_HUMAN, EXTL3_HUMAN, MANEA_HUMAN, MFS12_HUMAN, PDE3B_HUMAN, GPC5C_HUMAN, GP1BB_HUMAN, S47A1_HUMAN, S2552_HUMAN, FKRP_HUMAN, ZN707_HUMAN, CD244_HUMAN, LPAR6_HUMAN, P2Y12_HUMAN, DPOLB_HUMAN, PRRT2_HUMAN, OGFD3_HUMAN, SLAF1_HUMAN, TMM25_HUMAN, FAM9A_HUMAN, LYPD3_HUMAN, NR1I3_HUMAN, P2RY8_HUMAN, AT1B4_HUMAN, XRP2_HUMAN, SG196_HUMAN, SKAP1_HUMAN, RENR_HUMAN, DLK1_HUMAN, DEGS1_HUMAN, S26A6_HUMAN, HDGR3_HUMAN, RTEL1_HUMAN, VATC2_HUMAN, TEFF1_HUMAN, BTNL8_HUMAN, NIP7_HUMAN, STAU2_HUMAN, PUM2_HUMAN, CENPV_HUMAN, IMP4_HUMAN, PRP17_HUMAN, NAR3_HUMAN, FNTA_HUMAN, FNTB_HUMAN, PGLT1_HUMAN, B4GT3_HUMAN, CARD8_HUMAN, PPCEL_HUMAN, B3GN2_HUMAN, VSIG4_HUMAN, SCPDL_HUMAN, EDNRA_HUMAN, ENPP6_HUMAN, ZER1_HUMAN, KCNA6_HUMAN, MMP3_HUMAN, AZIN1_HUMAN, SERC2_HUMAN, SIAE_HUMAN, ANKL2_HUMAN, MTHR_HUMAN, FMC1_HUMAN, GCSP_HUMAN, AAKG1_HUMAN, STAR9_HUMAN, SPB7_HUMAN, ZN524_HUMAN, TPPC8_HUMAN, ISLR_HUMAN, PE2R3_HUMAN, ZACN_HUMAN, CHST8_HUMAN, TGON2_HUMAN, CHST9_HUMAN, BOLL_HUMAN, GSTM5_HUMAN, CD109_HUMAN, DHB3_HUMAN, MREG_HUMAN, PECR_HUMAN, SCN2B_HUMAN, HECA2_HUMAN, 5HT3C_HUMAN, NYX_HUMAN, OPN4_HUMAN, S38A6_HUMAN, TSP3_HUMAN, SAP3_HUMAN, LRRT2_HUMAN, CP1A1_HUMAN, KLRF1_HUMAN, SACA4_HUMAN, OXLD1_HUMAN, AKA28_HUMAN, GOG7B_HUMAN, IFNA5_HUMAN, NP1L5_HUMAN, NDUC2_HUMAN, RBM24_HUMAN, TUSC5_HUMAN, ZFP41_HUMAN, IER2_HUMAN, PILRA_HUMAN, ZNT6_HUMAN, CX6B1_HUMAN, LRAD4_HUMAN, SOX4_HUMAN, DNAI1_HUMAN, DNAI2_HUMAN, 5HT6R_HUMAN, SKAP_HUMAN, L2GL2_HUMAN, MAP1S_HUMAN, RASF9_HUMAN, VPS11_HUMAN, VPS16_HUMAN, VPS18_HUMAN, MLXIP_HUMAN, MLXPL_HUMAN, ARH40_HUMAN, DOCK4_HUMAN, TRIO_HUMAN, LGR5_HUMAN, PCDGK_HUMAN, LRRN3_HUMAN, ACV1B_HUMAN, TGM3_HUMAN, DSC1_HUMAN, D3DNK7_HUMAN.LEKR1_HUMAN, BT1A1_HUMAN, SYT4_HUMAN, RB15B_HUMAN, PTPRS_HUMAN, LIPB1_HUMAN, INT6_HUMAN, ARHGB_HUMAN, NSMA3_HUMAN, UNC5B_HUMAN, DDR2_HUMAN, XPR1_HUMAN, CO7_HUMAN, MSTO1_HUMAN, DPM1_HUMAN, FIP1_HUMAN, S12A2_HUMAN, TAF6L_HUMAN, ARAP3_HUMAN, SPTC2_HUMAN, IQGA3_HUMAN, VANG2_HUMAN, UNC5C_HUMAN, PTK7_HUMAN, ROR2_HUMAN, CNDD3_HUMAN, CEP97_HUMAN, PCAT2_HUMAN, CWC22_HUMAN, F1711_HUMAN, PLXB2_HUMAN, TMM59_HUMAN, RPRD2_HUMAN, FARP1_HUMAN, PRRT4_HUMAN, PCDB3_HUMAN, AGRL2_HUMAN, RASL2_HUMAN, GRDN_HUMAN, S11IP_HUMAN, ESYT2_HUMAN, GCP6_HUMAN, RSBNL_HUMAN, ARHGC_HUMAN, ATP7A_HUMAN, IGSF3_HUMAN, SPA5L_HUMAN, PDE4B_HUMAN, PP1RA_HUMAN, IDH3A_HUMAN, OFUT1_HUMAN, PIR_HUMAN, LGUL_HUMAN, BCS1_HUMAN, AK1A1_HUMAN, AK1C2_HUMAN, AL4A1_HUMAN, RPE_HUMAN, ARL8A_HUMAN, NPM3_HUMAN, VATD_HUMAN, ST1C3_HUMAN, BCAT2_HUMAN, APMAP_HUMAN, AT2B3_HUMAN, CCS_HUMAN, EHD2_HUMAN, PDCL3_HUMAN, CRIP1_HUMAN, CIP4_HUMAN, CPIN1_HUMAN, RDH13_HUMAN, API5_HUMAN, RNZ2_HUMAN, HYEP_HUMAN, LDH6A_HUMAN, FABP7_HUMAN, FAAA_HUMAN, IMPA2_HUMAN, LYAG_HUMAN, GLRX2_HUMAN, GMDS_HUMAN, MMSA_HUMAN, MAOX_HUMAN, GLYG_HUMAN, HIBCH_HUMAN, JUPI1_HUMAN, MYG1_HUMAN.Q86UA3_HUMAN, CPNE3_HUMAN, MSRA_HUMAN, DHPR_HUMAN, CMTR1_HUMAN, IMPA1_HUMAN, ITPA_HUMAN, KDSR_HUMAN, KIF4B_HUMAN, KIN17_HUMAN, NRDC_HUMAN, RPR1B_HUMAN, GUAD_HUMAN, LDB3_HUMAN, LDH6B_HUMAN, LDHC_HUMAN, GALK2_HUMAN, CSTF1_HUMAN, MCMBP_HUMAN, MECR_HUMAN, MED11_HUMAN, MED22_HUMAN, MTMRC_HUMAN, MYH6_HUMAN, MYH7B_HUMAN, LMAN2_HUMAN, NDUS5_HUMAN, NIT1_HUMAN, UAP1_HUMAN, PAPOB_HUMAN, PCF11_HUMAN, TRIM3_HUMAN, PGK2_HUMAN, PGM2L_HUMAN, PI42C_HUMAN, PMM2_HUMAN, MYP2_HUMAN, DPOE4_HUMAN, IPYR_HUMAN, IPYR2_HUMAN, AIFM3_HUMAN, CAPG_HUMAN, PR38B_HUMAN, RBM19_HUMAN, RGN_HUMAN, RNH2C_HUMAN, RS30_HUMAN.UBIM_HUMAN, RPC2_HUMAN, NOMO2_HUMAN, RLP24_HUMAN, SCD5_HUMAN, SC31B_HUMAN, IREB2_HUMAN, ISY1_HUMAN, SSBP3_HUMAN, CATL2_HUMAN, SYAP1_HUMAN, ABHEB_HUMAN, RPIA_HUMAN, GTR9_HUMAN, HMGCL_HUMAN, TARA_HUMAN, TRM6_HUMAN, TRM61_HUMAN, CP27A_HUMAN, WDHD1_HUMAN, WDR74_HUMAN, ZN830_HUMAN, ZPR1_HUMAN, PUM1_HUMAN, LSG1_HUMAN, TM10C_HUMAN, DHTK1_HUMAN, NAA16_HUMAN, KIFA3_HUMAN, SCAF8_HUMAN, STXB3_HUMAN, CTF18_HUMAN, PPP6_HUMAN, TPPC9_HUMAN, MYO9B_HUMAN, SMAL1_HUMAN, DOCK1_HUMAN, PLPP_HUMAN, CNOT3_HUMAN, EDEM3_HUMAN, EPMIP_HUMAN, MCE1_HUMAN, ZN598_HUMAN, IDH3B_HUMAN, PHX2A_HUMAN, HAUS5_HUMAN, KPBB_HUMAN, ATLA1_HUMAN, ELP3_HUMAN, MICA1_HUMAN, HSDL1_HUMAN, GPSM1_HUMAN, I2BPL_HUMAN, KIF2A_HUMAN, SYRM_HUMAN, ABCD2_HUMAN, GBF1_HUMAN, GTPB1_HUMAN, WASC4_HUMAN, TPC12_HUMAN, SRPRA_HUMAN, NAA35_HUMAN, CP131_HUMAN, BRE1B_HUMAN, TPC11_HUMAN, NAMPT_HUMAN, SOGA3_HUMAN, BRAT1_HUMAN, VP26B_HUMAN, AMPB_HUMAN, KI21A_HUMAN, ARHG1_HUMAN, ISLR2_HUMAN, AFTIN_HUMAN, PANK4_HUMAN, WASC5_HUMAN, CNOT9_HUMAN, VP33A_HUMAN, MCM10_HUMAN, AVL9_HUMAN, TGO1_HUMAN, MPP6_HUMAN, XPF_HUMAN, ERC6L_HUMAN, GCP60_HUMAN, GRIN1_HUMAN, RTL1_HUMAN, ARVC_HUMAN, SYT1_HUMAN, ROCK1_HUMAN, H90B2_HUMAN, SPSY_HUMAN, FOCAD_HUMAN, RB3GP_HUMAN, WAC2A_HUMAN, AGAP3_HUMAN, CBPD_HUMAN, PRUN1_HUMAN, DBR1_HUMAN, BICD1_HUMAN, DPYL4_HUMAN, TAOK1_HUMAN, PPWD1_HUMAN, TXLNG_HUMAN, NELFE_HUMAN, TIM_HUMAN, PPIL4_HUMAN, HOOK3_HUMAN, SYDM_HUMAN, RHG35_HUMAN, DOPO_HUMAN, EMAL4_HUMAN, CSN1_HUMAN, DCTN4_HUMAN, STRA6_HUMAN, NUF2_HUMAN, GDAP1_HUMAN, DPP9_HUMAN, CTNA2_HUMAN, SE6L2_HUMAN, NELFA_HUMAN, NRCAM_HUMAN, HTSF1_HUMAN, RSRC1_HUMAN, CD166_HUMAN, PAX5_HUMAN, SEPR_HUMAN, FGF13_HUMAN, PURG_HUMAN, GLRB_HUMAN, CPED1_HUMAN, ROBO3_HUMAN, FES_HUMAN, NCTR1_HUMAN, SIA7F_HUMAN, GPR15_HUMAN, TSP4_HUMAN, RFX5_HUMAN, LMF2_HUMAN, EPCAM_HUMAN, FOXK2_HUMAN, ENL_HUMAN, NUP53_HUMAN, MOONR_HUMAN, CIZ1_HUMAN, ATAD5_HUMAN, MORC2_HUMAN, ANLN_HUMAN, BOREA_HUMAN, PHF2_HUMAN, BRD2_HUMAN, ZKSC4_HUMAN, ZN362_HUMAN, ELF2_HUMAN, ACOT2_HUMAN, ZN174_HUMAN, BRD8_HUMAN, M18BP_HUMAN, MS3L1_HUMAN, GON4L_HUMAN, MTA70_HUMAN, CKAP2_HUMAN, ZMAT2_HUMAN, RNH2A_HUMAN, KI20A_HUMAN, ZN226_HUMAN, KI18A_HUMAN, EME1_HUMAN, ESCO2_HUMAN, KDM2A_HUMAN, FRG1_HUMAN, KDM1B_HUMAN, UNG_HUMAN, FOXC1_HUMAN, MUS81_HUMAN, RLF_HUMAN, ESS2_HUMAN, HXB9_HUMAN, LIN9_HUMAN, RNH2B_HUMAN, AR6P4_HUMAN, MPP8_HUMAN, PARG_HUMAN, SLBP_HUMAN, PCGF1_HUMAN, TDIF1_HUMAN, JADE3_HUMAN, SPAG7_HUMAN, PRD15_HUMAN, MIER1_HUMAN, TPPC5_HUMAN, EYA3_HUMAN, ANO1_HUMAN, MLX_HUMAN, PFD6_HUMAN, ZHX3_HUMAN, BCL9_HUMAN, BCL9L_HUMAN, CEP85_HUMAN, CECR2_HUMAN, NRBF2_HUMAN, NSE2_HUMAN, IF5AL_HUMAN, SOX7_HUMAN, PNISR_HUMAN, SPDLY_HUMAN, CRTC3_HUMAN, NUCKS_HUMAN, UBN2_HUMAN, PAX9_HUMAN, HME2_HUMAN, AN32E_HUMAN, MEG11_HUMAN, CTF8A_HUMAN.CTF8_HUMAN, OTX1_HUMAN, T2EA_HUMAN, GMEB2_HUMAN, AREL1_HUMAN, CE162_HUMAN, LCA5_HUMAN, B9D1_HUMAN, B9D2_HUMAN, MKS1_HUMAN, TECT3_HUMAN, CE120_HUMAN, CE152_HUMAN, CNTRB_HUMAN, FR1OP_HUMAN, SPICE_HUMAN, CE128_HUMAN, CP135_HUMAN, CEP89_HUMAN, NINL_HUMAN, NIN_HUMAN, NPHP1_HUMAN, CEP19_HUMAN, POC5_HUMAN, ADDG_HUMAN, CT2NL_HUMAN, LIN54_HUMAN, MA7D3_HUMAN, GWL_HUMAN, MOC2A_HUMAN.MOC2B_HUMAN, KNL1_HUMAN, IQEC1_HUMAN, MTUS1_HUMAN, SYNRG_HUMAN, NEK8_HUMAN, SAS6_HUMAN, STIL_HUMAN, TECT1_HUMAN, TMM17_HUMAN, TM216_HUMAN, MKS3_HUMAN, DPS1_HUMAN, NDUAB_HUMAN, ABCA2_HUMAN, PARP4_HUMAN, RHOG_HUMAN, MBOA1_HUMAN, XRCC3_HUMAN, ACATN_HUMAN, RETR2_HUMAN, VAS1_HUMAN, CHSTF_HUMAN, GTSE1_HUMAN, ARX_HUMAN, CO7A1_HUMAN, CBPM_HUMAN, DAPK3_HUMAN, EXTL2_HUMAN, GLGB_HUMAN, GLE1_HUMAN, NDST1_HUMAN, CNOT2_HUMAN, TF2H5_HUMAN, MSH5_HUMAN, MYO5B_HUMAN, NFIB_HUMAN, PCDH7_HUMAN, CHM1A_HUMAN, P52K_HUMAN, ROBO2_HUMAN, LDHD_HUMAN, PHF12_HUMAN, SIPA1_HUMAN, NEIL3_HUMAN, PCDBF_HUMAN, SPAST_HUMAN, TAF4B_HUMAN, NLRP3_HUMAN, COR2A_HUMAN, ZN207_HUMAN, BRPF1_HUMAN, OAZ1_HUMAN, AP4AT_HUMAN, PKP4_HUMAN, OSMR_HUMAN, VPS4B_HUMAN, PTGES_HUMAN, PIEZ1_HUMAN, IST1_HUMAN, RUSC2_HUMAN, CWC27_HUMAN, CEPT1_HUMAN, TM9S1_HUMAN, RPP29_HUMAN, TXN4A_HUMAN, TMED1_HUMAN, NUPL2_HUMAN, PKP3_HUMAN, B4GT7_HUMAN, NBEL2_HUMAN, CSTFT_HUMAN, JADE2_HUMAN, IP6K3_HUMAN, PANX1_HUMAN, PR40B_HUMAN, TES_HUMAN, CAR10_HUMAN, SENP1_HUMAN, PKN3_HUMAN, PNMA3_HUMAN, HM20A_HUMAN, RMD1_HUMAN, FA8A1_HUMAN, AP1S2_HUMAN, PPIL3_HUMAN, RBM27_HUMAN, CHPF2_HUMAN, RHOF_HUMAN, RC3H2_HUMAN, RAIN_HUMAN, P3H2_HUMAN, BMP2K_HUMAN, NEB1_HUMAN, ASAP3_HUMAN, YETS2_HUMAN, PLRKT_HUMAN, MUC13_HUMAN, DHX33_HUMAN, C42S2_HUMAN, RGPA2_HUMAN, THA11_HUMAN, MICA3_HUMAN, PITM2_HUMAN, DEN1A_HUMAN, SUCO_HUMAN, INF2_HUMAN, DCTP1_HUMAN, RIOX1_HUMAN, ZMYM1_HUMAN, PEAK1_HUMAN, REEP4_HUMAN, SGPP1_HUMAN, DOCK8_HUMAN, ARP5L_HUMAN, SEH1_HUMAN, PITM3_HUMAN, NSRP1_HUMAN, SPIR2_HUMAN, RIOX2_HUMAN, ATAD1_HUMAN, ZCRB1_HUMAN, SPB12_HUMAN, PP4P1_HUMAN, ACBD5_HUMAN, NEXN_HUMAN, MYADM_HUMAN, CYTSB_HUMAN, TBC31_HUMAN, ESCO1_HUMAN, TOP1M_HUMAN, CMTD1_HUMAN, MITD1_HUMAN, K2C72_HUMAN, MIB2_HUMAN, RHG42_HUMAN.TM133_HUMAN, PTGR2_HUMAN, UBX2A_HUMAN, PLBL2_HUMAN, C2D1B_HUMAN, TPRN_HUMAN, RGPD8_HUMAN, A0A087WY75_HUMAN.P121C_HUMAN, BRNP1_HUMAN, MEFV_HUMAN, GRIK2_HUMAN, FOXA1_HUMAN, FOXA3_HUMAN, FOXB1_HUMAN, KLF10_HUMAN, HECW1_HUMAN, FOXC2_HUMAN, FOXD3_HUMAN, FOXE1_HUMAN, FOXI2_HUMAN, FOXJ2_HUMAN, GAN_HUMAN, FOXL1_HUMAN, P2R3A_HUMAN, PATZ1_HUMAN, FOXL2_HUMAN, ALKB3_HUMAN, FOXP1_HUMAN, FKB15_HUMAN, FOXQ1_HUMAN, FOXS1_HUMAN, EP2A2_HUMAN.EPM2A_HUMAN, RN111_HUMAN, FBSP1_HUMAN, HXD9_HUMAN, HXC10_HUMAN, S2538_HUMAN, GAS6_HUMAN, RRF2M_HUMAN, RHOU_HUMAN, DNM3L_HUMAN, KLHL3_HUMAN, TFEB_HUMAN, DTX3L_HUMAN, UBX2B_HUMAN, ACACB_HUMAN, FA71B_HUMAN, ING4_HUMAN, PCLO_HUMAN, TMTC1_HUMAN, TOR3A_HUMAN, ZBTB2_HUMAN, ZN157_HUMAN, ZN467_HUMAN, NFIP1_HUMAN, IVD_HUMAN, COQ9_HUMAN, COX7C_HUMAN, TIM21_HUMAN, MIC27_HUMAN, COX8A_HUMAN, COX20_HUMAN, KGUA_HUMAN, CX6A1_HUMAN, USMG5_HUMAN, NMES1_HUMAN, ADCK5_HUMAN, UQCC1_HUMAN, COQ8B_HUMAN, SFXN4_HUMAN, ADCK1_HUMAN, CISD3_HUMAN, PRLD1_HUMAN, COX11_HUMAN, TM205_HUMAN, NDUF8_HUMAN, ODBA_HUMAN, PPA6_HUMAN, SCO1_HUMAN, COQ5_HUMAN, CQ10B_HUMAN, GHITM_HUMAN, MTHFS_HUMAN, COQ7_HUMAN, COQ2_HUMAN, AIFM2_HUMAN, F136A_HUMAN, FXRD1_HUMAN, HINT3_HUMAN, SPRY4_HUMAN, DDAH1_HUMAN, TAM41_HUMAN, CHTOP_HUMAN, H2AJ_HUMAN, HCLS1_HUMAN, LRRF1_HUMAN, ADCY5_HUMAN, STH_HUMAN, RC3H1_HUMAN, GGT1_HUMAN, UBP22_HUMAN, SOCS1_HUMAN, FGF10_HUMAN, UD16_HUMAN, UD11_HUMAN, SNF8_HUMAN, CHSTB_HUMAN, TM258_HUMAN, NEPRO_HUMAN, SPAT5_HUMAN, F210A_HUMAN, NECT1_HUMAN, AGAP1_HUMAN, AGAP2_HUMAN, EPC1_HUMAN, FANCJ_HUMAN, FBX8_HUMAN, ATOH1_HUMAN, K2C5_HUMAN, K1C9_HUMAN, K1C12_HUMAN, SPD2A_HUMAN, SIA4A_HUMAN, ZF64A_HUMAN.ZF64B_HUMAN, RFX1_HUMAN, EYA1_HUMAN, SIX4_HUMAN, BCKD_HUMAN, SLN11_HUMAN, PPM1E_HUMAN, PTN18_HUMAN, PTN4_HUMAN, CNEP1_HUMAN, PHLP1_HUMAN, PTPRN_HUMAN, PTPR2_HUMAN, PPA5_HUMAN, DS13A_HUMAN.DS13B_HUMAN, DUS22_HUMAN, DUS8_HUMAN, MTM1_HUMAN, MTMR6_HUMAN, MTMR7_HUMAN, MTMR8_HUMAN, IFN21_HUMAN, PCDAA_HUMAN, CP4FC_HUMAN, HKDC1_HUMAN, DZIP3_HUMAN, IFNA7_HUMAN, PCDA7_HUMAN, PCDA9_HUMAN, DOCK5_HUMAN, F8VWT9_HUMAN.HECD4_HUMAN, PCDAB_HUMAN, S13A2_HUMAN, PCDA1_HUMAN, KITM_HUMAN, SAT2_HUMAN, PCDAC_HUMAN, SEP10_HUMAN, NRX3A_HUMAN.NRX3B_HUMAN, MIGA2_HUMAN, DLP1_HUMAN, LG3BP_HUMAN, FOXP4_HUMAN, IFNA8_HUMAN, EPC2_HUMAN, JAZF1_HUMAN, IFNA1_HUMAN, BCD1_HUMAN, FRMD6_HUMAN, SYT12_HUMAN, CSPG2_HUMAN, EAF6_HUMAN, TFB1M_HUMAN, SEM7A_HUMAN, CERKL_HUMAN, MTG2_HUMAN, SNX25_HUMAN, F189B_HUMAN, RT4I1_HUMAN, TUSC3_HUMAN, ZN169_HUMAN, KLDC3_HUMAN, TF2LY_HUMAN, PKNX1_HUMAN, ZN785_HUMAN, IFNA2_HUMAN, PIGA_HUMAN, MYCL_HUMAN, PR20A_HUMAN.PR20B_HUMAN.PR20C_HUMAN.PR20D_HUMAN.PR20E_HUMAN, CO9_HUMAN, A0A0J9YY34_HUMAN.NHSL2_HUMAN, CD320_HUMAN, F172A_HUMAN, Z324B_HUMAN, H1T_HUMAN, MIPEP_HUMAN, TM38B_HUMAN, SPP2B_HUMAN, S22AN_HUMAN, DSG4_HUMAN, PPIP2_HUMAN, NPT3_HUMAN, TM40L_HUMAN, SEM4D_HUMAN, NK1R_HUMAN, SRS12_HUMAN, PDCD1_HUMAN, PP14C_HUMAN, AUHM_HUMAN, S27A6_HUMAN, GLMP_HUMAN, INHBE_HUMAN, VSIG8_HUMAN, UPK1A_HUMAN, B2L15_HUMAN, VMAT1_HUMAN, SULF2_HUMAN, ADA33_HUMAN, CHLE_HUMAN, SIA8C_HUMAN, S22A9_HUMAN, GRM1C_HUMAN, ELOV2_HUMAN, GRM1B_HUMAN, FEM1B_HUMAN, MAS_HUMAN, OXND1_HUMAN, MMP10_HUMAN, SPT13_HUMAN, GPR21_HUMAN, ACADL_HUMAN, MYL3_HUMAN, AP3S1_HUMAN, GDPD5_HUMAN, AT5G3_HUMAN, GNAT3_HUMAN, ZN550_HUMAN, RETN_HUMAN, SMAG1_HUMAN, CD1E_HUMAN, SNTG2_HUMAN, IQCN_HUMAN, HPHL1_HUMAN, IL1R2_HUMAN, GP107_HUMAN, NRN1_HUMAN, PCDA3_HUMAN, RM33_HUMAN, GMEB1_HUMAN, HPSE_HUMAN, DQX1_HUMAN, MLRV_HUMAN, SNX19_HUMAN, HLAG_HUMAN, CP8B1_HUMAN, GRM1A_HUMAN, RHG22_HUMAN, PKHG5_HUMAN, CO6A2_HUMAN, K319L_HUMAN, RAE2_HUMAN, KIME_HUMAN, I17RC_HUMAN, ADA21_HUMAN, LRFN1_HUMAN, SCNND_HUMAN, STXB6_HUMAN, LPCT4_HUMAN, GTR12_HUMAN, SC5A8_HUMAN, PDXL2_HUMAN, NEUR2_HUMAN, RF1ML_HUMAN, IFG15_HUMAN.TOIP2_HUMAN, CCG5_HUMAN, ACHD_HUMAN, THOC5_HUMAN, WNT7A_HUMAN, KCD15_HUMAN, REG3A_HUMAN, CLC4E_HUMAN, BODG_HUMAN, KCND2_HUMAN, P2RX2_HUMAN, MPPD2_HUMAN, FIGL1_HUMAN, MRCKA_HUMAN, DHB7_HUMAN, TMPS3_HUMAN, BMAL2_HUMAN, ALX3_HUMAN, FOXD4_HUMAN, MAP7_HUMAN, MYORG_HUMAN, S27A3_HUMAN, DFB4A_HUMAN, NSMA_HUMAN, GXLT1_HUMAN, CSPG5_HUMAN, HXK3_HUMAN, S20A2_HUMAN, NRROS_HUMAN, CHST6_HUMAN, TR16L_HUMAN, IFFO1_HUMAN, BRNP3_HUMAN, CNNM1_HUMAN, ACTBL_HUMAN, FCF1_HUMAN, S6A15_HUMAN, TSN2_HUMAN, I13R2_HUMAN, TMPSC_HUMAN, PEX13_HUMAN, FABPL_HUMAN, ZN581_HUMAN, TM206_HUMAN, TMEM5_HUMAN, KI3L2_HUMAN, FBX40_HUMAN, FXL14_HUMAN, VSIG1_HUMAN, CP1A2_HUMAN, CD97_HUMAN, NR3L1_HUMAN, LRRN2_HUMAN, TM223_HUMAN, TMUB2_HUMAN, ECP_HUMAN, NOX5_HUMAN, TACC1_HUMAN, GDF9_HUMAN, ZPLD1_HUMAN, ST4A1_HUMAN, PLCH1_HUMAN, PROD_HUMAN, AG10B_HUMAN, KLDC2_HUMAN, HYAL3_HUMAN, NTCP7_HUMAN, INTU_HUMAN, ATS4_HUMAN, P4HA3_HUMAN, RELL1_HUMAN, CETN1_HUMAN, B3GN3_HUMAN, FA11_HUMAN, CD1B_HUMAN, SIA8D_HUMAN, ARSG_HUMAN, LRRT1_HUMAN, TULP2_HUMAN, SESQ1_HUMAN, PROZ_HUMAN, DPEP3_HUMAN, C3AR_HUMAN, GALT6_HUMAN, TIMP3_HUMAN, NECA2_HUMAN, CC50B_HUMAN, PA2GX_HUMAN, GBRG2_HUMAN, ADA30_HUMAN, P2RX5_HUMAN, PKHG6_HUMAN, TM11B_HUMAN, ACM4_HUMAN, STS_HUMAN, ALG5_HUMAN, I27RA_HUMAN, IKZF5_HUMAN, CC85C_HUMAN, STK39_HUMAN, AMGO3_HUMAN, PNMT_HUMAN, RTN4R_HUMAN, PAL4G_HUMAN, NGN3_HUMAN, ASIC4_HUMAN, HAOX2_HUMAN, RB39B_HUMAN, BRNP2_HUMAN, RFIP5_HUMAN, PEDF_HUMAN, CHIA_HUMAN, RA51D_HUMAN, SC6A5_HUMAN, FREM2_HUMAN, MUC20_HUMAN, NMNA3_HUMAN, KLK15_HUMAN, RPF1_HUMAN, S22AI_HUMAN, TYSD1_HUMAN, CIDEC_HUMAN, TYRP2_HUMAN, SIA4B_HUMAN, KCNV2_HUMAN, ZNF2_HUMAN, E4F1_HUMAN, ST1C2_HUMAN, ZCHC7_HUMAN, WNT16_HUMAN, ACADS_HUMAN, SACA1_HUMAN, GATB_HUMAN, ARV1_HUMAN, ABC3D_HUMAN.Q6ICH2_HUMAN, E2AK4_HUMAN, MA7D1_HUMAN, GTR5_HUMAN, OPCM_HUMAN, CRIS2_HUMAN, PSG1_HUMAN, PCDC1_HUMAN, KKCC1_HUMAN, VIPR1_HUMAN, GALNS_HUMAN, SCRN1_HUMAN, P3H3_HUMAN, PDGFB_HUMAN, MRM2_HUMAN, PDD2L_HUMAN, AVIL_HUMAN, PCDBG_HUMAN, S39AC_HUMAN, ESAM_HUMAN, LPAR1_HUMAN, NCEH1_HUMAN, YBEY_HUMAN, RT63_HUMAN, DET1_HUMAN, KAPCG_HUMAN, TSN15_HUMAN, F174A_HUMAN, NPAS1_HUMAN, MFS4B_HUMAN, CCNJL_HUMAN, LIPH_HUMAN, FITM2_HUMAN, CHSTC_HUMAN, KCNC4_HUMAN, PPTC7_HUMAN, FPR2_HUMAN, UBE3D_HUMAN, CTGE5_HUMAN.MIA2_HUMAN, ANGT_HUMAN, AGRG5_HUMAN, T179B_HUMAN, STIM2_HUMAN, LRC15_HUMAN, SPC25_HUMAN, P2RX1_HUMAN, RAE1E_HUMAN, TMCO3_HUMAN, HYAL1_HUMAN, GATC_HUMAN, CTNA3_HUMAN, AGRL1_HUMAN, BCAM_HUMAN, TULP3_HUMAN, TMM9B_HUMAN, PCDB7_HUMAN, MTO1_HUMAN, PRDM5_HUMAN, HXC9_HUMAN, CD276_HUMAN, SPT19_HUMAN, JPH4_HUMAN, ENPP1_HUMAN, TSHB_HUMAN, KLHL2_HUMAN, IPPK_HUMAN, SPB11_HUMAN, TTC25_HUMAN, FUT9_HUMAN, MRPP3_HUMAN, UFSP2_HUMAN, ARP3B_HUMAN, ITM2A_HUMAN, GLPK2_HUMAN, A4GAT_HUMAN, TM39A_HUMAN, PMEL_HUMAN, IGSF6_HUMAN, TRHDE_HUMAN, CXB7_HUMAN, ZN331_HUMAN, CSCL1_HUMAN, S22AC_HUMAN, TTC1_HUMAN, AT8B2_HUMAN, GP141_HUMAN, PTCD2_HUMAN, TSYL6_HUMAN, CQ080_HUMAN, PPCT_HUMAN, CHSTE_HUMAN, TMED6_HUMAN, LYZL2_HUMAN, TPGS2_HUMAN, CLC5A_HUMAN, CP2A6_HUMAN, CH3L1_HUMAN, RCCD1_HUMAN, PTPRA_HUMAN, TPTE_HUMAN, ITSN2_HUMAN, ASCC3_HUMAN, CHP1_HUMAN, KCTD7_HUMAN, SDC4_HUMAN, PCMD1_HUMAN, TPSN_HUMAN, UBP32_HUMAN, ELOV5_HUMAN, S38A5_HUMAN, ERGI2_HUMAN, TTF2_HUMAN, SC5A6_HUMAN, LMTK2_HUMAN, TENS3_HUMAN, STYX_HUMAN, EAPP_HUMAN, ERH_HUMAN, ACOT8_HUMAN, S35A4_HUMAN.S35U4_HUMAN, PLIN1_HUMAN, GRK4_HUMAN, IPMK_HUMAN, MTF1_HUMAN, 5HT2A_HUMAN, BAALC_HUMAN, UBP6_HUMAN, MINY3_HUMAN, AT7L3_HUMAN, NRL_HUMAN, AQP2_HUMAN, MTSS1_HUMAN, NDRG3_HUMAN, STK40_HUMAN, MTG16_HUMAN, PSB10_HUMAN, CAD11_HUMAN, UBD_HUMAN, CLC14_HUMAN, CPEB2_HUMAN, ABCB5_HUMAN, HGF_HUMAN, MET_HUMAN, SCAI_HUMAN, SPR1B_HUMAN, WIZ_HUMAN, Z518A_HUMAN, Z518B_HUMAN, ZN292_HUMAN, ZN462_HUMAN, SENP7_HUMAN, ZN689_HUMAN, PHC3_HUMAN, TRI14_HUMAN, Q9H4D1_HUMAN.RIPK4_HUMAN, PHAR3_HUMAN, R144A_HUMAN, TRI11_HUMAN, RAB15_HUMAN, FOPNL_HUMAN, EGLN2_HUMAN, CRYL1_HUMAN, ZN217_HUMAN, DCTN5_HUMAN, PX11B_HUMAN, HNF1B_HUMAN, GMPPA_HUMAN, NPRL2_HUMAN, OXSM_HUMAN, OGG1_HUMAN, HECD3_HUMAN, IFIX_HUMAN, GDE_HUMAN, GSH0_HUMAN, B4DRS2_HUMAN.K2C4_HUMAN, SPB6_HUMAN, HIG1A_HUMAN, H2B3B_HUMAN, SOCS2_HUMAN, K2C6C_HUMAN, EVI1_HUMAN.MDS1_HUMAN, K2C6B_HUMAN, ZKSC1_HUMAN, OZF_HUMAN, ZKSC8_HUMAN, ZN592_HUMAN, ZBTB5_HUMAN, SATB2_HUMAN, NGDN_HUMAN, ZN687_HUMAN, PAXB1_HUMAN, K2C80_HUMAN, K2C78_HUMAN, K1C13_HUMAN, K1H2_HUMAN, LCORL_HUMAN, K2C73_HUMAN, CTAG2_HUMAN, HOOK1_HUMAN, RARB_HUMAN, HAVR1_HUMAN, CENPX_HUMAN, RIOK1_HUMAN, KY_HUMAN, IRX2_HUMAN, ITPR2_HUMAN, CBPA4_HUMAN, B2CL1_HUMAN.BCL2_HUMAN, NGAL_HUMAN, RN169_HUMAN, H2A1B_HUMAN.H2B1J_HUMAN, CKS2_HUMAN, TRBC2_HUMAN, TCA_HUMAN, 2B14_HUMAN, QCR10_HUMAN, IGHG1_HUMAN, IGKC_HUMAN, TCA_HUMAN.TVA21_HUMAN, A0A578_HUMAN.TRBC2_HUMAN, 1A01_HUMAN, RNF38_HUMAN, PI4KB_HUMAN, OTUB1_HUMAN.UB2D2_HUMAN, IQEC2_HUMAN, A0A5B6_HUMAN.K7N5M4_HUMAN, K7N5N2_HUMAN.TVA4_HUMAN, 1A02_HUMAN, HEBP2_HUMAN, CO6A1_HUMAN, GPC6_HUMAN, MARCO_HUMAN, GPC3_HUMAN, GPC5_HUMAN, PGCB_HUMAN, CSH1_HUMAN.CSH2_HUMAN, ZN212_HUMAN, TTL12_HUMAN, LMX1A_HUMAN, HHEX_HUMAN, HAUS7_HUMAN, MAGB2_HUMAN, ZMY10_HUMAN, HEN1_HUMAN, S29A1_HUMAN, SENP6_HUMAN, CAMP2_HUMAN, TRAP1_HUMAN, OCTC_HUMAN, SIL1_HUMAN, AGRG6_HUMAN, CYTM_HUMAN, PYRG1_HUMAN, EID3_HUMAN, SIGL7_HUMAN, TBCA_HUMAN, ABC3A_HUMAN, EMAL2_HUMAN, PDIA2_HUMAN, HHIP_HUMAN, ZBP1_HUMAN, SPHK2_HUMAN, PAHO_HUMAN, PISD_HUMAN, SSA27_HUMAN, PTPRU_HUMAN, NAA30_HUMAN, RIP_HUMAN, DIAP2_HUMAN, FOXA2_HUMAN, SMAP_HUMAN, MTPN_HUMAN, FETA_HUMAN, HGFL_HUMAN, MAF_HUMAN, CASK_HUMAN, K154L_HUMAN, TGT_HUMAN, SIAT6_HUMAN, STAG1_HUMAN, DHI1_HUMAN, ZN521_HUMAN, FIL1L_HUMAN, NUDT5_HUMAN, LRC26_HUMAN, PCD16_HUMAN, ABEC2_HUMAN, ZIC2_HUMAN, TIAF1_HUMAN, VPP4_HUMAN, LAGE3_HUMAN, SIX3_HUMAN, S29A2_HUMAN, ISL2_HUMAN, LRC40_HUMAN, MOB2_HUMAN.YYAP1_HUMAN, KCC4_HUMAN, CUX1_HUMAN, GSTM2_HUMAN, CATL1_HUMAN, NAF1_HUMAN.TNIP1_HUMAN, TBA3C_HUMAN.TBA4A_HUMAN, SP16H_HUMAN.SPT16_HUMAN, SH21A_HUMAN, CAR16_HUMAN.RFWD2_HUMAN, CAR14_HUMAN, NFASC_HUMAN, PSD3_HUMAN, CRIPT_HUMAN, GBRL3_HUMAN, 4EBP3_HUMAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q86V21</t>
   </si>
   <si>
@@ -57,6 +102,51 @@
   </si>
   <si>
     <t xml:space="preserve">STING_HUMAN, TBK1_HUMAN, PAR14_HUMAN, ETS1_HUMAN, CEBPB_HUMAN, CEBPA_HUMAN, MK01_HUMAN, H31T_HUMAN, STA5A_HUMAN.STA5B_HUMAN.STAT1_HUMAN.STAT2_HUMAN.STAT3_HUMAN.STAT4_HUMAN.STAT6_HUMAN, ITA2B_HUMAN, IRF4_HUMAN, PRDM1_HUMAN, STAT2_HUMAN, IRF9_HUMAN, SRC_HUMAN, IRF1_HUMAN, LITAF_HUMAN, PTN2_HUMAN, JAK3_HUMAN, STAT1_HUMAN, HNF1A_HUMAN, VP37B_HUMAN, VP37C_HUMAN, VP37A_HUMAN, BAG4_HUMAN, KT33B_HUMAN, MGRN1_HUMAN, IQGA1_HUMAN, CEP55_HUMAN, PDC6I_HUMAN, ZWINT_HUMAN, ROCK1_HUMAN, HGS_HUMAN, LNX1_HUMAN, COPE_HUMAN, HNRL1_HUMAN, LRSM1_HUMAN, GGA1_HUMAN, CC88B_HUMAN, AMPL_HUMAN, K1H1_HUMAN, ASPP1_HUMAN, A0A087WTE7_HUMAN.LENG8_HUMAN, RNF41_HUMAN, HAUS1_HUMAN, HSH2D_HUMAN, PDLI7_HUMAN, CD2AP_HUMAN, VPS28_HUMAN, TRI23_HUMAN, SYCE1_HUMAN, MIC60_HUMAN, CSN6_HUMAN, DCTN2_HUMAN, VRK3_HUMAN, NDUAD_HUMAN, PIGQ_HUMAN, SMRC2_HUMAN, CDS2_HUMAN, EP300_HUMAN, A1A4E9_HUMAN, AP2C_HUMAN, K1C18_HUMAN, TAXB1_HUMAN, RBPMS_HUMAN, F110A_HUMAN, VPS11_HUMAN, CBY1_HUMAN, NELFD_HUMAN, INCA1_HUMAN, RN111_HUMAN, K1C15_HUMAN, DAXX_HUMAN, TRI54_HUMAN, THOC7_HUMAN, PKNX2_HUMAN, MZB1_HUMAN, KRT34_HUMAN, SCRIB_HUMAN, TNIP1_HUMAN, THRSP_HUMAN, PDCD6_HUMAN, SNG3_HUMAN, TFP11_HUMAN, TRI35_HUMAN, UBB_HUMAN.UBC_HUMAN, TM1L1_HUMAN, NEDD4_HUMAN, MAVS_HUMAN, KIFC3_HUMAN, TSP50_HUMAN, FAM9B_HUMAN, UBC_HUMAN, B4DTS2_HUMAN.KPCD2_HUMAN, K1C16_HUMAN, DMAP1_HUMAN, PTN23_HUMAN, AJUBA_HUMAN, DPOD2_HUMAN, RIR2_HUMAN, CEP63_HUMAN, STK11_HUMAN, ORC1_HUMAN, FRIL_HUMAN, KRT35_HUMAN, KLK6_HUMAN, MTA3_HUMAN, HCK_HUMAN, NMI_HUMAN, DZIP3_HUMAN, PLEC_HUMAN, RAD18_HUMAN, FPPS_HUMAN, ENOA_HUMAN, GLYR1_HUMAN, K1C27_HUMAN, CCHCR_HUMAN, DDT4L_HUMAN, ARFP2_HUMAN, RSLAB_HUMAN, SCAM1_HUMAN, AT5F1_HUMAN, ECHP_HUMAN.TBA8_HUMAN, RPRM_HUMAN, BCAS3_HUMAN.BCAS4_HUMAN, K2C75_HUMAN, ABCB6_HUMAN, SCAR5_HUMAN, ACAD8_HUMAN, TRAIP_HUMAN, GGA3_HUMAN, CDN1A_HUMAN, SNF8_HUMAN, AATF_HUMAN, GMCL1_HUMAN, JAK1_HUMAN, ARF3_HUMAN, RL40_HUMAN, SND1_HUMAN, NCOA1_HUMAN, SCAM3_HUMAN, DNMT1_HUMAN, GTR4_HUMAN, MDM2_HUMAN, RB27A_HUMAN, NFKB1_HUMAN, CBP_HUMAN, H32_HUMAN, RB27B_HUMAN, GCR_HUMAN, KPCZ_HUMAN, VPS36_HUMAN, TF65_HUMAN, VP37D_HUMAN, P53_HUMAN, PTN6_HUMAN, ANDR_HUMAN, ARF1_HUMAN, LMNA_HUMAN, DHX9_HUMAN, KIF5A_HUMAN, ITSN1_HUMAN, THB_HUMAN, ARF5_HUMAN, SCNNA_HUMAN, BCR_HUMAN, STAT3_HUMAN, TIF1A_HUMAN, CEBPZ_HUMAN, WWP1_HUMAN, RNF12_HUMAN, ZN407_HUMAN, ZBTB2_HUMAN, ZNF92_HUMAN, NCOA3_HUMAN, NCOA2_HUMAN, JUN_HUMAN, CXA1_HUMAN, BIRC2_HUMAN, SFPQ_HUMAN, TNNT3_HUMAN, MB12A_HUMAN, MB12B_HUMAN, ATX2_HUMAN, BAG6_HUMAN, CAPR1_HUMAN, CPSF7_HUMAN, DDX6_HUMAN, EWS_HUMAN, FAS_HUMAN, IF4B_HUMAN, NFKB2_HUMAN, NONO_HUMAN, NUFP2_HUMAN, ODP2_HUMAN, PABP1_HUMAN, RENT1_HUMAN, S23IP_HUMAN, SC16A_HUMAN, SC24B_HUMAN, TB182_HUMAN, TFG_HUMAN, TRI47_HUMAN, VASP_HUMAN, WDR26_HUMAN, ALG2_HUMAN, TOM1_HUMAN, ASZ1_HUMAN, AKAP9_HUMAN, UBAP1_HUMAN, RFIP4_HUMAN, RFIP3_HUMAN, CEBPE_HUMAN, GRB2_HUMAN, XPO1_HUMAN, WDR12_HUMAN, SRXN1_HUMAN, PPM1G_HUMAN, RD23B_HUMAN, SC24A_HUMAN, NUBP2_HUMAN, SAHH2_HUMAN, DEST_HUMAN, IGBP1_HUMAN, SH3L1_HUMAN, SERC_HUMAN, ZFYV9_HUMAN, TERA_HUMAN, TIF1B_HUMAN, RCN3_HUMAN, EF1A1_HUMAN, API5_HUMAN, VATC1_HUMAN, TSNAX_HUMAN, YAP1_HUMAN, DNM1L_HUMAN, EHD1_HUMAN, IDE_HUMAN, PDE12_HUMAN, ANM3_HUMAN, GLYM_HUMAN, UBP8_HUMAN, CUL5_HUMAN, ADRB2_HUMAN, DAPK3_HUMAN, K1C13_HUMAN, PPARG_HUMAN, PICK1_HUMAN, AACS_HUMAN, ACTN4_HUMAN, AK1A1_HUMAN, ARFG2_HUMAN, PURA2_HUMAN, G6PD_HUMAN, PUR2_HUMAN, DHB8_HUMAN, PFKAM_HUMAN, PFKAP_HUMAN, PP2BA_HUMAN, PLPHP_HUMAN, SYSC_HUMAN, SC24D_HUMAN, GLYC_HUMAN, FCL_HUMAN, ATOX1_HUMAN, DNJB1_HUMAN, DPH2_HUMAN, DPYL2_HUMAN, ECH1_HUMAN, FLNB_HUMAN, HIP1R_HUMAN, KDM3A_HUMAN, LYPA1_HUMAN, NDRG1_HUMAN, NIF3L_HUMAN, PA1B2_HUMAN, PALLD_HUMAN, PGM2L_HUMAN, DHPR_HUMAN, SH3K1_HUMAN, SMHD1_HUMAN, STIP1_HUMAN, TATD1_HUMAN, TBCA_HUMAN, TRI25_HUMAN, STAM2_HUMAN, UBC9_HUMAN, PICAL_HUMAN, SYWC_HUMAN, NTRK1_HUMAN, BCAS3_HUMAN, DYLT1_HUMAN, TMM17_HUMAN, TM216_HUMAN, KIF22_HUMAN, POLK_HUMAN, PCKGM_HUMAN, CHM4B_HUMAN, WDR5_HUMAN, YBOX1_HUMAN, MERL_HUMAN, CDC5L_HUMAN, CBL_HUMAN, BCAR1_HUMAN, CRK_HUMAN, EPHA2_HUMAN, RAB5A_HUMAN, RAB7A_HUMAN, CHMP6_HUMAN, CHMP5_HUMAN, CADH1_HUMAN, EGFR_HUMAN, HSP7C_HUMAN, FBX7_HUMAN, EGLN3_HUMAN, MYD88_HUMAN, DMRTB_HUMAN, SHLB2_HUMAN, CDN2D_HUMAN, QKI_HUMAN, CNOT7_HUMAN, CCND3_HUMAN, PIAS1_HUMAN, TNIP2_HUMAN, PROM1_HUMAN, RS27A_HUMAN, ACTN1_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q9HD40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sep (O-phosphoserine) tRNA:Sec (selenocysteine) tRNA synthase [Source:HGNC Symbol;Acc:HGNC:30605]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPCS_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTX2_HUMAN, SOX2_HUMAN, XPO1_HUMAN, SUH_HUMAN, MTMR2_HUMAN, RFWD2_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PO5F1_HUMAN, CDX2_HUMAN, NANOG_HUMAN, DKK1_HUMAN, EOMES_HUMAN, GSC_HUMAN, HHEX_HUMAN, T22D1_HUMAN, DPPA4_HUMAN, EPHA1_HUMAN, FGF2_HUMAN, FOXD3_HUMAN, SALL1_HUMAN, STAT3_HUMAN, TDGF1_HUMAN, ZIC3_HUMAN, MTMR5_HUMAN, MTMRD_HUMAN, MTMRC_HUMAN, 1433Z_HUMAN, CTNB1_HUMAN, CBY1_HUMAN, NOTC1_HUMAN, SNW1_HUMAN, P53_HUMAN, SMUF1_HUMAN, SMAD7_HUMAN, CTBP1_HUMAN, KDM1A_HUMAN, MINT_HUMAN, CTIP_HUMAN, HEY1_HUMAN, HES1_HUMAN, RAN_HUMAN, NU214_HUMAN, NCOR1_HUMAN, NCOR2_HUMAN, HDAC1_HUMAN, CIR1_HUMAN, FHL1_HUMAN, NOTC2_HUMAN, NOTC4_HUMAN, NOTC1_HUMAN.NOTC2_HUMAN.NOTC3_HUMAN.NOTC4_HUMAN, DTX1_HUMAN.DTX2_HUMAN.DTX3_HUMAN, SKIL_HUMAN.SKI_HUMAN.TLE1_HUMAN.TLE2_HUMAN.TLE3_HUMAN.TLE4_HUMAN, G3P_HUMAN, FOXO4_HUMAN, SNTA1_HUMAN, IRF5_HUMAN, WASP_HUMAN, IRF3_HUMAN, RING2_HUMAN, TBX15_HUMAN, ETS2_HUMAN, ERBB2_HUMAN, 4ET_HUMAN, RBPMS_HUMAN, ETV1_HUMAN, ATX1_HUMAN, ATX1L_HUMAN, HDAC3_HUMAN, VRK1_HUMAN, MTA2_HUMAN, TOP2A_HUMAN, EZH2_HUMAN, TRIB3_HUMAN, ETS1_HUMAN, NCALD_HUMAN, CSN6_HUMAN, SPN1_HUMAN, POGZ_HUMAN, NXF1_HUMAN, ROA1_HUMAN, NCBP1_HUMAN, HNRPC_HUMAN, MS18B_HUMAN, VGLL3_HUMAN, ALKB4_HUMAN, SYQ_HUMAN, ZN774_HUMAN, 1433S_HUMAN, ATM_HUMAN, NIF3L_HUMAN, RITA1_HUMAN, KLC3_HUMAN, COQ8A_HUMAN, SPCS_HUMAN, FHL2_HUMAN, ARI5A_HUMAN, PHB_HUMAN, SOLH1_HUMAN, MED27_HUMAN, SPG21_HUMAN, GLCTK_HUMAN, UB2D3_HUMAN, LMBL2_HUMAN, HGS_HUMAN, COA6_HUMAN, HXB2_HUMAN, KDM6B_HUMAN, ATPO_HUMAN, MAML1_HUMAN, HXA1_HUMAN, RFX6_HUMAN, PKHF2_HUMAN, UB2D1_HUMAN, NEMO_HUMAN, DICER_HUMAN, AGO2_HUMAN, DHX9_HUMAN, RHXF2_HUMAN, Q49A12_HUMAN, PHF8_HUMAN, MVP_HUMAN, BIRC5_HUMAN, ZN503_HUMAN, MPIP1_HUMAN, PSB4_HUMAN, RUSC1_HUMAN, LNX1_HUMAN, ZN764_HUMAN, HAX1_HUMAN, B4DTS2_HUMAN.KPCD2_HUMAN, PAX5_HUMAN.ZN521_HUMAN, IPKA_HUMAN, FHL5_HUMAN, NFL_HUMAN, TEKT5_HUMAN, C1AS1_HUMAN, FOXI1_HUMAN, NDUAD_HUMAN, SAMD1_HUMAN, A0A024R9F6_HUMAN, LMBL3_HUMAN, HSPB1_HUMAN, SUMO1_HUMAN, FRYL_HUMAN, GLD2_HUMAN, B2L11_HUMAN, ACLY_HUMAN, PARG_HUMAN, STK40_HUMAN, ATF6A_HUMAN, TRI35_HUMAN, TRIB2_HUMAN, SMCA4_HUMAN, ZN620_HUMAN, PCH2_HUMAN, EYA2_HUMAN, KPCI_HUMAN, THOC4_HUMAN, DDX3X_HUMAN, DCAF8_HUMAN, CSN5_HUMAN, KS6A6_HUMAN, RCC1_HUMAN, MYC_HUMAN, KLF4_HUMAN, MBD3_HUMAN, UBQL4_HUMAN, HLX_HUMAN, MB3L1_HUMAN, AGO1_HUMAN, TGS1_HUMAN, LR2BP_HUMAN, IF4G1_HUMAN, IKZF3_HUMAN, GLYR1_HUMAN, MED19_HUMAN, SALL2_HUMAN, BRCA2_HUMAN, NMD3_HUMAN, GSK3B_HUMAN, DDB1_HUMAN, GRWD1_HUMAN, JUND_HUMAN, ECSIT_HUMAN, KDM6A_HUMAN, CLPP_HUMAN, AICDA_HUMAN, JUN_HUMAN, RAD51_HUMAN, GA45A_HUMAN, TE2IP_HUMAN, CASP8_HUMAN, PB1_HUMAN, CEBPD_HUMAN, HS90B_HUMAN, KPCD2_HUMAN, FADD_HUMAN, ERF_HUMAN, KS6B1_HUMAN, NXF3_HUMAN, NPM_HUMAN, RBP2_HUMAN, SIPA1_HUMAN, SNF5_HUMAN, NUP50_HUMAN, BECN1_HUMAN, NUP62_HUMAN, MERL_HUMAN, DSRAD_HUMAN, E2F5_HUMAN, DTX3_HUMAN, ORC1_HUMAN, CDN1B_HUMAN, ATF2_HUMAN, C2TA_HUMAN, HMGB1_HUMAN, NOTC3_HUMAN, SND1_HUMAN, DET1_HUMAN, NCBP2_HUMAN, PHAX_HUMAN, PO2F1_HUMAN, FGF4_HUMAN, TERT_HUMAN, AGFG1_HUMAN, SUFU_HUMAN, KAT2B_HUMAN, AHR_HUMAN, TOP2B_HUMAN, STAT1_HUMAN, STF1_HUMAN, MK06_HUMAN, NXT1_HUMAN, KIF17_HUMAN, IF5A1_HUMAN, SMAD1_HUMAN, ELAV1_HUMAN, AN32A_HUMAN, AN32B_HUMAN, ANM1_HUMAN, NRIP1_HUMAN, CRK_HUMAN, DTX1_HUMAN, RANB3_HUMAN, NU153_HUMAN, CUL4A_HUMAN, RBX1_HUMAN, AURKB_HUMAN, TYY1_HUMAN, RING1_HUMAN, CDK7_HUMAN, SPT6H_HUMAN, RPB1_HUMAN, EP300_HUMAN, CBP_HUMAN, PAX6_HUMAN, APC_HUMAN, SIN3A_HUMAN, KAT2A_HUMAN, RANG_HUMAN, CCND1_HUMAN, FOXO1_HUMAN, MECP2_HUMAN, CRTC2_HUMAN, PMS2_HUMAN, AIRE_HUMAN, HSP7C_HUMAN, HSP76_HUMAN, HSP72_HUMAN, TCPG_HUMAN, TCPA_HUMAN, TCPZ_HUMAN, TCPE_HUMAN, TCPQ_HUMAN, TCPH_HUMAN, TCPD_HUMAN, TCPB_HUMAN, CLN3_HUMAN, SRTD2_HUMAN, CDCA4_HUMAN, ALX4_HUMAN, CUL4B_HUMAN, WDR5_HUMAN, SAP25_HUMAN, CHK1_HUMAN, CSN2_HUMAN, CSN8_HUMAN, SET_HUMAN, HNF4A_HUMAN, BACH1_HUMAN, KDM5A_HUMAN, ETV5_HUMAN, ETV4_HUMAN, ZN281_HUMAN, KLF8_HUMAN, FBX7_HUMAN, HDAC5_HUMAN, MDM2_HUMAN, MDM4_HUMAN, ZN363_HUMAN, 1433B_HUMAN, BOREA_HUMAN, CHD4_HUMAN, MTA1_HUMAN, P66B_HUMAN, HDAC2_HUMAN, RBBP7_HUMAN, P66A_HUMAN, SALL3_HUMAN, TBL1R_HUMAN, SMRC2_HUMAN, RBBP4_HUMAN, ACL6A_HUMAN, SMRC1_HUMAN, SMRD1_HUMAN, ARI1A_HUMAN, RUVB2_HUMAN, RUVB1_HUMAN, CHD7_HUMAN, CASP_HUMAN.CUX1_HUMAN, ZEB1_HUMAN, SP16H_HUMAN, RFX3_HUMAN, SOX8_HUMAN, HXA5_HUMAN, MYEF2_HUMAN, NFIB_HUMAN, CTBP2_HUMAN, TEAD1_HUMAN, SMCA5_HUMAN, SOX5_HUMAN, TWST1_HUMAN, TFE2_HUMAN, ZNF24_HUMAN, DOCK7_HUMAN, RUNX3_HUMAN, XRCC1_HUMAN, MTG8_HUMAN, KAT5_HUMAN, SIR7_HUMAN, HDAC6_HUMAN, BCL6B_HUMAN, ESR1_HUMAN, FBX25_HUMAN, OTU7B_HUMAN, E2F4_HUMAN, CLUS_HUMAN, MRT4_HUMAN, TXN4B_HUMAN, CUL3_HUMAN, CSN3_HUMAN, CSN4_HUMAN, CSN7A_HUMAN, CSN7B_HUMAN, CUL1_HUMAN, SKP1_HUMAN, CUL2_HUMAN, ELOB_HUMAN, BTBD2_HUMAN, DDB2_HUMAN, ERCC8_HUMAN, DCAF1_HUMAN, DCA11_HUMAN, A4_HUMAN, PRS7_HUMAN, TBB4B_HUMAN, UBC9_HUMAN, XPO2_HUMAN, XPO7_HUMAN, QSOX2_HUMAN, ILF3_HUMAN, TS101_HUMAN, WDR12_HUMAN, DDX1_HUMAN, SRSF2_HUMAN, PYR1_HUMAN, SSU72_HUMAN, MPCP_HUMAN, DDTL_HUMAN, UBR1_HUMAN, URM1_HUMAN, DD19A_HUMAN, TBB5_HUMAN, UBP14_HUMAN, UBE2Z_HUMAN, SYEP_HUMAN, XRN2_HUMAN, RFC5_HUMAN, TLK2_HUMAN, VP37B_HUMAN, MDC1_HUMAN, PTN11_HUMAN, KCC4_HUMAN, CAH9_HUMAN, RBCC1_HUMAN, EPAS1_HUMAN, HS90A_HUMAN, RD23B_HUMAN, VCAM1_HUMAN, FINC_HUMAN, ITA4_HUMAN, CFTR_HUMAN, MMS19_HUMAN, ABL1_HUMAN, P73_HUMAN, NC2B_HUMAN, PAXI_HUMAN, STRAA_HUMAN, SIR2_HUMAN, CLN5_HUMAN, UBP7_HUMAN, MSI2H_HUMAN, SART3_HUMAN, GID8_HUMAN, CALR_HUMAN, IQGA3_HUMAN, TBB2A_HUMAN, SLN11_HUMAN, PHC3_HUMAN, NOL9_HUMAN, IPO7_HUMAN, GCN1_HUMAN, APC7_HUMAN, SRP68_HUMAN, LSM8_HUMAN, RAGP1_HUMAN, PHC2_HUMAN, PPIH_HUMAN, IMDH2_HUMAN, PATZ1_HUMAN, CND1_HUMAN, INT9_HUMAN, CSK22_HUMAN, LAS1L_HUMAN, PELP1_HUMAN, POP1_HUMAN, CCAR2_HUMAN, TBA4A_HUMAN, IPO4_HUMAN, IMA3_HUMAN, CHD9_HUMAN, IPO5_HUMAN, SUGP2_HUMAN, CTND1_HUMAN, DX39A_HUMAN, SENP3_HUMAN, SRP72_HUMAN, SGO2_HUMAN, EHMT2_HUMAN, INT1_HUMAN, DNJB6_HUMAN, LSM3_HUMAN, PIAS1_HUMAN, SMC2_HUMAN, CDC73_HUMAN, SPT5H_HUMAN, PKCB1_HUMAN, TBB3_HUMAN, RBM4_HUMAN, SRP54_HUMAN, NOM1_HUMAN, PAF1_HUMAN, XRCC5_HUMAN, MTREX_HUMAN, ZN687_HUMAN, TBB8_HUMAN, HCD2_HUMAN, TBA1A_HUMAN, RM04_HUMAN, ETV6_HUMAN, CCNT1_HUMAN, PRP4_HUMAN, RBM15_HUMAN, ASCC3_HUMAN, TEX10_HUMAN, TNPO3_HUMAN, ATPA_HUMAN, LSM2_HUMAN, SAHH2_HUMAN, AKA11_HUMAN, APC1_HUMAN, ANC2_HUMAN, APC4_HUMAN, APC5_HUMAN, AN32E_HUMAN, RHG01_HUMAN, ARI3A_HUMAN, ARI3B_HUMAN, ARI5B_HUMAN, BAG3_HUMAN, BAZ2B_HUMAN, BMI1_HUMAN, BRD8_HUMAN, BRX1_HUMAN, C1QBP_HUMAN, CAN2_HUMAN, KNL1_HUMAN, CBX2_HUMAN, CBX4_HUMAN, CDC23_HUMAN, CDC26_HUMAN, CDK1_HUMAN, CD11A_HUMAN, CAF1B_HUMAN, CHD3_HUMAN, CHD6_HUMAN, CHD8_HUMAN, CLOCK_HUMAN, CNOT3_HUMAN, COR1B_HUMAN, INT11_HUMAN, CTR9_HUMAN, CUL7_HUMAN, CUL9_HUMAN, RT29_HUMAN, DNM1L_HUMAN, EP400_HUMAN, ETV3_HUMAN, WAC2A_HUMAN, FERM2_HUMAN, FOXC1_HUMAN, FOXK2_HUMAN, FOXP4_HUMAN, GLI3_HUMAN, GLIS3_HUMAN, GPN1_HUMAN, ILK_HUMAN, INT2_HUMAN, INT3_HUMAN, INT7_HUMAN, I2BP1_HUMAN, KCTD5_HUMAN, LEO1_HUMAN, LONM_HUMAN, LSM6_HUMAN, MACF1_HUMAN, MAEA_HUMAN, MAGC2_HUMAN, MBD2_HUMAN, MDN1_HUMAN, EVI1_HUMAN.MDS1_HUMAN, MED22_HUMAN, MEIS2_HUMAN, MIER1_HUMAN, MKLN1_HUMAN, MLF2_HUMAN, RM01_HUMAN, RM12_HUMAN, RM15_HUMAN, RM39_HUMAN, RM41_HUMAN, RM09_HUMAN, RT22_HUMAN, RT26_HUMAN, RT35_HUMAN, RT09_HUMAN, MSL1_HUMAN, MS3L1_HUMAN, MTA3_HUMAN, NP1L4_HUMAN, NIP7_HUMAN, NUP93_HUMAN, OLA1_HUMAN, PARVA_HUMAN, PBX2_HUMAN, PFKAP_HUMAN, RPB3_HUMAN, 2A5G_HUMAN, 2A5D_HUMAN, PP6R1_HUMAN, KAP0_HUMAN, KAP3_HUMAN, PWP1_HUMAN, RAE1L_HUMAN, RALY_HUMAN, RBP10_HUMAN, RANB9_HUMAN, RFX1_HUMAN, MCE1_HUMAN, RINI_HUMAN, RPP30_HUMAN, RUNX1_HUMAN, SP130_HUMAN, SCFD1_HUMAN, SCYL2_HUMAN, SC16A_HUMAN, SETD2_HUMAN, SIN3B_HUMAN, SMCA2_HUMAN, SMC3_HUMAN, EST1A_HUMAN, SOX6_HUMAN, SP2_HUMAN, SRSF4_HUMAN, LA_HUMAN, TAF2_HUMAN, TAF6L_HUMAN, TBX3_HUMAN, HTF4_HUMAN, TSP1_HUMAN, TIA1_HUMAN, TIAR_HUMAN, TNPO1_HUMAN, TREF1_HUMAN, TRI33_HUMAN, TBG1_HUMAN, STPAP_HUMAN, UBR4_HUMAN, UBR5_HUMAN, USP9X_HUMAN, UT14A_HUMAN, VP33A_HUMAN, WDR26_HUMAN, WDR3_HUMAN, XPO5_HUMAN, ZBT10_HUMAN, ZBTB5_HUMAN, ZBT7A_HUMAN, ZCHC8_HUMAN, ZEB2_HUMAN, ZFHX4_HUMAN, ZMYM2_HUMAN, ZN462_HUMAN, ZN536_HUMAN, ZN609_HUMAN, ZN644_HUMAN, ZN787_HUMAN, CDX1_HUMAN, EGFR_HUMAN, GRP75_HUMAN, NUCB1_HUMAN, NUCB2_HUMAN, RCN2_HUMAN, RGS14_HUMAN, FZR1_HUMAN, HNRPK_HUMAN, PYRG2_HUMAN, EHD4_HUMAN, PLIN3_HUMAN, EFTU_HUMAN, VINC_HUMAN, XPP1_HUMAN, KCC1D_HUMAN, DCPS_HUMAN, EF2_HUMAN, GNAI3_HUMAN, HS71L_HUMAN, PP1A_HUMAN, PPP5_HUMAN, STK24_HUMAN, TWF2_HUMAN, UBA3_HUMAN, 1433E_HUMAN, 1433F_HUMAN, CD37L_HUMAN, STAU1_HUMAN, KEAP1_HUMAN, PTN1_HUMAN, ARNT2_HUMAN, UBP16_HUMAN, SETD7_HUMAN, PARP4_HUMAN, TRIB1_HUMAN, JUNB_HUMAN, HUWE1_HUMAN, DMAP1_HUMAN, TBX2_HUMAN, PTF1A_HUMAN, PPARG_HUMAN, OBSL1_HUMAN, CCDC8_HUMAN, DPA1_HUMAN, CD1B_HUMAN, ZN397_HUMAN, ANXA1_HUMAN, PLPHP_HUMAN, OXSM_HUMAN, RET1_HUMAN, PRDC1_HUMAN, CYB5_HUMAN, PAK2_HUMAN, PICAL_HUMAN, GINM1_HUMAN, ZN589_HUMAN, DCA16_HUMAN, ZN268_HUMAN, DMC1_HUMAN, FOSL2_HUMAN, LYPD3_HUMAN, FOS_HUMAN, PICK1_HUMAN, BASP1_HUMAN, CSTF2_HUMAN, CSTFT_HUMAN, CSTF3_HUMAN, DD19B_HUMAN, FPPS_HUMAN, GFPT1_HUMAN, GFPT2_HUMAN, IPO11_HUMAN, IPO9_HUMAN, ECM29_HUMAN, METK1_HUMAN, METK2_HUMAN, NDRG1_HUMAN, MDHM_HUMAN, RAVR1_HUMAN, STOM_HUMAN, TNPO2_HUMAN, G6PD_HUMAN, MAT2B_HUMAN, NCPR_HUMAN, FCL_HUMAN, NTRK1_HUMAN, MAML3_HUMAN, MAML2_HUMAN, NU107_HUMAN, MED23_HUMAN, ZN641_HUMAN, RN146_HUMAN, TFEB_HUMAN, PYM1_HUMAN, SEP10_HUMAN, CCNB1_HUMAN, GL1AD_HUMAN.GRL1A_HUMAN.MYZAP_HUMAN, DRG1_HUMAN, WEE1_HUMAN, HAUS7_HUMAN, PDLI7_HUMAN, LST8_HUMAN, AP3M2_HUMAN, RAD18_HUMAN, SDCG3_HUMAN, ABLM1_HUMAN, FBX9_HUMAN, RIMKB_HUMAN, FBLI1_HUMAN, CE030_HUMAN, LTV1_HUMAN, REN3B_HUMAN, SIN1_HUMAN, DVL3_HUMAN, MPLKI_HUMAN, HAUS1_HUMAN, GORS1_HUMAN, MEX3D_HUMAN, FARP2_HUMAN, DEN1B_HUMAN, UBIP1_HUMAN, TNIP2_HUMAN, KAP1_HUMAN, CEP78_HUMAN, MEX3C_HUMAN, CC85C_HUMAN, CRY1_HUMAN, TGFI1_HUMAN, RELB_HUMAN, TFE3_HUMAN, AVEN_HUMAN, NUFP1_HUMAN, HAUS8_HUMAN, UVRAG_HUMAN, ZCCHV_HUMAN, ZFYV1_HUMAN, SYDE1_HUMAN, SIK2_HUMAN, RENT2_HUMAN, TISB_HUMAN, NOC2L_HUMAN, BYST_HUMAN, FR1OP_HUMAN, ZC12A_HUMAN, ZC3HF_HUMAN, SEPT8_HUMAN, GLCI1_HUMAN, CEP41_HUMAN, CNOT4_HUMAN, EPN4_HUMAN, CEP55_HUMAN, TISD_HUMAN, TJAP1_HUMAN, NOB1_HUMAN, PAIP2_HUMAN, S7A6O_HUMAN, DVL2_HUMAN, DYR1A_HUMAN, RPAP2_HUMAN, HAUS5_HUMAN, AP2M1_HUMAN, HAUS4_HUMAN, KC1E_HUMAN, ARFG1_HUMAN, PAK4_HUMAN, ZNRF2_HUMAN, TAB2_HUMAN, ARRB2_HUMAN, SC23A_HUMAN, CHMP7_HUMAN, IF2B_HUMAN, CHM2B_HUMAN, ARFG2_HUMAN, STK3_HUMAN, AJUBA_HUMAN, DTBP1_HUMAN, EIF3D_HUMAN, DEN1A_HUMAN, TRIM5_HUMAN, SC24B_HUMAN, NUMBL_HUMAN, MAP2_HUMAN, SEPT7_HUMAN, ADDG_HUMAN, DCP1A_HUMAN, STK4_HUMAN, PDD2L_HUMAN, MEF2D_HUMAN, RIPK1_HUMAN, PPM1B_HUMAN, CNOT2_HUMAN, IQEC1_HUMAN, AP3S2_HUMAN, ZYX_HUMAN, GMIP_HUMAN, AP4M1_HUMAN, RL24_HUMAN, HAUS3_HUMAN, GBB1_HUMAN, GOGA2_HUMAN, AP3M1_HUMAN, SC23B_HUMAN, IKBE_HUMAN, TBK1_HUMAN, AP1G2_HUMAN, LPIN1_HUMAN, EDC3_HUMAN, MKNK1_HUMAN, ECD_HUMAN, DDX6_HUMAN, EI2BD_HUMAN, SNX17_HUMAN, DGKZ_HUMAN, CLSPN_HUMAN, BL1S5_HUMAN, ESPL1_HUMAN, SNP29_HUMAN, EPN1_HUMAN, IF4E2_HUMAN, AP4B1_HUMAN, HIRP3_HUMAN, PDPK1_HUMAN, AFTIN_HUMAN, NACC1_HUMAN, TCOF_HUMAN, EI2BE_HUMAN, OCRL_HUMAN, UBAP1_HUMAN, TOM1_HUMAN, ARFG3_HUMAN, TRIP6_HUMAN, DAB2_HUMAN, RABL6_HUMAN, LIMD1_HUMAN, PJA2_HUMAN, PEX19_HUMAN, HAUS6_HUMAN, DDX5_HUMAN, IKBA_HUMAN, PP4R1_HUMAN, ABCF1_HUMAN, RAPH1_HUMAN, SC24D_HUMAN, XPA_HUMAN, SQSTM_HUMAN, STAT2_HUMAN, C2D1A_HUMAN, SEPT9_HUMAN, SPN90_HUMAN, SYNRG_HUMAN, RAF1_HUMAN, GPSM1_HUMAN, SHRM1_HUMAN, CDC20_HUMAN, A16L1_HUMAN, CEP97_HUMAN, MYPN_HUMAN, STRN3_HUMAN, NOLC1_HUMAN, STK10_HUMAN, AP3B1_HUMAN, AP1M1_HUMAN, GPN3_HUMAN, SC24C_HUMAN, HAUS2_HUMAN, SEPT2_HUMAN, EPS15_HUMAN, BCR_HUMAN, HIF1N_HUMAN, RL23A_HUMAN, EIF3E_HUMAN, BL1S4_HUMAN, IF2P_HUMAN, WIPI4_HUMAN, COPD_HUMAN, ADDA_HUMAN, MALT1_HUMAN, IF4G2_HUMAN, COPG2_HUMAN, IF2A_HUMAN, AP3D1_HUMAN, AP3S1_HUMAN, IRS2_HUMAN, AAK1_HUMAN, CLAP2_HUMAN, PI4KB_HUMAN, RICTR_HUMAN, SYSC_HUMAN, SSH2_HUMAN, EI2BG_HUMAN, ATG5_HUMAN, T2FA_HUMAN, AURKA_HUMAN, SMAD4_HUMAN, SYAP1_HUMAN, KIBRA_HUMAN, ERC6L_HUMAN, ZN330_HUMAN, AP4E1_HUMAN, NP1L1_HUMAN, COPB_HUMAN, MB12A_HUMAN, SHQ1_HUMAN, IF2G_HUMAN, ENAH_HUMAN, COPB2_HUMAN, DMD_HUMAN, CNOT7_HUMAN, NAF1_HUMAN, IF5_HUMAN, VASP_HUMAN, COPG1_HUMAN, BUB1B_HUMAN, KC1A_HUMAN, DKC1_HUMAN, RS2_HUMAN, ATG3_HUMAN, UBA5_HUMAN, AP2B1_HUMAN, COPA_HUMAN, IF4B_HUMAN, VP37A_HUMAN, CBL_HUMAN, GRDN_HUMAN, VPS28_HUMAN, GORS2_HUMAN, BCAS3_HUMAN, ARP3_HUMAN, AP1B1_HUMAN, CSDE1_HUMAN, BICD2_HUMAN, DCAF7_HUMAN, SRP19_HUMAN, CNOT9_HUMAN, TR150_HUMAN, GBB2_HUMAN, SMAD5_HUMAN, CE170_HUMAN, TBL1X_HUMAN, TNIP1_HUMAN, MTOR_HUMAN, CCDC6_HUMAN, ARC1A_HUMAN, COPE_HUMAN, RS17_HUMAN, EIF3L_HUMAN, MK07_HUMAN, ARAP3_HUMAN, HPS6_HUMAN, M4K4_HUMAN, AP1S2_HUMAN, NHP2_HUMAN, EDC4_HUMAN, BUB3_HUMAN, WNK1_HUMAN, LS14A_HUMAN, DHX16_HUMAN, M3K7_HUMAN, RPB2_HUMAN, RPAB1_HUMAN, MKL2_HUMAN, TRADD_HUMAN, FERM1_HUMAN, IKBB_HUMAN, DBR1_HUMAN, PASK_HUMAN, AP1G1_HUMAN, PDCD4_HUMAN, DAXX_HUMAN, SETB1_HUMAN, RPB7_HUMAN, BCL10_HUMAN, PDCD6_HUMAN, KAPCB_HUMAN, SEC13_HUMAN, WASC5_HUMAN, T2FB_HUMAN, EIF3C_HUMAN, EI2BB_HUMAN, ABCE1_HUMAN, SHC1_HUMAN, CPSF6_HUMAN, MCTS1_HUMAN, DNJA4_HUMAN, PRP31_HUMAN, RPB9_HUMAN, FKB15_HUMAN, AP1S1_HUMAN, RS3A_HUMAN, TAB1_HUMAN, IWS1_HUMAN, CNOT1_HUMAN, GGA2_HUMAN, RS3_HUMAN, NED4L_HUMAN, PIHD1_HUMAN, ZO2_HUMAN, TMED8_HUMAN, COPZ1_HUMAN, WRIP1_HUMAN, RS10_HUMAN, PPP6_HUMAN, RS7_HUMAN, SCYL1_HUMAN, LSM4_HUMAN, YAP1_HUMAN, FYCO1_HUMAN, RU2A_HUMAN, TB182_HUMAN, WASC4_HUMAN, SRRT_HUMAN, KPRA_HUMAN, RS9_HUMAN, ARP2_HUMAN, YBOX1_HUMAN, RS16_HUMAN, MP2K7_HUMAN, RPAB4_HUMAN, RPAP1_HUMAN, NEK9_HUMAN, RS18_HUMAN, RS8_HUMAN, ARPC3_HUMAN, CSK21_HUMAN, AP2A1_HUMAN, RS4X_HUMAN, PDLI5_HUMAN, EIF3H_HUMAN, PP4C_HUMAN, KAP2_HUMAN, LSM1_HUMAN, RS23_HUMAN, PI3R4_HUMAN, 2ABA_HUMAN, WDHD1_HUMAN, ARPC4_HUMAN, DPOA2_HUMAN, CD123_HUMAN, RS11_HUMAN, ERF1_HUMAN, PP6R3_HUMAN, EI2BA_HUMAN, ARP5L_HUMAN, CSK2B_HUMAN, LIN9_HUMAN, GRB10_HUMAN, SLAI2_HUMAN, CRTC1_HUMAN, TTLL4_HUMAN, TCAM1_HUMAN, SPA5L_HUMAN, CRTC3_HUMAN, CDC27_HUMAN, SMAP2_HUMAN, KCTD3_HUMAN, SHKB1_HUMAN, RL18_HUMAN, PUM1_HUMAN, IRAK1_HUMAN, LPIN3_HUMAN, RPGP1_HUMAN, UBP2L_HUMAN, RPGP2_HUMAN, PEX5_HUMAN, HOOK2_HUMAN, IASPP_HUMAN, PATL1_HUMAN, TYSD1_HUMAN, LPP_HUMAN, SMAP1_HUMAN, VIME_HUMAN, RPC4_HUMAN, REL_HUMAN, RPGF6_HUMAN, NFKB1_HUMAN, RN216_HUMAN, SMU1_HUMAN, ASCC1_HUMAN, PABP4_HUMAN, SC31A_HUMAN, TF65_HUMAN, MADD_HUMAN, KDM3B_HUMAN, SC24A_HUMAN, PABP1_HUMAN, RTCB_HUMAN, MTMR9_HUMAN, RTN3_HUMAN, RENT1_HUMAN, CLAP1_HUMAN, AKP8L_HUMAN, P3C2B_HUMAN, NFKB2_HUMAN, NCOA3_HUMAN, SNX24_HUMAN, MP2K2_HUMAN, MYO10_HUMAN, CAMP2_HUMAN, RIC8B_HUMAN, ZO1_HUMAN, MKL1_HUMAN, ALEX_HUMAN.GNAS1_HUMAN.GNAS2_HUMAN.GNAS3_HUMAN, S23IP_HUMAN, IKKA_HUMAN, AR6P4_HUMAN, WDR34_HUMAN, TBB4A_HUMAN, DPOD1_HUMAN, FOXK1_HUMAN, RS13_HUMAN, EP15R_HUMAN, SSRP1_HUMAN, SNRPA_HUMAN, ARPC2_HUMAN, KAPCA_HUMAN, SHIP2_HUMAN, CHM2A_HUMAN, PELO_HUMAN, LIN7C_HUMAN, AAGAB_HUMAN, ABRX2_HUMAN, RU2B_HUMAN, GPKOW_HUMAN, DPOD3_HUMAN, M3K20_HUMAN, WDR61_HUMAN, RS25_HUMAN, WDR82_HUMAN, RSSA_HUMAN, MAPK2_HUMAN, TBA1B_HUMAN, RL5_HUMAN, ANM3_HUMAN, GBRL1_HUMAN, GAPD1_HUMAN, ETFB_HUMAN, ARC1B_HUMAN, RIPR1_HUMAN, RHG29_HUMAN, TELO2_HUMAN, STRAP_HUMAN, DPOD2_HUMAN, RS14_HUMAN, EF2K_HUMAN, ARHG1_HUMAN, 1433G_HUMAN, SERA_HUMAN, RS5_HUMAN, CEP85_HUMAN, RPTOR_HUMAN, LEG7_HUMAN, VAC14_HUMAN, UBP47_HUMAN, AKTS1_HUMAN, ANKS6_HUMAN, MEF2A_HUMAN, CRY2_HUMAN, KAT7_HUMAN, SESQ1_HUMAN, ARP3B_HUMAN, RL7A_HUMAN, FOXO3_HUMAN, PTTG1_HUMAN, LORI_HUMAN, JADE3_HUMAN, HNRPM_HUMAN, PITX1_HUMAN, CCNB2_HUMAN, DEK_HUMAN, BIN3_HUMAN, GPS2_HUMAN, SIK1_HUMAN, TTP_HUMAN, SAPC2_HUMAN, S10A7_HUMAN, RS6_HUMAN, CDC7_HUMAN, ESS2_HUMAN, DDX17_HUMAN, PKP3_HUMAN, SNTB2_HUMAN, ANR54_HUMAN, SNX21_HUMAN, CLASR_HUMAN, KC1D_HUMAN, RL28_HUMAN, UTP15_HUMAN, PR38A_HUMAN, RL8_HUMAN, NFIA_HUMAN, GAB2_HUMAN, GO45_HUMAN, LS14B_HUMAN, PPIL4_HUMAN, RMP_HUMAN, SESQ2_HUMAN, SMN_HUMAN, TAF13_HUMAN, MAX_HUMAN, M3K8_HUMAN, DAB2P_HUMAN, TRI37_HUMAN, CHM4C_HUMAN, GANP_HUMAN, HSPB8_HUMAN, NEK4_HUMAN, RASF9_HUMAN, BORG5_HUMAN, DJC11_HUMAN, MLXIP_HUMAN, MLXPL_HUMAN, GPBL1_HUMAN, RFWD3_HUMAN, RL6_HUMAN, EAF1_HUMAN, RL4_HUMAN, TAF12_HUMAN, ERRFI_HUMAN, RL10A_HUMAN, ERCC2_HUMAN, SRSF1_HUMAN, RBMS2_HUMAN, MITF_HUMAN, ACD_HUMAN, IQCB1_HUMAN, CASC3_HUMAN, STN1_HUMAN, DI3L1_HUMAN, CARF_HUMAN, LIN37_HUMAN, TCF25_HUMAN, BCLF1_HUMAN, PJA1_HUMAN, POC5_HUMAN, PWP2_HUMAN, DHX35_HUMAN, NEK1_HUMAN, RBMS1_HUMAN, A16L2_HUMAN, KLF5_HUMAN, RUSC2_HUMAN, CINP_HUMAN, OCAD1_HUMAN, PRP4B_HUMAN, RPGF2_HUMAN, WDR43_HUMAN, PNO1_HUMAN, FBXW5_HUMAN, RED_HUMAN, UTP4_HUMAN, RNF10_HUMAN, CDT1_HUMAN, MCRS1_HUMAN, SPAT2_HUMAN, T2H2L_HUMAN, WDR74_HUMAN, TTF2_HUMAN, CBPC1_HUMAN, AGO3_HUMAN, KSR1_HUMAN, SRSF6_HUMAN, SMG7_HUMAN, PER1_HUMAN, LSM11_HUMAN, BL1S3_HUMAN, GTSE1_HUMAN, RHG12_HUMAN, PNISR_HUMAN, NIPS2_HUMAN, PKRI1_HUMAN, RASF1_HUMAN, GBB4_HUMAN, FIP1_HUMAN, FA98B_HUMAN, AAAS_HUMAN, GCP3_HUMAN, KI20A_HUMAN, TNKS1_HUMAN, AATF_HUMAN, SKT_HUMAN, MPIP2_HUMAN, TF3C5_HUMAN, LUC7L_HUMAN, MSH5_HUMAN, NCOA4_HUMAN, TRAK1_HUMAN, CYLD_HUMAN, PAN3_HUMAN, PRCC_HUMAN, CP110_HUMAN, EID1_HUMAN, RASF3_HUMAN, NEDD1_HUMAN, RL21_HUMAN, RPRD2_HUMAN, SNX18_HUMAN, SPICE_HUMAN, SRSF7_HUMAN, SNX16_HUMAN, FBXW8_HUMAN, M3K3_HUMAN, RCL1_HUMAN, SPF45_HUMAN, RU17_HUMAN, TFPT_HUMAN, TRAK2_HUMAN, DUS7_HUMAN, DVL1_HUMAN, WDTC1_HUMAN, MIS12_HUMAN, SNPC2_HUMAN, FANCG_HUMAN, APC10_HUMAN, RNPS1_HUMAN, SMCE1_HUMAN, GNPAT_HUMAN, MED12_HUMAN, PLK2_HUMAN, FBXL4_HUMAN, FRM4B_HUMAN, LZTS2_HUMAN, NOP58_HUMAN, PRKX_HUMAN, K0556_HUMAN, NONO_HUMAN, SLU7_HUMAN, UTP18_HUMAN, NIPS1_HUMAN, XRN1_HUMAN, ERI1_HUMAN, EVL_HUMAN, RFIP1_HUMAN, TOB2_HUMAN, FKBPL_HUMAN, SRSF5_HUMAN, HM20B_HUMAN, XRCC3_HUMAN, AMER1_HUMAN, SNRK_HUMAN, TF3C3_HUMAN, TRIP4_HUMAN, DOCK6_HUMAN, HNRH3_HUMAN, STXB3_HUMAN, SOX13_HUMAN, NCS1_HUMAN, ARHG3_HUMAN, DCP1B_HUMAN, M3K1_HUMAN, PAR12_HUMAN, IF2B1_HUMAN, PCGF5_HUMAN, RASF7_HUMAN, TNIK_HUMAN, MKS1_HUMAN, FBRL_HUMAN, NFX1_HUMAN, PLD2_HUMAN, HP1B3_HUMAN, EXOS5_HUMAN, ERG7_HUMAN, DDX47_HUMAN, EID2_HUMAN, KLDC3_HUMAN, SNR40_HUMAN, ADIP_HUMAN, CE350_HUMAN, HEXI2_HUMAN, SPAS2_HUMAN, RHOF_HUMAN, SCHI1_HUMAN, PAXI1_HUMAN, REN3A_HUMAN, CNTRB_HUMAN, GEMI2_HUMAN, KCD20_HUMAN, ERBIN_HUMAN, STAM2_HUMAN, NR4A1_HUMAN, YETS4_HUMAN, MCM8_HUMAN, CPSF4_HUMAN, ASH2L_HUMAN, RHG21_HUMAN, EAF2_HUMAN, PLRG1_HUMAN, TOLIP_HUMAN, COIL_HUMAN, NDE1_HUMAN, DBF4A_HUMAN, BACD2_HUMAN, SNPC3_HUMAN, WRP73_HUMAN, DDX56_HUMAN, F10C1_HUMAN, SUGP1_HUMAN, AXIN1_HUMAN, BMP2K_HUMAN, PITM2_HUMAN, TDIF1_HUMAN, UTP6_HUMAN, N4BP3_HUMAN, Z3H7A_HUMAN, RL18A_HUMAN, VPS52_HUMAN, ENKD1_HUMAN, AF9_HUMAN, MPP9_HUMAN, PSRC1_HUMAN, PDE4B_HUMAN, RNC_HUMAN, KLH20_HUMAN, RFIP5_HUMAN, ZBTB1_HUMAN, CHP1_HUMAN, TERF1_HUMAN, GCP2_HUMAN, SOSB2_HUMAN, CEPT1_HUMAN, NBEL2_HUMAN, ORC3_HUMAN, BRE1A_HUMAN, LCOR_HUMAN, RECQ1_HUMAN, FNBP1_HUMAN, NKX61_HUMAN, TPX2_HUMAN, PF21A_HUMAN, JHD2C_HUMAN, SMBT1_HUMAN, SMCA1_HUMAN, HXA10_HUMAN, HXB9_HUMAN, PSIP1_HUMAN, DLX5_HUMAN, FBP1L_HUMAN, H2AY_HUMAN, KDM2A_HUMAN, NKX25_HUMAN, SATB2_HUMAN, TPM1_HUMAN, HXC13_HUMAN, HXD13_HUMAN, KIF2C_HUMAN, MA7D3_HUMAN, SATB1_HUMAN, TBP_HUMAN, TFAP4_HUMAN, TXND5_HUMAN, CAMP1_HUMAN, CGBP1_HUMAN, CREM_HUMAN, TF3C4_HUMAN, MBD1_HUMAN, MYH7_HUMAN, NFAC1_HUMAN, NFIC_HUMAN, NFIX_HUMAN, COT2_HUMAN, OGT1_HUMAN, PBX1_HUMAN, PITX2_HUMAN, TPM2_HUMAN, ZN143_HUMAN, DDX24_HUMAN, RFA2_HUMAN, MCM2_HUMAN, ZMIZ1_HUMAN, SMUF2_HUMAN, MTMR1_HUMAN, PTPRE_HUMAN, EYA3_HUMAN, NUD16_HUMAN, G45IP_HUMAN, AROS_HUMAN, EBP2_HUMAN, RL3L_HUMAN, SPOP_HUMAN, F120B_HUMAN, 2ABD_HUMAN, NSMF_HUMAN, TAXB1_HUMAN, JPH1_HUMAN, TSKS_HUMAN, NFIL3_HUMAN, PP2AA_HUMAN, CE164_HUMAN, KCC2D_HUMAN, KHDR2_HUMAN, TCPW_HUMAN, ZN263_HUMAN, PAK1_HUMAN, DDAH2_HUMAN, PDLI1_HUMAN, HIBCH_HUMAN, APJ_HUMAN, ERBB4_HUMAN, ERBB3_HUMAN, FANCA_HUMAN, PLPL2_HUMAN, FOXA1_HUMAN, BRCA1_HUMAN, EGLN3_HUMAN, Q9H4D1_HUMAN.RIPK4_HUMAN, HACD1_HUMAN, HIF1A_HUMAN, TXNIP_HUMAN, RNF4_HUMAN, UB2R1_HUMAN, NUPL2_HUMAN, NF2L2_HUMAN, ARNT_HUMAN, RIPK2_HUMAN, CAR16_HUMAN.RFWD2_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P49908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenoprotein P [Source:HGNC Symbol;Acc:HGNC:10751]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEPP1_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGFR_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGF_HUMAN, SHC1_HUMAN, GRB2_HUMAN, SOS1_HUMAN, AP2C_HUMAN, HBEGF_HUMAN, ERBB2_HUMAN, NOTC3_HUMAN, HS90A_HUMAN, CDC37_HUMAN, P85A_HUMAN, GAB1_HUMAN, PLCG1_HUMAN, CBL_HUMAN, L1CAM_HUMAN, GPNMB_HUMAN, IQEC1_HUMAN, SDC3_HUMAN, TGFA_HUMAN, GNAI1_HUMAN, GNAI3_HUMAN, PK3CB_HUMAN, EREG_HUMAN, ERBB3_HUMAN, NRG4_HUMAN, ERBB4_HUMAN, AREG_HUMAN, BTC_HUMAN, NRG1_HUMAN, SRC_HUMAN, ANDR_HUMAN, SHIP2_HUMAN, RGS16_HUMAN, PLEC_HUMAN, ARF4_HUMAN, K1C18_HUMAN, RASA1_HUMAN, FRS2_HUMAN, PLD1_HUMAN, KPCA_HUMAN, STAT3_HUMAN, NCK2_HUMAN, NCK1_HUMAN, RIPK1_HUMAN, MP2K1_HUMAN, P3C2B_HUMAN, I17RD_HUMAN, CSK_HUMAN, KAP0_HUMAN, PTK6_HUMAN, ERRFI_HUMAN, STABP_HUMAN, PTN1_HUMAN, HD_HUMAN, STA5A_HUMAN, C2D1A_HUMAN, GRB10_HUMAN, SOCS1_HUMAN, STAT1_HUMAN, PTN11_HUMAN, M3K14_HUMAN, PAK1_HUMAN, PTN6_HUMAN, STA5B_HUMAN, DOK2_HUMAN, VAV2_HUMAN, VAV_HUMAN, CBLB_HUMAN, CAV1_HUMAN, CBLC_HUMAN, PLS1_HUMAN, K1C17_HUMAN, K2C8_HUMAN, K2C7_HUMAN, SMD2_HUMAN, ATX2_HUMAN, SOCS3_HUMAN, MK01_HUMAN, FOS_HUMAN, CAV2_HUMAN, TLR4_HUMAN, AT1A1_HUMAN, S10A7_HUMAN, CLCA_HUMAN, JAK2_HUMAN, 1433S_HUMAN, JAK1_HUMAN, MUC1_HUMAN, CASP1_HUMAN, CASP7_HUMAN, G3P_HUMAN, ITB4_HUMAN, LEG3_HUMAN, LYN_HUMAN, S10A9_HUMAN, EGR1_HUMAN, BAG1_HUMAN, AT1B1_HUMAN, HXC10_HUMAN, 4F2_HUMAN, SEC13_HUMAN, TLR2_HUMAN, CASP3_HUMAN, TBA1A_HUMAN, FAK2_HUMAN, GOLM1_HUMAN, EXOC7_HUMAN, CRKL_HUMAN, MET_HUMAN, KPCE_HUMAN, SRC8_HUMAN, CRK_HUMAN, FKBP8_HUMAN, SYN1_HUMAN, PTPRG_HUMAN, HDAC6_HUMAN, ERCC1_HUMAN, HSP7C_HUMAN, MK08_HUMAN, SH3G2_HUMAN, BAKOR_HUMAN, PK3C3_HUMAN, RUBIC_HUMAN, BECN1_HUMAN, UVRAG_HUMAN, SNP25_HUMAN, HS71B_HUMAN.HSP77_HUMAN, PLCG2_HUMAN, SH2B1_HUMAN, SLAP1_HUMAN, PHOCN_HUMAN, MAST1_HUMAN, SH2B3_HUMAN, THIO_HUMAN, ANXA2_HUMAN, GRAP2_HUMAN, ARF6_HUMAN, UBC_HUMAN, TBA1A_HUMAN.TBA1B_HUMAN, ESR1_HUMAN, ANS1B_HUMAN, ROR1_HUMAN, AGO2_HUMAN, GCR_HUMAN, SRBS2_HUMAN, ESR2_HUMAN, S10A4_HUMAN, ITB2_HUMAN, ABL1_HUMAN, MATR3_HUMAN, EXOC4_HUMAN, CAN7_HUMAN, IST1_HUMAN, GRP75_HUMAN, EXOC6_HUMAN, SH22A_HUMAN, NUMBL_HUMAN, DJC13_HUMAN, RBNS5_HUMAN, RIN1_HUMAN, COF1_HUMAN, TRAF2_HUMAN, TENS3_HUMAN, EXOC8_HUMAN, EXOC3_HUMAN, PSA7_HUMAN, 1433T_HUMAN, TAU_HUMAN, JIP1_HUMAN, PHAG1_HUMAN, KPCB_HUMAN, PIN4_HUMAN, YES_HUMAN, AIP_HUMAN, NEDD4_HUMAN, ANS1A_HUMAN, RAGE_HUMAN, LAP4B_HUMAN, DICER_HUMAN, AURKA_HUMAN, A4_HUMAN, RACK1_HUMAN, ABL2_HUMAN, P55G_HUMAN, LIGO1_HUMAN, LCP2_HUMAN, FKBP4_HUMAN, P85B_HUMAN, IRS1_HUMAN, HSPB1_HUMAN, PDC6I_HUMAN, SC5A1_HUMAN, SPCS2_HUMAN, PP2AB_HUMAN, A0A0A0MT22_HUMAN.PTPRC_HUMAN.X6R433_HUMAN, STAM2_HUMAN, EXOC2_HUMAN, ARBK1_HUMAN, MIF_HUMAN, PTPRB_HUMAN, AKT1_HUMAN, ARRB2_HUMAN, SH3K1_HUMAN, DP13A_HUMAN, PPP5_HUMAN, TM1L1_HUMAN, ZAP70_HUMAN, IQGA1_HUMAN, CALM1_HUMAN.CALM2_HUMAN.CALM3_HUMAN, UFO_HUMAN, JIP2_HUMAN, FGR_HUMAN, RAB7A_HUMAN, CAVN1_HUMAN, EHD4_HUMAN, CAV3_HUMAN, GDIA_HUMAN, LAT_HUMAN, PTN22_HUMAN, XPF_HUMAN, FAAA_HUMAN, ITSN2_HUMAN, STAP2_HUMAN, IBP3_HUMAN, CHIP_HUMAN, ANXA1_HUMAN.B5BU38_HUMAN, APBB1_HUMAN, FRK_HUMAN, STAT2_HUMAN, M3K12_HUMAN, AHNK_HUMAN, CYLC2_HUMAN, PRKDC_HUMAN, TCTP_HUMAN, ATPG_HUMAN, PSMD4_HUMAN, RAB3A_HUMAN, LRP1_HUMAN, VAPA_HUMAN, EPS15_HUMAN, RABX5_HUMAN, CADH1_HUMAN, CBR1_HUMAN, FES_HUMAN, ITK_HUMAN, RET_HUMAN, SH21A_HUMAN, FKBP5_HUMAN, GELS_HUMAN, MAPK3_HUMAN, WASL_HUMAN, MPIP3_HUMAN, IMA5_HUMAN, KSYK_HUMAN, HDAC7_HUMAN, OAZ1_HUMAN, CSRP1_HUMAN, SHC4_HUMAN, FINC_HUMAN, STIP1_HUMAN, UCHL1_HUMAN, ENPL_HUMAN, PTN12_HUMAN, CDK1_HUMAN, AP2A1_HUMAN, EEA1_HUMAN, PIM1_HUMAN, TAB1_HUMAN, SLAP2_HUMAN, CKLF8_HUMAN, ARPC5_HUMAN, PLAK_HUMAN, TRBP2_HUMAN, CD59_HUMAN, GBRL2_HUMAN, EF1G_HUMAN, ARRB1_HUMAN, RGS4_HUMAN, CHIA_HUMAN, AP2M1_HUMAN, BMX_HUMAN, KPCZ_HUMAN, CTND1_HUMAN, BLK_HUMAN, NEMO_HUMAN, ZN510_HUMAN, CAMLG_HUMAN, HCK_HUMAN, 1433B_HUMAN, TLN1_HUMAN, Q6PK50_HUMAN, SOCS6_HUMAN, PLCH1_HUMAN, AKA12_HUMAN, PRDX1_HUMAN, AMPO_HUMAN, TPIS_HUMAN, KAP1_HUMAN, DOK1_HUMAN, IRS4_HUMAN, NECD_HUMAN, MK14_HUMAN, SNX9_HUMAN, RAPH1_HUMAN, TGFB1_HUMAN, HSP74_HUMAN, ACTN4_HUMAN, PTN18_HUMAN, PLPL2_HUMAN, ADRM1_HUMAN, LAMP1_HUMAN, 1433Z_HUMAN, CNTN2_HUMAN, DCTN2_HUMAN, PTPRJ_HUMAN, VP33B_HUMAN, CHD5_HUMAN, STX17_HUMAN, CO9A3_HUMAN, PGFRA_HUMAN, MK09_HUMAN, DNJC4_HUMAN, DYHC1_HUMAN, FAK1_HUMAN, UB2V2_HUMAN, SYUA_HUMAN, SOS2_HUMAN, NUMB_HUMAN, ITSN1_HUMAN, RB11A_HUMAN, SH3L3_HUMAN, Q96D37_HUMAN, H31_HUMAN, RAF1_HUMAN, NOE1_HUMAN, RPGF1_HUMAN, SH3G3_HUMAN, M3K3_HUMAN, TENS4_HUMAN, PDK3_HUMAN, ARHG7_HUMAN, HGS_HUMAN, SEPP1_HUMAN, ALDOA_HUMAN, MDHC_HUMAN, P3C2A_HUMAN, NTRK2_HUMAN, CTNA1_HUMAN, MCM5_HUMAN, MCM7_HUMAN, KCTD9_HUMAN, TNR1A_HUMAN, BAIP2_HUMAN, WASF3_HUMAN, GAB2_HUMAN, FANCC_HUMAN, AHSA1_HUMAN, EZRI_HUMAN, PTGDS_HUMAN, SNX1_HUMAN, PTN2_HUMAN, ANXA1_HUMAN, XRCC6_HUMAN, TBA4A_HUMAN, ICAM1_HUMAN, SCAM1_HUMAN, SCAM3_HUMAN, KCC2A_HUMAN, TENA_HUMAN, CEBPB_HUMAN, KCC2G_HUMAN, PLD2_HUMAN, NHRF1_HUMAN, TNR6_HUMAN, GRB7_HUMAN, KAPCA_HUMAN, GRB14_HUMAN, CLH2_HUMAN, 41_HUMAN, CD44_HUMAN, AGTR1_HUMAN, ACTS_HUMAN, DEGS1_HUMAN, RPGP1_HUMAN, BRAF_HUMAN, VAV3_HUMAN, SNX6_HUMAN, SNX4_HUMAN, SNX2_HUMAN, CD82_HUMAN, MPIP1_HUMAN, ITA5_HUMAN, GNAI2_HUMAN, UBB_HUMAN, CD166_HUMAN, CTNB1_HUMAN, MIS_HUMAN, ZO1_HUMAN, CEAM1_HUMAN, ACK1_HUMAN, FER_HUMAN, PGFRB_HUMAN, KPCD_HUMAN, PTPRS_HUMAN, ZPR1_HUMAN, KPCD1_HUMAN, H31T_HUMAN, ELF3_HUMAN, EPHA2_HUMAN, PGS2_HUMAN, PTEN_HUMAN, Q3V639_HUMAN, Q5U5U6_HUMAN, CDCP1_HUMAN, SIA10_HUMAN, ITB3_HUMAN, ITAV_HUMAN, PRKN_HUMAN, WASP_HUMAN, DUS3_HUMAN, IGF1R_HUMAN, NCAM1_HUMAN, HS71A_HUMAN.HS71B_HUMAN, TPM1_HUMAN, CCD50_HUMAN, UBP8_HUMAN, PCNA_HUMAN, EPN1_HUMAN, LRIG1_HUMAN, UBS3B_HUMAN, NFIP1_HUMAN, NFIP2_HUMAN, LEG1_HUMAN, LST2_HUMAN, ACTA_HUMAN, SMUF2_HUMAN, OTU7B_HUMAN, UBP2_HUMAN, YAP1_HUMAN, CD2AP_HUMAN, H2AX_HUMAN, P2R3A_HUMAN, SC61B_HUMAN, EMD_HUMAN, RBM10_HUMAN, HNRH1_HUMAN, BCLF1_HUMAN, DOCK4_HUMAN, MYCBP_HUMAN, HCFC1_HUMAN, IRS2_HUMAN, PICAL_HUMAN, MPV17_HUMAN, CALU_HUMAN, TRPV1_HUMAN, BIP_HUMAN, CTGF_HUMAN, MLP3A_HUMAN, PTN23_HUMAN, CHM4A_HUMAN, DNJA3_HUMAN, FBX25_HUMAN, IGKC_HUMAN.KVD16_HUMAN, TBB5_HUMAN, TBB4B_HUMAN, TBB4A_HUMAN, TBB2A_HUMAN, TBB3_HUMAN, TBB6_HUMAN, HBA_HUMAN, XPO2_HUMAN, EF1A1_HUMAN, KRT86_HUMAN, AP1S1_HUMAN, ATX10_HUMAN, IMB1_HUMAN, SMD1_HUMAN, HSP72_HUMAN, XPO1_HUMAN, CIP2A_HUMAN, AP1M2_HUMAN, IPO7_HUMAN, XPOT_HUMAN, TNPO1_HUMAN, IPO5_HUMAN, 2AAA_HUMAN, DNJA1_HUMAN, DHB12_HUMAN, SGPL1_HUMAN, 2ABA_HUMAN, GCN1_HUMAN, EI2BB_HUMAN, SERA_HUMAN, FBX6_HUMAN, LANC2_HUMAN, SAAL1_HUMAN, SPTC1_HUMAN, GEMI6_HUMAN, HOOK2_HUMAN, RANG_HUMAN, PEX19_HUMAN, ARL1_HUMAN, PPP6_HUMAN, AP1G2_HUMAN, 2A5E_HUMAN, AP2B1_HUMAN, RPN1_HUMAN, S61A1_HUMAN, TPPC3_HUMAN, PDIA3_HUMAN, COG7_HUMAN, IQGA3_HUMAN, MMS19_HUMAN, STRAP_HUMAN, MON2_HUMAN, EI2BG_HUMAN, COG5_HUMAN, RCN2_HUMAN, COG6_HUMAN, THEM6_HUMAN, S39AB_HUMAN, COG4_HUMAN, PFKAP_HUMAN, TECR_HUMAN, BUB3_HUMAN, TIM50_HUMAN, AP1M1_HUMAN, VATH_HUMAN, OS9_HUMAN, XPO7_HUMAN, PDIA1_HUMAN, IPO4_HUMAN, PP6R1_HUMAN, SE1L1_HUMAN, USP9X_HUMAN, PFKAL_HUMAN, XPO5_HUMAN, AP2A2_HUMAN, ITIH2_HUMAN, PHLA1_HUMAN, DDX20_HUMAN, LEG8_HUMAN, PSMD2_HUMAN, TPP1_HUMAN, EXC6B_HUMAN, FAKD4_HUMAN, ZW10_HUMAN, ARHG5_HUMAN, AP1G1_HUMAN, IPO8_HUMAN, COG1_HUMAN, AT2A2_HUMAN, NUP85_HUMAN, XPO6_HUMAN, GEMI4_HUMAN, AL3A2_HUMAN, NUP93_HUMAN, RAGP1_HUMAN, BIG1_HUMAN, TELO2_HUMAN, EI2BE_HUMAN, PRGC1_HUMAN, BIG3_HUMAN, MTOR_HUMAN, DOP2_HUMAN, CNDG2_HUMAN, GBF1_HUMAN, SMC2_HUMAN, RN213_HUMAN, ATR_HUMAN, NBEL2_HUMAN, FDFT_HUMAN, SYRC_HUMAN, ACOT9_HUMAN, VAC14_HUMAN, BIRC3_HUMAN, BIRC2_HUMAN, CNOT9_HUMAN, RFA3_HUMAN, RFA2_HUMAN, RFA1_HUMAN, PANK4_HUMAN, HUWE1_HUMAN, AAKG1_HUMAN, KS6A3_HUMAN, PLK1_HUMAN, F263_HUMAN, DNM1L_HUMAN, SAE2_HUMAN, MP2K2_HUMAN, HXK2_HUMAN, MP2K4_HUMAN, AP3D1_HUMAN, DYN2_HUMAN, UBR4_HUMAN, S12A2_HUMAN, MP2K3_HUMAN, HXK1_HUMAN, ATP5L_HUMAN, PTPRF_HUMAN, RHG01_HUMAN, ITCH_HUMAN, PDK1_HUMAN, TBK1_HUMAN, PLD3_HUMAN, STK26_HUMAN, 2A5G_HUMAN, UB2G2_HUMAN, AP3M1_HUMAN, PFKAM_HUMAN, AAPK1_HUMAN, AP1S2_HUMAN, AP1B1_HUMAN, KC1A_HUMAN, PPAC_HUMAN, CSK21_HUMAN, AP2S1_HUMAN, CDK5_HUMAN, E2AK2_HUMAN, UBE2S_HUMAN, AP3S1_HUMAN, VRK1_HUMAN, AKT2_HUMAN, DERL1_HUMAN, PML_HUMAN, DCBD2_HUMAN, LRSM1_HUMAN, DSG2_HUMAN, SSBP_HUMAN, MYO1B_HUMAN, NGLY1_HUMAN, CALX_HUMAN, DPM1_HUMAN, DJB11_HUMAN, HCD2_HUMAN, DC1L1_HUMAN, FAF2_HUMAN, SYYC_HUMAN, IDHP_HUMAN, ECM29_HUMAN, ST1A1_HUMAN, TFR1_HUMAN, CLPX_HUMAN, SRPRA_HUMAN, MRT4_HUMAN, EIF3M_HUMAN, TIM23_HUMAN, SSRD_HUMAN, RPR1A_HUMAN, MYO1D_HUMAN, FBRL_HUMAN, ECHB_HUMAN, AFG32_HUMAN, SMC1A_HUMAN, SMC3_HUMAN, NDUA9_HUMAN, ITPA_HUMAN, SLN11_HUMAN, LONM_HUMAN, RL38_HUMAN, RU2A_HUMAN, COPA_HUMAN, NSF_HUMAN, ATAD1_HUMAN, AIFM1_HUMAN, PDIP2_HUMAN, WDR6_HUMAN, SCFD1_HUMAN, NDUS1_HUMAN, MGST1_HUMAN, NDUS3_HUMAN, RUXF_HUMAN, CN37_HUMAN, ORC5_HUMAN, EI2BD_HUMAN, TRUA_HUMAN, SDF2L_HUMAN, MIC60_HUMAN, ARP2_HUMAN, EI2BA_HUMAN, 1A01_HUMAN.1A02_HUMAN.1A03_HUMAN.1A11_HUMAN.1A23_HUMAN.1A24_HUMAN.1A25_HUMAN.1A26_HUMAN.1A29_HUMAN.1A30_HUMAN.1A31_HUMAN.1A32_HUMAN.1A33_HUMAN.1A34_HUMAN.1A36_HUMAN.1A43_HUMAN.1A66_HUMAN.1A68_HUMAN.1A69_HUMAN.1A74_HUMAN.1A80_HUMAN, VPS4B_HUMAN, EHD1_HUMAN, P5CR2_HUMAN, MYO1C_HUMAN, CUL4B_HUMAN, DRS7B_HUMAN, RFC5_HUMAN, OSBP1_HUMAN, YBEY_HUMAN, EF1B_HUMAN, GSH0_HUMAN, MIC10_HUMAN, PELO_HUMAN, RM10_HUMAN, FACR1_HUMAN, CTBP1_HUMAN, ABCF2_HUMAN, MPC2_HUMAN, LIMA1_HUMAN, CND3_HUMAN, EIF3K_HUMAN, MIC19_HUMAN, PUM1_HUMAN, TOIP1_HUMAN, ALEX_HUMAN.GNAS1_HUMAN.GNAS2_HUMAN.GNAS3_HUMAN, EIF3F_HUMAN, RS15A_HUMAN, SGMR2_HUMAN, CND2_HUMAN, RFC3_HUMAN, TOM22_HUMAN, STT3A_HUMAN, GCP2_HUMAN, PON2_HUMAN, ABCD3_HUMAN, CDIPT_HUMAN, SDF2_HUMAN, DIM1_HUMAN, BCCIP_HUMAN, TEBP_HUMAN, PYC_HUMAN, SRPRB_HUMAN, UTP15_HUMAN, GBB2_HUMAN, COQ8A_HUMAN, RER1_HUMAN, LRWD1_HUMAN, CF120_HUMAN, BZW1_HUMAN, AAAT_HUMAN, NSUN2_HUMAN, SFXN3_HUMAN, UFL1_HUMAN, ELP1_HUMAN, PDS5A_HUMAN, TR10B_HUMAN, ACACA_HUMAN, HYOU1_HUMAN, AT5F1_HUMAN, FLOT2_HUMAN, NTPCR_HUMAN, CERS2_HUMAN, ACOD_HUMAN, QCR2_HUMAN, AT2B1_HUMAN, IF4G2_HUMAN, SAM50_HUMAN, DJC11_HUMAN, NCLN_HUMAN, SKIV2_HUMAN, RRP44_HUMAN, LSR_HUMAN, CALR_HUMAN, PRI1_HUMAN, MRM3_HUMAN, AAMP_HUMAN, RAB18_HUMAN, RL23_HUMAN, AAAS_HUMAN, CTBP2_HUMAN, KIF1A_HUMAN, TPPC5_HUMAN, CMC2_HUMAN, TBL3_HUMAN, CLUS_HUMAN, ARHG2_HUMAN, ATPA_HUMAN, RL22_HUMAN, DHC24_HUMAN, FADS2_HUMAN, CKAP2_HUMAN, CEBPZ_HUMAN, DSRAD_HUMAN, NU153_HUMAN, LPPRC_HUMAN, OPA1_HUMAN, STOM_HUMAN, RFC4_HUMAN, TBG1_HUMAN, LANC1_HUMAN, TAF4_HUMAN, PSPC1_HUMAN, EWS_HUMAN, AAMDC_HUMAN, GRN_HUMAN, PSMD1_HUMAN, TPM3_HUMAN, CAP2_HUMAN, RL4_HUMAN, BLM_HUMAN, PLST_HUMAN, TPM4_HUMAN, XRCC5_HUMAN, H1X_HUMAN, RM09_HUMAN, CADH5_HUMAN, TMM25_HUMAN, PTC1_HUMAN, PTPRK_HUMAN, AKTIP_HUMAN, NTRK1_HUMAN, PIGS_HUMAN, RHG32_HUMAN, PPARG_HUMAN, KEAP1_HUMAN, NELL1_HUMAN, CYTA_HUMAN, ANO5_HUMAN, COHA1_HUMAN, CTNA2_HUMAN, H2A1A_HUMAN, RS15_HUMAN, RBM25_HUMAN, SPR1A_HUMAN, SRAC1_HUMAN, SFPQ_HUMAN, PTPRD_HUMAN, GSTT1_HUMAN, DBR1_HUMAN, LAT1_HUMAN, RL17_HUMAN, AT2B4_HUMAN, APOB_HUMAN, ERR2_HUMAN, OSMR_HUMAN, ACTB_HUMAN, MYH9_HUMAN, PTPRU_HUMAN, LRIG2_HUMAN, BBC3B_HUMAN.BBC3_HUMAN, GSTP1_HUMAN, RAD_HUMAN, HIP1_HUMAN, CLCN5_HUMAN, MCM4_HUMAN, APEX1_HUMAN, NUCL_HUMAN, NPM_HUMAN, PARP1_HUMAN, LMNA_HUMAN, FUS_HUMAN, ERCC2_HUMAN, TIF1B_HUMAN, MCM3_HUMAN, MCM6_HUMAN, FEN1_HUMAN, ILF2_HUMAN, ILF3_HUMAN, DHX9_HUMAN, BABA2_HUMAN, TOP1_HUMAN, LTK_HUMAN, IBP2_HUMAN, CADH2_HUMAN, ITB1_HUMAN, GRDN_HUMAN, PDP1_HUMAN, PTPRR_HUMAN, PTN7_HUMAN, PTPRA_HUMAN, PTPRH_HUMAN, PTPRT_HUMAN, PPM1A_HUMAN, PPM1F_HUMAN, MPZL2_HUMAN, SSH1_HUMAN, SRRM4_HUMAN, CLM7_HUMAN, E9PPJ3_HUMAN.SMTL1_HUMAN, KR161_HUMAN, MYO9A_HUMAN, IGLL5_HUMAN, RAS4B_HUMAN, PGRC1_HUMAN, SPT5H_HUMAN, ACACB_HUMAN, IF1AY_HUMAN, SC16A_HUMAN, E41L2_HUMAN, FOXO3_HUMAN, HTSF1_HUMAN, DYRK3_HUMAN, DHX16_HUMAN, NPHP4_HUMAN, SPAG7_HUMAN, TOM70_HUMAN, OR2F2_HUMAN, LC7L3_HUMAN, ABCA1_HUMAN, HERC2_HUMAN, PAK4_HUMAN, 1B07_HUMAN.1B08_HUMAN.1B13_HUMAN.1B14_HUMAN.1B15_HUMAN.1B18_HUMAN.1B27_HUMAN.1B35_HUMAN.1B37_HUMAN.1B38_HUMAN.1B39_HUMAN.1B40_HUMAN.1B41_HUMAN.1B42_HUMAN.1B44_HUMAN.1B45_HUMAN.1B46_HUMAN.1B47_HUMAN.1B48_HUMAN.1B49_HUMAN.1B50_HUMAN.1B51_HUMAN.1B52_HUMAN.1B53_HUMAN.1B54_HUMAN.1B55_HUMAN.1B56_HUMAN.1B57_HUMAN.1B58_HUMAN.1B59_HUMAN.1B67_HUMAN.1B73_HUMAN.1B78_HUMAN.1B81_HUMAN.1B82_HUMAN, CO1A1_HUMAN, FETUA_HUMAN, MAS_HUMAN, K2C1_HUMAN, HMGN2_HUMAN, RLA2_HUMAN, LA_HUMAN, CATD_HUMAN, CO1A2_HUMAN, K1C16_HUMAN, HMGB1_HUMAN, KCRU_HUMAN, DRD2_HUMAN, GLNA_HUMAN, HMGA1_HUMAN, DDX5_HUMAN, TCPA_HUMAN, RL7_HUMAN, LFA3_HUMAN, NF1_HUMAN, PPIB_HUMAN, RS3_HUMAN, IF4B_HUMAN, PSA3_HUMAN, PSA4_HUMAN, U2AF2_HUMAN, CNTF_HUMAN, HMGB2_HUMAN, DPP4_HUMAN, MAP4_HUMAN, DHI1_HUMAN, RPB1_HUMAN, GBRA3_HUMAN, K1C9_HUMAN, TRI23_HUMAN, RL3_HUMAN, RS27_HUMAN, GRIK4_HUMAN, EFTU_HUMAN, RL14_HUMAN, IDH3G_HUMAN, IRAK1_HUMAN, KCNQ1_HUMAN, HDGF_HUMAN, BTAF1_HUMAN, TCP4_HUMAN, EIF3B_HUMAN, SESN2_HUMAN, KR109_HUMAN, RS20_HUMAN, S10AA_HUMAN, HNRPK_HUMAN, CNBP_HUMAN, RAB1A_HUMAN, TRA2B_HUMAN, YBOX1_HUMAN, NTH_HUMAN, XIAP_HUMAN, SRSF2_HUMAN, AK17A_HUMAN, RL6_HUMAN, SRS11_HUMAN, SLC31_HUMAN, SSRP1_HUMAN, BPTF_HUMAN, CSTF3_HUMAN, G3BP1_HUMAN, TCOF_HUMAN, VPP3_HUMAN, HDAC1_HUMAN, CDK13_HUMAN, CIRBP_HUMAN, LRP8_HUMAN, PDE1C_HUMAN, UBP2L_HUMAN, CAPR1_HUMAN, RBM39_HUMAN, DIP2A_HUMAN, CBX2_HUMAN, GRM4_HUMAN, STIL_HUMAN, DIXC1_HUMAN, HERC1_HUMAN, E2F4_HUMAN, MICB_HUMAN, KR151_HUMAN, RHG29_HUMAN, DOP1_HUMAN, CE170_HUMAN, EYS_HUMAN, SKT_HUMAN, MCAF2_HUMAN, EST4A_HUMAN, NADE_HUMAN, PKHA7_HUMAN, MAST2_HUMAN, SCYL2_HUMAN, EMAL6_HUMAN, ZCCHV_HUMAN, PCLI1_HUMAN, SETX_HUMAN, OR2W3_HUMAN, PRS42_HUMAN, ZN573_HUMAN, S13A5_HUMAN, SRRM1_HUMAN, ZZZ3_HUMAN, CENPL_HUMAN, MIER1_HUMAN, RM43_HUMAN, ZN114_HUMAN, PAIRB_HUMAN, LS14A_HUMAN, MK15_HUMAN, CHD6_HUMAN, MUC16_HUMAN, DYH7_HUMAN, TITIN_HUMAN, ROBO4_HUMAN, S39A7_HUMAN, EDEM1_HUMAN, PRP16_HUMAN, LFG3_HUMAN, ELP4_HUMAN, MTMR8_HUMAN, DYH8_HUMAN, SCYL1_HUMAN, PRIC1_HUMAN, SPB12_HUMAN, MINT_HUMAN, TS101_HUMAN, SPAG8_HUMAN, SOSB1_HUMAN, ZFY21_HUMAN, SYT17_HUMAN, CNPY3_HUMAN, ASHWN_HUMAN, PLVAP_HUMAN, API5_HUMAN, NXF2_HUMAN, KTBL1_HUMAN, NUCKS_HUMAN, REEP4_HUMAN, NOL6_HUMAN, RPF1_HUMAN, IRPL2_HUMAN, MLXPL_HUMAN, INCE_HUMAN, EXOS3_HUMAN, RNF12_HUMAN, RCC2_HUMAN, TEKT2_HUMAN, SO3A1_HUMAN, JUPI1_HUMAN, TNIK_HUMAN, TRHDE_HUMAN, BAG5_HUMAN, GRID1_HUMAN, S45A2_HUMAN, ING4_HUMAN, CBPC1_HUMAN, SRRM2_HUMAN, RUVB2_HUMAN, COA3_HUMAN, NOSIP_HUMAN, CBY1_HUMAN, WIPI2_HUMAN, PCDG3_HUMAN, K2C3_HUMAN, K1C10_HUMAN, K22E_HUMAN, K2C5_HUMAN, GOGB1_HUMAN, GP149_HUMAN, MERL_HUMAN, SG1D4_HUMAN, DEF1_HUMAN, SIA8D_HUMAN, 5HT3A_HUMAN, PCDBB_HUMAN, RAB31_HUMAN, PP2BB_HUMAN, PPM1B_HUMAN, DUS19_HUMAN, STYX_HUMAN, RGS2_HUMAN, HEPS_HUMAN, UB2J2_HUMAN, CFTR_HUMAN, PK3CA_HUMAN, CYLD_HUMAN, EPGN_HUMAN, PKP2_HUMAN, CCR5_HUMAN, H14_HUMAN, FHL2_HUMAN, 1433E_HUMAN, PAXI_HUMAN, ATPB_HUMAN, MPCP_HUMAN, TE2IP_HUMAN, KRIT1_HUMAN, S10AB_HUMAN, H2B1N_HUMAN, RS27A_HUMAN, EFNB1_HUMAN, CH60_HUMAN, BCAR1_HUMAN, K1C14_HUMAN, K2C6A_HUMAN, CKAP4_HUMAN, HNRPF_HUMAN, ADT2_HUMAN, PTPRC_HUMAN, EPHB4_HUMAN, HEBP1_HUMAN, H2B1C_HUMAN.H2B1D_HUMAN, PGH2_HUMAN, LRC59_HUMAN, AP180_HUMAN, CCND1_HUMAN, MYL9_HUMAN, CALM3_HUMAN, WASF1_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q9H1K1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iron-sulfur cluster assembly enzyme [Source:HGNC Symbol;Acc:HGNC:29882]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCU_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPERT_HUMAN, TRIM1_HUMAN, SDHB_HUMAN, HSC20_HUMAN, GRP75_HUMAN, LYRM7_HUMAN, UCRI_HUMAN, GOGA2_HUMAN, NUP62_HUMAN, FAM9B_HUMAN, BANP_HUMAN, LNX1_HUMAN, SDHF1_HUMAN, NECA2_HUMAN, IKZF1_HUMAN, ATRAP_HUMAN, NDUS8_HUMAN, NDUS1_HUMAN, SDHA_HUMAN, 1433B_HUMAN, HPRT_HUMAN, NDUV2_HUMAN, NFS1_HUMAN, IMPA1_HUMAN, LYRM4_HUMAN, FRDA_HUMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P53_HUMAN, GORS1_HUMAN, RAF1_HUMAN, BRAF_HUMAN.K1549_HUMAN, KSR1_HUMAN, MARK3_HUMAN, NUP58_HUMAN, NUP54_HUMAN, MPIP3_HUMAN, HDAC5_HUMAN, HDAC4_HUMAN, RBP2_HUMAN, PO210_HUMAN, NU214_HUMAN, NU153_HUMAN, RON_HUMAN, B2L11_HUMAN, M3K3_HUMAN, 1433B_HUMAN.1433E_HUMAN.1433F_HUMAN.1433G_HUMAN.1433S_HUMAN.1433T_HUMAN.1433Z_HUMAN, BAX_HUMAN, BAD_HUMAN, DHSD_HUMAN, C560_HUMAN, PA1B3_HUMAN, TSC2_HUMAN, IKKB_HUMAN, ADT3_HUMAN, BYST_HUMAN, RIN1_HUMAN, TBB5_HUMAN, BFSP1_HUMAN, UBB_HUMAN, FOXO3_HUMAN, ATX7_HUMAN, KPCD_HUMAN, AES_HUMAN, GASP1_HUMAN, TNAP3_HUMAN, BARD1_HUMAN, ACTN1_HUMAN, HEM0_HUMAN, HNF1A_HUMAN, ADRB2_HUMAN, CY24A_HUMAN, CARD9_HUMAN, A4_HUMAN, THIC_HUMAN, BIEA_HUMAN, CDN1B_HUMAN, RING2_HUMAN, GORS2_HUMAN, NDK7_HUMAN, TOX4_HUMAN, DDX6_HUMAN, PAR6B_HUMAN, Q96F82_HUMAN, GOG6A_HUMAN, PNMA1_HUMAN, 1433E_HUMAN, BCL6_HUMAN, RBTN2_HUMAN, SPG21_HUMAN, CKS1_HUMAN, HNRH1_HUMAN, FL2D_HUMAN, M3K14_HUMAN, SRPK1_HUMAN, ZBT16_HUMAN, FHL2_HUMAN, SCEL_HUMAN, MED28_HUMAN, ARHG6_HUMAN, RAB2B_HUMAN, CDK14_HUMAN, UB2E2_HUMAN, AAPK2_HUMAN, CCHCR_HUMAN, CDD_HUMAN, OR7AA_HUMAN, CHCH2_HUMAN, CCDC6_HUMAN.RET_HUMAN, NTF2_HUMAN, TCL1A_HUMAN, IP6K3_HUMAN, DEMA_HUMAN, MTNB_HUMAN, EPN2_HUMAN, THAP1_HUMAN, ISCU_HUMAN, SPF27_HUMAN, DPYL1_HUMAN, CC88B_HUMAN, SRBS2_HUMAN, AQP1_HUMAN, EGLN3_HUMAN, P66B_HUMAN, LMO4_HUMAN, UBC_HUMAN, CRBN_HUMAN, ARPC3_HUMAN, PFD5_HUMAN, SP2_HUMAN, SCND1_HUMAN, LEG3_HUMAN, ALKB3_HUMAN, RT27_HUMAN, PRS4_HUMAN, WASC3_HUMAN, RA51D_HUMAN, RPC2_HUMAN, HYLS1_HUMAN, SYT17_HUMAN, BAG6_HUMAN, FAS_HUMAN, UB2D1_HUMAN, TLE4_HUMAN, THIOM_HUMAN, DBLOH_HUMAN, TFAP4_HUMAN, IF4E2_HUMAN, NECA1_HUMAN, USF3_HUMAN, PSA1_HUMAN, MMAB_HUMAN, RGS20_HUMAN, DCAF6_HUMAN, SH24A_HUMAN, NOTO_HUMAN, CCD91_HUMAN, RBY1A_HUMAN.RBY1C_HUMAN, HSF4_HUMAN, DAXX_HUMAN, PRPF3_HUMAN, ELOA1_HUMAN, MTEF3_HUMAN, F161A_HUMAN, SYQ_HUMAN, CDIPT_HUMAN, NXF1_HUMAN, NTAQ1_HUMAN, PRP31_HUMAN, RRFM_HUMAN, FAKD3_HUMAN, ZN581_HUMAN, SPY2_HUMAN, FOXK1_HUMAN, ZFY21_HUMAN, MO4L2_HUMAN, CIRBP_HUMAN, CDX4_HUMAN, RUSC2_HUMAN, DCTD_HUMAN, RBTN1_HUMAN, FAKD4_HUMAN, PHS_HUMAN, KCC2D_HUMAN, RN135_HUMAN, TESK1_HUMAN, FXL12_HUMAN, FBF1_HUMAN, PIMRE_HUMAN, GTPBA_HUMAN, IL7RA_HUMAN, UBE2K_HUMAN, GATA2_HUMAN, ZN655_HUMAN, NDUBA_HUMAN, TXLNB_HUMAN, SYYM_HUMAN, CPNS1_HUMAN, HSF2B_HUMAN, MID51_HUMAN, RLP24_HUMAN, ABI2_HUMAN, TRAF5_HUMAN, TCEA2_HUMAN, HELZ_HUMAN, PNPO_HUMAN, COX5B_HUMAN, TRAF1_HUMAN, REL1_HUMAN.REL2_HUMAN, PITX1_HUMAN, STK25_HUMAN, RAB3I_HUMAN, RPH3L_HUMAN, BAHD1_HUMAN, IMA1_HUMAN, CCNG1_HUMAN, IN80B_HUMAN, GLRX5_HUMAN, PKP4_HUMAN, STK3_HUMAN, NFYB_HUMAN, MEMO1_HUMAN, MD2L2_HUMAN, NXT2_HUMAN, RSMB_HUMAN, AMPL_HUMAN, K2C1_HUMAN, RBPMS_HUMAN, MAX_HUMAN, REQU_HUMAN, FLOT1_HUMAN, SDHF2_HUMAN, PCLI1_HUMAN, GMCL2_HUMAN, K2C75_HUMAN, RUVB2_HUMAN, KPCZ_HUMAN, RABX5_HUMAN, TPM1_HUMAN, MTG8_HUMAN.RUNX1_HUMAN, IMPA2_HUMAN, SPTN1_HUMAN, STAR_HUMAN, RPAB5_HUMAN, GCP60_HUMAN, RMD3_HUMAN, PSA4_HUMAN, TS101_HUMAN, RU2B_HUMAN, K1C20_HUMAN, APC10_HUMAN, DYN2_HUMAN, ATPA_HUMAN, GDIA_HUMAN, CDKL3_HUMAN, NEK6_HUMAN, KIFC3_HUMAN, NUD14_HUMAN, TEANC_HUMAN, SYFM_HUMAN, OTU7B_HUMAN, SPA24_HUMAN, DAPK2_HUMAN, ZN417_HUMAN, TRI10_HUMAN, XPO6_HUMAN, DCX_HUMAN, GMCL1_HUMAN, DNPEP_HUMAN, ARH40_HUMAN, RUXF_HUMAN, SNX20_HUMAN, RITA1_HUMAN, SDCB1_HUMAN, PPR18_HUMAN, PPL13_HUMAN, SFI1_HUMAN, RCL1_HUMAN, NDUS3_HUMAN, NDUS2_HUMAN, PHB_HUMAN, ATAD5_HUMAN, HAUS1_HUMAN, KLC3_HUMAN, EXOS5_HUMAN, TANK_HUMAN, LZTS1_HUMAN, MYCPP_HUMAN, SHLB1_HUMAN, 1433S_HUMAN, NKG7_HUMAN, SAT1_HUMAN, NEBL_HUMAN, MCRS1_HUMAN, COQ8A_HUMAN, KIF23_HUMAN, CBX8_HUMAN, DCE1_HUMAN, NADK_HUMAN, TCF19_HUMAN, NOC4L_HUMAN, CHRC1_HUMAN, SCNM1_HUMAN, UBE2N_HUMAN, HXB9_HUMAN, CEP55_HUMAN, DJC15_HUMAN, AXIN1_HUMAN, EXOS8_HUMAN, GOPC_HUMAN, CASL_HUMAN, MYEF2_HUMAN, ZNF41_HUMAN, FIP1_HUMAN, MGN2_HUMAN, MTMR9_HUMAN, SEN54_HUMAN, SYCE1_HUMAN, PCY1A_HUMAN, MET17_HUMAN, CAND1_HUMAN, KDM1A_HUMAN, LASP1_HUMAN, MO4L1_HUMAN, LIN7A_HUMAN, BEX3_HUMAN, MCM7_HUMAN, MK09_HUMAN, ACINU_HUMAN, DYLT1_HUMAN, ENKD1_HUMAN, FHL5_HUMAN, CDC7_HUMAN, MPIP2_HUMAN, ZZZ3_HUMAN, TBCEL_HUMAN, ERCC3_HUMAN, EXOS4_HUMAN, P85B_HUMAN, TERF2_HUMAN, CENPL_HUMAN, ITB5_HUMAN, PAK5_HUMAN, TEAD4_HUMAN, DPPA3_HUMAN, FAD1_HUMAN, SMCE1_HUMAN, RAD18_HUMAN, GRAP2_HUMAN, K2C6A_HUMAN, SNAPN_HUMAN, NAB1_HUMAN, CINP_HUMAN, H4G_HUMAN, GEM_HUMAN, CYH4_HUMAN, NCK2_HUMAN, SNF8_HUMAN, PIN1_HUMAN, GAPD1_HUMAN, VIME_HUMAN, MTG8_HUMAN, ZGPAT_HUMAN, CDC37_HUMAN, ODPX_HUMAN, TYDP2_HUMAN, CRX_HUMAN, APC11_HUMAN, EFC4B_HUMAN, MDM1_HUMAN, SRC_HUMAN, AIMP2_HUMAN, LCP2_HUMAN, MS18B_HUMAN, GFAP_HUMAN, ZBTB4_HUMAN, P73_HUMAN, STOX1_HUMAN, PTBP2_HUMAN, PSME2_HUMAN, POGZ_HUMAN, NRIP2_HUMAN, SLU7_HUMAN, IKBE_HUMAN, ACPM_HUMAN, IFT25_HUMAN, ACY3_HUMAN, ZN564_HUMAN, EGFR_HUMAN, GCC1_HUMAN, TFP11_HUMAN, PTN3_HUMAN, AAKB2_HUMAN, M3K8_HUMAN, ATRIP_HUMAN, EHBP1_HUMAN, CRDL2_HUMAN, MCEE_HUMAN, FA50B_HUMAN, MLH1_HUMAN, KAP1_HUMAN, PTN9_HUMAN, VATC2_HUMAN, ARL4A_HUMAN, GGA2_HUMAN, RMD2_HUMAN, ARIP4_HUMAN, PICK1_HUMAN, TFAM_HUMAN, A0AVN2_HUMAN, OGT1_HUMAN, PCM1_HUMAN, MBD3_HUMAN, SSNA1_HUMAN, KI20B_HUMAN, CSPP1_HUMAN, CEP95_HUMAN, SKT_HUMAN, PKHA2_HUMAN, AKAP9_HUMAN, XRCC4_HUMAN, NDRG4_HUMAN, MYCB2_HUMAN, SOCS6_HUMAN, DHYS_HUMAN, TTC25_HUMAN, DPOLL_HUMAN, VATG1_HUMAN, ADA15_HUMAN, FXR1_HUMAN, CTBP1_HUMAN, PRP18_HUMAN, SUCB2_HUMAN, SNX5_HUMAN, F110A_HUMAN, LMNB2_HUMAN, CBL_HUMAN, GRAM4_HUMAN, RM28_HUMAN, VP37C_HUMAN, SUOX_HUMAN, SON_HUMAN, TOP3B_HUMAN, M1IP1_HUMAN, 5HT6R_HUMAN, HNRPR_HUMAN, EFCB6_HUMAN, PML_HUMAN.RARA_HUMAN, ING5_HUMAN, GRM5_HUMAN, RAB1B_HUMAN, IKZF3_HUMAN, PP16B_HUMAN, ZN764_HUMAN, ADAP1_HUMAN, NELFB_HUMAN, MID49_HUMAN, TRI27_HUMAN, PIN4_HUMAN, RM10_HUMAN, ZN580_HUMAN, ACTN4_HUMAN, SPT5H_HUMAN, BL1S6_HUMAN, BICD2_HUMAN, LCLT1_HUMAN, CEP72_HUMAN, GGN_HUMAN, KAT5_HUMAN, SPF45_HUMAN, CASP6_HUMAN, NOS3_HUMAN, PDCD6_HUMAN, PF21A_HUMAN, ARI5A_HUMAN, E5KS60_HUMAN, PTH_HUMAN, CDC73_HUMAN, IKBA_HUMAN, TRIP6_HUMAN, PGK1_HUMAN, FKBP4_HUMAN, 1433F_HUMAN, GPAA1_HUMAN, CENPP_HUMAN, ITB1_HUMAN, STX1A_HUMAN, ZC12A_HUMAN, GLRX3_HUMAN, EAF2_HUMAN, CEP44_HUMAN, SDS3_HUMAN, IFT20_HUMAN, ABT1_HUMAN, TRAF4_HUMAN, AFF4_HUMAN, RGS8_HUMAN, PSME3_HUMAN, FANCG_HUMAN, KLF15_HUMAN, RHNO1_HUMAN, FBXW5_HUMAN, CC106_HUMAN, IF2B2_HUMAN, Q6IAQ1_HUMAN, KANL1_HUMAN, SNPC5_HUMAN, NFYA_HUMAN, MGST3_HUMAN, MGN_HUMAN, UN45A_HUMAN, CBX4_HUMAN, VMAC_HUMAN, Q6IQ43_HUMAN, GOGA7_HUMAN, ESCO2_HUMAN, GSTK1_HUMAN, PTN11_HUMAN, ZN263_HUMAN, CUL5_HUMAN, CALX_HUMAN, SMN_HUMAN, CCNH_HUMAN, COR1A_HUMAN, CEP76_HUMAN, P5CS_HUMAN, K2C6B_HUMAN, CDK2_HUMAN, THG1_HUMAN, MB12B_HUMAN, ENPP7_HUMAN, DCE2_HUMAN, DYR1A_HUMAN, ZFHX3_HUMAN, SENP2_HUMAN, TRI18_HUMAN, F214B_HUMAN, BIRC2_HUMAN, ASPP1_HUMAN, MSRB3_HUMAN, K1C18_HUMAN, XIAP_HUMAN, AKP13_HUMAN, HOOK2_HUMAN, NB5R2_HUMAN, GATA1_HUMAN, FOXR1_HUMAN, ZFY26_HUMAN, FOXK2_HUMAN, ACSF2_HUMAN, SRRM2_HUMAN, IKKE_HUMAN, LMBL2_HUMAN, RCOR3_HUMAN, RRF2M_HUMAN, TRI69_HUMAN, TRAF3_HUMAN, NQO2_HUMAN, MUTYH_HUMAN, COAC_HUMAN, STK38_HUMAN, DC1I2_HUMAN, GAB2_HUMAN, BTBD1_HUMAN, HSPB1_HUMAN, ZN410_HUMAN, NDOR1_HUMAN, LHX8_HUMAN, LYRM2_HUMAN, DCAF7_HUMAN, STMN4_HUMAN, CPSF4_HUMAN, RBM25_HUMAN, KCNK5_HUMAN, DTBP1_HUMAN, ARFP2_HUMAN, FRMD6_HUMAN, TRIM3_HUMAN, CIC_HUMAN, PPIA_HUMAN, ARGL1_HUMAN, GLCTK_HUMAN, PTPS_HUMAN, FATE1_HUMAN, NDUA5_HUMAN, AFAD_HUMAN, DCTN4_HUMAN, PATL1_HUMAN, NXP20_HUMAN, LZTS2_HUMAN, ATF7_HUMAN, MLX_HUMAN, RM09_HUMAN, Q6IB29_HUMAN, NDC80_HUMAN, CPSF5_HUMAN, LSM2_HUMAN, EPMIP_HUMAN, EFTU_HUMAN, RAB2A_HUMAN, RGS3_HUMAN, UBC9_HUMAN, ZN567_HUMAN, RBM39_HUMAN, BEX2_HUMAN, CLIP3_HUMAN, THAP7_HUMAN, AP3M1_HUMAN, E41L2_HUMAN, A0A0C4DFT9_HUMAN.WHRN_HUMAN, RND3_HUMAN, GOLM1_HUMAN, SP110_HUMAN, FOXP2_HUMAN, RUSC1_HUMAN, LRIF1_HUMAN, MD1L1_HUMAN, APOA4_HUMAN, DCTP1_HUMAN, ATPF2_HUMAN, ZMAT2_HUMAN, MTEF4_HUMAN, TBK1_HUMAN, YAP1_HUMAN, PO6F2_HUMAN, NCF2_HUMAN, GCP2_HUMAN, TRAF6_HUMAN, 1433G_HUMAN, P121A_HUMAN.P121C_HUMAN, JAK3_HUMAN, LIPA3_HUMAN, ZBT42_HUMAN, ALS2_HUMAN, LBX1_HUMAN, AKIP_HUMAN, K1C27_HUMAN, LIN54_HUMAN, CENPO_HUMAN, TSYL2_HUMAN, HIF1A_HUMAN, ARNT_HUMAN, MRM1_HUMAN, IKBB_HUMAN, M3K7_HUMAN, CTBP2_HUMAN, PNKP_HUMAN, NOL4_HUMAN, PRKRA_HUMAN, AEN_HUMAN, SNW1_HUMAN, SUCB1_HUMAN, AURKA_HUMAN, ZN346_HUMAN, TRI54_HUMAN, KCMF1_HUMAN, PSMD4_HUMAN, UBR4_HUMAN, HGS_HUMAN, SAHH_HUMAN, IQCN_HUMAN, CD79A_HUMAN, PPCT_HUMAN, NDKA_HUMAN, PAHX_HUMAN, MTA1_HUMAN, HSF2_HUMAN, RIOX2_HUMAN, RO52_HUMAN, AFG1L_HUMAN, RBM28_HUMAN, PIGS_HUMAN, CSK21_HUMAN, ING1_HUMAN.KLK5_HUMAN, TEKT4_HUMAN, PMGT1_HUMAN, BY55_HUMAN, HNRPD_HUMAN, HXB5_HUMAN, PEPL_HUMAN, SRC8_HUMAN, 1433Z_HUMAN, IF2B3_HUMAN, GBRL2_HUMAN, IGFN1_HUMAN, Q548N1_HUMAN, CBY1_HUMAN, RING1_HUMAN, BMI1_HUMAN, PHC1_HUMAN, KATL2_HUMAN, IKIP_HUMAN, PIAS2_HUMAN, MAD3_HUMAN, LCOR_HUMAN, SHPRH_HUMAN, G6PI_HUMAN, SRRM4_HUMAN, KIF9_HUMAN, TCHP_HUMAN, TRAF2_HUMAN, CND3_HUMAN, SEPT1_HUMAN, PNMT_HUMAN, HSP74_HUMAN, SYHM_HUMAN, IFT27_HUMAN, MOT4_HUMAN, PPIF_HUMAN, RIPK1_HUMAN, A4D2J0_HUMAN, ULK2_HUMAN, PRDC1_HUMAN, TTPA_HUMAN, UB2E3_HUMAN, TPD53_HUMAN, MCM10_HUMAN, ZN148_HUMAN, WEE1_HUMAN, BID_HUMAN, PDE3B_HUMAN, T23O_HUMAN, TTHY_HUMAN, TRIM8_HUMAN, GO45_HUMAN, DTX2_HUMAN, AAPK1_HUMAN, G45IP_HUMAN, DTNB_HUMAN, TAF6_HUMAN, STAU1_HUMAN, K1C40_HUMAN, TBA1A_HUMAN.TBA1B_HUMAN, GRB2_HUMAN, MTUS2_HUMAN, CRTC2_HUMAN, MB212_HUMAN, BL1S2_HUMAN, 1433T_HUMAN, ATG9A_HUMAN, TXLNA_HUMAN, UBS3A_HUMAN, IF4H_HUMAN, MPRIP_HUMAN, OAS1_HUMAN, UBP2_HUMAN, PRAF1_HUMAN, HDAC1_HUMAN, K22O_HUMAN, RB39B_HUMAN, DNJC1_HUMAN, ERGI3_HUMAN, EIF3G_HUMAN, IF4A3_HUMAN, EBP2_HUMAN, GNL3L_HUMAN, HS90B_HUMAN, NT2NL_HUMAN, LBR_HUMAN, FOXC2_HUMAN, CDC5L_HUMAN, DACT1_HUMAN, NCOR1_HUMAN, HIP1_HUMAN, MAST1_HUMAN, MAGI2_HUMAN, CDC23_HUMAN, CACO2_HUMAN, NEMO_HUMAN, PAK4_HUMAN, CCAR1_HUMAN, CLK3_HUMAN, ECH1_HUMAN, CAPS1_HUMAN, GNMT_HUMAN, PKN3_HUMAN, SMG9_HUMAN, Q96AL5_HUMAN, RMND1_HUMAN, V9HW56_HUMAN, GRB14_HUMAN, PBX2_HUMAN, RM11_HUMAN, E41L3_HUMAN, SNX1_HUMAN, TXK_HUMAN, MP2K1_HUMAN, DYRK2_HUMAN, UBP8_HUMAN, TACO1_HUMAN, SYT6_HUMAN, FHL3_HUMAN, PAQRB_HUMAN, USO1_HUMAN, GOGB1_HUMAN, RAB1A_HUMAN, KANK1_HUMAN, CH60_HUMAN, WASL_HUMAN, CCNC_HUMAN, TAXB1_HUMAN, Z512B_HUMAN, SCAF8_HUMAN, PDIP2_HUMAN, KLC4_HUMAN, CCDB1_HUMAN, CALR_HUMAN, BECN1_HUMAN, BCL2_HUMAN, MCL1_HUMAN, DERL1_HUMAN, F16A2_HUMAN, 1B42_HUMAN, DRG1_HUMAN, ITPR1_HUMAN, KLC1_HUMAN, PAX6_HUMAN, SRPK2_HUMAN, RIPK3_HUMAN, AP1M1_HUMAN, INT10_HUMAN, COG6_HUMAN, NFU1_HUMAN, PSDE_HUMAN, CLK1_HUMAN, RYBP_HUMAN, NDEL1_HUMAN, ALKB2_HUMAN, RNPS1_HUMAN, CRNL1_HUMAN, S100B_HUMAN, TRI68_HUMAN, GRPE1_HUMAN, OLA1_HUMAN, M3K5_HUMAN, PI3R5_HUMAN, B2L13_HUMAN, NUP88_HUMAN, LRC59_HUMAN, GAS8_HUMAN, RL9_HUMAN, REPS2_HUMAN, ZN572_HUMAN, TF65_HUMAN, C1T9A_HUMAN.C1T9B_HUMAN, SP4_HUMAN, RBFA_HUMAN, RIC8A_HUMAN, ARF3_HUMAN, QORL1_HUMAN, CDA7L_HUMAN, V9HW80_HUMAN, LRC45_HUMAN, MCSP_HUMAN, CDKN3_HUMAN, UPP2_HUMAN, ANKS6_HUMAN, CENPU_HUMAN, KIF24_HUMAN, ECM29_HUMAN, MEP50_HUMAN, DDB1_HUMAN, CUL4A_HUMAN, STK26_HUMAN, KS6A1_HUMAN, SSH1_HUMAN, LRFN1_HUMAN, HMBX1_HUMAN, PARD3_HUMAN.PKHD1_HUMAN, NDUF3_HUMAN, VHL_HUMAN, RPP25_HUMAN, CRCM_HUMAN, NICA_HUMAN, RPAC1_HUMAN, MARE2_HUMAN, SEC13_HUMAN, MARK2_HUMAN, CAH8_HUMAN, SYEP_HUMAN, MPIP1_HUMAN, ECHP_HUMAN.TBA8_HUMAN, SRSF3_HUMAN, VDAC1_HUMAN, SOX5_HUMAN, PRKDC_HUMAN, M3K2_HUMAN, IGF1_HUMAN, HMHA1_HUMAN, ALDOC_HUMAN, MDM4_HUMAN, TOX_HUMAN, 2AAA_HUMAN, HNRPF_HUMAN, TF2H1_HUMAN, CEP85_HUMAN, RGPS2_HUMAN, AXIN2_HUMAN, SYTL2_HUMAN, HES1_HUMAN, SPC25_HUMAN, RIDA_HUMAN, 3HIDH_HUMAN, TF3C1_HUMAN, VMAT1_HUMAN, EDC3_HUMAN, TRI50_HUMAN, VEZF1_HUMAN, ZN488_HUMAN, CEP70_HUMAN, RGAP1_HUMAN, RABE1_HUMAN, AIF1_HUMAN, PPM1A_HUMAN, HSFY1_HUMAN, E2F7_HUMAN, CHSP1_HUMAN, SRS10_HUMAN, FAM9A_HUMAN, PSMF1_HUMAN, CSK2B_HUMAN, PRDM6_HUMAN, SH22A_HUMAN, ZRAN1_HUMAN, IRS2_HUMAN, CDN1A_HUMAN, DFFA_HUMAN, TRI14_HUMAN, CDN2D_HUMAN, FA156_HUMAN, A0A0A0MQR8_HUMAN.A0A0A0MST9_HUMAN.A0A0A0MT23_HUMAN.MARK3_HUMAN, PUR6_HUMAN, CING_HUMAN, SSX3_HUMAN, MAT1_HUMAN, TRI35_HUMAN, PTCD2_HUMAN, PPIB_HUMAN, RNF8_HUMAN, PKN1_HUMAN, MIC19_HUMAN, LRRK2_HUMAN, AP5Z1_HUMAN, IKKA_HUMAN, ZN587_HUMAN, SOAT1_HUMAN, LHX4_HUMAN, TEKT1_HUMAN, GP152_HUMAN, RAB30_HUMAN, LTOR5_HUMAN, UB2D3_HUMAN, TSN_HUMAN, ST38L_HUMAN, ZN395_HUMAN, CIDEB_HUMAN, K2C6C_HUMAN, TAB2_HUMAN, GLP3L_HUMAN, PO4F3_HUMAN, HCK_HUMAN, ACES_HUMAN, QCR8_HUMAN, QCR9_HUMAN, QCR1_HUMAN, QCR2_HUMAN, QCR7_HUMAN, MK07_HUMAN, E4F1_HUMAN, RBM23_HUMAN, CLIC1_HUMAN, RUBIC_HUMAN, SEBP2_HUMAN, AQP6_HUMAN, GDN_HUMAN, NB5R3_HUMAN, DDT4L_HUMAN, VPS28_HUMAN, UBP7_HUMAN, MILK1_HUMAN, BIG1_HUMAN, NUCL_HUMAN, FBRL_HUMAN, REL_HUMAN, RASL3_HUMAN, VPS52_HUMAN, HXB3_HUMAN, ZN614_HUMAN, SURF6_HUMAN, KINH_HUMAN, PELI2_HUMAN, AKTS1_HUMAN, ACTN3_HUMAN, ATPO_HUMAN, DLX3_HUMAN, PNPT1_HUMAN, PSMD9_HUMAN, RXRB_HUMAN, SCRIB_HUMAN, RU2A_HUMAN, DVL2_HUMAN, HOIL1_HUMAN, KI2L3_HUMAN, GEMI_HUMAN, NINL_HUMAN, V9HWB8_HUMAN, CSN5_HUMAN, KPRP_HUMAN, DLGP5_HUMAN, VP37B_HUMAN, TEAN2_HUMAN, IQUB_HUMAN, MBOA7_HUMAN, K2C79_HUMAN, BACD2_HUMAN, FAKD5_HUMAN, CCNA2_HUMAN, CTNL1_HUMAN, INSR_HUMAN, LIMS2_HUMAN, BIP_HUMAN, ZN622_HUMAN, RPB3_HUMAN, PI3R4_HUMAN, GA2L2_HUMAN, ARHG5_HUMAN, SPART_HUMAN, ABL1_HUMAN, DVL3_HUMAN, FX4L3_HUMAN, UBP32_HUMAN, DUPD1_HUMAN, MARE3_HUMAN, TPRX1_HUMAN, FOS_HUMAN, ANM5_HUMAN, PIM1_HUMAN, PI4KB_HUMAN, RPIA_HUMAN, CCD62_HUMAN, IL16_HUMAN, UBP16_HUMAN, INP5K_HUMAN, TBA1B_HUMAN, MYOTI_HUMAN, TRI41_HUMAN, LYPA1_HUMAN, LSM4_HUMAN, M3K1_HUMAN, UT14C_HUMAN, HEYL_HUMAN, TAB1_HUMAN, HEXI2_HUMAN, RPC3_HUMAN, HS71B_HUMAN.HSP77_HUMAN, HSP7E_HUMAN, CE164_HUMAN, PPIH_HUMAN, GPX8_HUMAN, APC_HUMAN, PCNA_HUMAN, KC1G1_HUMAN, FYN_HUMAN, SNP29_HUMAN, ETFA_HUMAN, SRP19_HUMAN, ZN785_HUMAN, LMBL3_HUMAN, CATZ_HUMAN, RN213_HUMAN, HD_HUMAN, NDUA9_HUMAN, GBG5_HUMAN, ATP5E_HUMAN, K2C3_HUMAN, UTP23_HUMAN, RNF4_HUMAN, PNRC2_HUMAN, ATF2_HUMAN, SNX18_HUMAN, THIO_HUMAN, U520_HUMAN, GBF1_HUMAN, RELB_HUMAN, PRDM9_HUMAN, P121A_HUMAN, DHX15_HUMAN, CWC22_HUMAN, RBM22_HUMAN, IRX3_HUMAN, RHOH_HUMAN, ZO2_HUMAN, RHG01_HUMAN, H2B1H_HUMAN, EXOS1_HUMAN, A0A1W2PKR9_HUMAN.M3K21_HUMAN.X6R610_HUMAN, A0A0S2Z4G9_HUMAN, AKT1_HUMAN, DDX5_HUMAN, NFL_HUMAN, RT06_HUMAN, RA51B_HUMAN, TNR1A_HUMAN, F16P1_HUMAN, PASK_HUMAN, ETFR1_HUMAN, CC85B_HUMAN, CCD70_HUMAN, DERL2_HUMAN, ATPB_HUMAN, FZD1_HUMAN, RBM26_HUMAN, SNP47_HUMAN, IRF3_HUMAN, EXOC8_HUMAN, AL3B1_HUMAN, SAP18_HUMAN, AAKB1_HUMAN, PR20D_HUMAN.PR20E_HUMAN, NOL10_HUMAN, K1H1_HUMAN, ZN438_HUMAN, ZDH17_HUMAN, MIEAP_HUMAN, TGS1_HUMAN, RAI14_HUMAN, THYN1_HUMAN, C1QBP_HUMAN, GA45A_HUMAN, J3KN16_HUMAN, HIKES_HUMAN, TRI23_HUMAN, OPTN_HUMAN, T2EB_HUMAN, STN1_HUMAN, NSMF_HUMAN, U5S1_HUMAN, NOA1_HUMAN, RT29_HUMAN, RM12_HUMAN, SIAS_HUMAN, SRSF1_HUMAN, IPYR_HUMAN, ZN250_HUMAN, ZMYM6_HUMAN, MAGAB_HUMAN, SPNS1_HUMAN, AP2M1_HUMAN, RHG32_HUMAN, GPS2_HUMAN, FER3L_HUMAN, UBE2Z_HUMAN, PKP1_HUMAN, DOCK4_HUMAN, PGM1_HUMAN, DEN1B_HUMAN, GFI1B_HUMAN, SKP2_HUMAN, STOM_HUMAN, RYR2_HUMAN, NFKB2_HUMAN, GNPI2_HUMAN, ORML1_HUMAN, TSC1_HUMAN, CHK1_HUMAN, TE2IP_HUMAN, ARL3_HUMAN, CLPX_HUMAN, CLPP_HUMAN, CUTC_HUMAN, ING1_HUMAN, NFKB1_HUMAN, VTA1_HUMAN, CAN3_HUMAN, BRAF_HUMAN, Q9UG07_HUMAN, ELYS_HUMAN, FXR2_HUMAN, GCP4_HUMAN, UCP2_HUMAN, IMB1_HUMAN, XPO1_HUMAN, DDX3X_HUMAN, TBP_HUMAN, IGBP1_HUMAN, IRS1_HUMAN, MDHM_HUMAN, HS71A_HUMAN.HS71B_HUMAN, BCR_HUMAN, MINK1_HUMAN, CDK1_HUMAN, MVD1_HUMAN, SYUA_HUMAN, MPPB_HUMAN, TY3H_HUMAN, NXF2_HUMAN, CD11B_HUMAN, TF2B_HUMAN, CHD3_HUMAN, IKZF2_HUMAN, IKZF4_HUMAN, SIN3B_HUMAN, SIN3A_HUMAN, AGTR1_HUMAN, E41L1_HUMAN, PTMA_HUMAN, ENPL_HUMAN, NAC2_HUMAN, NAC1_HUMAN, NAC3_HUMAN, KPCG_HUMAN, ABCA1_HUMAN, RGS7_HUMAN, KIF1C_HUMAN, PARD3_HUMAN, LYST_HUMAN, TESK2_HUMAN, CY1_HUMAN, CALB1_HUMAN, IPO5_HUMAN, DAPK1_HUMAN, CTIP_HUMAN, HDAC2_HUMAN, SMCA4_HUMAN, FER_HUMAN, FSBP_HUMAN.RA54B_HUMAN, TTP_HUMAN, NUP98_HUMAN, RACK1_HUMAN, PP2AA_HUMAN, RB33B_HUMAN, UCP3_HUMAN, TAU_HUMAN, 41_HUMAN, MLXIP_HUMAN, MARK4_HUMAN, PBX3_HUMAN, FGF1_HUMAN, TMED2_HUMAN, CXAR_HUMAN, TIM44_HUMAN, GRPE2_HUMAN, RBL1_HUMAN, RBL2_HUMAN, NDUS7_HUMAN, NDUS4_HUMAN, RGRF1_HUMAN, NCOR2_HUMAN, CHD4_HUMAN, HDAC7_HUMAN, HDAC3_HUMAN, IMA5_HUMAN, IKZF5_HUMAN, TRI32_HUMAN, RAB6A_HUMAN, PRP6_HUMAN, AGTR2_HUMAN, CASP3_HUMAN, TIM14_HUMAN, G3BP1_HUMAN, RAE1L_HUMAN, TF2AA_HUMAN, TBPL1_HUMAN, ROA1_HUMAN, MDM2_HUMAN, KCC2A_HUMAN, KCC2B_HUMAN, EMD_HUMAN, SAMN1_HUMAN, EXO1_HUMAN, CAF1A_HUMAN, PML_HUMAN, H2AX_HUMAN, HAX1_HUMAN, MYC_HUMAN, NED4L_HUMAN, ICT1_HUMAN, AGO3_HUMAN, SIR1_HUMAN, SIR3_HUMAN, RHOC_HUMAN, MP2K2_HUMAN, RFWD2_HUMAN, MIC10_HUMAN, PSA3_HUMAN, DNLZ_HUMAN, BAP1_HUMAN, H31_HUMAN, PCKGC_HUMAN, RN146_HUMAN, HDGF_HUMAN, ITSN2_HUMAN, ARRB1_HUMAN, ARRB2_HUMAN, SIR7_HUMAN, SP1_HUMAN, CTNB1_HUMAN, UB2E1_HUMAN, PRKN_HUMAN, AURKB_HUMAN, AURKC_HUMAN, CK2N2_HUMAN, SHOT1_HUMAN, RT24_HUMAN, NKD2_HUMAN, PKHG5_HUMAN, PPID_HUMAN, SCLT1_HUMAN, SYUB_HUMAN, PTGR3_HUMAN, WWP1_HUMAN, TM14C_HUMAN, STX5_HUMAN, PAK6_HUMAN, TYK2_HUMAN, KPCA_HUMAN, CUL3_HUMAN, CUL4B_HUMAN, CUL2_HUMAN, CUL1_HUMAN, CSN6_HUMAN, DCNL1_HUMAN, NEDD8_HUMAN, ITB2_HUMAN, INSC_HUMAN, MDR1_HUMAN, KALRN_HUMAN, CLD17_HUMAN, GP142_HUMAN, NMDZ1_HUMAN, RHG06_HUMAN, SSR3_HUMAN, TYRO3_HUMAN, CITE1_HUMAN, ARVC_HUMAN, CTND2_HUMAN, ILF3_HUMAN, CATO_HUMAN, VRK2_HUMAN, STRN_HUMAN, ARHGG_HUMAN, PQBP1_HUMAN, BORG4_HUMAN, ORML3_HUMAN, ABR_HUMAN, NUP37_HUMAN, 5HT2B_HUMAN, PTN14_HUMAN, DNJA3_HUMAN, MEX3B_HUMAN, KI13B_HUMAN, RBBP4_HUMAN, GRK5_HUMAN, SHIP2_HUMAN, SHC1_HUMAN, CRK_HUMAN, EPS15_HUMAN, FBX6_HUMAN, NDUV1_HUMAN, NDUB4_HUMAN, NDUV3_HUMAN, NDUB9_HUMAN, NDUAC_HUMAN, NDUAA_HUMAN, NDUB5_HUMAN, NDUS6_HUMAN, SUCA_HUMAN, ATPG_HUMAN, SURF1_HUMAN, APT_HUMAN, DNJA1_HUMAN, SAM50_HUMAN, SYNE2_HUMAN, SFR15_HUMAN, NPTN_HUMAN, GHC1_HUMAN, RBM14_HUMAN, TIM50_HUMAN, SBP1_HUMAN, PYRD_HUMAN, IWS1_HUMAN, PPAL_HUMAN, LRC8A_HUMAN, BCS1_HUMAN, TOM7_HUMAN, MDHC_HUMAN, A0A087WU62_HUMAN.RM45_HUMAN, COX15_HUMAN, PREP_HUMAN, OPA1_HUMAN, NOTC2_HUMAN, ACTA_HUMAN, TMED9_HUMAN, TOM70_HUMAN, TAP1_HUMAN, TM14B_HUMAN, VAPB_HUMAN, HIG1A_HUMAN, MOGS_HUMAN, SCOT1_HUMAN, RAI3_HUMAN, THTM_HUMAN, SC24C_HUMAN, TIM9_HUMAN, RM01_HUMAN, HNRPQ_HUMAN, HNRL2_HUMAN, RAB14_HUMAN, LTOR2_HUMAN, TOM40_HUMAN, RLA0_HUMAN, RT09_HUMAN, CH10_HUMAN, NHRF1_HUMAN, MPCP_HUMAN, PSN1_HUMAN, FKBP8_HUMAN, RL27_HUMAN, ZO1_HUMAN, NDUB6_HUMAN, FUBP3_HUMAN, NDUBB_HUMAN, SEPT9_HUMAN, STX12_HUMAN, MGT4B_HUMAN, IF4A1_HUMAN, XRCC6_HUMAN, RT10_HUMAN, MARC1_HUMAN, ERGI1_HUMAN, RAB5B_HUMAN, RT05_HUMAN, RM20_HUMAN, IMPA3_HUMAN, THIL_HUMAN, SFXN1_HUMAN, MRP2_HUMAN, SSBP_HUMAN, OXA1L_HUMAN, HS902_HUMAN, GCN1_HUMAN, MPV17_HUMAN, CPSM_HUMAN, IQGA1_HUMAN, PSMD1_HUMAN, EPCR_HUMAN, GTR14_HUMAN, TM9S4_HUMAN, ATG4B_HUMAN, PCYOX_HUMAN, CPT1A_HUMAN, MIRO2_HUMAN, S27A2_HUMAN, RM13_HUMAN, EF2_HUMAN, SQSTM_HUMAN, ODPA_HUMAN, AT5F1_HUMAN, RM40_HUMAN, SVIL_HUMAN, OCAD1_HUMAN, ESR1_HUMAN, NPM_HUMAN, ECT2_HUMAN, TP53B_HUMAN, NOTC1_HUMAN, TERA_HUMAN, PKD2_HUMAN, MIPT3_HUMAN, HS90A_HUMAN, BTK_HUMAN, VCAM1_HUMAN, FINC_HUMAN, TISB_HUMAN, IQCB1_HUMAN, NOS2_HUMAN, UBL4A_HUMAN, ITA4_HUMAN, PAN2_HUMAN, YIPF3_HUMAN, HDA11_HUMAN, KCJ11_HUMAN, BAG3_HUMAN, MUC1_HUMAN, NUP93_HUMAN, EP300_HUMAN, YTDC1_HUMAN, TDG_HUMAN, LSM8_HUMAN, XRN1_HUMAN, KLC2_HUMAN, RASF2_HUMAN, ABLM1_HUMAN, ANS1A_HUMAN, ARHG2_HUMAN, CP131_HUMAN, BAIP2_HUMAN, SPE39_HUMAN, KKCC1_HUMAN, CCDC6_HUMAN, BORG5_HUMAN, CE170_HUMAN, CLAP1_HUMAN, CLAP2_HUMAN, CRTC3_HUMAN, CYFP2_HUMAN, CYLD_HUMAN, DEN1A_HUMAN, DOC11_HUMAN, GRIP1_HUMAN, C170B_HUMAN, KIF1B_HUMAN, LIMA1_HUMAN, LMO7_HUMAN, LUZP1_HUMAN, MARK1_HUMAN, MAST2_HUMAN, MTMRC_HUMAN, NAV1_HUMAN, SPN90_HUMAN, NF1_HUMAN, F262_HUMAN, PHLB2_HUMAN, P3C2A_HUMAN, PKHA7_HUMAN, LIPA1_HUMAN, 2A5D_HUMAN, PTN13_HUMAN, PUM1_HUMAN, R3HD2_HUMAN, RFIP1_HUMAN, RFIP2_HUMAN, RPGF6_HUMAN, NGAP_HUMAN, RICTR_HUMAN, SPD2A_HUMAN, SH3R1_HUMAN, SHRM3_HUMAN, MTREX_HUMAN, SRBS1_HUMAN, SRGP2_HUMAN, STAM1_HUMAN, TBCD1_HUMAN, TBCD4_HUMAN, ASPP2_HUMAN, VP33B_HUMAN, WDR62_HUMAN, NELFA_HUMAN, WNK1_HUMAN, M3K20_HUMAN, ZCHC8_HUMAN, TISD_HUMAN, ARF_HUMAN.CDN2A_HUMAN, AIP_HUMAN, CAZA1_HUMAN, CNBP_HUMAN, ECHM_HUMAN, IF4E_HUMAN, IF6_HUMAN, G3P_HUMAN, PSF3_HUMAN, AATC_HUMAN, ASSY_HUMAN, ATG3_HUMAN, IF5_HUMAN, FERM2_HUMAN, PUR4_HUMAN, TFIP8_HUMAN, VINC_HUMAN, MTAP_HUMAN, NDKB_HUMAN, PA1B2_HUMAN, PAK2_HUMAN, 6PGD_HUMAN, SERC_HUMAN, TEBP_HUMAN, SPSY_HUMAN, BCCIP_HUMAN, TKFC_HUMAN, G6PD_HUMAN, GSHB_HUMAN, LDHB_HUMAN, RRAGB_HUMAN, SGTA_HUMAN, TBB4B_HUMAN, SPKAP_HUMAN, GRSF1_HUMAN, SIK3_HUMAN, PPA6_HUMAN, ANR11_HUMAN, ARNT2_HUMAN, CPLX1_HUMAN, DGCR6_HUMAN, GPX1_HUMAN, IQCE_HUMAN, KIF1A_HUMAN, MVP_HUMAN, NDE1_HUMAN, NECD_HUMAN, SPRTN_HUMAN, CDC20_HUMAN, CP250_HUMAN, CEP57_HUMAN, HAUS2_HUMAN, NEDD1_HUMAN, TBG1_HUMAN, DDIT4_HUMAN, DTL_HUMAN, FUS_HUMAN, PARP1_HUMAN, ECHP_HUMAN, ORC1_HUMAN, SRSF2_HUMAN, RU1C_HUMAN, LATS1_HUMAN, TPX2_HUMAN, VATD_HUMAN, FXL18_HUMAN.Q96D16_HUMAN, T22D4_HUMAN, PDIP3_HUMAN, YKT6_HUMAN, DNJC4_HUMAN, KPYM_HUMAN, TPM4_HUMAN, NR1D2_HUMAN, BET1_HUMAN, ST3L1_HUMAN, MID51_HUMAN.MIDUO_HUMAN, PRP39_HUMAN, ZN471_HUMAN, CU067_HUMAN, ZF64A_HUMAN.ZF64B_HUMAN, MYG1_HUMAN.Q86UA3_HUMAN, PELI3_HUMAN, BRCA1_HUMAN, BAP18_HUMAN, CUL7_HUMAN, OBSL1_HUMAN, EED_HUMAN, RN115_HUMAN, SUMO2_HUMAN, TNK1_HUMAN, ABCE1_HUMAN, FBW1A_HUMAN, FBW1B_HUMAN, STX7_HUMAN, ZWINT_HUMAN, SGF29_HUMAN, UBXN1_HUMAN, HOGA1_HUMAN, IPYR2_HUMAN, ATF6B_HUMAN, ODPB_HUMAN, DLDH_HUMAN, RASF1_HUMAN, EPN3_HUMAN, ECSIT_HUMAN, DPB1_HUMAN, DCR1C_HUMAN, DD19A_HUMAN, NDUA8_HUMAN, KIBRA_HUMAN, KS6B2_HUMAN, MRP1_HUMAN, ACADM_HUMAN, AFG32_HUMAN, GDE_HUMAN, AHNK_HUMAN, AL1B1_HUMAN, THOC4_HUMAN, NNRE_HUMAN, AT1A1_HUMAN, AT1B1_HUMAN, RENR_HUMAN, VA0D1_HUMAN, CCD58_HUMAN, COF1_HUMAN, CISD1_HUMAN, CLH1_HUMAN, COX41_HUMAN, CX6B1_HUMAN, CPNE3_HUMAN, CYC_HUMAN, ODP2_HUMAN, DNJB1_HUMAN, DNJC3_HUMAN, DNJC8_HUMAN, DUT_HUMAN, LYAG_HUMAN, GBB2_HUMAN, GPDM_HUMAN, HNRPU_HUMAN, HCD2_HUMAN, HSP72_HUMAN, HS74L_HUMAN, HSP7C_HUMAN, EF1A1_HUMAN, HNRPL_HUMAN, RAB7A_HUMAN, SODC_HUMAN, HS105_HUMAN, NUDT9_HUMAN, 6PGL_HUMAN, ITPA_HUMAN, LDHA_HUMAN, MTCH1_HUMAN, NDUA2_HUMAN, NDUA6_HUMAN, AT1B3_HUMAN, MTCH2_HUMAN, VATE1_HUMAN, VDAC3_HUMAN, PRS7_HUMAN, ACOX1_HUMAN, MCM3_HUMAN, ODPAT_HUMAN, PHB2_HUMAN, PUR1_HUMAN, PRDX6_HUMAN, PTBP1_HUMAN, RS15_HUMAN, ACLY_HUMAN, CISY_HUMAN, GLOD4_HUMAN, METK2_HUMAN, RM48_HUMAN, RAB8A_HUMAN, UAP1_HUMAN, STMN1_HUMAN, TECR_HUMAN, TKT_HUMAN, TPIS_HUMAN, UGDH_HUMAN, ATP5J_HUMAN, ATIF1_HUMAN, CYB5B_HUMAN, GSTO1_HUMAN, NDUB8_HUMAN, OAT_HUMAN, SERA_HUMAN, VAPA_HUMAN, CNDD3_HUMAN, SLK_HUMAN, NTRK1_HUMAN, HSPB2_HUMAN, IF16_HUMAN, MK01_HUMAN, KHDR1_HUMAN, HDAC6_HUMAN, NUP85_HUMAN, NUP53_HUMAN, H2B1C_HUMAN, LCA5_HUMAN, TECT2_HUMAN, TECT3_HUMAN, CE128_HUMAN, FTM_HUMAN, TMM17_HUMAN, MKS3_HUMAN, IF4A2_HUMAN, NDUS5_HUMAN, NDUAB_HUMAN, NDUAD_HUMAN, CIA30_HUMAN, TIDC1_HUMAN, MYH13_HUMAN, SC16A_HUMAN, NEST_HUMAN, GOT1B_HUMAN, GTSE1_HUMAN, RAB5C_HUMAN, FGOP2_HUMAN, MMGT1_HUMAN, CENPJ_HUMAN, CTR9_HUMAN, TACC3_HUMAN, BCOR_HUMAN, CARF_HUMAN, NU107_HUMAN, ATM_HUMAN, JUN_HUMAN, FOXB1_HUMAN, ID2_HUMAN, FOXG1_HUMAN, GAN_HUMAN, PPARG_HUMAN, SKI_HUMAN, CRY1_HUMAN, CRY2_HUMAN, FOXS1_HUMAN, MCM2_HUMAN, MCM5_HUMAN, SPAG5_HUMAN, ASPM_HUMAN, PSMD3_HUMAN, PSD11_HUMAN, PSMD2_HUMAN, PSB5_HUMAN, MERL_HUMAN, UBX2A_HUMAN, OTUB1_HUMAN, ERR2_HUMAN, NANOG_HUMAN, PO5F1_HUMAN, COQ9_HUMAN, NDUA4_HUMAN, NDUF4_HUMAN, COQ3_HUMAN, MPPA_HUMAN, CISD3_HUMAN, NMES1_HUMAN, DDAH1_HUMAN, PTPM1_HUMAN, NDUF8_HUMAN, ODBA_HUMAN, SCOT2_HUMAN, SDHF3_HUMAN, U2AF2_HUMAN, NFAC2_HUMAN, NFAC1_HUMAN, ERRFI_HUMAN, AIFM1_HUMAN, CADH1_HUMAN, DS13A_HUMAN.DS13B_HUMAN, DUS16_HUMAN, DUS4_HUMAN, DUS9_HUMAN, MTMR4_HUMAN, SDHF4_HUMAN, SAPC2_HUMAN, RB6I2_HUMAN, DLP1_HUMAN, NECA3_HUMAN, DPS1_HUMAN, KIF11_HUMAN, ACBD5_HUMAN, PDP1_HUMAN, POC1A_HUMAN, CSR2B_HUMAN, YETS2_HUMAN, SPICE_HUMAN, TOP3A_HUMAN, FLCN_HUMAN, TRI11_HUMAN, D2HDH_HUMAN, ACAD9_HUMAN, APBP2_HUMAN, SPT13_HUMAN, MBIP1_HUMAN, KLDC3_HUMAN, PFD4_HUMAN, ACD11_HUMAN, MAVS_HUMAN, PCGF2_HUMAN, RAN_HUMAN, MTA3_HUMAN, GOGA4_HUMAN, SSX2_HUMAN, PDPR_HUMAN, DPOG1_HUMAN, MMAD_HUMAN, A0A0J9YY34_HUMAN.NHSL2_HUMAN, PPCEL_HUMAN, DHB4_HUMAN, ENPP6_HUMAN, WDR26_HUMAN, P66A_HUMAN, MKLN1_HUMAN, ASAP3_HUMAN, CKAP5_HUMAN, ACSF3_HUMAN, RSAD1_HUMAN, TFEB_HUMAN, HXC9_HUMAN, BPNT1_HUMAN, RBP10_HUMAN, MTA2_HUMAN, GALC_HUMAN, NPS3A_HUMAN, DC1L1_HUMAN, SYLM_HUMAN, PTN4_HUMAN, DNM1L_HUMAN, PARK7_HUMAN, SC22B_HUMAN, ML12A_HUMAN.ML12B_HUMAN, BAF_HUMAN, KCRB_HUMAN, RL30_HUMAN, HNRH3_HUMAN, H2A1D_HUMAN, TCPB_HUMAN, TCPQ_HUMAN, RL26_HUMAN, EF1G_HUMAN, ADT2_HUMAN, RPN2_HUMAN, ATP5H_HUMAN, RL12_HUMAN, LDH6A_HUMAN, PDIA3_HUMAN, PRAF3_HUMAN, PMVK_HUMAN, RAB10_HUMAN, CKAP4_HUMAN, SERPH_HUMAN, TMEDA_HUMAN, PDIA6_HUMAN, RAB21_HUMAN, EF1B_HUMAN, GANAB_HUMAN, TM109_HUMAN, GLYM_HUMAN, PGAM1_HUMAN, PRDX3_HUMAN, TCPH_HUMAN, EMC2_HUMAN, IF2A_HUMAN, APEX1_HUMAN, ELAV1_HUMAN, LMNA_HUMAN, NFIP2_HUMAN, DJB11_HUMAN, 1B07_HUMAN.1B08_HUMAN.1B13_HUMAN.1B14_HUMAN.1B15_HUMAN.1B18_HUMAN.1B27_HUMAN.1B35_HUMAN.1B37_HUMAN.1B38_HUMAN.1B39_HUMAN.1B40_HUMAN.1B41_HUMAN.1B42_HUMAN.1B44_HUMAN.1B45_HUMAN.1B46_HUMAN.1B47_HUMAN.1B48_HUMAN.1B49_HUMAN.1B50_HUMAN.1B51_HUMAN.1B52_HUMAN.1B53_HUMAN.1B54_HUMAN.1B55_HUMAN.1B56_HUMAN.1B57_HUMAN.1B58_HUMAN.1B59_HUMAN.1B67_HUMAN.1B73_HUMAN.1B78_HUMAN.1B81_HUMAN.1B82_HUMAN, 1A01_HUMAN.1A02_HUMAN.1A03_HUMAN.1A11_HUMAN.1A23_HUMAN.1A24_HUMAN.1A25_HUMAN.1A26_HUMAN.1A29_HUMAN.1A30_HUMAN.1A31_HUMAN.1A32_HUMAN.1A33_HUMAN.1A34_HUMAN.1A36_HUMAN.1A43_HUMAN.1A66_HUMAN.1A68_HUMAN.1A69_HUMAN.1A74_HUMAN.1A80_HUMAN, IDH3A_HUMAN, PLAK_HUMAN, PRS8_HUMAN, PAIRB_HUMAN, PERI_HUMAN, NAMPT_HUMAN, SYDC_HUMAN, SYFA_HUMAN, ASNS_HUMAN, LMNB1_HUMAN, RPN1_HUMAN, SSRP1_HUMAN, DESP_HUMAN, DDX1_HUMAN, NEC1_HUMAN, DGKG_HUMAN, MCM6_HUMAN, SYAM_HUMAN, TPR_HUMAN, SMC3_HUMAN, COPA_HUMAN, VIGLN_HUMAN, H2A1B_HUMAN, H2B1C_HUMAN.H2B1D_HUMAN, FOXA1_HUMAN, IDHC_HUMAN, SNF5_HUMAN, WT1_HUMAN, MTF1_HUMAN, RMP_HUMAN, MK08_HUMAN, BRD1_HUMAN, FOXP1_HUMAN, ATX3_HUMAN, USP9X_HUMAN, SYIC_HUMAN, KIF14_HUMAN, PEX1_HUMAN, RL4_HUMAN, NUMBL_HUMAN, PLEK_HUMAN, PP1A_HUMAN, AP2A1_HUMAN, SYLC_HUMAN, RS27L_HUMAN, ERC2_HUMAN, KC1D_HUMAN, PEX6_HUMAN, FBX11_HUMAN, ELOC_HUMAN, SPEB_HUMAN, RM04_HUMAN, LMAN2_HUMAN, EIF3H_HUMAN, MYH9_HUMAN, DLRB1_HUMAN, RL36L_HUMAN, ZKSC8_HUMAN, SPB3_HUMAN, DZIP3_HUMAN, FLOT2_HUMAN, GRWD1_HUMAN, PIGR_HUMAN, CTRO_HUMAN, SYMC_HUMAN, SMC4_HUMAN, ELP1_HUMAN, TMED5_HUMAN, TMED4_HUMAN, SYGP1_HUMAN, CFTR_HUMAN, CPEB2_HUMAN, FBX7_HUMAN, DPOD1_HUMAN, TXTP_HUMAN, Q9H4D1_HUMAN.RIPK4_HUMAN, LAP2A_HUMAN.LAP2B_HUMAN, PPM1D_HUMAN, PP1G_HUMAN, PPP5_HUMAN, PPTC7_HUMAN, MED9_HUMAN, PCBP1_HUMAN, TGFB1_HUMAN, ACON_HUMAN, PURA2_HUMAN, API5_HUMAN, BMR1A_HUMAN, CDK9_HUMAN, CRYL1_HUMAN, KC1A_HUMAN, GSK3A_HUMAN, RASK_HUMAN, MP2K3_HUMAN, PPIE_HUMAN, TRIP4_HUMAN, YAF2_HUMAN, PRP8_HUMAN, PIHD1_HUMAN, TNIP2_HUMAN, NKX21_HUMAN, RARA_HUMAN, RXRA_HUMAN, RARB_HUMAN, DGUOK_HUMAN, FIBA_HUMAN, RNF6_HUMAN, MEOX2_HUMAN, PR20A_HUMAN.PR20B_HUMAN.PR20C_HUMAN.PR20D_HUMAN.PR20E_HUMAN, HNRLL_HUMAN, UB2R1_HUMAN, CHIP_HUMAN, DISC1_HUMAN, NDUA7_HUMAN, NU155_HUMAN, NU205_HUMAN, QCR10_HUMAN, MYPT1_HUMAN, CBR1_HUMAN, MTP_HUMAN, TBA1A_HUMAN, RIP_HUMAN, MED19_HUMAN, M4K4_HUMAN, NAA10_HUMAN, OCTC_HUMAN, TAOK1_HUMAN, PRI1_HUMAN, SYF1_HUMAN, HSPB8_HUMAN</t>
   </si>
   <si>
     <t xml:space="preserve">Q2M2I8</t>
@@ -461,82 +551,256 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="n">
+        <v>0.00584795321637427</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" t="n">
-        <v>0.00199828718241507</v>
+        <v>0.00138127906441365</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="n">
+        <v>0.00220264317180617</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" t="n">
-        <v>0.00119018447859418</v>
+        <v>0.00130568356374808</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="n">
+        <v>0.00179533213644524</v>
+      </c>
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="n">
+        <v>0.00131752305665349</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="n">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.00199828718241507</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.00148872820076563</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.00144374548829535</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.00135547272111149</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.00119018447859418</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed Archive package Working Form Correct Output
</commit_message>
<xml_diff>
--- a/Project_Output/POIs_sorted.xlsx
+++ b/Project_Output/POIs_sorted.xlsx
@@ -476,7 +476,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -521,7 +521,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0150975810802536</v>
+        <v>0.015099929233531</v>
       </c>
     </row>
     <row r="3">
@@ -535,7 +535,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0526315789473684</v>
+        <v>0.0540540540540541</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -544,7 +544,7 @@
         <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>6.09422906604821</v>
+        <v>5.90806584989691</v>
       </c>
     </row>
     <row r="4">
@@ -558,7 +558,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05</v>
+        <v>0.0526315789473684</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -567,7 +567,7 @@
         <v>18</v>
       </c>
       <c r="G4" t="n">
-        <v>2.90489511964124</v>
+        <v>2.81192265581059</v>
       </c>
     </row>
     <row r="5">
@@ -581,7 +581,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0465116279069767</v>
+        <v>0.0476190476190476</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -590,7 +590,7 @@
         <v>21</v>
       </c>
       <c r="G5" t="n">
-        <v>3.30671353906589</v>
+        <v>3.20813890652545</v>
       </c>
     </row>
     <row r="6">
@@ -613,7 +613,7 @@
         <v>26</v>
       </c>
       <c r="G6" t="n">
-        <v>3.02365118426608</v>
+        <v>2.9381759817832</v>
       </c>
     </row>
     <row r="7">
@@ -636,7 +636,7 @@
         <v>31</v>
       </c>
       <c r="G7" t="n">
-        <v>2.31334502757633</v>
+        <v>2.26966306455418</v>
       </c>
     </row>
     <row r="8">
@@ -659,7 +659,7 @@
         <v>34</v>
       </c>
       <c r="G8" t="n">
-        <v>2.27543123935373</v>
+        <v>2.23384916725504</v>
       </c>
     </row>
     <row r="9">
@@ -682,7 +682,7 @@
         <v>37</v>
       </c>
       <c r="G9" t="n">
-        <v>1.37959306612601</v>
+        <v>1.36020209880448</v>
       </c>
     </row>
     <row r="10">
@@ -705,7 +705,7 @@
         <v>41</v>
       </c>
       <c r="G10" t="n">
-        <v>0.340125586489395</v>
+        <v>0.332138464774045</v>
       </c>
     </row>
     <row r="11">
@@ -728,7 +728,7 @@
         <v>44</v>
       </c>
       <c r="G11" t="n">
-        <v>0.308935676622387</v>
+        <v>0.308404536242237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>